<commit_message>
Changes associated with bulldoze
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716" firstSheet="12" activeTab="22"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716" firstSheet="12" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Skills" sheetId="1" r:id="rId1"/>
@@ -700,7 +700,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="702">
   <si>
     <t>Fishing</t>
   </si>
@@ -2797,6 +2797,15 @@
   </si>
   <si>
     <t>Jump on to target unoccupied tile, ignores spear wall</t>
+  </si>
+  <si>
+    <t>Hazer</t>
+  </si>
+  <si>
+    <t>Orc, 3</t>
+  </si>
+  <si>
+    <t>Hitting a taunted target causes a HoT for 15% of dmg done over 5 turns</t>
   </si>
 </sst>
 </file>
@@ -6734,10 +6743,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7629,6 +7638,20 @@
       </c>
       <c r="G83" t="s">
         <v>689</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>699</v>
+      </c>
+      <c r="B84" t="s">
+        <v>700</v>
+      </c>
+      <c r="G84" t="s">
+        <v>701</v>
+      </c>
+      <c r="H84">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -7646,7 +7669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding stun, charge, and fixes
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716" firstSheet="12" activeTab="21"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716" firstSheet="12" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Skills" sheetId="1" r:id="rId1"/>
@@ -2840,7 +2840,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2862,6 +2862,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3097,7 +3103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3203,6 +3209,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6745,7 +6754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
@@ -7669,8 +7678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8439,7 +8448,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="39" t="s">
         <v>693</v>
       </c>
       <c r="B40" s="37" t="s">

</xml_diff>

<commit_message>
Cleaning up icons for weapons
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -701,7 +701,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1969" uniqueCount="947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1973" uniqueCount="949">
   <si>
     <t>Fishing</t>
   </si>
@@ -3277,9 +3277,6 @@
     <t>Finish Trollish</t>
   </si>
   <si>
-    <t>Lash</t>
-  </si>
-  <si>
     <t>Weapon Abilities</t>
   </si>
   <si>
@@ -3542,6 +3539,15 @@
   </si>
   <si>
     <t>Bottlenecks</t>
+  </si>
+  <si>
+    <t>Shield Bash</t>
+  </si>
+  <si>
+    <t>Pull</t>
+  </si>
+  <si>
+    <t>Poke</t>
   </si>
 </sst>
 </file>
@@ -4721,24 +4727,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4758,6 +4746,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5109,10 +5115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C154"/>
+  <dimension ref="A1:C158"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5127,29 +5133,29 @@
       <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="138" t="s">
+      <c r="A2" s="132" t="s">
         <v>847</v>
       </c>
-      <c r="B2" s="139"/>
-      <c r="C2" s="140"/>
+      <c r="B2" s="133"/>
+      <c r="C2" s="134"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="116">
         <v>1</v>
       </c>
-      <c r="B3" s="141" t="s">
+      <c r="B3" s="135" t="s">
         <v>848</v>
       </c>
-      <c r="C3" s="142"/>
+      <c r="C3" s="136"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="117">
         <v>2</v>
       </c>
-      <c r="B4" s="132" t="s">
+      <c r="B4" s="139" t="s">
         <v>849</v>
       </c>
-      <c r="C4" s="133"/>
+      <c r="C4" s="140"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="117"/>
@@ -5172,7 +5178,7 @@
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="117"/>
       <c r="B7" s="121" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C7" s="122" t="s">
         <v>112</v>
@@ -5182,54 +5188,54 @@
       <c r="A8" s="117">
         <v>3</v>
       </c>
-      <c r="B8" s="134" t="s">
+      <c r="B8" s="141" t="s">
         <v>850</v>
       </c>
-      <c r="C8" s="135"/>
+      <c r="C8" s="142"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="117">
         <v>4</v>
       </c>
-      <c r="B9" s="136" t="s">
+      <c r="B9" s="143" t="s">
         <v>851</v>
       </c>
-      <c r="C9" s="137"/>
+      <c r="C9" s="144"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="117">
         <v>5</v>
       </c>
-      <c r="B10" s="136" t="s">
+      <c r="B10" s="143" t="s">
         <v>852</v>
       </c>
-      <c r="C10" s="137"/>
+      <c r="C10" s="144"/>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="118">
         <v>6</v>
       </c>
-      <c r="B11" s="143" t="s">
+      <c r="B11" s="137" t="s">
         <v>857</v>
       </c>
-      <c r="C11" s="144"/>
+      <c r="C11" s="138"/>
     </row>
     <row r="12" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="138" t="s">
+      <c r="A13" s="132" t="s">
         <v>208</v>
       </c>
-      <c r="B13" s="139"/>
-      <c r="C13" s="140"/>
+      <c r="B13" s="133"/>
+      <c r="C13" s="134"/>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="116">
         <v>1</v>
       </c>
-      <c r="B14" s="141" t="s">
-        <v>859</v>
-      </c>
-      <c r="C14" s="142"/>
+      <c r="B14" s="135" t="s">
+        <v>858</v>
+      </c>
+      <c r="C14" s="136"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="117"/>
@@ -5237,7 +5243,7 @@
         <v>853</v>
       </c>
       <c r="C15" s="120" t="s">
-        <v>858</v>
+        <v>946</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5246,22 +5252,22 @@
         <v>854</v>
       </c>
       <c r="C16" s="126" t="s">
-        <v>63</v>
+        <v>695</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="117"/>
       <c r="B17" s="125" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C17" s="126" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="117"/>
       <c r="B18" s="125" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C18" s="126" t="s">
         <v>735</v>
@@ -5269,1082 +5275,1158 @@
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="117"/>
-      <c r="B19" s="121" t="s">
-        <v>865</v>
-      </c>
-      <c r="C19" s="122" t="s">
+      <c r="B19" s="128" t="s">
+        <v>864</v>
+      </c>
+      <c r="C19" s="129" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="117"/>
+      <c r="B20" s="128" t="s">
+        <v>895</v>
+      </c>
+      <c r="C20" s="129" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="117"/>
+      <c r="B21" s="128" t="s">
+        <v>897</v>
+      </c>
+      <c r="C21" s="129" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="117"/>
+      <c r="B22" s="128" t="s">
+        <v>899</v>
+      </c>
+      <c r="C22" s="129" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="117"/>
+      <c r="B23" s="121" t="s">
+        <v>900</v>
+      </c>
+      <c r="C23" s="122" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="132" t="s">
         <v>861</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="138" t="s">
+      <c r="B25" s="133"/>
+      <c r="C25" s="134"/>
+    </row>
+    <row r="26" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="116">
+        <v>1</v>
+      </c>
+      <c r="B26" s="135" t="s">
+        <v>847</v>
+      </c>
+      <c r="C26" s="136"/>
+    </row>
+    <row r="27" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="117"/>
+      <c r="B27" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C27" s="120" t="s">
         <v>862</v>
       </c>
-      <c r="B21" s="139"/>
-      <c r="C21" s="140"/>
-    </row>
-    <row r="22" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="116">
-        <v>1</v>
-      </c>
-      <c r="B22" s="141" t="s">
-        <v>847</v>
-      </c>
-      <c r="C22" s="142"/>
-    </row>
-    <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="117"/>
-      <c r="B23" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C23" s="120" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="117"/>
-      <c r="B24" s="125" t="s">
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="117"/>
+      <c r="B28" s="125" t="s">
         <v>854</v>
       </c>
-      <c r="C24" s="126" t="s">
+      <c r="C28" s="126" t="s">
         <v>856</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="117"/>
-      <c r="B25" s="125" t="s">
-        <v>860</v>
-      </c>
-      <c r="C25" s="126" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="117"/>
-      <c r="B26" s="121" t="s">
-        <v>864</v>
-      </c>
-      <c r="C26" s="122" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="117">
-        <v>2</v>
-      </c>
-      <c r="B27" s="132" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="133"/>
-    </row>
-    <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="117"/>
-      <c r="B28" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C28" s="120" t="s">
-        <v>869</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="117"/>
-      <c r="B29" s="121"/>
-      <c r="C29" s="122"/>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="B29" s="125" t="s">
+        <v>859</v>
+      </c>
+      <c r="C29" s="126" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="117"/>
+      <c r="B30" s="121" t="s">
+        <v>863</v>
+      </c>
+      <c r="C30" s="122" t="s">
+        <v>867</v>
+      </c>
+    </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="138" t="s">
+      <c r="A31" s="117">
+        <v>2</v>
+      </c>
+      <c r="B31" s="139" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="140"/>
+    </row>
+    <row r="32" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="117"/>
+      <c r="B32" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C32" s="120" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="117"/>
+      <c r="B33" s="121"/>
+      <c r="C33" s="122"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="132" t="s">
+        <v>869</v>
+      </c>
+      <c r="B35" s="133"/>
+      <c r="C35" s="134"/>
+    </row>
+    <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="116">
+        <v>1</v>
+      </c>
+      <c r="B36" s="135" t="s">
         <v>870</v>
       </c>
-      <c r="B31" s="139"/>
-      <c r="C31" s="140"/>
-    </row>
-    <row r="32" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="116">
-        <v>1</v>
-      </c>
-      <c r="B32" s="141" t="s">
+      <c r="C36" s="136"/>
+    </row>
+    <row r="37" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="117"/>
+      <c r="B37" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C37" s="120" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="117"/>
+      <c r="B38" s="125" t="s">
+        <v>854</v>
+      </c>
+      <c r="C38" s="126" t="s">
         <v>871</v>
       </c>
-      <c r="C32" s="142"/>
-    </row>
-    <row r="33" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="117"/>
-      <c r="B33" s="119" t="s">
+    </row>
+    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="117"/>
+      <c r="B39" s="125" t="s">
+        <v>859</v>
+      </c>
+      <c r="C39" s="126" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="117"/>
+      <c r="B40" s="121" t="s">
+        <v>863</v>
+      </c>
+      <c r="C40" s="122" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="132" t="s">
+        <v>874</v>
+      </c>
+      <c r="B42" s="133"/>
+      <c r="C42" s="134"/>
+    </row>
+    <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="116">
+        <v>1</v>
+      </c>
+      <c r="B43" s="135" t="s">
+        <v>875</v>
+      </c>
+      <c r="C43" s="136"/>
+    </row>
+    <row r="44" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="117"/>
+      <c r="B44" s="119" t="s">
         <v>853</v>
       </c>
-      <c r="C33" s="120" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="117"/>
-      <c r="B34" s="125" t="s">
+      <c r="C44" s="120" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="127"/>
+      <c r="B45" s="121" t="s">
         <v>854</v>
       </c>
-      <c r="C34" s="126" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="117"/>
-      <c r="B35" s="125" t="s">
-        <v>860</v>
-      </c>
-      <c r="C35" s="126" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="117"/>
-      <c r="B36" s="121" t="s">
-        <v>864</v>
-      </c>
-      <c r="C36" s="122" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="138" t="s">
-        <v>875</v>
-      </c>
-      <c r="B38" s="139"/>
-      <c r="C38" s="140"/>
-    </row>
-    <row r="39" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="116">
-        <v>1</v>
-      </c>
-      <c r="B39" s="141" t="s">
-        <v>876</v>
-      </c>
-      <c r="C39" s="142"/>
-    </row>
-    <row r="40" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="117"/>
-      <c r="B40" s="119" t="s">
+      <c r="C45" s="122" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="116">
+        <v>1</v>
+      </c>
+      <c r="B46" s="135" t="s">
+        <v>877</v>
+      </c>
+      <c r="C46" s="136"/>
+    </row>
+    <row r="47" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="117"/>
+      <c r="B47" s="119" t="s">
         <v>853</v>
       </c>
-      <c r="C40" s="120" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="127"/>
-      <c r="B41" s="121" t="s">
+      <c r="C47" s="120" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="117"/>
+      <c r="B48" s="125" t="s">
         <v>854</v>
       </c>
-      <c r="C41" s="122" t="s">
+      <c r="C48" s="126" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="117"/>
+      <c r="B49" s="125" t="s">
+        <v>859</v>
+      </c>
+      <c r="C49" s="126" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="117"/>
+      <c r="B50" s="121"/>
+      <c r="C50" s="122"/>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="132" t="s">
+        <v>213</v>
+      </c>
+      <c r="B52" s="133"/>
+      <c r="C52" s="134"/>
+    </row>
+    <row r="53" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="116">
+        <v>1</v>
+      </c>
+      <c r="B53" s="135" t="s">
         <v>882</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="116">
-        <v>1</v>
-      </c>
-      <c r="B42" s="141" t="s">
-        <v>878</v>
-      </c>
-      <c r="C42" s="142"/>
-    </row>
-    <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="117"/>
-      <c r="B43" s="119" t="s">
+      <c r="C53" s="136"/>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="132" t="s">
+        <v>855</v>
+      </c>
+      <c r="B55" s="133"/>
+      <c r="C55" s="134"/>
+    </row>
+    <row r="56" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="116">
+        <v>1</v>
+      </c>
+      <c r="B56" s="141" t="s">
+        <v>848</v>
+      </c>
+      <c r="C56" s="142"/>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="117">
+        <v>2</v>
+      </c>
+      <c r="B57" s="145" t="s">
+        <v>849</v>
+      </c>
+      <c r="C57" s="146"/>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="117">
+        <v>3</v>
+      </c>
+      <c r="B58" s="143" t="s">
+        <v>850</v>
+      </c>
+      <c r="C58" s="144"/>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="117">
+        <v>4</v>
+      </c>
+      <c r="B59" s="143" t="s">
+        <v>851</v>
+      </c>
+      <c r="C59" s="144"/>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="117">
+        <v>5</v>
+      </c>
+      <c r="B60" s="143" t="s">
+        <v>852</v>
+      </c>
+      <c r="C60" s="144"/>
+    </row>
+    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="118">
+        <v>6</v>
+      </c>
+      <c r="B61" s="137" t="s">
+        <v>857</v>
+      </c>
+      <c r="C61" s="138"/>
+    </row>
+    <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="132" t="s">
+        <v>883</v>
+      </c>
+      <c r="B63" s="133"/>
+      <c r="C63" s="134"/>
+    </row>
+    <row r="64" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="116">
+        <v>1</v>
+      </c>
+      <c r="B64" s="141" t="s">
+        <v>848</v>
+      </c>
+      <c r="C64" s="142"/>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="117">
+        <v>2</v>
+      </c>
+      <c r="B65" s="145" t="s">
+        <v>849</v>
+      </c>
+      <c r="C65" s="146"/>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="117">
+        <v>3</v>
+      </c>
+      <c r="B66" s="143" t="s">
+        <v>850</v>
+      </c>
+      <c r="C66" s="144"/>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="117">
+        <v>4</v>
+      </c>
+      <c r="B67" s="143" t="s">
+        <v>851</v>
+      </c>
+      <c r="C67" s="144"/>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="117">
+        <v>5</v>
+      </c>
+      <c r="B68" s="143" t="s">
+        <v>852</v>
+      </c>
+      <c r="C68" s="144"/>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="118">
+        <v>6</v>
+      </c>
+      <c r="B69" s="137" t="s">
+        <v>857</v>
+      </c>
+      <c r="C69" s="138"/>
+    </row>
+    <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="132" t="s">
+        <v>884</v>
+      </c>
+      <c r="B71" s="133"/>
+      <c r="C71" s="134"/>
+    </row>
+    <row r="72" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="116">
+        <v>1</v>
+      </c>
+      <c r="B72" s="141" t="s">
+        <v>848</v>
+      </c>
+      <c r="C72" s="142"/>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="117">
+        <v>2</v>
+      </c>
+      <c r="B73" s="145" t="s">
+        <v>849</v>
+      </c>
+      <c r="C73" s="146"/>
+    </row>
+    <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="117">
+        <v>3</v>
+      </c>
+      <c r="B74" s="143" t="s">
+        <v>850</v>
+      </c>
+      <c r="C74" s="144"/>
+    </row>
+    <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="117">
+        <v>4</v>
+      </c>
+      <c r="B75" s="143" t="s">
+        <v>851</v>
+      </c>
+      <c r="C75" s="144"/>
+    </row>
+    <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="117">
+        <v>5</v>
+      </c>
+      <c r="B76" s="143" t="s">
+        <v>852</v>
+      </c>
+      <c r="C76" s="144"/>
+    </row>
+    <row r="77" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="118">
+        <v>6</v>
+      </c>
+      <c r="B77" s="137" t="s">
+        <v>857</v>
+      </c>
+      <c r="C77" s="138"/>
+    </row>
+    <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="132" t="s">
+        <v>934</v>
+      </c>
+      <c r="B79" s="133"/>
+      <c r="C79" s="134"/>
+    </row>
+    <row r="80" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="116">
+        <v>1</v>
+      </c>
+      <c r="B80" s="135" t="s">
+        <v>102</v>
+      </c>
+      <c r="C80" s="136"/>
+    </row>
+    <row r="81" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="127"/>
+      <c r="B81" s="119" t="s">
         <v>853</v>
       </c>
-      <c r="C43" s="120" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="117"/>
-      <c r="B44" s="125" t="s">
-        <v>854</v>
-      </c>
-      <c r="C44" s="126" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="117"/>
-      <c r="B45" s="125" t="s">
-        <v>860</v>
-      </c>
-      <c r="C45" s="126" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="117"/>
-      <c r="B46" s="121"/>
-      <c r="C46" s="122"/>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="138" t="s">
-        <v>213</v>
-      </c>
-      <c r="B48" s="139"/>
-      <c r="C48" s="140"/>
-    </row>
-    <row r="49" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="116">
-        <v>1</v>
-      </c>
-      <c r="B49" s="141" t="s">
-        <v>883</v>
-      </c>
-      <c r="C49" s="142"/>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="138" t="s">
-        <v>855</v>
-      </c>
-      <c r="B51" s="139"/>
-      <c r="C51" s="140"/>
-    </row>
-    <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="116">
-        <v>1</v>
-      </c>
-      <c r="B52" s="134" t="s">
-        <v>848</v>
-      </c>
-      <c r="C52" s="135"/>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="117">
-        <v>2</v>
-      </c>
-      <c r="B53" s="145" t="s">
-        <v>849</v>
-      </c>
-      <c r="C53" s="146"/>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="117">
-        <v>3</v>
-      </c>
-      <c r="B54" s="136" t="s">
-        <v>850</v>
-      </c>
-      <c r="C54" s="137"/>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="117">
-        <v>4</v>
-      </c>
-      <c r="B55" s="136" t="s">
-        <v>851</v>
-      </c>
-      <c r="C55" s="137"/>
-    </row>
-    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="117">
-        <v>5</v>
-      </c>
-      <c r="B56" s="136" t="s">
-        <v>852</v>
-      </c>
-      <c r="C56" s="137"/>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="118">
-        <v>6</v>
-      </c>
-      <c r="B57" s="143" t="s">
-        <v>857</v>
-      </c>
-      <c r="C57" s="144"/>
-    </row>
-    <row r="58" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="138" t="s">
-        <v>884</v>
-      </c>
-      <c r="B59" s="139"/>
-      <c r="C59" s="140"/>
-    </row>
-    <row r="60" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="116">
-        <v>1</v>
-      </c>
-      <c r="B60" s="134" t="s">
-        <v>848</v>
-      </c>
-      <c r="C60" s="135"/>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="117">
-        <v>2</v>
-      </c>
-      <c r="B61" s="145" t="s">
-        <v>849</v>
-      </c>
-      <c r="C61" s="146"/>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="117">
-        <v>3</v>
-      </c>
-      <c r="B62" s="136" t="s">
-        <v>850</v>
-      </c>
-      <c r="C62" s="137"/>
-    </row>
-    <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="117">
-        <v>4</v>
-      </c>
-      <c r="B63" s="136" t="s">
-        <v>851</v>
-      </c>
-      <c r="C63" s="137"/>
-    </row>
-    <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="117">
-        <v>5</v>
-      </c>
-      <c r="B64" s="136" t="s">
-        <v>852</v>
-      </c>
-      <c r="C64" s="137"/>
-    </row>
-    <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="118">
-        <v>6</v>
-      </c>
-      <c r="B65" s="143" t="s">
-        <v>857</v>
-      </c>
-      <c r="C65" s="144"/>
-    </row>
-    <row r="66" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="138" t="s">
-        <v>885</v>
-      </c>
-      <c r="B67" s="139"/>
-      <c r="C67" s="140"/>
-    </row>
-    <row r="68" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="116">
-        <v>1</v>
-      </c>
-      <c r="B68" s="134" t="s">
-        <v>848</v>
-      </c>
-      <c r="C68" s="135"/>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="117">
-        <v>2</v>
-      </c>
-      <c r="B69" s="145" t="s">
-        <v>849</v>
-      </c>
-      <c r="C69" s="146"/>
-    </row>
-    <row r="70" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="117">
-        <v>3</v>
-      </c>
-      <c r="B70" s="136" t="s">
-        <v>850</v>
-      </c>
-      <c r="C70" s="137"/>
-    </row>
-    <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="117">
-        <v>4</v>
-      </c>
-      <c r="B71" s="136" t="s">
-        <v>851</v>
-      </c>
-      <c r="C71" s="137"/>
-    </row>
-    <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="117">
-        <v>5</v>
-      </c>
-      <c r="B72" s="136" t="s">
-        <v>852</v>
-      </c>
-      <c r="C72" s="137"/>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="118">
-        <v>6</v>
-      </c>
-      <c r="B73" s="143" t="s">
-        <v>857</v>
-      </c>
-      <c r="C73" s="144"/>
-    </row>
-    <row r="74" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="138" t="s">
-        <v>935</v>
-      </c>
-      <c r="B75" s="139"/>
-      <c r="C75" s="140"/>
-    </row>
-    <row r="76" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="116">
-        <v>1</v>
-      </c>
-      <c r="B76" s="141" t="s">
-        <v>102</v>
-      </c>
-      <c r="C76" s="142"/>
-    </row>
-    <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="127"/>
-      <c r="B77" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C77" s="120" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="127"/>
-      <c r="B78" s="130" t="s">
-        <v>854</v>
-      </c>
-      <c r="C78" s="131" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="127"/>
-      <c r="B79" s="130" t="s">
-        <v>860</v>
-      </c>
-      <c r="C79" s="131" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="127"/>
-      <c r="B80" s="130" t="s">
-        <v>864</v>
-      </c>
-      <c r="C80" s="131" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="127"/>
-      <c r="B81" s="130" t="s">
-        <v>865</v>
-      </c>
-      <c r="C81" s="131" t="s">
-        <v>916</v>
+      <c r="C81" s="120" t="s">
+        <v>911</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="127"/>
       <c r="B82" s="130" t="s">
-        <v>896</v>
+        <v>854</v>
       </c>
       <c r="C82" s="131" t="s">
-        <v>917</v>
+        <v>912</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="127"/>
       <c r="B83" s="130" t="s">
-        <v>898</v>
+        <v>859</v>
       </c>
       <c r="C83" s="131" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="127"/>
       <c r="B84" s="130" t="s">
-        <v>900</v>
+        <v>863</v>
       </c>
       <c r="C84" s="131" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="127"/>
       <c r="B85" s="130" t="s">
-        <v>901</v>
+        <v>864</v>
       </c>
       <c r="C85" s="131" t="s">
-        <v>920</v>
+        <v>915</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="117"/>
-      <c r="B86" s="125" t="s">
-        <v>902</v>
-      </c>
-      <c r="C86" s="126" t="s">
-        <v>921</v>
+      <c r="A86" s="127"/>
+      <c r="B86" s="130" t="s">
+        <v>895</v>
+      </c>
+      <c r="C86" s="131" t="s">
+        <v>916</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="117"/>
-      <c r="B87" s="125" t="s">
-        <v>903</v>
-      </c>
-      <c r="C87" s="126" t="s">
-        <v>922</v>
+      <c r="A87" s="127"/>
+      <c r="B87" s="130" t="s">
+        <v>897</v>
+      </c>
+      <c r="C87" s="131" t="s">
+        <v>917</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="117"/>
-      <c r="B88" s="125" t="s">
-        <v>904</v>
-      </c>
-      <c r="C88" s="126" t="s">
-        <v>923</v>
+      <c r="A88" s="127"/>
+      <c r="B88" s="130" t="s">
+        <v>899</v>
+      </c>
+      <c r="C88" s="131" t="s">
+        <v>918</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="117"/>
-      <c r="B89" s="125" t="s">
-        <v>905</v>
-      </c>
-      <c r="C89" s="126" t="s">
-        <v>924</v>
+      <c r="A89" s="127"/>
+      <c r="B89" s="130" t="s">
+        <v>900</v>
+      </c>
+      <c r="C89" s="131" t="s">
+        <v>919</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="117"/>
       <c r="B90" s="125" t="s">
-        <v>906</v>
+        <v>901</v>
       </c>
       <c r="C90" s="126" t="s">
-        <v>925</v>
+        <v>920</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="117"/>
       <c r="B91" s="125" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="C91" s="126" t="s">
-        <v>926</v>
+        <v>921</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="117"/>
       <c r="B92" s="125" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
       <c r="C92" s="126" t="s">
-        <v>35</v>
+        <v>922</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="117"/>
       <c r="B93" s="125" t="s">
-        <v>909</v>
+        <v>904</v>
       </c>
       <c r="C93" s="126" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="117"/>
       <c r="B94" s="125" t="s">
-        <v>910</v>
-      </c>
-      <c r="C94" s="126"/>
+        <v>905</v>
+      </c>
+      <c r="C94" s="126" t="s">
+        <v>924</v>
+      </c>
     </row>
     <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="117"/>
-      <c r="B95" s="121" t="s">
-        <v>911</v>
-      </c>
-      <c r="C95" s="122"/>
-    </row>
-    <row r="96" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="117">
-        <v>2</v>
-      </c>
-      <c r="B96" s="132" t="s">
-        <v>886</v>
-      </c>
-      <c r="C96" s="133"/>
-    </row>
-    <row r="97" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="125" t="s">
+        <v>906</v>
+      </c>
+      <c r="C95" s="126" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="117"/>
+      <c r="B96" s="125" t="s">
+        <v>907</v>
+      </c>
+      <c r="C96" s="126" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="117"/>
-      <c r="B97" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C97" s="120" t="s">
-        <v>899</v>
+      <c r="B97" s="125" t="s">
+        <v>908</v>
+      </c>
+      <c r="C97" s="126" t="s">
+        <v>926</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="117"/>
       <c r="B98" s="125" t="s">
-        <v>854</v>
-      </c>
-      <c r="C98" s="126" t="s">
-        <v>928</v>
-      </c>
+        <v>909</v>
+      </c>
+      <c r="C98" s="126"/>
     </row>
     <row r="99" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="117"/>
-      <c r="B99" s="125" t="s">
-        <v>860</v>
-      </c>
-      <c r="C99" s="126" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="117"/>
-      <c r="B100" s="125" t="s">
-        <v>864</v>
-      </c>
-      <c r="C100" s="126" t="s">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="121" t="s">
+        <v>910</v>
+      </c>
+      <c r="C99" s="122"/>
+    </row>
+    <row r="100" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="117">
+        <v>2</v>
+      </c>
+      <c r="B100" s="139" t="s">
+        <v>885</v>
+      </c>
+      <c r="C100" s="140"/>
+    </row>
+    <row r="101" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="117"/>
-      <c r="B101" s="125" t="s">
-        <v>865</v>
-      </c>
-      <c r="C101" s="126" t="s">
-        <v>931</v>
+      <c r="B101" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C101" s="120" t="s">
+        <v>898</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="117"/>
-      <c r="B102" s="128" t="s">
-        <v>896</v>
-      </c>
-      <c r="C102" s="129" t="s">
-        <v>932</v>
+      <c r="B102" s="125" t="s">
+        <v>854</v>
+      </c>
+      <c r="C102" s="126" t="s">
+        <v>927</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="117"/>
-      <c r="B103" s="128" t="s">
-        <v>898</v>
-      </c>
-      <c r="C103" s="129" t="s">
-        <v>933</v>
+      <c r="B103" s="125" t="s">
+        <v>859</v>
+      </c>
+      <c r="C103" s="126" t="s">
+        <v>928</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="117"/>
-      <c r="B104" s="121" t="s">
-        <v>900</v>
-      </c>
-      <c r="C104" s="122" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="117">
-        <v>3</v>
-      </c>
-      <c r="B105" s="134" t="s">
-        <v>887</v>
-      </c>
-      <c r="C105" s="135"/>
-    </row>
-    <row r="106" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="125" t="s">
+        <v>863</v>
+      </c>
+      <c r="C104" s="126" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="117"/>
+      <c r="B105" s="125" t="s">
+        <v>864</v>
+      </c>
+      <c r="C105" s="126" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="117"/>
-      <c r="B106" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C106" s="120" t="s">
-        <v>893</v>
+      <c r="B106" s="128" t="s">
+        <v>895</v>
+      </c>
+      <c r="C106" s="129" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="117"/>
-      <c r="B107" s="125" t="s">
-        <v>854</v>
-      </c>
-      <c r="C107" s="126" t="s">
-        <v>894</v>
+      <c r="B107" s="128" t="s">
+        <v>897</v>
+      </c>
+      <c r="C107" s="129" t="s">
+        <v>932</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="117"/>
-      <c r="B108" s="125" t="s">
-        <v>860</v>
-      </c>
-      <c r="C108" s="126" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="117"/>
-      <c r="B109" s="128" t="s">
-        <v>864</v>
-      </c>
-      <c r="C109" s="129" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="121" t="s">
+        <v>899</v>
+      </c>
+      <c r="C108" s="122" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="117">
+        <v>3</v>
+      </c>
+      <c r="B109" s="141" t="s">
+        <v>886</v>
+      </c>
+      <c r="C109" s="142"/>
+    </row>
+    <row r="110" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="117"/>
-      <c r="B110" s="128" t="s">
-        <v>865</v>
-      </c>
-      <c r="C110" s="129" t="s">
-        <v>897</v>
+      <c r="B110" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C110" s="120" t="s">
+        <v>892</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="117"/>
-      <c r="B111" s="121"/>
-      <c r="C111" s="122"/>
-    </row>
-    <row r="112" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="116">
-        <v>4</v>
-      </c>
-      <c r="B112" s="136" t="s">
-        <v>888</v>
-      </c>
-      <c r="C112" s="137"/>
-    </row>
-    <row r="113" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="127"/>
-      <c r="B113" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C113" s="120" t="s">
-        <v>889</v>
+      <c r="B111" s="125" t="s">
+        <v>854</v>
+      </c>
+      <c r="C111" s="126" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="117"/>
+      <c r="B112" s="125" t="s">
+        <v>859</v>
+      </c>
+      <c r="C112" s="126" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="117"/>
+      <c r="B113" s="128" t="s">
+        <v>863</v>
+      </c>
+      <c r="C113" s="129" t="s">
+        <v>894</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="117"/>
-      <c r="B114" s="125" t="s">
-        <v>854</v>
-      </c>
-      <c r="C114" s="126" t="s">
-        <v>890</v>
+      <c r="B114" s="128" t="s">
+        <v>864</v>
+      </c>
+      <c r="C114" s="129" t="s">
+        <v>896</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="117"/>
-      <c r="B115" s="125" t="s">
-        <v>860</v>
-      </c>
-      <c r="C115" s="126" t="s">
+      <c r="B115" s="121"/>
+      <c r="C115" s="122"/>
+    </row>
+    <row r="116" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="116">
+        <v>4</v>
+      </c>
+      <c r="B116" s="143" t="s">
+        <v>887</v>
+      </c>
+      <c r="C116" s="144"/>
+    </row>
+    <row r="117" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="127"/>
+      <c r="B117" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C117" s="120" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="117"/>
+      <c r="B118" s="125" t="s">
+        <v>854</v>
+      </c>
+      <c r="C118" s="126" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="117"/>
+      <c r="B119" s="125" t="s">
+        <v>859</v>
+      </c>
+      <c r="C119" s="126" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="117"/>
+      <c r="B120" s="121" t="s">
+        <v>863</v>
+      </c>
+      <c r="C120" s="122" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="117"/>
-      <c r="B116" s="121" t="s">
-        <v>864</v>
-      </c>
-      <c r="C116" s="122" t="s">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="118" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="138" t="s">
+    <row r="121" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="132" t="s">
+        <v>935</v>
+      </c>
+      <c r="B122" s="133"/>
+      <c r="C122" s="134"/>
+    </row>
+    <row r="123" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="116">
+        <v>1</v>
+      </c>
+      <c r="B123" s="135" t="s">
         <v>936</v>
       </c>
-      <c r="B118" s="139"/>
-      <c r="C118" s="140"/>
-    </row>
-    <row r="119" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="116">
-        <v>1</v>
-      </c>
-      <c r="B119" s="141" t="s">
-        <v>937</v>
-      </c>
-      <c r="C119" s="142"/>
-    </row>
-    <row r="120" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="127"/>
-      <c r="B120" s="119" t="s">
+      <c r="C123" s="136"/>
+    </row>
+    <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="127"/>
+      <c r="B124" s="119" t="s">
         <v>853</v>
       </c>
-      <c r="C120" s="120" t="s">
+      <c r="C124" s="120" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="127"/>
-      <c r="B121" s="130" t="s">
-        <v>854</v>
-      </c>
-      <c r="C121" s="131" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="127"/>
-      <c r="B122" s="130" t="s">
-        <v>860</v>
-      </c>
-      <c r="C122" s="131" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="127"/>
-      <c r="B123" s="130" t="s">
-        <v>864</v>
-      </c>
-      <c r="C123" s="131" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="127"/>
-      <c r="B124" s="130" t="s">
-        <v>865</v>
-      </c>
-      <c r="C124" s="131"/>
     </row>
     <row r="125" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="127"/>
       <c r="B125" s="130" t="s">
-        <v>896</v>
-      </c>
-      <c r="C125" s="131"/>
+        <v>854</v>
+      </c>
+      <c r="C125" s="131" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="126" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="127"/>
       <c r="B126" s="130" t="s">
-        <v>898</v>
-      </c>
-      <c r="C126" s="131"/>
+        <v>859</v>
+      </c>
+      <c r="C126" s="131" t="s">
+        <v>886</v>
+      </c>
     </row>
     <row r="127" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="127"/>
       <c r="B127" s="130" t="s">
-        <v>900</v>
-      </c>
-      <c r="C127" s="131"/>
+        <v>863</v>
+      </c>
+      <c r="C127" s="131" t="s">
+        <v>887</v>
+      </c>
     </row>
     <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="127"/>
       <c r="B128" s="130" t="s">
-        <v>901</v>
+        <v>864</v>
       </c>
       <c r="C128" s="131"/>
     </row>
     <row r="129" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="117"/>
-      <c r="B129" s="125" t="s">
-        <v>902</v>
-      </c>
-      <c r="C129" s="126"/>
+      <c r="A129" s="127"/>
+      <c r="B129" s="130" t="s">
+        <v>895</v>
+      </c>
+      <c r="C129" s="131"/>
     </row>
     <row r="130" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="117"/>
-      <c r="B130" s="125" t="s">
-        <v>903</v>
-      </c>
-      <c r="C130" s="126"/>
+      <c r="A130" s="127"/>
+      <c r="B130" s="130" t="s">
+        <v>897</v>
+      </c>
+      <c r="C130" s="131"/>
     </row>
     <row r="131" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="117"/>
-      <c r="B131" s="125" t="s">
-        <v>904</v>
-      </c>
-      <c r="C131" s="126"/>
+      <c r="A131" s="127"/>
+      <c r="B131" s="130" t="s">
+        <v>899</v>
+      </c>
+      <c r="C131" s="131"/>
     </row>
     <row r="132" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="117"/>
-      <c r="B132" s="125" t="s">
-        <v>905</v>
-      </c>
-      <c r="C132" s="126"/>
+      <c r="A132" s="127"/>
+      <c r="B132" s="130" t="s">
+        <v>900</v>
+      </c>
+      <c r="C132" s="131"/>
     </row>
     <row r="133" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="117"/>
       <c r="B133" s="125" t="s">
-        <v>906</v>
+        <v>901</v>
       </c>
       <c r="C133" s="126"/>
     </row>
     <row r="134" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="117"/>
       <c r="B134" s="125" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="C134" s="126"/>
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="117"/>
       <c r="B135" s="125" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
       <c r="C135" s="126"/>
     </row>
     <row r="136" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="117"/>
       <c r="B136" s="125" t="s">
-        <v>909</v>
+        <v>904</v>
       </c>
       <c r="C136" s="126"/>
     </row>
     <row r="137" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="117"/>
       <c r="B137" s="125" t="s">
-        <v>910</v>
+        <v>905</v>
       </c>
       <c r="C137" s="126"/>
     </row>
     <row r="138" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="117"/>
-      <c r="B138" s="121" t="s">
-        <v>911</v>
-      </c>
-      <c r="C138" s="122"/>
-    </row>
-    <row r="139" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="117">
-        <v>2</v>
-      </c>
-      <c r="B139" s="132" t="s">
-        <v>938</v>
-      </c>
-      <c r="C139" s="133"/>
-    </row>
-    <row r="140" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B138" s="125" t="s">
+        <v>906</v>
+      </c>
+      <c r="C138" s="126"/>
+    </row>
+    <row r="139" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="117"/>
+      <c r="B139" s="125" t="s">
+        <v>907</v>
+      </c>
+      <c r="C139" s="126"/>
+    </row>
+    <row r="140" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="117"/>
-      <c r="B140" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C140" s="120" t="s">
-        <v>266</v>
-      </c>
+      <c r="B140" s="125" t="s">
+        <v>908</v>
+      </c>
+      <c r="C140" s="126"/>
     </row>
     <row r="141" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="117"/>
       <c r="B141" s="125" t="s">
-        <v>854</v>
-      </c>
-      <c r="C141" s="126" t="s">
-        <v>940</v>
-      </c>
+        <v>909</v>
+      </c>
+      <c r="C141" s="126"/>
     </row>
     <row r="142" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="117"/>
-      <c r="B142" s="125" t="s">
-        <v>860</v>
-      </c>
-      <c r="C142" s="126" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="117"/>
-      <c r="B143" s="125" t="s">
-        <v>864</v>
-      </c>
-      <c r="C143" s="126" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B142" s="121" t="s">
+        <v>910</v>
+      </c>
+      <c r="C142" s="122"/>
+    </row>
+    <row r="143" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="117">
+        <v>2</v>
+      </c>
+      <c r="B143" s="139" t="s">
+        <v>937</v>
+      </c>
+      <c r="C143" s="140"/>
+    </row>
+    <row r="144" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="117"/>
-      <c r="B144" s="125" t="s">
-        <v>865</v>
-      </c>
-      <c r="C144" s="126"/>
+      <c r="B144" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C144" s="120" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="145" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="117"/>
-      <c r="B145" s="128" t="s">
-        <v>896</v>
-      </c>
-      <c r="C145" s="129"/>
+      <c r="B145" s="125" t="s">
+        <v>854</v>
+      </c>
+      <c r="C145" s="126" t="s">
+        <v>939</v>
+      </c>
     </row>
     <row r="146" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="117"/>
-      <c r="B146" s="128" t="s">
-        <v>898</v>
-      </c>
-      <c r="C146" s="129"/>
+      <c r="B146" s="125" t="s">
+        <v>859</v>
+      </c>
+      <c r="C146" s="126" t="s">
+        <v>940</v>
+      </c>
     </row>
     <row r="147" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="117"/>
-      <c r="B147" s="121" t="s">
-        <v>900</v>
-      </c>
-      <c r="C147" s="122"/>
-    </row>
-    <row r="148" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="117">
-        <v>3</v>
-      </c>
-      <c r="B148" s="134" t="s">
-        <v>939</v>
-      </c>
-      <c r="C148" s="135"/>
-    </row>
-    <row r="149" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B147" s="125" t="s">
+        <v>863</v>
+      </c>
+      <c r="C147" s="126" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="117"/>
+      <c r="B148" s="125" t="s">
+        <v>864</v>
+      </c>
+      <c r="C148" s="126"/>
+    </row>
+    <row r="149" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="117"/>
-      <c r="B149" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C149" s="120" t="s">
-        <v>944</v>
-      </c>
+      <c r="B149" s="128" t="s">
+        <v>895</v>
+      </c>
+      <c r="C149" s="129"/>
     </row>
     <row r="150" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="117"/>
-      <c r="B150" s="125" t="s">
-        <v>854</v>
-      </c>
-      <c r="C150" s="126" t="s">
-        <v>943</v>
-      </c>
+      <c r="B150" s="128" t="s">
+        <v>897</v>
+      </c>
+      <c r="C150" s="129"/>
     </row>
     <row r="151" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="117"/>
-      <c r="B151" s="125" t="s">
-        <v>860</v>
-      </c>
-      <c r="C151" s="126" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="117"/>
-      <c r="B152" s="128" t="s">
-        <v>864</v>
-      </c>
-      <c r="C152" s="129" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B151" s="121" t="s">
+        <v>899</v>
+      </c>
+      <c r="C151" s="122"/>
+    </row>
+    <row r="152" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="117">
+        <v>3</v>
+      </c>
+      <c r="B152" s="141" t="s">
+        <v>938</v>
+      </c>
+      <c r="C152" s="142"/>
+    </row>
+    <row r="153" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="117"/>
-      <c r="B153" s="128" t="s">
-        <v>865</v>
-      </c>
-      <c r="C153" s="129"/>
+      <c r="B153" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C153" s="120" t="s">
+        <v>943</v>
+      </c>
     </row>
     <row r="154" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="117"/>
-      <c r="B154" s="121" t="s">
-        <v>896</v>
-      </c>
-      <c r="C154" s="122"/>
+      <c r="B154" s="125" t="s">
+        <v>854</v>
+      </c>
+      <c r="C154" s="126" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="117"/>
+      <c r="B155" s="125" t="s">
+        <v>859</v>
+      </c>
+      <c r="C155" s="126" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="117"/>
+      <c r="B156" s="128" t="s">
+        <v>863</v>
+      </c>
+      <c r="C156" s="129" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="117"/>
+      <c r="B157" s="128" t="s">
+        <v>864</v>
+      </c>
+      <c r="C157" s="129"/>
+    </row>
+    <row r="158" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="117"/>
+      <c r="B158" s="121" t="s">
+        <v>895</v>
+      </c>
+      <c r="C158" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="A122:C122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B11:C11"/>
@@ -6354,46 +6436,6 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="A118:C118"/>
-    <mergeCell ref="B119:C119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -8885,9 +8927,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X300"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V63" sqref="V63:V66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13132,9 +13174,7 @@
       <c r="U63" s="44" t="s">
         <v>715</v>
       </c>
-      <c r="V63" s="44" t="s">
-        <v>718</v>
-      </c>
+      <c r="V63" s="44"/>
       <c r="W63" s="44"/>
       <c r="X63" s="45"/>
     </row>
@@ -13200,9 +13240,7 @@
       <c r="U64" s="44" t="s">
         <v>715</v>
       </c>
-      <c r="V64" s="44" t="s">
-        <v>718</v>
-      </c>
+      <c r="V64" s="44"/>
       <c r="W64" s="44"/>
       <c r="X64" s="45"/>
     </row>
@@ -13268,9 +13306,7 @@
       <c r="U65" s="44" t="s">
         <v>715</v>
       </c>
-      <c r="V65" s="44" t="s">
-        <v>718</v>
-      </c>
+      <c r="V65" s="44"/>
       <c r="W65" s="44"/>
       <c r="X65" s="45"/>
     </row>
@@ -13336,9 +13372,7 @@
       <c r="U66" s="44" t="s">
         <v>715</v>
       </c>
-      <c r="V66" s="44" t="s">
-        <v>718</v>
-      </c>
+      <c r="V66" s="44"/>
       <c r="W66" s="44"/>
       <c r="X66" s="45"/>
     </row>

</xml_diff>

<commit_message>
Implementing dead eyes on critters
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716"/>
   </bookViews>
   <sheets>
     <sheet name="TODO - Quick Battle" sheetId="37" r:id="rId1"/>
@@ -701,7 +701,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1973" uniqueCount="949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1971" uniqueCount="948">
   <si>
     <t>Fishing</t>
   </si>
@@ -3269,9 +3269,6 @@
   </si>
   <si>
     <t>Perks</t>
-  </si>
-  <si>
-    <t>Dead Eyes on Critters</t>
   </si>
   <si>
     <t>Finish Trollish</t>
@@ -4727,6 +4724,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4746,24 +4761,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5115,10 +5112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C158"/>
+  <dimension ref="A1:C157"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5133,29 +5130,29 @@
       <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="138" t="s">
         <v>847</v>
       </c>
-      <c r="B2" s="133"/>
-      <c r="C2" s="134"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="140"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="116">
         <v>1</v>
       </c>
-      <c r="B3" s="135" t="s">
+      <c r="B3" s="141" t="s">
         <v>848</v>
       </c>
-      <c r="C3" s="136"/>
+      <c r="C3" s="142"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="117">
         <v>2</v>
       </c>
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="132" t="s">
         <v>849</v>
       </c>
-      <c r="C4" s="140"/>
+      <c r="C4" s="133"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="117"/>
@@ -5178,7 +5175,7 @@
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="117"/>
       <c r="B7" s="121" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C7" s="122" t="s">
         <v>112</v>
@@ -5188,54 +5185,54 @@
       <c r="A8" s="117">
         <v>3</v>
       </c>
-      <c r="B8" s="141" t="s">
+      <c r="B8" s="134" t="s">
         <v>850</v>
       </c>
-      <c r="C8" s="142"/>
+      <c r="C8" s="135"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="117">
         <v>4</v>
       </c>
-      <c r="B9" s="143" t="s">
+      <c r="B9" s="136" t="s">
         <v>851</v>
       </c>
-      <c r="C9" s="144"/>
+      <c r="C9" s="137"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="117">
         <v>5</v>
       </c>
-      <c r="B10" s="143" t="s">
+      <c r="B10" s="136" t="s">
         <v>852</v>
       </c>
-      <c r="C10" s="144"/>
+      <c r="C10" s="137"/>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="118">
         <v>6</v>
       </c>
-      <c r="B11" s="137" t="s">
-        <v>857</v>
-      </c>
-      <c r="C11" s="138"/>
+      <c r="B11" s="143" t="s">
+        <v>856</v>
+      </c>
+      <c r="C11" s="144"/>
     </row>
     <row r="12" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="132" t="s">
+      <c r="A13" s="138" t="s">
         <v>208</v>
       </c>
-      <c r="B13" s="133"/>
-      <c r="C13" s="134"/>
+      <c r="B13" s="139"/>
+      <c r="C13" s="140"/>
     </row>
     <row r="14" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="116">
         <v>1</v>
       </c>
-      <c r="B14" s="135" t="s">
-        <v>858</v>
-      </c>
-      <c r="C14" s="136"/>
+      <c r="B14" s="141" t="s">
+        <v>857</v>
+      </c>
+      <c r="C14" s="142"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="117"/>
@@ -5243,7 +5240,7 @@
         <v>853</v>
       </c>
       <c r="C15" s="120" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5258,16 +5255,16 @@
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="117"/>
       <c r="B17" s="125" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C17" s="126" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="117"/>
       <c r="B18" s="125" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C18" s="126" t="s">
         <v>735</v>
@@ -5276,7 +5273,7 @@
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="117"/>
       <c r="B19" s="128" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C19" s="129" t="s">
         <v>718</v>
@@ -5285,7 +5282,7 @@
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="117"/>
       <c r="B20" s="128" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C20" s="129" t="s">
         <v>549</v>
@@ -5294,46 +5291,46 @@
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="117"/>
       <c r="B21" s="128" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C21" s="129" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="117"/>
       <c r="B22" s="128" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C22" s="129" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="117"/>
       <c r="B23" s="121" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C23" s="122" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="132" t="s">
-        <v>861</v>
-      </c>
-      <c r="B25" s="133"/>
-      <c r="C25" s="134"/>
+      <c r="A25" s="138" t="s">
+        <v>860</v>
+      </c>
+      <c r="B25" s="139"/>
+      <c r="C25" s="140"/>
     </row>
     <row r="26" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="116">
         <v>1</v>
       </c>
-      <c r="B26" s="135" t="s">
+      <c r="B26" s="141" t="s">
         <v>847</v>
       </c>
-      <c r="C26" s="136"/>
+      <c r="C26" s="142"/>
     </row>
     <row r="27" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="117"/>
@@ -5341,89 +5338,89 @@
         <v>853</v>
       </c>
       <c r="C27" s="120" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="117"/>
       <c r="B28" s="125" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="C28" s="126" t="s">
-        <v>856</v>
+        <v>865</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="117"/>
-      <c r="B29" s="125" t="s">
-        <v>859</v>
-      </c>
-      <c r="C29" s="126" t="s">
+      <c r="B29" s="121" t="s">
+        <v>862</v>
+      </c>
+      <c r="C29" s="122" t="s">
         <v>866</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="117"/>
-      <c r="B30" s="121" t="s">
-        <v>863</v>
-      </c>
-      <c r="C30" s="122" t="s">
+    <row r="30" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="117">
+        <v>2</v>
+      </c>
+      <c r="B30" s="132" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="133"/>
+    </row>
+    <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="117"/>
+      <c r="B31" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C31" s="120" t="s">
         <v>867</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="117">
-        <v>2</v>
-      </c>
-      <c r="B31" s="139" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="140"/>
-    </row>
-    <row r="32" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="117"/>
-      <c r="B32" s="119" t="s">
+      <c r="B32" s="121"/>
+      <c r="C32" s="122"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="138" t="s">
+        <v>868</v>
+      </c>
+      <c r="B34" s="139"/>
+      <c r="C34" s="140"/>
+    </row>
+    <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="116">
+        <v>1</v>
+      </c>
+      <c r="B35" s="141" t="s">
+        <v>869</v>
+      </c>
+      <c r="C35" s="142"/>
+    </row>
+    <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="117"/>
+      <c r="B36" s="119" t="s">
         <v>853</v>
       </c>
-      <c r="C32" s="120" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="117"/>
-      <c r="B33" s="121"/>
-      <c r="C33" s="122"/>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="132" t="s">
-        <v>869</v>
-      </c>
-      <c r="B35" s="133"/>
-      <c r="C35" s="134"/>
-    </row>
-    <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="116">
-        <v>1</v>
-      </c>
-      <c r="B36" s="135" t="s">
+      <c r="C36" s="120" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="117"/>
+      <c r="B37" s="125" t="s">
+        <v>854</v>
+      </c>
+      <c r="C37" s="126" t="s">
         <v>870</v>
-      </c>
-      <c r="C36" s="136"/>
-    </row>
-    <row r="37" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="117"/>
-      <c r="B37" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C37" s="120" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="117"/>
       <c r="B38" s="125" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="C38" s="126" t="s">
         <v>871</v>
@@ -5431,79 +5428,79 @@
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="117"/>
-      <c r="B39" s="125" t="s">
-        <v>859</v>
-      </c>
-      <c r="C39" s="126" t="s">
+      <c r="B39" s="121" t="s">
+        <v>862</v>
+      </c>
+      <c r="C39" s="122" t="s">
         <v>872</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="117"/>
-      <c r="B40" s="121" t="s">
-        <v>863</v>
-      </c>
-      <c r="C40" s="122" t="s">
+    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="138" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="B41" s="139"/>
+      <c r="C41" s="140"/>
+    </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="132" t="s">
+      <c r="A42" s="116">
+        <v>1</v>
+      </c>
+      <c r="B42" s="141" t="s">
         <v>874</v>
       </c>
-      <c r="B42" s="133"/>
-      <c r="C42" s="134"/>
+      <c r="C42" s="142"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="116">
-        <v>1</v>
-      </c>
-      <c r="B43" s="135" t="s">
+      <c r="A43" s="117"/>
+      <c r="B43" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C43" s="120" t="s">
         <v>875</v>
       </c>
-      <c r="C43" s="136"/>
-    </row>
-    <row r="44" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="117"/>
-      <c r="B44" s="119" t="s">
+    </row>
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="127"/>
+      <c r="B44" s="121" t="s">
+        <v>854</v>
+      </c>
+      <c r="C44" s="122" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="116">
+        <v>1</v>
+      </c>
+      <c r="B45" s="141" t="s">
+        <v>876</v>
+      </c>
+      <c r="C45" s="142"/>
+    </row>
+    <row r="46" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="117"/>
+      <c r="B46" s="119" t="s">
         <v>853</v>
       </c>
-      <c r="C44" s="120" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="127"/>
-      <c r="B45" s="121" t="s">
+      <c r="C46" s="120" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="117"/>
+      <c r="B47" s="125" t="s">
         <v>854</v>
       </c>
-      <c r="C45" s="122" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="116">
-        <v>1</v>
-      </c>
-      <c r="B46" s="135" t="s">
-        <v>877</v>
-      </c>
-      <c r="C46" s="136"/>
-    </row>
-    <row r="47" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="117"/>
-      <c r="B47" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C47" s="120" t="s">
+      <c r="C47" s="126" t="s">
         <v>878</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="117"/>
       <c r="B48" s="125" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="C48" s="126" t="s">
         <v>879</v>
@@ -5511,251 +5508,251 @@
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="117"/>
-      <c r="B49" s="125" t="s">
-        <v>859</v>
-      </c>
-      <c r="C49" s="126" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="117"/>
-      <c r="B50" s="121"/>
-      <c r="C50" s="122"/>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="B49" s="121"/>
+      <c r="C49" s="122"/>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="138" t="s">
+        <v>213</v>
+      </c>
+      <c r="B51" s="139"/>
+      <c r="C51" s="140"/>
+    </row>
     <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="132" t="s">
-        <v>213</v>
-      </c>
-      <c r="B52" s="133"/>
-      <c r="C52" s="134"/>
-    </row>
-    <row r="53" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="116">
-        <v>1</v>
-      </c>
-      <c r="B53" s="135" t="s">
-        <v>882</v>
-      </c>
-      <c r="C53" s="136"/>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="A52" s="116">
+        <v>1</v>
+      </c>
+      <c r="B52" s="141" t="s">
+        <v>881</v>
+      </c>
+      <c r="C52" s="142"/>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="138" t="s">
+        <v>855</v>
+      </c>
+      <c r="B54" s="139"/>
+      <c r="C54" s="140"/>
+    </row>
     <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="132" t="s">
-        <v>855</v>
-      </c>
-      <c r="B55" s="133"/>
-      <c r="C55" s="134"/>
-    </row>
-    <row r="56" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="116">
-        <v>1</v>
-      </c>
-      <c r="B56" s="141" t="s">
+      <c r="A55" s="116">
+        <v>1</v>
+      </c>
+      <c r="B55" s="134" t="s">
         <v>848</v>
       </c>
-      <c r="C56" s="142"/>
+      <c r="C55" s="135"/>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="117">
+        <v>2</v>
+      </c>
+      <c r="B56" s="145" t="s">
+        <v>849</v>
+      </c>
+      <c r="C56" s="146"/>
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="117">
-        <v>2</v>
-      </c>
-      <c r="B57" s="145" t="s">
-        <v>849</v>
-      </c>
-      <c r="C57" s="146"/>
+        <v>3</v>
+      </c>
+      <c r="B57" s="136" t="s">
+        <v>850</v>
+      </c>
+      <c r="C57" s="137"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="117">
-        <v>3</v>
-      </c>
-      <c r="B58" s="143" t="s">
-        <v>850</v>
-      </c>
-      <c r="C58" s="144"/>
+        <v>4</v>
+      </c>
+      <c r="B58" s="136" t="s">
+        <v>851</v>
+      </c>
+      <c r="C58" s="137"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="117">
-        <v>4</v>
-      </c>
-      <c r="B59" s="143" t="s">
-        <v>851</v>
-      </c>
-      <c r="C59" s="144"/>
+        <v>5</v>
+      </c>
+      <c r="B59" s="136" t="s">
+        <v>852</v>
+      </c>
+      <c r="C59" s="137"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="117">
-        <v>5</v>
+      <c r="A60" s="118">
+        <v>6</v>
       </c>
       <c r="B60" s="143" t="s">
-        <v>852</v>
+        <v>856</v>
       </c>
       <c r="C60" s="144"/>
     </row>
-    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="118">
-        <v>6</v>
-      </c>
-      <c r="B61" s="137" t="s">
-        <v>857</v>
-      </c>
-      <c r="C61" s="138"/>
-    </row>
-    <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="138" t="s">
+        <v>882</v>
+      </c>
+      <c r="B62" s="139"/>
+      <c r="C62" s="140"/>
+    </row>
     <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="132" t="s">
-        <v>883</v>
-      </c>
-      <c r="B63" s="133"/>
-      <c r="C63" s="134"/>
-    </row>
-    <row r="64" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="116">
-        <v>1</v>
-      </c>
-      <c r="B64" s="141" t="s">
+      <c r="A63" s="116">
+        <v>1</v>
+      </c>
+      <c r="B63" s="134" t="s">
         <v>848</v>
       </c>
-      <c r="C64" s="142"/>
+      <c r="C63" s="135"/>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="117">
+        <v>2</v>
+      </c>
+      <c r="B64" s="145" t="s">
+        <v>849</v>
+      </c>
+      <c r="C64" s="146"/>
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="117">
-        <v>2</v>
-      </c>
-      <c r="B65" s="145" t="s">
-        <v>849</v>
-      </c>
-      <c r="C65" s="146"/>
+        <v>3</v>
+      </c>
+      <c r="B65" s="136" t="s">
+        <v>850</v>
+      </c>
+      <c r="C65" s="137"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="117">
-        <v>3</v>
-      </c>
-      <c r="B66" s="143" t="s">
-        <v>850</v>
-      </c>
-      <c r="C66" s="144"/>
+        <v>4</v>
+      </c>
+      <c r="B66" s="136" t="s">
+        <v>851</v>
+      </c>
+      <c r="C66" s="137"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="117">
-        <v>4</v>
-      </c>
-      <c r="B67" s="143" t="s">
-        <v>851</v>
-      </c>
-      <c r="C67" s="144"/>
+        <v>5</v>
+      </c>
+      <c r="B67" s="136" t="s">
+        <v>852</v>
+      </c>
+      <c r="C67" s="137"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="117">
-        <v>5</v>
+      <c r="A68" s="118">
+        <v>6</v>
       </c>
       <c r="B68" s="143" t="s">
-        <v>852</v>
+        <v>856</v>
       </c>
       <c r="C68" s="144"/>
     </row>
-    <row r="69" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="118">
-        <v>6</v>
-      </c>
-      <c r="B69" s="137" t="s">
-        <v>857</v>
-      </c>
-      <c r="C69" s="138"/>
-    </row>
-    <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="138" t="s">
+        <v>883</v>
+      </c>
+      <c r="B70" s="139"/>
+      <c r="C70" s="140"/>
+    </row>
     <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="132" t="s">
-        <v>884</v>
-      </c>
-      <c r="B71" s="133"/>
-      <c r="C71" s="134"/>
-    </row>
-    <row r="72" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="116">
-        <v>1</v>
-      </c>
-      <c r="B72" s="141" t="s">
+      <c r="A71" s="116">
+        <v>1</v>
+      </c>
+      <c r="B71" s="134" t="s">
         <v>848</v>
       </c>
-      <c r="C72" s="142"/>
+      <c r="C71" s="135"/>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="117">
+        <v>2</v>
+      </c>
+      <c r="B72" s="145" t="s">
+        <v>849</v>
+      </c>
+      <c r="C72" s="146"/>
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="117">
-        <v>2</v>
-      </c>
-      <c r="B73" s="145" t="s">
-        <v>849</v>
-      </c>
-      <c r="C73" s="146"/>
+        <v>3</v>
+      </c>
+      <c r="B73" s="136" t="s">
+        <v>850</v>
+      </c>
+      <c r="C73" s="137"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="117">
-        <v>3</v>
-      </c>
-      <c r="B74" s="143" t="s">
-        <v>850</v>
-      </c>
-      <c r="C74" s="144"/>
+        <v>4</v>
+      </c>
+      <c r="B74" s="136" t="s">
+        <v>851</v>
+      </c>
+      <c r="C74" s="137"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="117">
-        <v>4</v>
-      </c>
-      <c r="B75" s="143" t="s">
-        <v>851</v>
-      </c>
-      <c r="C75" s="144"/>
+        <v>5</v>
+      </c>
+      <c r="B75" s="136" t="s">
+        <v>852</v>
+      </c>
+      <c r="C75" s="137"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="117">
-        <v>5</v>
+      <c r="A76" s="118">
+        <v>6</v>
       </c>
       <c r="B76" s="143" t="s">
-        <v>852</v>
+        <v>856</v>
       </c>
       <c r="C76" s="144"/>
     </row>
-    <row r="77" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="118">
-        <v>6</v>
-      </c>
-      <c r="B77" s="137" t="s">
-        <v>857</v>
-      </c>
-      <c r="C77" s="138"/>
-    </row>
-    <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="138" t="s">
+        <v>933</v>
+      </c>
+      <c r="B78" s="139"/>
+      <c r="C78" s="140"/>
+    </row>
     <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="132" t="s">
-        <v>934</v>
-      </c>
-      <c r="B79" s="133"/>
-      <c r="C79" s="134"/>
+      <c r="A79" s="116">
+        <v>1</v>
+      </c>
+      <c r="B79" s="141" t="s">
+        <v>102</v>
+      </c>
+      <c r="C79" s="142"/>
     </row>
     <row r="80" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="116">
-        <v>1</v>
-      </c>
-      <c r="B80" s="135" t="s">
-        <v>102</v>
-      </c>
-      <c r="C80" s="136"/>
-    </row>
-    <row r="81" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="127"/>
+      <c r="B80" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C80" s="120" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="127"/>
-      <c r="B81" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C81" s="120" t="s">
+      <c r="B81" s="130" t="s">
+        <v>854</v>
+      </c>
+      <c r="C81" s="131" t="s">
         <v>911</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="127"/>
       <c r="B82" s="130" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="C82" s="131" t="s">
         <v>912</v>
@@ -5764,7 +5761,7 @@
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="127"/>
       <c r="B83" s="130" t="s">
-        <v>859</v>
+        <v>862</v>
       </c>
       <c r="C83" s="131" t="s">
         <v>913</v>
@@ -5782,7 +5779,7 @@
     <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="127"/>
       <c r="B85" s="130" t="s">
-        <v>864</v>
+        <v>894</v>
       </c>
       <c r="C85" s="131" t="s">
         <v>915</v>
@@ -5791,7 +5788,7 @@
     <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="127"/>
       <c r="B86" s="130" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="C86" s="131" t="s">
         <v>916</v>
@@ -5800,7 +5797,7 @@
     <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="127"/>
       <c r="B87" s="130" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="C87" s="131" t="s">
         <v>917</v>
@@ -5816,11 +5813,11 @@
       </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="127"/>
-      <c r="B89" s="130" t="s">
+      <c r="A89" s="117"/>
+      <c r="B89" s="125" t="s">
         <v>900</v>
       </c>
-      <c r="C89" s="131" t="s">
+      <c r="C89" s="126" t="s">
         <v>919</v>
       </c>
     </row>
@@ -5875,7 +5872,7 @@
         <v>906</v>
       </c>
       <c r="C95" s="126" t="s">
-        <v>925</v>
+        <v>35</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5884,7 +5881,7 @@
         <v>907</v>
       </c>
       <c r="C96" s="126" t="s">
-        <v>35</v>
+        <v>925</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5892,46 +5889,46 @@
       <c r="B97" s="125" t="s">
         <v>908</v>
       </c>
-      <c r="C97" s="126" t="s">
-        <v>926</v>
-      </c>
+      <c r="C97" s="126"/>
     </row>
     <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="117"/>
-      <c r="B98" s="125" t="s">
+      <c r="B98" s="121" t="s">
         <v>909</v>
       </c>
-      <c r="C98" s="126"/>
-    </row>
-    <row r="99" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="117"/>
-      <c r="B99" s="121" t="s">
-        <v>910</v>
-      </c>
-      <c r="C99" s="122"/>
+      <c r="C98" s="122"/>
+    </row>
+    <row r="99" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="117">
+        <v>2</v>
+      </c>
+      <c r="B99" s="132" t="s">
+        <v>884</v>
+      </c>
+      <c r="C99" s="133"/>
     </row>
     <row r="100" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="117">
-        <v>2</v>
-      </c>
-      <c r="B100" s="139" t="s">
-        <v>885</v>
-      </c>
-      <c r="C100" s="140"/>
-    </row>
-    <row r="101" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="117"/>
+      <c r="B100" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C100" s="120" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="117"/>
-      <c r="B101" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C101" s="120" t="s">
-        <v>898</v>
+      <c r="B101" s="125" t="s">
+        <v>854</v>
+      </c>
+      <c r="C101" s="126" t="s">
+        <v>926</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="117"/>
       <c r="B102" s="125" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="C102" s="126" t="s">
         <v>927</v>
@@ -5940,7 +5937,7 @@
     <row r="103" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="117"/>
       <c r="B103" s="125" t="s">
-        <v>859</v>
+        <v>862</v>
       </c>
       <c r="C103" s="126" t="s">
         <v>928</v>
@@ -5957,17 +5954,17 @@
     </row>
     <row r="105" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="117"/>
-      <c r="B105" s="125" t="s">
-        <v>864</v>
-      </c>
-      <c r="C105" s="126" t="s">
+      <c r="B105" s="128" t="s">
+        <v>894</v>
+      </c>
+      <c r="C105" s="129" t="s">
         <v>930</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="117"/>
       <c r="B106" s="128" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="C106" s="129" t="s">
         <v>931</v>
@@ -5975,56 +5972,56 @@
     </row>
     <row r="107" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="117"/>
-      <c r="B107" s="128" t="s">
-        <v>897</v>
-      </c>
-      <c r="C107" s="129" t="s">
+      <c r="B107" s="121" t="s">
+        <v>898</v>
+      </c>
+      <c r="C107" s="122" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="117"/>
-      <c r="B108" s="121" t="s">
-        <v>899</v>
-      </c>
-      <c r="C108" s="122" t="s">
-        <v>933</v>
-      </c>
+    <row r="108" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="117">
+        <v>3</v>
+      </c>
+      <c r="B108" s="134" t="s">
+        <v>885</v>
+      </c>
+      <c r="C108" s="135"/>
     </row>
     <row r="109" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="117">
-        <v>3</v>
-      </c>
-      <c r="B109" s="141" t="s">
-        <v>886</v>
-      </c>
-      <c r="C109" s="142"/>
-    </row>
-    <row r="110" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="117"/>
+      <c r="B109" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C109" s="120" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="117"/>
-      <c r="B110" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C110" s="120" t="s">
+      <c r="B110" s="125" t="s">
+        <v>854</v>
+      </c>
+      <c r="C110" s="126" t="s">
         <v>892</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="117"/>
       <c r="B111" s="125" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="C111" s="126" t="s">
-        <v>893</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="117"/>
-      <c r="B112" s="125" t="s">
-        <v>859</v>
-      </c>
-      <c r="C112" s="126" t="s">
-        <v>90</v>
+      <c r="B112" s="128" t="s">
+        <v>862</v>
+      </c>
+      <c r="C112" s="129" t="s">
+        <v>893</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6033,45 +6030,45 @@
         <v>863</v>
       </c>
       <c r="C113" s="129" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="117"/>
-      <c r="B114" s="128" t="s">
-        <v>864</v>
-      </c>
-      <c r="C114" s="129" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="117"/>
-      <c r="B115" s="121"/>
-      <c r="C115" s="122"/>
+      <c r="B114" s="121"/>
+      <c r="C114" s="122"/>
+    </row>
+    <row r="115" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="116">
+        <v>4</v>
+      </c>
+      <c r="B115" s="136" t="s">
+        <v>886</v>
+      </c>
+      <c r="C115" s="137"/>
     </row>
     <row r="116" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="116">
-        <v>4</v>
-      </c>
-      <c r="B116" s="143" t="s">
+      <c r="A116" s="127"/>
+      <c r="B116" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C116" s="120" t="s">
         <v>887</v>
       </c>
-      <c r="C116" s="144"/>
-    </row>
-    <row r="117" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="127"/>
-      <c r="B117" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C117" s="120" t="s">
+    </row>
+    <row r="117" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="117"/>
+      <c r="B117" s="125" t="s">
+        <v>854</v>
+      </c>
+      <c r="C117" s="126" t="s">
         <v>888</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="117"/>
       <c r="B118" s="125" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="C118" s="126" t="s">
         <v>889</v>
@@ -6079,52 +6076,52 @@
     </row>
     <row r="119" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="117"/>
-      <c r="B119" s="125" t="s">
-        <v>859</v>
-      </c>
-      <c r="C119" s="126" t="s">
+      <c r="B119" s="121" t="s">
+        <v>862</v>
+      </c>
+      <c r="C119" s="122" t="s">
         <v>890</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="117"/>
-      <c r="B120" s="121" t="s">
-        <v>863</v>
-      </c>
-      <c r="C120" s="122" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="138" t="s">
+        <v>934</v>
+      </c>
+      <c r="B121" s="139"/>
+      <c r="C121" s="140"/>
+    </row>
     <row r="122" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="132" t="s">
+      <c r="A122" s="116">
+        <v>1</v>
+      </c>
+      <c r="B122" s="141" t="s">
         <v>935</v>
       </c>
-      <c r="B122" s="133"/>
-      <c r="C122" s="134"/>
+      <c r="C122" s="142"/>
     </row>
     <row r="123" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="116">
-        <v>1</v>
-      </c>
-      <c r="B123" s="135" t="s">
-        <v>936</v>
-      </c>
-      <c r="C123" s="136"/>
-    </row>
-    <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="127"/>
+      <c r="B123" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C123" s="120" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="127"/>
-      <c r="B124" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C124" s="120" t="s">
-        <v>102</v>
+      <c r="B124" s="130" t="s">
+        <v>854</v>
+      </c>
+      <c r="C124" s="131" t="s">
+        <v>884</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="127"/>
       <c r="B125" s="130" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="C125" s="131" t="s">
         <v>885</v>
@@ -6133,7 +6130,7 @@
     <row r="126" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="127"/>
       <c r="B126" s="130" t="s">
-        <v>859</v>
+        <v>862</v>
       </c>
       <c r="C126" s="131" t="s">
         <v>886</v>
@@ -6144,28 +6141,26 @@
       <c r="B127" s="130" t="s">
         <v>863</v>
       </c>
-      <c r="C127" s="131" t="s">
-        <v>887</v>
-      </c>
+      <c r="C127" s="131"/>
     </row>
     <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="127"/>
       <c r="B128" s="130" t="s">
-        <v>864</v>
+        <v>894</v>
       </c>
       <c r="C128" s="131"/>
     </row>
     <row r="129" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="127"/>
       <c r="B129" s="130" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="C129" s="131"/>
     </row>
     <row r="130" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="127"/>
       <c r="B130" s="130" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="C130" s="131"/>
     </row>
@@ -6177,11 +6172,11 @@
       <c r="C131" s="131"/>
     </row>
     <row r="132" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="127"/>
-      <c r="B132" s="130" t="s">
+      <c r="A132" s="117"/>
+      <c r="B132" s="125" t="s">
         <v>900</v>
       </c>
-      <c r="C132" s="131"/>
+      <c r="C132" s="126"/>
     </row>
     <row r="133" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="117"/>
@@ -6241,40 +6236,42 @@
     </row>
     <row r="141" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="117"/>
-      <c r="B141" s="125" t="s">
+      <c r="B141" s="121" t="s">
         <v>909</v>
       </c>
-      <c r="C141" s="126"/>
-    </row>
-    <row r="142" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="117"/>
-      <c r="B142" s="121" t="s">
-        <v>910</v>
-      </c>
-      <c r="C142" s="122"/>
+      <c r="C141" s="122"/>
+    </row>
+    <row r="142" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="117">
+        <v>2</v>
+      </c>
+      <c r="B142" s="132" t="s">
+        <v>936</v>
+      </c>
+      <c r="C142" s="133"/>
     </row>
     <row r="143" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="117">
-        <v>2</v>
-      </c>
-      <c r="B143" s="139" t="s">
-        <v>937</v>
-      </c>
-      <c r="C143" s="140"/>
-    </row>
-    <row r="144" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="117"/>
+      <c r="B143" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C143" s="120" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="117"/>
-      <c r="B144" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C144" s="120" t="s">
-        <v>266</v>
+      <c r="B144" s="125" t="s">
+        <v>854</v>
+      </c>
+      <c r="C144" s="126" t="s">
+        <v>938</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="117"/>
       <c r="B145" s="125" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="C145" s="126" t="s">
         <v>939</v>
@@ -6283,7 +6280,7 @@
     <row r="146" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="117"/>
       <c r="B146" s="125" t="s">
-        <v>859</v>
+        <v>862</v>
       </c>
       <c r="C146" s="126" t="s">
         <v>940</v>
@@ -6294,71 +6291,71 @@
       <c r="B147" s="125" t="s">
         <v>863</v>
       </c>
-      <c r="C147" s="126" t="s">
-        <v>941</v>
-      </c>
+      <c r="C147" s="126"/>
     </row>
     <row r="148" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="117"/>
-      <c r="B148" s="125" t="s">
-        <v>864</v>
-      </c>
-      <c r="C148" s="126"/>
+      <c r="B148" s="128" t="s">
+        <v>894</v>
+      </c>
+      <c r="C148" s="129"/>
     </row>
     <row r="149" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="117"/>
       <c r="B149" s="128" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="C149" s="129"/>
     </row>
     <row r="150" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="117"/>
-      <c r="B150" s="128" t="s">
-        <v>897</v>
-      </c>
-      <c r="C150" s="129"/>
-    </row>
-    <row r="151" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="117"/>
-      <c r="B151" s="121" t="s">
-        <v>899</v>
-      </c>
-      <c r="C151" s="122"/>
+      <c r="B150" s="121" t="s">
+        <v>898</v>
+      </c>
+      <c r="C150" s="122"/>
+    </row>
+    <row r="151" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="117">
+        <v>3</v>
+      </c>
+      <c r="B151" s="134" t="s">
+        <v>937</v>
+      </c>
+      <c r="C151" s="135"/>
     </row>
     <row r="152" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="117">
-        <v>3</v>
-      </c>
-      <c r="B152" s="141" t="s">
-        <v>938</v>
-      </c>
-      <c r="C152" s="142"/>
-    </row>
-    <row r="153" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="117"/>
+      <c r="B152" s="119" t="s">
+        <v>853</v>
+      </c>
+      <c r="C152" s="120" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="117"/>
-      <c r="B153" s="119" t="s">
-        <v>853</v>
-      </c>
-      <c r="C153" s="120" t="s">
-        <v>943</v>
+      <c r="B153" s="125" t="s">
+        <v>854</v>
+      </c>
+      <c r="C153" s="126" t="s">
+        <v>941</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="117"/>
       <c r="B154" s="125" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="C154" s="126" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="117"/>
-      <c r="B155" s="125" t="s">
-        <v>859</v>
-      </c>
-      <c r="C155" s="126" t="s">
+      <c r="B155" s="128" t="s">
+        <v>862</v>
+      </c>
+      <c r="C155" s="129" t="s">
         <v>944</v>
       </c>
     </row>
@@ -6367,66 +6364,17 @@
       <c r="B156" s="128" t="s">
         <v>863</v>
       </c>
-      <c r="C156" s="129" t="s">
-        <v>945</v>
-      </c>
+      <c r="C156" s="129"/>
     </row>
     <row r="157" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="117"/>
-      <c r="B157" s="128" t="s">
-        <v>864</v>
-      </c>
-      <c r="C157" s="129"/>
-    </row>
-    <row r="158" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="117"/>
-      <c r="B158" s="121" t="s">
-        <v>895</v>
-      </c>
-      <c r="C158" s="122"/>
+      <c r="B157" s="121" t="s">
+        <v>894</v>
+      </c>
+      <c r="C157" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="B152:C152"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="A122:C122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="B36:C36"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B11:C11"/>
@@ -6436,6 +6384,46 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="A121:C121"/>
+    <mergeCell ref="B122:C122"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -8927,7 +8915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="V63" sqref="V63:V66"/>
     </sheetView>

</xml_diff>

<commit_message>
Implementing surrounded/heigh delta logic
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -642,7 +642,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2173" uniqueCount="1034">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="1033">
   <si>
     <t>Fishing</t>
   </si>
@@ -3101,12 +3101,6 @@
     <t>Area Suppression</t>
   </si>
   <si>
-    <t>Height Bonuses/Penalties</t>
-  </si>
-  <si>
-    <t>Surrounded bonuses/penalties</t>
-  </si>
-  <si>
     <t>Implement</t>
   </si>
   <si>
@@ -3744,6 +3738,9 @@
   </si>
   <si>
     <t>Soul Farmer</t>
+  </si>
+  <si>
+    <t>attack of opportunity</t>
   </si>
 </sst>
 </file>
@@ -4918,24 +4915,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4955,6 +4934,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5305,8 +5302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5321,29 +5318,29 @@
       <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="145" t="s">
+      <c r="A2" s="139" t="s">
         <v>803</v>
       </c>
-      <c r="B2" s="146"/>
-      <c r="C2" s="147"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="141"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="116">
         <v>1</v>
       </c>
-      <c r="B3" s="148" t="s">
+      <c r="B3" s="142" t="s">
         <v>804</v>
       </c>
-      <c r="C3" s="149"/>
+      <c r="C3" s="143"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="117">
         <v>2</v>
       </c>
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="146" t="s">
         <v>805</v>
       </c>
-      <c r="C4" s="140"/>
+      <c r="C4" s="147"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="117"/>
@@ -5378,7 +5375,7 @@
         <v>816</v>
       </c>
       <c r="C8" s="124" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5394,10 +5391,10 @@
       <c r="A10" s="117">
         <v>3</v>
       </c>
-      <c r="B10" s="141" t="s">
+      <c r="B10" s="148" t="s">
         <v>806</v>
       </c>
-      <c r="C10" s="142"/>
+      <c r="C10" s="149"/>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="117"/>
@@ -5405,17 +5402,17 @@
         <v>809</v>
       </c>
       <c r="C11" s="120" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="117">
         <v>4</v>
       </c>
-      <c r="B12" s="143" t="s">
+      <c r="B12" s="150" t="s">
         <v>807</v>
       </c>
-      <c r="C12" s="144"/>
+      <c r="C12" s="151"/>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="117"/>
@@ -5423,17 +5420,17 @@
         <v>809</v>
       </c>
       <c r="C13" s="120" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="117">
         <v>5</v>
       </c>
-      <c r="B14" s="143" t="s">
+      <c r="B14" s="150" t="s">
         <v>808</v>
       </c>
-      <c r="C14" s="144"/>
+      <c r="C14" s="151"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="117"/>
@@ -5441,17 +5438,17 @@
         <v>809</v>
       </c>
       <c r="C15" s="120" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="118">
         <v>6</v>
       </c>
-      <c r="B16" s="150" t="s">
+      <c r="B16" s="144" t="s">
         <v>812</v>
       </c>
-      <c r="C16" s="151"/>
+      <c r="C16" s="145"/>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="117"/>
@@ -5459,43 +5456,43 @@
         <v>809</v>
       </c>
       <c r="C17" s="120" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="118">
         <v>7</v>
       </c>
-      <c r="B18" s="150" t="s">
-        <v>944</v>
-      </c>
-      <c r="C18" s="151"/>
+      <c r="B18" s="144" t="s">
+        <v>942</v>
+      </c>
+      <c r="C18" s="145"/>
     </row>
     <row r="19" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="134">
         <v>8</v>
       </c>
-      <c r="B19" s="150" t="s">
-        <v>945</v>
-      </c>
-      <c r="C19" s="151"/>
+      <c r="B19" s="144" t="s">
+        <v>943</v>
+      </c>
+      <c r="C19" s="145"/>
     </row>
     <row r="20" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="145" t="s">
+      <c r="A21" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="B21" s="146"/>
-      <c r="C21" s="147"/>
+      <c r="B21" s="140"/>
+      <c r="C21" s="141"/>
     </row>
     <row r="22" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="116">
         <v>1</v>
       </c>
-      <c r="B22" s="148" t="s">
+      <c r="B22" s="142" t="s">
         <v>813</v>
       </c>
-      <c r="C22" s="149"/>
+      <c r="C22" s="143"/>
     </row>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="117"/>
@@ -5503,7 +5500,7 @@
         <v>809</v>
       </c>
       <c r="C23" s="120" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5545,7 +5542,7 @@
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="117"/>
       <c r="B28" s="126" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C28" s="127" t="s">
         <v>510</v>
@@ -5554,64 +5551,60 @@
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="117"/>
       <c r="B29" s="126" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="C29" s="127" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="117"/>
       <c r="B30" s="121" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="C30" s="122" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="145" t="s">
+      <c r="A32" s="139" t="s">
         <v>815</v>
       </c>
-      <c r="B32" s="146"/>
-      <c r="C32" s="147"/>
+      <c r="B32" s="140"/>
+      <c r="C32" s="141"/>
     </row>
     <row r="33" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="116">
         <v>1</v>
       </c>
-      <c r="B33" s="148" t="s">
+      <c r="B33" s="142" t="s">
         <v>803</v>
       </c>
-      <c r="C33" s="149"/>
+      <c r="C33" s="143"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="117"/>
       <c r="B34" s="123" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
       <c r="C34" s="124" t="s">
-        <v>819</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="117"/>
-      <c r="B35" s="123" t="s">
-        <v>816</v>
-      </c>
-      <c r="C35" s="124" t="s">
-        <v>820</v>
-      </c>
+      <c r="B35" s="123"/>
+      <c r="C35" s="124"/>
     </row>
     <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="117">
         <v>2</v>
       </c>
-      <c r="B36" s="139" t="s">
+      <c r="B36" s="146" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="140"/>
+      <c r="C36" s="147"/>
     </row>
     <row r="37" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="117"/>
@@ -5619,7 +5612,7 @@
         <v>809</v>
       </c>
       <c r="C37" s="120" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5631,10 +5624,10 @@
       <c r="A39" s="117">
         <v>2</v>
       </c>
-      <c r="B39" s="139" t="s">
-        <v>941</v>
-      </c>
-      <c r="C39" s="140"/>
+      <c r="B39" s="146" t="s">
+        <v>939</v>
+      </c>
+      <c r="C39" s="147"/>
     </row>
     <row r="40" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="117"/>
@@ -5642,7 +5635,7 @@
         <v>809</v>
       </c>
       <c r="C40" s="120" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5651,25 +5644,25 @@
         <v>810</v>
       </c>
       <c r="C41" s="132" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="145" t="s">
-        <v>822</v>
-      </c>
-      <c r="B43" s="146"/>
-      <c r="C43" s="147"/>
+      <c r="A43" s="139" t="s">
+        <v>820</v>
+      </c>
+      <c r="B43" s="140"/>
+      <c r="C43" s="141"/>
     </row>
     <row r="44" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="116">
         <v>1</v>
       </c>
-      <c r="B44" s="148" t="s">
-        <v>823</v>
-      </c>
-      <c r="C44" s="149"/>
+      <c r="B44" s="142" t="s">
+        <v>821</v>
+      </c>
+      <c r="C44" s="143"/>
     </row>
     <row r="45" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="117"/>
@@ -5686,7 +5679,7 @@
         <v>810</v>
       </c>
       <c r="C46" s="124" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5695,7 +5688,7 @@
         <v>814</v>
       </c>
       <c r="C47" s="124" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5704,25 +5697,25 @@
         <v>816</v>
       </c>
       <c r="C48" s="122" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="145" t="s">
-        <v>827</v>
-      </c>
-      <c r="B50" s="146"/>
-      <c r="C50" s="147"/>
+      <c r="A50" s="139" t="s">
+        <v>825</v>
+      </c>
+      <c r="B50" s="140"/>
+      <c r="C50" s="141"/>
     </row>
     <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="116">
         <v>1</v>
       </c>
-      <c r="B51" s="148" t="s">
-        <v>828</v>
-      </c>
-      <c r="C51" s="149"/>
+      <c r="B51" s="142" t="s">
+        <v>826</v>
+      </c>
+      <c r="C51" s="143"/>
     </row>
     <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="117"/>
@@ -5730,7 +5723,7 @@
         <v>809</v>
       </c>
       <c r="C52" s="120" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5739,17 +5732,17 @@
         <v>810</v>
       </c>
       <c r="C53" s="122" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="116">
         <v>1</v>
       </c>
-      <c r="B54" s="148" t="s">
-        <v>830</v>
-      </c>
-      <c r="C54" s="149"/>
+      <c r="B54" s="142" t="s">
+        <v>828</v>
+      </c>
+      <c r="C54" s="143"/>
     </row>
     <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="117"/>
@@ -5757,7 +5750,7 @@
         <v>809</v>
       </c>
       <c r="C55" s="120" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5766,7 +5759,7 @@
         <v>810</v>
       </c>
       <c r="C56" s="124" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5775,7 +5768,7 @@
         <v>814</v>
       </c>
       <c r="C57" s="124" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5785,37 +5778,37 @@
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="145" t="s">
+      <c r="A60" s="139" t="s">
         <v>188</v>
       </c>
-      <c r="B60" s="146"/>
-      <c r="C60" s="147"/>
+      <c r="B60" s="140"/>
+      <c r="C60" s="141"/>
     </row>
     <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="116">
         <v>1</v>
       </c>
-      <c r="B61" s="148" t="s">
-        <v>835</v>
-      </c>
-      <c r="C61" s="149"/>
+      <c r="B61" s="142" t="s">
+        <v>833</v>
+      </c>
+      <c r="C61" s="143"/>
     </row>
     <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="145" t="s">
+      <c r="A63" s="139" t="s">
         <v>811</v>
       </c>
-      <c r="B63" s="146"/>
-      <c r="C63" s="147"/>
+      <c r="B63" s="140"/>
+      <c r="C63" s="141"/>
     </row>
     <row r="64" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="116">
         <v>1</v>
       </c>
-      <c r="B64" s="141" t="s">
+      <c r="B64" s="148" t="s">
         <v>804</v>
       </c>
-      <c r="C64" s="142"/>
+      <c r="C64" s="149"/>
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="117">
@@ -5830,54 +5823,54 @@
       <c r="A66" s="117">
         <v>3</v>
       </c>
-      <c r="B66" s="143" t="s">
+      <c r="B66" s="150" t="s">
         <v>806</v>
       </c>
-      <c r="C66" s="144"/>
+      <c r="C66" s="151"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="117">
         <v>4</v>
       </c>
-      <c r="B67" s="143" t="s">
+      <c r="B67" s="150" t="s">
         <v>807</v>
       </c>
-      <c r="C67" s="144"/>
+      <c r="C67" s="151"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="117">
         <v>5</v>
       </c>
-      <c r="B68" s="143" t="s">
+      <c r="B68" s="150" t="s">
         <v>808</v>
       </c>
-      <c r="C68" s="144"/>
+      <c r="C68" s="151"/>
     </row>
     <row r="69" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="118">
         <v>6</v>
       </c>
-      <c r="B69" s="150" t="s">
+      <c r="B69" s="144" t="s">
         <v>812</v>
       </c>
-      <c r="C69" s="151"/>
+      <c r="C69" s="145"/>
     </row>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="145" t="s">
-        <v>836</v>
-      </c>
-      <c r="B71" s="146"/>
-      <c r="C71" s="147"/>
+      <c r="A71" s="139" t="s">
+        <v>834</v>
+      </c>
+      <c r="B71" s="140"/>
+      <c r="C71" s="141"/>
     </row>
     <row r="72" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="116">
         <v>1</v>
       </c>
-      <c r="B72" s="141" t="s">
+      <c r="B72" s="148" t="s">
         <v>804</v>
       </c>
-      <c r="C72" s="142"/>
+      <c r="C72" s="149"/>
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="117">
@@ -5892,54 +5885,54 @@
       <c r="A74" s="117">
         <v>3</v>
       </c>
-      <c r="B74" s="143" t="s">
+      <c r="B74" s="150" t="s">
         <v>806</v>
       </c>
-      <c r="C74" s="144"/>
+      <c r="C74" s="151"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="117">
         <v>4</v>
       </c>
-      <c r="B75" s="143" t="s">
+      <c r="B75" s="150" t="s">
         <v>807</v>
       </c>
-      <c r="C75" s="144"/>
+      <c r="C75" s="151"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="117">
         <v>5</v>
       </c>
-      <c r="B76" s="143" t="s">
+      <c r="B76" s="150" t="s">
         <v>808</v>
       </c>
-      <c r="C76" s="144"/>
+      <c r="C76" s="151"/>
     </row>
     <row r="77" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="118">
         <v>6</v>
       </c>
-      <c r="B77" s="150" t="s">
+      <c r="B77" s="144" t="s">
         <v>812</v>
       </c>
-      <c r="C77" s="151"/>
+      <c r="C77" s="145"/>
     </row>
     <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="145" t="s">
-        <v>837</v>
-      </c>
-      <c r="B79" s="146"/>
-      <c r="C79" s="147"/>
+      <c r="A79" s="139" t="s">
+        <v>835</v>
+      </c>
+      <c r="B79" s="140"/>
+      <c r="C79" s="141"/>
     </row>
     <row r="80" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="116">
         <v>1</v>
       </c>
-      <c r="B80" s="141" t="s">
+      <c r="B80" s="148" t="s">
         <v>804</v>
       </c>
-      <c r="C80" s="142"/>
+      <c r="C80" s="149"/>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="117">
@@ -5954,54 +5947,54 @@
       <c r="A82" s="117">
         <v>3</v>
       </c>
-      <c r="B82" s="143" t="s">
+      <c r="B82" s="150" t="s">
         <v>806</v>
       </c>
-      <c r="C82" s="144"/>
+      <c r="C82" s="151"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="117">
         <v>4</v>
       </c>
-      <c r="B83" s="143" t="s">
+      <c r="B83" s="150" t="s">
         <v>807</v>
       </c>
-      <c r="C83" s="144"/>
+      <c r="C83" s="151"/>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="117">
         <v>5</v>
       </c>
-      <c r="B84" s="143" t="s">
+      <c r="B84" s="150" t="s">
         <v>808</v>
       </c>
-      <c r="C84" s="144"/>
+      <c r="C84" s="151"/>
     </row>
     <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="118">
         <v>6</v>
       </c>
-      <c r="B85" s="150" t="s">
+      <c r="B85" s="144" t="s">
         <v>812</v>
       </c>
-      <c r="C85" s="151"/>
+      <c r="C85" s="145"/>
     </row>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="87" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="145" t="s">
-        <v>887</v>
-      </c>
-      <c r="B87" s="146"/>
-      <c r="C87" s="147"/>
+      <c r="A87" s="139" t="s">
+        <v>885</v>
+      </c>
+      <c r="B87" s="140"/>
+      <c r="C87" s="141"/>
     </row>
     <row r="88" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="116">
         <v>1</v>
       </c>
-      <c r="B88" s="148" t="s">
+      <c r="B88" s="142" t="s">
         <v>101</v>
       </c>
-      <c r="C88" s="149"/>
+      <c r="C88" s="143"/>
     </row>
     <row r="89" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="125"/>
@@ -6009,7 +6002,7 @@
         <v>809</v>
       </c>
       <c r="C89" s="120" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6018,7 +6011,7 @@
         <v>810</v>
       </c>
       <c r="C90" s="129" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6027,7 +6020,7 @@
         <v>814</v>
       </c>
       <c r="C91" s="129" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6036,7 +6029,7 @@
         <v>816</v>
       </c>
       <c r="C92" s="129" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6045,103 +6038,103 @@
         <v>817</v>
       </c>
       <c r="C93" s="129" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="125"/>
       <c r="B94" s="128" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C94" s="129" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="125"/>
       <c r="B95" s="128" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="C95" s="129" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="125"/>
       <c r="B96" s="128" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="C96" s="129" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="125"/>
       <c r="B97" s="128" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="C97" s="129" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="117"/>
       <c r="B98" s="123" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="C98" s="124" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="117"/>
       <c r="B99" s="123" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="C99" s="124" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="117"/>
       <c r="B100" s="123" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="C100" s="124" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="117"/>
       <c r="B101" s="123" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="C101" s="124" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="117"/>
       <c r="B102" s="123" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="C102" s="124" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="117"/>
       <c r="B103" s="123" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="C103" s="124" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="117"/>
       <c r="B104" s="123" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="C104" s="124" t="s">
         <v>35</v>
@@ -6150,23 +6143,23 @@
     <row r="105" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="117"/>
       <c r="B105" s="123" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="C105" s="124" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="117"/>
       <c r="B106" s="123" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="C106" s="124"/>
     </row>
     <row r="107" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="117"/>
       <c r="B107" s="121" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="C107" s="122"/>
     </row>
@@ -6174,10 +6167,10 @@
       <c r="A108" s="117">
         <v>2</v>
       </c>
-      <c r="B108" s="139" t="s">
-        <v>838</v>
-      </c>
-      <c r="C108" s="140"/>
+      <c r="B108" s="146" t="s">
+        <v>836</v>
+      </c>
+      <c r="C108" s="147"/>
     </row>
     <row r="109" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="117"/>
@@ -6185,7 +6178,7 @@
         <v>809</v>
       </c>
       <c r="C109" s="120" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6194,7 +6187,7 @@
         <v>810</v>
       </c>
       <c r="C110" s="124" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6203,7 +6196,7 @@
         <v>814</v>
       </c>
       <c r="C111" s="124" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6212,7 +6205,7 @@
         <v>816</v>
       </c>
       <c r="C112" s="124" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6221,44 +6214,44 @@
         <v>817</v>
       </c>
       <c r="C113" s="124" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="117"/>
       <c r="B114" s="126" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C114" s="127" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="117"/>
       <c r="B115" s="126" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="C115" s="127" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="117"/>
       <c r="B116" s="121" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="C116" s="122" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="117">
         <v>3</v>
       </c>
-      <c r="B117" s="141" t="s">
-        <v>839</v>
-      </c>
-      <c r="C117" s="142"/>
+      <c r="B117" s="148" t="s">
+        <v>837</v>
+      </c>
+      <c r="C117" s="149"/>
     </row>
     <row r="118" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="117"/>
@@ -6266,7 +6259,7 @@
         <v>809</v>
       </c>
       <c r="C118" s="120" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6275,7 +6268,7 @@
         <v>810</v>
       </c>
       <c r="C119" s="124" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6293,7 +6286,7 @@
         <v>816</v>
       </c>
       <c r="C121" s="127" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6302,7 +6295,7 @@
         <v>817</v>
       </c>
       <c r="C122" s="127" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6314,10 +6307,10 @@
       <c r="A124" s="116">
         <v>4</v>
       </c>
-      <c r="B124" s="143" t="s">
-        <v>840</v>
-      </c>
-      <c r="C124" s="144"/>
+      <c r="B124" s="150" t="s">
+        <v>838</v>
+      </c>
+      <c r="C124" s="151"/>
     </row>
     <row r="125" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="125"/>
@@ -6325,7 +6318,7 @@
         <v>809</v>
       </c>
       <c r="C125" s="120" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6334,7 +6327,7 @@
         <v>810</v>
       </c>
       <c r="C126" s="124" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6343,7 +6336,7 @@
         <v>814</v>
       </c>
       <c r="C127" s="124" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6352,25 +6345,25 @@
         <v>816</v>
       </c>
       <c r="C128" s="122" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="145" t="s">
-        <v>888</v>
-      </c>
-      <c r="B130" s="146"/>
-      <c r="C130" s="147"/>
+      <c r="A130" s="139" t="s">
+        <v>886</v>
+      </c>
+      <c r="B130" s="140"/>
+      <c r="C130" s="141"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="116">
         <v>1</v>
       </c>
-      <c r="B131" s="148" t="s">
-        <v>889</v>
-      </c>
-      <c r="C131" s="149"/>
+      <c r="B131" s="142" t="s">
+        <v>887</v>
+      </c>
+      <c r="C131" s="143"/>
     </row>
     <row r="132" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="125"/>
@@ -6387,7 +6380,7 @@
         <v>810</v>
       </c>
       <c r="C133" s="129" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6396,7 +6389,7 @@
         <v>814</v>
       </c>
       <c r="C134" s="129" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6405,7 +6398,7 @@
         <v>816</v>
       </c>
       <c r="C135" s="129" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6418,98 +6411,98 @@
     <row r="137" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="125"/>
       <c r="B137" s="128" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C137" s="129"/>
     </row>
     <row r="138" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="125"/>
       <c r="B138" s="128" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="C138" s="129"/>
     </row>
     <row r="139" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="125"/>
       <c r="B139" s="128" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="C139" s="129"/>
     </row>
     <row r="140" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="125"/>
       <c r="B140" s="128" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="C140" s="129"/>
     </row>
     <row r="141" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="117"/>
       <c r="B141" s="123" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="C141" s="124"/>
     </row>
     <row r="142" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="117"/>
       <c r="B142" s="123" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="C142" s="124"/>
     </row>
     <row r="143" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="117"/>
       <c r="B143" s="123" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="C143" s="124"/>
     </row>
     <row r="144" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="117"/>
       <c r="B144" s="123" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="C144" s="124"/>
     </row>
     <row r="145" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="117"/>
       <c r="B145" s="123" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="C145" s="124"/>
     </row>
     <row r="146" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="117"/>
       <c r="B146" s="123" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="C146" s="124"/>
     </row>
     <row r="147" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="117"/>
       <c r="B147" s="123" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="C147" s="124"/>
     </row>
     <row r="148" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="117"/>
       <c r="B148" s="123" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="C148" s="124"/>
     </row>
     <row r="149" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="117"/>
       <c r="B149" s="123" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="C149" s="124"/>
     </row>
     <row r="150" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="117"/>
       <c r="B150" s="121" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="C150" s="122"/>
     </row>
@@ -6517,10 +6510,10 @@
       <c r="A151" s="117">
         <v>2</v>
       </c>
-      <c r="B151" s="139" t="s">
-        <v>890</v>
-      </c>
-      <c r="C151" s="140"/>
+      <c r="B151" s="146" t="s">
+        <v>888</v>
+      </c>
+      <c r="C151" s="147"/>
     </row>
     <row r="152" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="117"/>
@@ -6537,7 +6530,7 @@
         <v>810</v>
       </c>
       <c r="C153" s="124" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6546,7 +6539,7 @@
         <v>814</v>
       </c>
       <c r="C154" s="124" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6555,7 +6548,7 @@
         <v>816</v>
       </c>
       <c r="C155" s="124" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6568,21 +6561,21 @@
     <row r="157" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="117"/>
       <c r="B157" s="126" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C157" s="127"/>
     </row>
     <row r="158" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="117"/>
       <c r="B158" s="126" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="C158" s="127"/>
     </row>
     <row r="159" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="117"/>
       <c r="B159" s="121" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="C159" s="122"/>
     </row>
@@ -6590,10 +6583,10 @@
       <c r="A160" s="117">
         <v>3</v>
       </c>
-      <c r="B160" s="141" t="s">
-        <v>891</v>
-      </c>
-      <c r="C160" s="142"/>
+      <c r="B160" s="148" t="s">
+        <v>889</v>
+      </c>
+      <c r="C160" s="149"/>
     </row>
     <row r="161" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="117"/>
@@ -6601,7 +6594,7 @@
         <v>809</v>
       </c>
       <c r="C161" s="120" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6610,7 +6603,7 @@
         <v>810</v>
       </c>
       <c r="C162" s="124" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6619,7 +6612,7 @@
         <v>814</v>
       </c>
       <c r="C163" s="124" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6628,7 +6621,7 @@
         <v>816</v>
       </c>
       <c r="C164" s="127" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6641,34 +6634,30 @@
     <row r="166" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="117"/>
       <c r="B166" s="121" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C166" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="A130:C130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="A63:C63"/>
@@ -6681,24 +6670,28 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B160:C160"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="A130:C130"/>
-    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B18:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -12998,7 +12991,7 @@
         <v>679</v>
       </c>
       <c r="X54" s="45" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
@@ -13068,7 +13061,7 @@
         <v>679</v>
       </c>
       <c r="X55" s="45" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
@@ -13138,7 +13131,7 @@
         <v>679</v>
       </c>
       <c r="X56" s="45" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
@@ -13208,7 +13201,7 @@
         <v>679</v>
       </c>
       <c r="X57" s="45" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
@@ -13278,7 +13271,7 @@
         <v>679</v>
       </c>
       <c r="X58" s="45" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
@@ -22361,10 +22354,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="84" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="C16" s="44"/>
       <c r="D16" s="44"/>
@@ -22375,7 +22368,7 @@
       <c r="I16" s="44"/>
       <c r="J16" s="45"/>
       <c r="K16" s="90" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="L16" s="88"/>
     </row>
@@ -22643,7 +22636,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="84" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B30" s="49"/>
       <c r="C30" s="44"/>
@@ -22655,7 +22648,7 @@
       <c r="I30" s="44"/>
       <c r="J30" s="45"/>
       <c r="K30" s="90" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="L30" s="88">
         <v>3</v>
@@ -22743,7 +22736,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="84" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="B35" s="49"/>
       <c r="C35" s="44"/>
@@ -22755,13 +22748,13 @@
       <c r="I35" s="44"/>
       <c r="J35" s="45"/>
       <c r="K35" s="90" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="L35" s="88"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="84" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="B36" s="49"/>
       <c r="C36" s="44"/>
@@ -22773,7 +22766,7 @@
       <c r="I36" s="44"/>
       <c r="J36" s="45"/>
       <c r="K36" s="90" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="L36" s="88"/>
     </row>
@@ -22911,7 +22904,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="84" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="B44" s="49"/>
       <c r="C44" s="44"/>
@@ -22929,7 +22922,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="84" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="B45" s="49"/>
       <c r="C45" s="44"/>
@@ -22941,7 +22934,7 @@
       <c r="I45" s="44"/>
       <c r="J45" s="45"/>
       <c r="K45" s="90" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="L45" s="88">
         <v>3</v>
@@ -23607,7 +23600,7 @@
       <c r="I79" s="44"/>
       <c r="J79" s="45"/>
       <c r="K79" s="90" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="L79" s="88"/>
     </row>
@@ -23965,7 +23958,7 @@
         <v>372</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F3" s="130"/>
       <c r="G3" s="31"/>
@@ -23992,7 +23985,7 @@
         <v>382</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="F4" s="130"/>
       <c r="G4" s="31"/>
@@ -24108,7 +24101,7 @@
         <v>493</v>
       </c>
       <c r="E9" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="F9" s="135" t="s">
         <v>766</v>
@@ -24423,7 +24416,7 @@
         <v>488</v>
       </c>
       <c r="E24" s="135" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="L24" s="35">
         <v>4</v>
@@ -24501,7 +24494,7 @@
         <v>372</v>
       </c>
       <c r="E28" s="135" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="L28" s="35">
         <v>7</v>
@@ -24525,7 +24518,7 @@
         <v>422</v>
       </c>
       <c r="E29" s="135" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="L29" s="35">
         <v>0</v>
@@ -24546,13 +24539,13 @@
         <v>382</v>
       </c>
       <c r="E30" s="135" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="L30" s="35">
         <v>3</v>
       </c>
       <c r="M30" s="35" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -24787,7 +24780,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="130" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="B42" s="130" t="s">
         <v>603</v>
@@ -24796,12 +24789,12 @@
         <v>488</v>
       </c>
       <c r="M42" s="130" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="130" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="B43" s="130" t="s">
         <v>603</v>
@@ -24811,7 +24804,7 @@
       </c>
       <c r="L43" s="32"/>
       <c r="M43" s="130" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="N43"/>
     </row>
@@ -24826,22 +24819,22 @@
         <v>488</v>
       </c>
       <c r="M44" s="130" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="130" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="130" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="130" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="B47" s="130" t="s">
         <v>603</v>
@@ -24850,15 +24843,15 @@
         <v>488</v>
       </c>
       <c r="E47" s="130" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="M47" s="130" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="130" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="B48" s="130" t="s">
         <v>374</v>
@@ -24867,10 +24860,10 @@
         <v>488</v>
       </c>
       <c r="E48" s="130" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="M48" s="130" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="N48" s="34">
         <v>5</v>
@@ -24878,7 +24871,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="130" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="B49" s="130" t="s">
         <v>374</v>
@@ -24887,15 +24880,15 @@
         <v>488</v>
       </c>
       <c r="E49" s="130" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="M49" s="130" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="130" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="B50" s="130" t="s">
         <v>374</v>
@@ -24904,15 +24897,15 @@
         <v>488</v>
       </c>
       <c r="E50" s="130" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="M50" s="130" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="130" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="B51" s="130" t="s">
         <v>374</v>
@@ -24921,15 +24914,15 @@
         <v>488</v>
       </c>
       <c r="E51" s="130" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="M51" s="130" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="130" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="B52" s="130" t="s">
         <v>374</v>
@@ -24938,10 +24931,10 @@
         <v>488</v>
       </c>
       <c r="E52" s="130" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="M52" s="130" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="N52" s="34">
         <v>5</v>
@@ -24958,12 +24951,12 @@
         <v>488</v>
       </c>
       <c r="M53" s="131" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="131" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="B54" s="131" t="s">
         <v>603</v>
@@ -24972,41 +24965,41 @@
         <v>488</v>
       </c>
       <c r="M54" s="131" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="131" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="B55" s="131" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="D55" s="131" t="s">
         <v>488</v>
       </c>
       <c r="E55" s="131" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="M55" s="131" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="131" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="B56" s="131" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="D56" s="131" t="s">
         <v>488</v>
       </c>
       <c r="E56" s="131" t="s">
+        <v>955</v>
+      </c>
+      <c r="M56" s="131" t="s">
         <v>957</v>
-      </c>
-      <c r="M56" s="131" t="s">
-        <v>959</v>
       </c>
       <c r="N56" s="34">
         <v>3</v>
@@ -25014,7 +25007,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="133" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="B57" s="133" t="s">
         <v>374</v>
@@ -25023,10 +25016,10 @@
         <v>488</v>
       </c>
       <c r="E57" s="133" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="M57" s="133" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="N57" s="34">
         <v>3</v>
@@ -25034,7 +25027,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="133" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B58" s="133" t="s">
         <v>374</v>
@@ -25043,10 +25036,10 @@
         <v>488</v>
       </c>
       <c r="E58" s="133" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="M58" s="133" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="N58" s="34">
         <v>3</v>
@@ -25054,7 +25047,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="133" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="B59" s="133" t="s">
         <v>374</v>
@@ -25063,10 +25056,10 @@
         <v>488</v>
       </c>
       <c r="E59" s="133" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="M59" s="133" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="N59" s="34">
         <v>3</v>
@@ -25074,7 +25067,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="135" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="B60" s="135" t="s">
         <v>374</v>
@@ -25083,10 +25076,10 @@
         <v>422</v>
       </c>
       <c r="E60" s="135" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="M60" s="135" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="N60" s="34">
         <v>3</v>
@@ -25094,7 +25087,7 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="136" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="B61" s="136" t="s">
         <v>375</v>
@@ -25103,16 +25096,16 @@
         <v>493</v>
       </c>
       <c r="E61" s="136" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="F61" s="136" t="s">
         <v>766</v>
       </c>
       <c r="G61" s="136" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="M61" s="136" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="N61" s="34">
         <v>3</v>
@@ -25120,7 +25113,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="136" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="B62" s="136" t="s">
         <v>375</v>
@@ -25129,30 +25122,30 @@
         <v>493</v>
       </c>
       <c r="E62" s="136" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="F62" s="136" t="s">
         <v>766</v>
       </c>
       <c r="M62" s="136" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="136" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B63" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D63" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E63" s="136" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="M63" s="136" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="N63" s="34">
         <v>3</v>
@@ -25160,19 +25153,19 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="136" t="s">
+        <v>984</v>
+      </c>
+      <c r="B64" s="136" t="s">
         <v>986</v>
-      </c>
-      <c r="B64" s="136" t="s">
-        <v>988</v>
       </c>
       <c r="D64" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E64" s="136" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="M64" s="136" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="N64" s="34">
         <v>3</v>
@@ -25180,53 +25173,53 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="136" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="B65" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D65" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E65" s="136" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="M65" s="136" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="136" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B66" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D66" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E66" s="136" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="M66" s="136" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="136" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B67" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D67" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E67" s="136" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="M67" s="136" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="N67" s="34">
         <v>3</v>
@@ -25234,19 +25227,19 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="136" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="B68" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D68" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E68" s="136" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="M68" s="136" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="N68" s="34">
         <v>3</v>
@@ -25254,19 +25247,19 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="136" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="B69" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D69" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E69" s="136" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="M69" s="137" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="N69" s="138">
         <v>3</v>
@@ -25276,19 +25269,19 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="136" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="B70" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D70" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E70" s="136" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="M70" s="136" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="N70" s="34">
         <v>3</v>
@@ -25296,19 +25289,19 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="136" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="B71" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D71" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E71" s="136" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="M71" s="136" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="N71" s="34">
         <v>3</v>
@@ -25316,19 +25309,19 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="136" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="B72" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D72" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E72" s="136" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="M72" s="136" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="N72" s="34">
         <v>3</v>
@@ -25336,19 +25329,19 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="136" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="B73" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D73" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E73" s="136" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="M73" s="136" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="N73" s="34">
         <v>3</v>
@@ -25356,53 +25349,53 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="136" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="B74" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D74" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E74" s="136" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="M74" s="136" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="136" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="B75" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D75" s="136" t="s">
         <v>382</v>
       </c>
       <c r="E75" s="136" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="M75" s="136" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="136" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B76" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D76" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E76" s="136" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="M76" s="136" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="N76" s="34">
         <v>3</v>
@@ -25410,19 +25403,19 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="136" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="B77" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D77" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E77" s="136" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="M77" s="136" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="N77" s="34">
         <v>3</v>
@@ -25430,19 +25423,19 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="136" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="B78" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D78" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E78" s="136" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="M78" s="136" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="N78" s="34">
         <v>4</v>
@@ -25450,19 +25443,19 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="136" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="B79" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D79" s="136" t="s">
         <v>422</v>
       </c>
       <c r="E79" s="136" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="M79" s="136" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="N79" s="34">
         <v>3</v>
@@ -25470,36 +25463,36 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="136" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="B80" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D80" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E80" s="136" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="M80" s="136" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="136" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="B81" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D81" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E81" s="136" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="M81" s="136" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="N81" s="34">
         <v>3</v>
@@ -25507,19 +25500,19 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="136" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="B82" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D82" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E82" s="136" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="M82" s="136" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
@@ -25527,16 +25520,16 @@
         <v>483</v>
       </c>
       <c r="B83" s="136" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D83" s="136" t="s">
         <v>488</v>
       </c>
       <c r="E83" s="136" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="M83" s="136" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
     </row>
   </sheetData>
@@ -26702,10 +26695,10 @@
     </row>
     <row r="19" spans="1:15" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="105" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -27212,7 +27205,7 @@
         <v>278</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -27465,19 +27458,19 @@
         <v>794</v>
       </c>
       <c r="K61" s="77" t="s">
+        <v>934</v>
+      </c>
+      <c r="L61" s="77" t="s">
+        <v>935</v>
+      </c>
+      <c r="M61" s="77" t="s">
         <v>936</v>
       </c>
-      <c r="L61" s="77" t="s">
+      <c r="N61" s="77" t="s">
         <v>937</v>
       </c>
-      <c r="M61" s="77" t="s">
+      <c r="O61" s="75" t="s">
         <v>938</v>
-      </c>
-      <c r="N61" s="77" t="s">
-        <v>939</v>
-      </c>
-      <c r="O61" s="75" t="s">
-        <v>940</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Adding melee check to surrounded/melee bonus
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -642,7 +642,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2172" uniqueCount="1035">
   <si>
     <t>Fishing</t>
   </si>
@@ -3741,6 +3741,12 @@
   </si>
   <si>
     <t>attack of opportunity</t>
+  </si>
+  <si>
+    <t>Make Injuries recalculate stats</t>
+  </si>
+  <si>
+    <t>bullets hitting random targets</t>
   </si>
 </sst>
 </file>
@@ -3840,7 +3846,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="56">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -4593,11 +4599,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4915,6 +4943,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4934,24 +4980,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4998,6 +5026,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5300,10 +5334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C166"/>
+  <dimension ref="A1:C167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5318,29 +5352,29 @@
       <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="139" t="s">
+      <c r="A2" s="145" t="s">
         <v>803</v>
       </c>
-      <c r="B2" s="140"/>
-      <c r="C2" s="141"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="147"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="116">
         <v>1</v>
       </c>
-      <c r="B3" s="142" t="s">
+      <c r="B3" s="148" t="s">
         <v>804</v>
       </c>
-      <c r="C3" s="143"/>
+      <c r="C3" s="149"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="117">
         <v>2</v>
       </c>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="139" t="s">
         <v>805</v>
       </c>
-      <c r="C4" s="147"/>
+      <c r="C4" s="140"/>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="117"/>
@@ -5391,10 +5425,10 @@
       <c r="A10" s="117">
         <v>3</v>
       </c>
-      <c r="B10" s="148" t="s">
+      <c r="B10" s="141" t="s">
         <v>806</v>
       </c>
-      <c r="C10" s="149"/>
+      <c r="C10" s="142"/>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="117"/>
@@ -5409,10 +5443,10 @@
       <c r="A12" s="117">
         <v>4</v>
       </c>
-      <c r="B12" s="150" t="s">
+      <c r="B12" s="143" t="s">
         <v>807</v>
       </c>
-      <c r="C12" s="151"/>
+      <c r="C12" s="144"/>
     </row>
     <row r="13" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="117"/>
@@ -5427,10 +5461,10 @@
       <c r="A14" s="117">
         <v>5</v>
       </c>
-      <c r="B14" s="150" t="s">
+      <c r="B14" s="143" t="s">
         <v>808</v>
       </c>
-      <c r="C14" s="151"/>
+      <c r="C14" s="144"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="117"/>
@@ -5445,10 +5479,10 @@
       <c r="A16" s="118">
         <v>6</v>
       </c>
-      <c r="B16" s="144" t="s">
+      <c r="B16" s="150" t="s">
         <v>812</v>
       </c>
-      <c r="C16" s="145"/>
+      <c r="C16" s="151"/>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="117"/>
@@ -5463,36 +5497,36 @@
       <c r="A18" s="118">
         <v>7</v>
       </c>
-      <c r="B18" s="144" t="s">
+      <c r="B18" s="150" t="s">
         <v>942</v>
       </c>
-      <c r="C18" s="145"/>
+      <c r="C18" s="151"/>
     </row>
     <row r="19" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="134">
         <v>8</v>
       </c>
-      <c r="B19" s="144" t="s">
+      <c r="B19" s="150" t="s">
         <v>943</v>
       </c>
-      <c r="C19" s="145"/>
+      <c r="C19" s="151"/>
     </row>
     <row r="20" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="139" t="s">
+      <c r="A21" s="145" t="s">
         <v>183</v>
       </c>
-      <c r="B21" s="140"/>
-      <c r="C21" s="141"/>
+      <c r="B21" s="146"/>
+      <c r="C21" s="147"/>
     </row>
     <row r="22" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="116">
         <v>1</v>
       </c>
-      <c r="B22" s="142" t="s">
+      <c r="B22" s="148" t="s">
         <v>813</v>
       </c>
-      <c r="C22" s="143"/>
+      <c r="C22" s="149"/>
     </row>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="117"/>
@@ -5568,20 +5602,20 @@
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="139" t="s">
+      <c r="A32" s="145" t="s">
         <v>815</v>
       </c>
-      <c r="B32" s="140"/>
-      <c r="C32" s="141"/>
+      <c r="B32" s="146"/>
+      <c r="C32" s="147"/>
     </row>
     <row r="33" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="116">
         <v>1</v>
       </c>
-      <c r="B33" s="142" t="s">
+      <c r="B33" s="148" t="s">
         <v>803</v>
       </c>
-      <c r="C33" s="143"/>
+      <c r="C33" s="149"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="117"/>
@@ -5594,17 +5628,21 @@
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="117"/>
-      <c r="B35" s="123"/>
-      <c r="C35" s="124"/>
+      <c r="B35" s="123" t="s">
+        <v>810</v>
+      </c>
+      <c r="C35" s="124" t="s">
+        <v>1034</v>
+      </c>
     </row>
     <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="117">
         <v>2</v>
       </c>
-      <c r="B36" s="146" t="s">
+      <c r="B36" s="139" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="147"/>
+      <c r="C36" s="140"/>
     </row>
     <row r="37" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="117"/>
@@ -5624,1063 +5662,1031 @@
       <c r="A39" s="117">
         <v>2</v>
       </c>
-      <c r="B39" s="146" t="s">
+      <c r="B39" s="139" t="s">
         <v>939</v>
       </c>
-      <c r="C39" s="147"/>
+      <c r="C39" s="140"/>
     </row>
     <row r="40" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="117"/>
-      <c r="B40" s="119" t="s">
-        <v>809</v>
+      <c r="B40" s="119">
+        <v>1</v>
       </c>
       <c r="C40" s="120" t="s">
         <v>940</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="117"/>
-      <c r="B41" s="121" t="s">
-        <v>810</v>
-      </c>
-      <c r="C41" s="132" t="s">
+      <c r="B41" s="167">
+        <v>2</v>
+      </c>
+      <c r="C41" s="168" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="117"/>
+      <c r="B42" s="121">
+        <v>3</v>
+      </c>
+      <c r="C42" s="132" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="139" t="s">
+    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="145" t="s">
         <v>820</v>
       </c>
-      <c r="B43" s="140"/>
-      <c r="C43" s="141"/>
-    </row>
-    <row r="44" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="116">
-        <v>1</v>
-      </c>
-      <c r="B44" s="142" t="s">
+      <c r="B44" s="146"/>
+      <c r="C44" s="147"/>
+    </row>
+    <row r="45" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="116">
+        <v>1</v>
+      </c>
+      <c r="B45" s="148" t="s">
         <v>821</v>
       </c>
-      <c r="C44" s="143"/>
-    </row>
-    <row r="45" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="117"/>
-      <c r="B45" s="119" t="s">
+      <c r="C45" s="149"/>
+    </row>
+    <row r="46" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="117"/>
+      <c r="B46" s="119" t="s">
         <v>809</v>
       </c>
-      <c r="C45" s="120" t="s">
+      <c r="C46" s="120" t="s">
         <v>547</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="117"/>
-      <c r="B46" s="123" t="s">
-        <v>810</v>
-      </c>
-      <c r="C46" s="124" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="117"/>
       <c r="B47" s="123" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C47" s="124" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="117"/>
-      <c r="B48" s="121" t="s">
+      <c r="B48" s="123" t="s">
+        <v>814</v>
+      </c>
+      <c r="C48" s="124" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="117"/>
+      <c r="B49" s="121" t="s">
         <v>816</v>
       </c>
-      <c r="C48" s="122" t="s">
+      <c r="C49" s="122" t="s">
         <v>824</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="139" t="s">
+    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="145" t="s">
         <v>825</v>
       </c>
-      <c r="B50" s="140"/>
-      <c r="C50" s="141"/>
-    </row>
-    <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="116">
-        <v>1</v>
-      </c>
-      <c r="B51" s="142" t="s">
+      <c r="B51" s="146"/>
+      <c r="C51" s="147"/>
+    </row>
+    <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="116">
+        <v>1</v>
+      </c>
+      <c r="B52" s="148" t="s">
         <v>826</v>
       </c>
-      <c r="C51" s="143"/>
-    </row>
-    <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="117"/>
-      <c r="B52" s="119" t="s">
+      <c r="C52" s="149"/>
+    </row>
+    <row r="53" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="117"/>
+      <c r="B53" s="119" t="s">
         <v>809</v>
       </c>
-      <c r="C52" s="120" t="s">
+      <c r="C53" s="120" t="s">
         <v>827</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="125"/>
-      <c r="B53" s="121" t="s">
+    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="125"/>
+      <c r="B54" s="121" t="s">
         <v>810</v>
       </c>
-      <c r="C53" s="122" t="s">
+      <c r="C54" s="122" t="s">
         <v>832</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="116">
-        <v>1</v>
-      </c>
-      <c r="B54" s="142" t="s">
+    <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="116">
+        <v>1</v>
+      </c>
+      <c r="B55" s="148" t="s">
         <v>828</v>
       </c>
-      <c r="C54" s="143"/>
-    </row>
-    <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="117"/>
-      <c r="B55" s="119" t="s">
+      <c r="C55" s="149"/>
+    </row>
+    <row r="56" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="117"/>
+      <c r="B56" s="119" t="s">
         <v>809</v>
       </c>
-      <c r="C55" s="120" t="s">
+      <c r="C56" s="120" t="s">
         <v>829</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="117"/>
-      <c r="B56" s="123" t="s">
-        <v>810</v>
-      </c>
-      <c r="C56" s="124" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="117"/>
       <c r="B57" s="123" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C57" s="124" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="117"/>
-      <c r="B58" s="121"/>
-      <c r="C58" s="122"/>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="139" t="s">
+      <c r="B58" s="123" t="s">
+        <v>814</v>
+      </c>
+      <c r="C58" s="124" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="117"/>
+      <c r="B59" s="121"/>
+      <c r="C59" s="122"/>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="145" t="s">
         <v>188</v>
       </c>
-      <c r="B60" s="140"/>
-      <c r="C60" s="141"/>
-    </row>
-    <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="116">
-        <v>1</v>
-      </c>
-      <c r="B61" s="142" t="s">
+      <c r="B61" s="146"/>
+      <c r="C61" s="147"/>
+    </row>
+    <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="116">
+        <v>1</v>
+      </c>
+      <c r="B62" s="148" t="s">
         <v>833</v>
       </c>
-      <c r="C61" s="143"/>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="139" t="s">
+      <c r="C62" s="149"/>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="145" t="s">
         <v>811</v>
       </c>
-      <c r="B63" s="140"/>
-      <c r="C63" s="141"/>
-    </row>
-    <row r="64" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="116">
-        <v>1</v>
-      </c>
-      <c r="B64" s="148" t="s">
+      <c r="B64" s="146"/>
+      <c r="C64" s="147"/>
+    </row>
+    <row r="65" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="116">
+        <v>1</v>
+      </c>
+      <c r="B65" s="141" t="s">
         <v>804</v>
       </c>
-      <c r="C64" s="149"/>
-    </row>
-    <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="117">
-        <v>2</v>
-      </c>
-      <c r="B65" s="152" t="s">
-        <v>805</v>
-      </c>
-      <c r="C65" s="153"/>
+      <c r="C65" s="142"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="117">
-        <v>3</v>
-      </c>
-      <c r="B66" s="150" t="s">
-        <v>806</v>
-      </c>
-      <c r="C66" s="151"/>
+        <v>2</v>
+      </c>
+      <c r="B66" s="152" t="s">
+        <v>805</v>
+      </c>
+      <c r="C66" s="153"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="117">
-        <v>4</v>
-      </c>
-      <c r="B67" s="150" t="s">
-        <v>807</v>
-      </c>
-      <c r="C67" s="151"/>
+        <v>3</v>
+      </c>
+      <c r="B67" s="143" t="s">
+        <v>806</v>
+      </c>
+      <c r="C67" s="144"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="117">
+        <v>4</v>
+      </c>
+      <c r="B68" s="143" t="s">
+        <v>807</v>
+      </c>
+      <c r="C68" s="144"/>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="117">
         <v>5</v>
       </c>
-      <c r="B68" s="150" t="s">
+      <c r="B69" s="143" t="s">
         <v>808</v>
       </c>
-      <c r="C68" s="151"/>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="118">
+      <c r="C69" s="144"/>
+    </row>
+    <row r="70" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="118">
         <v>6</v>
       </c>
-      <c r="B69" s="144" t="s">
+      <c r="B70" s="150" t="s">
         <v>812</v>
       </c>
-      <c r="C69" s="145"/>
-    </row>
-    <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="139" t="s">
+      <c r="C70" s="151"/>
+    </row>
+    <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="145" t="s">
         <v>834</v>
       </c>
-      <c r="B71" s="140"/>
-      <c r="C71" s="141"/>
-    </row>
-    <row r="72" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="116">
-        <v>1</v>
-      </c>
-      <c r="B72" s="148" t="s">
+      <c r="B72" s="146"/>
+      <c r="C72" s="147"/>
+    </row>
+    <row r="73" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="116">
+        <v>1</v>
+      </c>
+      <c r="B73" s="141" t="s">
         <v>804</v>
       </c>
-      <c r="C72" s="149"/>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="117">
-        <v>2</v>
-      </c>
-      <c r="B73" s="152" t="s">
-        <v>805</v>
-      </c>
-      <c r="C73" s="153"/>
+      <c r="C73" s="142"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="117">
-        <v>3</v>
-      </c>
-      <c r="B74" s="150" t="s">
-        <v>806</v>
-      </c>
-      <c r="C74" s="151"/>
+        <v>2</v>
+      </c>
+      <c r="B74" s="152" t="s">
+        <v>805</v>
+      </c>
+      <c r="C74" s="153"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="117">
-        <v>4</v>
-      </c>
-      <c r="B75" s="150" t="s">
-        <v>807</v>
-      </c>
-      <c r="C75" s="151"/>
+        <v>3</v>
+      </c>
+      <c r="B75" s="143" t="s">
+        <v>806</v>
+      </c>
+      <c r="C75" s="144"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="117">
+        <v>4</v>
+      </c>
+      <c r="B76" s="143" t="s">
+        <v>807</v>
+      </c>
+      <c r="C76" s="144"/>
+    </row>
+    <row r="77" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="117">
         <v>5</v>
       </c>
-      <c r="B76" s="150" t="s">
+      <c r="B77" s="143" t="s">
         <v>808</v>
       </c>
-      <c r="C76" s="151"/>
-    </row>
-    <row r="77" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="118">
+      <c r="C77" s="144"/>
+    </row>
+    <row r="78" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="118">
         <v>6</v>
       </c>
-      <c r="B77" s="144" t="s">
+      <c r="B78" s="150" t="s">
         <v>812</v>
       </c>
-      <c r="C77" s="145"/>
-    </row>
-    <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="139" t="s">
+      <c r="C78" s="151"/>
+    </row>
+    <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="145" t="s">
         <v>835</v>
       </c>
-      <c r="B79" s="140"/>
-      <c r="C79" s="141"/>
-    </row>
-    <row r="80" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="116">
-        <v>1</v>
-      </c>
-      <c r="B80" s="148" t="s">
+      <c r="B80" s="146"/>
+      <c r="C80" s="147"/>
+    </row>
+    <row r="81" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="116">
+        <v>1</v>
+      </c>
+      <c r="B81" s="141" t="s">
         <v>804</v>
       </c>
-      <c r="C80" s="149"/>
-    </row>
-    <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="117">
-        <v>2</v>
-      </c>
-      <c r="B81" s="152" t="s">
-        <v>805</v>
-      </c>
-      <c r="C81" s="153"/>
+      <c r="C81" s="142"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="117">
-        <v>3</v>
-      </c>
-      <c r="B82" s="150" t="s">
-        <v>806</v>
-      </c>
-      <c r="C82" s="151"/>
+        <v>2</v>
+      </c>
+      <c r="B82" s="152" t="s">
+        <v>805</v>
+      </c>
+      <c r="C82" s="153"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="117">
-        <v>4</v>
-      </c>
-      <c r="B83" s="150" t="s">
-        <v>807</v>
-      </c>
-      <c r="C83" s="151"/>
+        <v>3</v>
+      </c>
+      <c r="B83" s="143" t="s">
+        <v>806</v>
+      </c>
+      <c r="C83" s="144"/>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="117">
+        <v>4</v>
+      </c>
+      <c r="B84" s="143" t="s">
+        <v>807</v>
+      </c>
+      <c r="C84" s="144"/>
+    </row>
+    <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="117">
         <v>5</v>
       </c>
-      <c r="B84" s="150" t="s">
+      <c r="B85" s="143" t="s">
         <v>808</v>
       </c>
-      <c r="C84" s="151"/>
-    </row>
-    <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="118">
+      <c r="C85" s="144"/>
+    </row>
+    <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="118">
         <v>6</v>
       </c>
-      <c r="B85" s="144" t="s">
+      <c r="B86" s="150" t="s">
         <v>812</v>
       </c>
-      <c r="C85" s="145"/>
-    </row>
-    <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="139" t="s">
+      <c r="C86" s="151"/>
+    </row>
+    <row r="87" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="145" t="s">
         <v>885</v>
       </c>
-      <c r="B87" s="140"/>
-      <c r="C87" s="141"/>
-    </row>
-    <row r="88" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="116">
-        <v>1</v>
-      </c>
-      <c r="B88" s="142" t="s">
+      <c r="B88" s="146"/>
+      <c r="C88" s="147"/>
+    </row>
+    <row r="89" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="116">
+        <v>1</v>
+      </c>
+      <c r="B89" s="148" t="s">
         <v>101</v>
       </c>
-      <c r="C88" s="143"/>
-    </row>
-    <row r="89" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="125"/>
-      <c r="B89" s="119" t="s">
+      <c r="C89" s="149"/>
+    </row>
+    <row r="90" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="125"/>
+      <c r="B90" s="119" t="s">
         <v>809</v>
       </c>
-      <c r="C89" s="120" t="s">
+      <c r="C90" s="120" t="s">
         <v>862</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="125"/>
-      <c r="B90" s="128" t="s">
-        <v>810</v>
-      </c>
-      <c r="C90" s="129" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="125"/>
       <c r="B91" s="128" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C91" s="129" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="125"/>
       <c r="B92" s="128" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="C92" s="129" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="125"/>
       <c r="B93" s="128" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C93" s="129" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="125"/>
       <c r="B94" s="128" t="s">
-        <v>846</v>
+        <v>817</v>
       </c>
       <c r="C94" s="129" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="125"/>
       <c r="B95" s="128" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C95" s="129" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="125"/>
       <c r="B96" s="128" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="C96" s="129" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="125"/>
       <c r="B97" s="128" t="s">
+        <v>850</v>
+      </c>
+      <c r="C97" s="129" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="125"/>
+      <c r="B98" s="128" t="s">
         <v>851</v>
       </c>
-      <c r="C97" s="129" t="s">
+      <c r="C98" s="129" t="s">
         <v>870</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="117"/>
-      <c r="B98" s="123" t="s">
-        <v>852</v>
-      </c>
-      <c r="C98" s="124" t="s">
-        <v>871</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="117"/>
       <c r="B99" s="123" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C99" s="124" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="117"/>
       <c r="B100" s="123" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C100" s="124" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="117"/>
       <c r="B101" s="123" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C101" s="124" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="117"/>
       <c r="B102" s="123" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C102" s="124" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="117"/>
       <c r="B103" s="123" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C103" s="124" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="117"/>
       <c r="B104" s="123" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C104" s="124" t="s">
-        <v>35</v>
+        <v>876</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="117"/>
       <c r="B105" s="123" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C105" s="124" t="s">
-        <v>877</v>
+        <v>35</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="117"/>
       <c r="B106" s="123" t="s">
-        <v>860</v>
-      </c>
-      <c r="C106" s="124"/>
+        <v>859</v>
+      </c>
+      <c r="C106" s="124" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="107" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="117"/>
-      <c r="B107" s="121" t="s">
+      <c r="B107" s="123" t="s">
+        <v>860</v>
+      </c>
+      <c r="C107" s="124"/>
+    </row>
+    <row r="108" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="117"/>
+      <c r="B108" s="121" t="s">
         <v>861</v>
       </c>
-      <c r="C107" s="122"/>
-    </row>
-    <row r="108" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="117">
+      <c r="C108" s="122"/>
+    </row>
+    <row r="109" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="117">
         <v>2</v>
       </c>
-      <c r="B108" s="146" t="s">
+      <c r="B109" s="139" t="s">
         <v>836</v>
       </c>
-      <c r="C108" s="147"/>
-    </row>
-    <row r="109" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="117"/>
-      <c r="B109" s="119" t="s">
+      <c r="C109" s="140"/>
+    </row>
+    <row r="110" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="117"/>
+      <c r="B110" s="119" t="s">
         <v>809</v>
       </c>
-      <c r="C109" s="120" t="s">
+      <c r="C110" s="120" t="s">
         <v>849</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="117"/>
-      <c r="B110" s="123" t="s">
-        <v>810</v>
-      </c>
-      <c r="C110" s="124" t="s">
-        <v>878</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="117"/>
       <c r="B111" s="123" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C111" s="124" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="117"/>
       <c r="B112" s="123" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="C112" s="124" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="117"/>
       <c r="B113" s="123" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C113" s="124" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="117"/>
-      <c r="B114" s="126" t="s">
-        <v>846</v>
-      </c>
-      <c r="C114" s="127" t="s">
-        <v>882</v>
+      <c r="B114" s="123" t="s">
+        <v>817</v>
+      </c>
+      <c r="C114" s="124" t="s">
+        <v>881</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="117"/>
       <c r="B115" s="126" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C115" s="127" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="117"/>
-      <c r="B116" s="121" t="s">
+      <c r="B116" s="126" t="s">
+        <v>848</v>
+      </c>
+      <c r="C116" s="127" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="117"/>
+      <c r="B117" s="121" t="s">
         <v>850</v>
       </c>
-      <c r="C116" s="122" t="s">
+      <c r="C117" s="122" t="s">
         <v>884</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="117">
+    <row r="118" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="117">
         <v>3</v>
       </c>
-      <c r="B117" s="148" t="s">
+      <c r="B118" s="141" t="s">
         <v>837</v>
       </c>
-      <c r="C117" s="149"/>
-    </row>
-    <row r="118" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="117"/>
-      <c r="B118" s="119" t="s">
+      <c r="C118" s="142"/>
+    </row>
+    <row r="119" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="117"/>
+      <c r="B119" s="119" t="s">
         <v>809</v>
       </c>
-      <c r="C118" s="120" t="s">
+      <c r="C119" s="120" t="s">
         <v>843</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="117"/>
-      <c r="B119" s="123" t="s">
-        <v>810</v>
-      </c>
-      <c r="C119" s="124" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="117"/>
       <c r="B120" s="123" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C120" s="124" t="s">
-        <v>89</v>
+        <v>844</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="117"/>
-      <c r="B121" s="126" t="s">
-        <v>816</v>
-      </c>
-      <c r="C121" s="127" t="s">
-        <v>845</v>
+      <c r="B121" s="123" t="s">
+        <v>814</v>
+      </c>
+      <c r="C121" s="124" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="117"/>
       <c r="B122" s="126" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C122" s="127" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="117"/>
-      <c r="B123" s="121"/>
-      <c r="C123" s="122"/>
-    </row>
-    <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="116">
+      <c r="B123" s="126" t="s">
+        <v>817</v>
+      </c>
+      <c r="C123" s="127" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="117"/>
+      <c r="B124" s="121"/>
+      <c r="C124" s="122"/>
+    </row>
+    <row r="125" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="116">
         <v>4</v>
       </c>
-      <c r="B124" s="150" t="s">
+      <c r="B125" s="143" t="s">
         <v>838</v>
       </c>
-      <c r="C124" s="151"/>
-    </row>
-    <row r="125" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="125"/>
-      <c r="B125" s="119" t="s">
+      <c r="C125" s="144"/>
+    </row>
+    <row r="126" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="125"/>
+      <c r="B126" s="119" t="s">
         <v>809</v>
       </c>
-      <c r="C125" s="120" t="s">
+      <c r="C126" s="120" t="s">
         <v>839</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="117"/>
-      <c r="B126" s="123" t="s">
-        <v>810</v>
-      </c>
-      <c r="C126" s="124" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="117"/>
       <c r="B127" s="123" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C127" s="124" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="117"/>
-      <c r="B128" s="121" t="s">
+      <c r="B128" s="123" t="s">
+        <v>814</v>
+      </c>
+      <c r="C128" s="124" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="117"/>
+      <c r="B129" s="121" t="s">
         <v>816</v>
       </c>
-      <c r="C128" s="122" t="s">
+      <c r="C129" s="122" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="130" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="139" t="s">
+    <row r="130" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="145" t="s">
         <v>886</v>
       </c>
-      <c r="B130" s="140"/>
-      <c r="C130" s="141"/>
-    </row>
-    <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="116">
-        <v>1</v>
-      </c>
-      <c r="B131" s="142" t="s">
+      <c r="B131" s="146"/>
+      <c r="C131" s="147"/>
+    </row>
+    <row r="132" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="116">
+        <v>1</v>
+      </c>
+      <c r="B132" s="148" t="s">
         <v>887</v>
       </c>
-      <c r="C131" s="143"/>
-    </row>
-    <row r="132" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="125"/>
-      <c r="B132" s="119" t="s">
+      <c r="C132" s="149"/>
+    </row>
+    <row r="133" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="125"/>
+      <c r="B133" s="119" t="s">
         <v>809</v>
       </c>
-      <c r="C132" s="120" t="s">
+      <c r="C133" s="120" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="125"/>
-      <c r="B133" s="128" t="s">
-        <v>810</v>
-      </c>
-      <c r="C133" s="129" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="125"/>
       <c r="B134" s="128" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C134" s="129" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="125"/>
       <c r="B135" s="128" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="C135" s="129" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="125"/>
       <c r="B136" s="128" t="s">
-        <v>817</v>
-      </c>
-      <c r="C136" s="129"/>
+        <v>816</v>
+      </c>
+      <c r="C136" s="129" t="s">
+        <v>838</v>
+      </c>
     </row>
     <row r="137" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="125"/>
       <c r="B137" s="128" t="s">
-        <v>846</v>
+        <v>817</v>
       </c>
       <c r="C137" s="129"/>
     </row>
     <row r="138" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="125"/>
       <c r="B138" s="128" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C138" s="129"/>
     </row>
     <row r="139" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="125"/>
       <c r="B139" s="128" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="C139" s="129"/>
     </row>
     <row r="140" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="125"/>
       <c r="B140" s="128" t="s">
+        <v>850</v>
+      </c>
+      <c r="C140" s="129"/>
+    </row>
+    <row r="141" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="125"/>
+      <c r="B141" s="128" t="s">
         <v>851</v>
       </c>
-      <c r="C140" s="129"/>
-    </row>
-    <row r="141" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="117"/>
-      <c r="B141" s="123" t="s">
-        <v>852</v>
-      </c>
-      <c r="C141" s="124"/>
+      <c r="C141" s="129"/>
     </row>
     <row r="142" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="117"/>
       <c r="B142" s="123" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C142" s="124"/>
     </row>
     <row r="143" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="117"/>
       <c r="B143" s="123" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C143" s="124"/>
     </row>
     <row r="144" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="117"/>
       <c r="B144" s="123" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C144" s="124"/>
     </row>
     <row r="145" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="117"/>
       <c r="B145" s="123" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C145" s="124"/>
     </row>
     <row r="146" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="117"/>
       <c r="B146" s="123" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C146" s="124"/>
     </row>
     <row r="147" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="117"/>
       <c r="B147" s="123" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C147" s="124"/>
     </row>
     <row r="148" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="117"/>
       <c r="B148" s="123" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C148" s="124"/>
     </row>
     <row r="149" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="117"/>
       <c r="B149" s="123" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C149" s="124"/>
     </row>
     <row r="150" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="117"/>
-      <c r="B150" s="121" t="s">
+      <c r="B150" s="123" t="s">
+        <v>860</v>
+      </c>
+      <c r="C150" s="124"/>
+    </row>
+    <row r="151" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="117"/>
+      <c r="B151" s="121" t="s">
         <v>861</v>
       </c>
-      <c r="C150" s="122"/>
-    </row>
-    <row r="151" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="117">
+      <c r="C151" s="122"/>
+    </row>
+    <row r="152" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="117">
         <v>2</v>
       </c>
-      <c r="B151" s="146" t="s">
+      <c r="B152" s="139" t="s">
         <v>888</v>
       </c>
-      <c r="C151" s="147"/>
-    </row>
-    <row r="152" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="117"/>
-      <c r="B152" s="119" t="s">
+      <c r="C152" s="140"/>
+    </row>
+    <row r="153" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="117"/>
+      <c r="B153" s="119" t="s">
         <v>809</v>
       </c>
-      <c r="C152" s="120" t="s">
+      <c r="C153" s="120" t="s">
         <v>241</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="117"/>
-      <c r="B153" s="123" t="s">
-        <v>810</v>
-      </c>
-      <c r="C153" s="124" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="117"/>
       <c r="B154" s="123" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C154" s="124" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="117"/>
       <c r="B155" s="123" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="C155" s="124" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="117"/>
       <c r="B156" s="123" t="s">
-        <v>817</v>
-      </c>
-      <c r="C156" s="124"/>
+        <v>816</v>
+      </c>
+      <c r="C156" s="124" t="s">
+        <v>892</v>
+      </c>
     </row>
     <row r="157" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="117"/>
-      <c r="B157" s="126" t="s">
-        <v>846</v>
-      </c>
-      <c r="C157" s="127"/>
+      <c r="B157" s="123" t="s">
+        <v>817</v>
+      </c>
+      <c r="C157" s="124"/>
     </row>
     <row r="158" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="117"/>
       <c r="B158" s="126" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C158" s="127"/>
     </row>
     <row r="159" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="117"/>
-      <c r="B159" s="121" t="s">
+      <c r="B159" s="126" t="s">
+        <v>848</v>
+      </c>
+      <c r="C159" s="127"/>
+    </row>
+    <row r="160" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="117"/>
+      <c r="B160" s="121" t="s">
         <v>850</v>
       </c>
-      <c r="C159" s="122"/>
-    </row>
-    <row r="160" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="117">
+      <c r="C160" s="122"/>
+    </row>
+    <row r="161" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="117">
         <v>3</v>
       </c>
-      <c r="B160" s="148" t="s">
+      <c r="B161" s="141" t="s">
         <v>889</v>
       </c>
-      <c r="C160" s="149"/>
-    </row>
-    <row r="161" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="117"/>
-      <c r="B161" s="119" t="s">
+      <c r="C161" s="142"/>
+    </row>
+    <row r="162" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="117"/>
+      <c r="B162" s="119" t="s">
         <v>809</v>
       </c>
-      <c r="C161" s="120" t="s">
+      <c r="C162" s="120" t="s">
         <v>894</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="117"/>
-      <c r="B162" s="123" t="s">
-        <v>810</v>
-      </c>
-      <c r="C162" s="124" t="s">
-        <v>893</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="117"/>
       <c r="B163" s="123" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C163" s="124" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="117"/>
-      <c r="B164" s="126" t="s">
-        <v>816</v>
-      </c>
-      <c r="C164" s="127" t="s">
-        <v>896</v>
+      <c r="B164" s="123" t="s">
+        <v>814</v>
+      </c>
+      <c r="C164" s="124" t="s">
+        <v>895</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="117"/>
       <c r="B165" s="126" t="s">
-        <v>817</v>
-      </c>
-      <c r="C165" s="127"/>
+        <v>816</v>
+      </c>
+      <c r="C165" s="127" t="s">
+        <v>896</v>
+      </c>
     </row>
     <row r="166" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="117"/>
-      <c r="B166" s="121" t="s">
+      <c r="B166" s="126" t="s">
+        <v>817</v>
+      </c>
+      <c r="C166" s="127"/>
+    </row>
+    <row r="167" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="117"/>
+      <c r="B167" s="121" t="s">
         <v>846</v>
       </c>
-      <c r="C166" s="122"/>
+      <c r="C167" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B160:C160"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="A130:C130"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B39:C39"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B16:C16"/>
@@ -6692,6 +6698,47 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="A131:C131"/>
+    <mergeCell ref="B132:C132"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Reimplementing raycast as well as fighting fatality
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -5043,16 +5043,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5070,16 +5076,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5433,8 +5433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5449,29 +5449,29 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="144" t="s">
+      <c r="A2" s="146" t="s">
         <v>782</v>
       </c>
-      <c r="B2" s="145"/>
-      <c r="C2" s="146"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="148"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="115">
         <v>1</v>
       </c>
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="149" t="s">
         <v>783</v>
       </c>
-      <c r="C3" s="148"/>
+      <c r="C3" s="150"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B4" s="149" t="s">
+      <c r="B4" s="140" t="s">
         <v>784</v>
       </c>
-      <c r="C4" s="150"/>
+      <c r="C4" s="141"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="116"/>
@@ -5522,10 +5522,10 @@
       <c r="A10" s="116">
         <v>3</v>
       </c>
-      <c r="B10" s="151" t="s">
+      <c r="B10" s="142" t="s">
         <v>785</v>
       </c>
-      <c r="C10" s="152"/>
+      <c r="C10" s="143"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="116"/>
@@ -5540,10 +5540,10 @@
       <c r="A12" s="116">
         <v>4</v>
       </c>
-      <c r="B12" s="140" t="s">
+      <c r="B12" s="144" t="s">
         <v>786</v>
       </c>
-      <c r="C12" s="141"/>
+      <c r="C12" s="145"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="116"/>
@@ -5558,10 +5558,10 @@
       <c r="A14" s="116">
         <v>5</v>
       </c>
-      <c r="B14" s="140" t="s">
+      <c r="B14" s="144" t="s">
         <v>787</v>
       </c>
-      <c r="C14" s="141"/>
+      <c r="C14" s="145"/>
     </row>
     <row r="15" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="116"/>
@@ -5576,10 +5576,10 @@
       <c r="A16" s="117">
         <v>6</v>
       </c>
-      <c r="B16" s="142" t="s">
+      <c r="B16" s="151" t="s">
         <v>791</v>
       </c>
-      <c r="C16" s="143"/>
+      <c r="C16" s="152"/>
     </row>
     <row r="17" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="116"/>
@@ -5594,45 +5594,45 @@
       <c r="A18" s="117">
         <v>7</v>
       </c>
-      <c r="B18" s="142" t="s">
+      <c r="B18" s="151" t="s">
         <v>916</v>
       </c>
-      <c r="C18" s="143"/>
+      <c r="C18" s="152"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="132">
         <v>8</v>
       </c>
-      <c r="B19" s="142" t="s">
+      <c r="B19" s="151" t="s">
         <v>1004</v>
       </c>
-      <c r="C19" s="143"/>
+      <c r="C19" s="152"/>
     </row>
     <row r="20" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="132">
         <v>9</v>
       </c>
-      <c r="B20" s="142" t="s">
+      <c r="B20" s="151" t="s">
         <v>917</v>
       </c>
-      <c r="C20" s="143"/>
+      <c r="C20" s="152"/>
     </row>
     <row r="21" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="144" t="s">
+      <c r="A22" s="146" t="s">
         <v>183</v>
       </c>
-      <c r="B22" s="145"/>
-      <c r="C22" s="146"/>
+      <c r="B22" s="147"/>
+      <c r="C22" s="148"/>
     </row>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="115">
         <v>1</v>
       </c>
-      <c r="B23" s="147" t="s">
+      <c r="B23" s="149" t="s">
         <v>792</v>
       </c>
-      <c r="C23" s="148"/>
+      <c r="C23" s="150"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="116"/>
@@ -5681,20 +5681,20 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="144" t="s">
+      <c r="A30" s="146" t="s">
         <v>794</v>
       </c>
-      <c r="B30" s="145"/>
-      <c r="C30" s="146"/>
+      <c r="B30" s="147"/>
+      <c r="C30" s="148"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="115">
         <v>1</v>
       </c>
-      <c r="B31" s="147" t="s">
+      <c r="B31" s="149" t="s">
         <v>782</v>
       </c>
-      <c r="C31" s="148"/>
+      <c r="C31" s="150"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="116"/>
@@ -5718,10 +5718,10 @@
       <c r="A34" s="116">
         <v>2</v>
       </c>
-      <c r="B34" s="149" t="s">
+      <c r="B34" s="140" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="150"/>
+      <c r="C34" s="141"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="116"/>
@@ -5741,10 +5741,10 @@
       <c r="A37" s="116">
         <v>3</v>
       </c>
-      <c r="B37" s="149" t="s">
+      <c r="B37" s="140" t="s">
         <v>1005</v>
       </c>
-      <c r="C37" s="150"/>
+      <c r="C37" s="141"/>
     </row>
     <row r="38" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="116"/>
@@ -5766,20 +5766,20 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="144" t="s">
+      <c r="A41" s="146" t="s">
         <v>799</v>
       </c>
-      <c r="B41" s="145"/>
-      <c r="C41" s="146"/>
+      <c r="B41" s="147"/>
+      <c r="C41" s="148"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="115">
         <v>1</v>
       </c>
-      <c r="B42" s="147" t="s">
+      <c r="B42" s="149" t="s">
         <v>800</v>
       </c>
-      <c r="C42" s="148"/>
+      <c r="C42" s="150"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="116"/>
@@ -5819,20 +5819,20 @@
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="144" t="s">
+      <c r="A48" s="146" t="s">
         <v>804</v>
       </c>
-      <c r="B48" s="145"/>
-      <c r="C48" s="146"/>
+      <c r="B48" s="147"/>
+      <c r="C48" s="148"/>
     </row>
     <row r="49" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="115">
         <v>1</v>
       </c>
-      <c r="B49" s="147" t="s">
+      <c r="B49" s="149" t="s">
         <v>805</v>
       </c>
-      <c r="C49" s="148"/>
+      <c r="C49" s="150"/>
     </row>
     <row r="50" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="116"/>
@@ -5856,10 +5856,10 @@
       <c r="A52" s="115">
         <v>1</v>
       </c>
-      <c r="B52" s="147" t="s">
+      <c r="B52" s="149" t="s">
         <v>807</v>
       </c>
-      <c r="C52" s="148"/>
+      <c r="C52" s="150"/>
     </row>
     <row r="53" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="116"/>
@@ -5895,37 +5895,37 @@
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="144" t="s">
+      <c r="A58" s="146" t="s">
         <v>188</v>
       </c>
-      <c r="B58" s="145"/>
-      <c r="C58" s="146"/>
+      <c r="B58" s="147"/>
+      <c r="C58" s="148"/>
     </row>
     <row r="59" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="115">
         <v>1</v>
       </c>
-      <c r="B59" s="147" t="s">
+      <c r="B59" s="149" t="s">
         <v>812</v>
       </c>
-      <c r="C59" s="148"/>
+      <c r="C59" s="150"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="144" t="s">
+      <c r="A61" s="146" t="s">
         <v>790</v>
       </c>
-      <c r="B61" s="145"/>
-      <c r="C61" s="146"/>
+      <c r="B61" s="147"/>
+      <c r="C61" s="148"/>
     </row>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="115">
         <v>1</v>
       </c>
-      <c r="B62" s="151" t="s">
+      <c r="B62" s="142" t="s">
         <v>783</v>
       </c>
-      <c r="C62" s="152"/>
+      <c r="C62" s="143"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="116">
@@ -5940,54 +5940,54 @@
       <c r="A64" s="116">
         <v>3</v>
       </c>
-      <c r="B64" s="140" t="s">
+      <c r="B64" s="144" t="s">
         <v>785</v>
       </c>
-      <c r="C64" s="141"/>
+      <c r="C64" s="145"/>
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="116">
         <v>4</v>
       </c>
-      <c r="B65" s="140" t="s">
+      <c r="B65" s="144" t="s">
         <v>786</v>
       </c>
-      <c r="C65" s="141"/>
+      <c r="C65" s="145"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="116">
         <v>5</v>
       </c>
-      <c r="B66" s="140" t="s">
+      <c r="B66" s="144" t="s">
         <v>787</v>
       </c>
-      <c r="C66" s="141"/>
+      <c r="C66" s="145"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="117">
         <v>6</v>
       </c>
-      <c r="B67" s="142" t="s">
+      <c r="B67" s="151" t="s">
         <v>791</v>
       </c>
-      <c r="C67" s="143"/>
+      <c r="C67" s="152"/>
     </row>
     <row r="68" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="144" t="s">
+      <c r="A69" s="146" t="s">
         <v>813</v>
       </c>
-      <c r="B69" s="145"/>
-      <c r="C69" s="146"/>
+      <c r="B69" s="147"/>
+      <c r="C69" s="148"/>
     </row>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="115">
         <v>1</v>
       </c>
-      <c r="B70" s="151" t="s">
+      <c r="B70" s="142" t="s">
         <v>783</v>
       </c>
-      <c r="C70" s="152"/>
+      <c r="C70" s="143"/>
     </row>
     <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="116">
@@ -6002,52 +6002,52 @@
       <c r="A72" s="116">
         <v>3</v>
       </c>
-      <c r="B72" s="140" t="s">
+      <c r="B72" s="144" t="s">
         <v>785</v>
       </c>
-      <c r="C72" s="141"/>
+      <c r="C72" s="145"/>
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="116">
         <v>4</v>
       </c>
-      <c r="B73" s="140" t="s">
+      <c r="B73" s="144" t="s">
         <v>786</v>
       </c>
-      <c r="C73" s="141"/>
+      <c r="C73" s="145"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="116">
         <v>5</v>
       </c>
-      <c r="B74" s="140" t="s">
+      <c r="B74" s="144" t="s">
         <v>787</v>
       </c>
-      <c r="C74" s="141"/>
+      <c r="C74" s="145"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="117">
         <v>6</v>
       </c>
-      <c r="B75" s="142" t="s">
+      <c r="B75" s="151" t="s">
         <v>791</v>
       </c>
-      <c r="C75" s="143"/>
+      <c r="C75" s="152"/>
     </row>
     <row r="76" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="144" t="s">
+      <c r="A77" s="146" t="s">
         <v>1005</v>
       </c>
-      <c r="B77" s="145"/>
-      <c r="C77" s="146"/>
+      <c r="B77" s="147"/>
+      <c r="C77" s="148"/>
     </row>
     <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="115">
         <v>1</v>
       </c>
-      <c r="B78" s="151"/>
-      <c r="C78" s="152"/>
+      <c r="B78" s="142"/>
+      <c r="C78" s="143"/>
     </row>
     <row r="79" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="116"/>
@@ -6056,40 +6056,40 @@
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="116"/>
-      <c r="B80" s="140"/>
-      <c r="C80" s="141"/>
+      <c r="B80" s="144"/>
+      <c r="C80" s="145"/>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="116"/>
-      <c r="B81" s="140"/>
-      <c r="C81" s="141"/>
+      <c r="B81" s="144"/>
+      <c r="C81" s="145"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="116"/>
-      <c r="B82" s="140"/>
-      <c r="C82" s="141"/>
+      <c r="B82" s="144"/>
+      <c r="C82" s="145"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="117"/>
-      <c r="B83" s="142"/>
-      <c r="C83" s="143"/>
+      <c r="B83" s="151"/>
+      <c r="C83" s="152"/>
     </row>
     <row r="84" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="144" t="s">
+      <c r="A85" s="146" t="s">
         <v>814</v>
       </c>
-      <c r="B85" s="145"/>
-      <c r="C85" s="146"/>
+      <c r="B85" s="147"/>
+      <c r="C85" s="148"/>
     </row>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="115">
         <v>1</v>
       </c>
-      <c r="B86" s="151" t="s">
+      <c r="B86" s="142" t="s">
         <v>783</v>
       </c>
-      <c r="C86" s="152"/>
+      <c r="C86" s="143"/>
     </row>
     <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="116">
@@ -6104,54 +6104,54 @@
       <c r="A88" s="116">
         <v>3</v>
       </c>
-      <c r="B88" s="140" t="s">
+      <c r="B88" s="144" t="s">
         <v>785</v>
       </c>
-      <c r="C88" s="141"/>
+      <c r="C88" s="145"/>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="116">
         <v>4</v>
       </c>
-      <c r="B89" s="140" t="s">
+      <c r="B89" s="144" t="s">
         <v>786</v>
       </c>
-      <c r="C89" s="141"/>
+      <c r="C89" s="145"/>
     </row>
     <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="116">
         <v>5</v>
       </c>
-      <c r="B90" s="140" t="s">
+      <c r="B90" s="144" t="s">
         <v>787</v>
       </c>
-      <c r="C90" s="141"/>
+      <c r="C90" s="145"/>
     </row>
     <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="117">
         <v>6</v>
       </c>
-      <c r="B91" s="142" t="s">
+      <c r="B91" s="151" t="s">
         <v>791</v>
       </c>
-      <c r="C91" s="143"/>
+      <c r="C91" s="152"/>
     </row>
     <row r="92" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="93" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="144" t="s">
+      <c r="A93" s="146" t="s">
         <v>864</v>
       </c>
-      <c r="B93" s="145"/>
-      <c r="C93" s="146"/>
+      <c r="B93" s="147"/>
+      <c r="C93" s="148"/>
     </row>
     <row r="94" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="115">
         <v>1</v>
       </c>
-      <c r="B94" s="147" t="s">
+      <c r="B94" s="149" t="s">
         <v>101</v>
       </c>
-      <c r="C94" s="148"/>
+      <c r="C94" s="150"/>
     </row>
     <row r="95" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="124"/>
@@ -6324,10 +6324,10 @@
       <c r="A114" s="116">
         <v>2</v>
       </c>
-      <c r="B114" s="149" t="s">
+      <c r="B114" s="140" t="s">
         <v>815</v>
       </c>
-      <c r="C114" s="150"/>
+      <c r="C114" s="141"/>
     </row>
     <row r="115" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="116"/>
@@ -6405,10 +6405,10 @@
       <c r="A123" s="116">
         <v>3</v>
       </c>
-      <c r="B123" s="151" t="s">
+      <c r="B123" s="142" t="s">
         <v>816</v>
       </c>
-      <c r="C123" s="152"/>
+      <c r="C123" s="143"/>
     </row>
     <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="116"/>
@@ -6464,10 +6464,10 @@
       <c r="A130" s="115">
         <v>4</v>
       </c>
-      <c r="B130" s="140" t="s">
+      <c r="B130" s="144" t="s">
         <v>817</v>
       </c>
-      <c r="C130" s="141"/>
+      <c r="C130" s="145"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="124"/>
@@ -6507,20 +6507,20 @@
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="136" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="144" t="s">
+      <c r="A136" s="146" t="s">
         <v>865</v>
       </c>
-      <c r="B136" s="145"/>
-      <c r="C136" s="146"/>
+      <c r="B136" s="147"/>
+      <c r="C136" s="148"/>
     </row>
     <row r="137" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="115">
         <v>1</v>
       </c>
-      <c r="B137" s="147" t="s">
+      <c r="B137" s="149" t="s">
         <v>866</v>
       </c>
-      <c r="C137" s="148"/>
+      <c r="C137" s="150"/>
     </row>
     <row r="138" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="124"/>
@@ -6667,10 +6667,10 @@
       <c r="A157" s="116">
         <v>2</v>
       </c>
-      <c r="B157" s="149" t="s">
+      <c r="B157" s="140" t="s">
         <v>867</v>
       </c>
-      <c r="C157" s="150"/>
+      <c r="C157" s="141"/>
     </row>
     <row r="158" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="116"/>
@@ -6740,10 +6740,10 @@
       <c r="A166" s="116">
         <v>3</v>
       </c>
-      <c r="B166" s="151" t="s">
+      <c r="B166" s="142" t="s">
         <v>868</v>
       </c>
-      <c r="C166" s="152"/>
+      <c r="C166" s="143"/>
     </row>
     <row r="167" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="116"/>
@@ -6797,12 +6797,44 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="A136:C136"/>
-    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
     <mergeCell ref="B114:C114"/>
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="B75:C75"/>
@@ -6819,44 +6851,12 @@
     <mergeCell ref="B78:C78"/>
     <mergeCell ref="B79:C79"/>
     <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="A136:C136"/>
+    <mergeCell ref="B137:C137"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Tweaking effects and particles, fixing unity update
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -5043,22 +5043,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5076,10 +5070,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5433,8 +5433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5449,29 +5449,29 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="144" t="s">
         <v>782</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="148"/>
+      <c r="B2" s="145"/>
+      <c r="C2" s="146"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="115">
         <v>1</v>
       </c>
-      <c r="B3" s="149" t="s">
+      <c r="B3" s="147" t="s">
         <v>783</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="148"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="149" t="s">
         <v>784</v>
       </c>
-      <c r="C4" s="141"/>
+      <c r="C4" s="150"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="116"/>
@@ -5522,10 +5522,10 @@
       <c r="A10" s="116">
         <v>3</v>
       </c>
-      <c r="B10" s="142" t="s">
+      <c r="B10" s="151" t="s">
         <v>785</v>
       </c>
-      <c r="C10" s="143"/>
+      <c r="C10" s="152"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="116"/>
@@ -5540,10 +5540,10 @@
       <c r="A12" s="116">
         <v>4</v>
       </c>
-      <c r="B12" s="144" t="s">
+      <c r="B12" s="140" t="s">
         <v>786</v>
       </c>
-      <c r="C12" s="145"/>
+      <c r="C12" s="141"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="116"/>
@@ -5558,10 +5558,10 @@
       <c r="A14" s="116">
         <v>5</v>
       </c>
-      <c r="B14" s="144" t="s">
+      <c r="B14" s="140" t="s">
         <v>787</v>
       </c>
-      <c r="C14" s="145"/>
+      <c r="C14" s="141"/>
     </row>
     <row r="15" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="116"/>
@@ -5576,10 +5576,10 @@
       <c r="A16" s="117">
         <v>6</v>
       </c>
-      <c r="B16" s="151" t="s">
+      <c r="B16" s="142" t="s">
         <v>791</v>
       </c>
-      <c r="C16" s="152"/>
+      <c r="C16" s="143"/>
     </row>
     <row r="17" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="116"/>
@@ -5594,45 +5594,45 @@
       <c r="A18" s="117">
         <v>7</v>
       </c>
-      <c r="B18" s="151" t="s">
+      <c r="B18" s="142" t="s">
         <v>916</v>
       </c>
-      <c r="C18" s="152"/>
+      <c r="C18" s="143"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="132">
         <v>8</v>
       </c>
-      <c r="B19" s="151" t="s">
+      <c r="B19" s="142" t="s">
         <v>1004</v>
       </c>
-      <c r="C19" s="152"/>
+      <c r="C19" s="143"/>
     </row>
     <row r="20" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="132">
         <v>9</v>
       </c>
-      <c r="B20" s="151" t="s">
+      <c r="B20" s="142" t="s">
         <v>917</v>
       </c>
-      <c r="C20" s="152"/>
+      <c r="C20" s="143"/>
     </row>
     <row r="21" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="146" t="s">
+      <c r="A22" s="144" t="s">
         <v>183</v>
       </c>
-      <c r="B22" s="147"/>
-      <c r="C22" s="148"/>
+      <c r="B22" s="145"/>
+      <c r="C22" s="146"/>
     </row>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="115">
         <v>1</v>
       </c>
-      <c r="B23" s="149" t="s">
+      <c r="B23" s="147" t="s">
         <v>792</v>
       </c>
-      <c r="C23" s="150"/>
+      <c r="C23" s="148"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="116"/>
@@ -5681,20 +5681,20 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="146" t="s">
+      <c r="A30" s="144" t="s">
         <v>794</v>
       </c>
-      <c r="B30" s="147"/>
-      <c r="C30" s="148"/>
+      <c r="B30" s="145"/>
+      <c r="C30" s="146"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="115">
         <v>1</v>
       </c>
-      <c r="B31" s="149" t="s">
+      <c r="B31" s="147" t="s">
         <v>782</v>
       </c>
-      <c r="C31" s="150"/>
+      <c r="C31" s="148"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="116"/>
@@ -5718,10 +5718,10 @@
       <c r="A34" s="116">
         <v>2</v>
       </c>
-      <c r="B34" s="140" t="s">
+      <c r="B34" s="149" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="141"/>
+      <c r="C34" s="150"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="116"/>
@@ -5741,10 +5741,10 @@
       <c r="A37" s="116">
         <v>3</v>
       </c>
-      <c r="B37" s="140" t="s">
+      <c r="B37" s="149" t="s">
         <v>1005</v>
       </c>
-      <c r="C37" s="141"/>
+      <c r="C37" s="150"/>
     </row>
     <row r="38" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="116"/>
@@ -5766,20 +5766,20 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="146" t="s">
+      <c r="A41" s="144" t="s">
         <v>799</v>
       </c>
-      <c r="B41" s="147"/>
-      <c r="C41" s="148"/>
+      <c r="B41" s="145"/>
+      <c r="C41" s="146"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="115">
         <v>1</v>
       </c>
-      <c r="B42" s="149" t="s">
+      <c r="B42" s="147" t="s">
         <v>800</v>
       </c>
-      <c r="C42" s="150"/>
+      <c r="C42" s="148"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="116"/>
@@ -5819,20 +5819,20 @@
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="146" t="s">
+      <c r="A48" s="144" t="s">
         <v>804</v>
       </c>
-      <c r="B48" s="147"/>
-      <c r="C48" s="148"/>
+      <c r="B48" s="145"/>
+      <c r="C48" s="146"/>
     </row>
     <row r="49" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="115">
         <v>1</v>
       </c>
-      <c r="B49" s="149" t="s">
+      <c r="B49" s="147" t="s">
         <v>805</v>
       </c>
-      <c r="C49" s="150"/>
+      <c r="C49" s="148"/>
     </row>
     <row r="50" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="116"/>
@@ -5856,10 +5856,10 @@
       <c r="A52" s="115">
         <v>1</v>
       </c>
-      <c r="B52" s="149" t="s">
+      <c r="B52" s="147" t="s">
         <v>807</v>
       </c>
-      <c r="C52" s="150"/>
+      <c r="C52" s="148"/>
     </row>
     <row r="53" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="116"/>
@@ -5895,37 +5895,37 @@
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="146" t="s">
+      <c r="A58" s="144" t="s">
         <v>188</v>
       </c>
-      <c r="B58" s="147"/>
-      <c r="C58" s="148"/>
+      <c r="B58" s="145"/>
+      <c r="C58" s="146"/>
     </row>
     <row r="59" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="115">
         <v>1</v>
       </c>
-      <c r="B59" s="149" t="s">
+      <c r="B59" s="147" t="s">
         <v>812</v>
       </c>
-      <c r="C59" s="150"/>
+      <c r="C59" s="148"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="146" t="s">
+      <c r="A61" s="144" t="s">
         <v>790</v>
       </c>
-      <c r="B61" s="147"/>
-      <c r="C61" s="148"/>
+      <c r="B61" s="145"/>
+      <c r="C61" s="146"/>
     </row>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="115">
         <v>1</v>
       </c>
-      <c r="B62" s="142" t="s">
+      <c r="B62" s="151" t="s">
         <v>783</v>
       </c>
-      <c r="C62" s="143"/>
+      <c r="C62" s="152"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="116">
@@ -5940,54 +5940,54 @@
       <c r="A64" s="116">
         <v>3</v>
       </c>
-      <c r="B64" s="144" t="s">
+      <c r="B64" s="140" t="s">
         <v>785</v>
       </c>
-      <c r="C64" s="145"/>
+      <c r="C64" s="141"/>
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="116">
         <v>4</v>
       </c>
-      <c r="B65" s="144" t="s">
+      <c r="B65" s="140" t="s">
         <v>786</v>
       </c>
-      <c r="C65" s="145"/>
+      <c r="C65" s="141"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="116">
         <v>5</v>
       </c>
-      <c r="B66" s="144" t="s">
+      <c r="B66" s="140" t="s">
         <v>787</v>
       </c>
-      <c r="C66" s="145"/>
+      <c r="C66" s="141"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="117">
         <v>6</v>
       </c>
-      <c r="B67" s="151" t="s">
+      <c r="B67" s="142" t="s">
         <v>791</v>
       </c>
-      <c r="C67" s="152"/>
+      <c r="C67" s="143"/>
     </row>
     <row r="68" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="146" t="s">
+      <c r="A69" s="144" t="s">
         <v>813</v>
       </c>
-      <c r="B69" s="147"/>
-      <c r="C69" s="148"/>
+      <c r="B69" s="145"/>
+      <c r="C69" s="146"/>
     </row>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="115">
         <v>1</v>
       </c>
-      <c r="B70" s="142" t="s">
+      <c r="B70" s="151" t="s">
         <v>783</v>
       </c>
-      <c r="C70" s="143"/>
+      <c r="C70" s="152"/>
     </row>
     <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="116">
@@ -6002,52 +6002,52 @@
       <c r="A72" s="116">
         <v>3</v>
       </c>
-      <c r="B72" s="144" t="s">
+      <c r="B72" s="140" t="s">
         <v>785</v>
       </c>
-      <c r="C72" s="145"/>
+      <c r="C72" s="141"/>
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="116">
         <v>4</v>
       </c>
-      <c r="B73" s="144" t="s">
+      <c r="B73" s="140" t="s">
         <v>786</v>
       </c>
-      <c r="C73" s="145"/>
+      <c r="C73" s="141"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="116">
         <v>5</v>
       </c>
-      <c r="B74" s="144" t="s">
+      <c r="B74" s="140" t="s">
         <v>787</v>
       </c>
-      <c r="C74" s="145"/>
+      <c r="C74" s="141"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="117">
         <v>6</v>
       </c>
-      <c r="B75" s="151" t="s">
+      <c r="B75" s="142" t="s">
         <v>791</v>
       </c>
-      <c r="C75" s="152"/>
+      <c r="C75" s="143"/>
     </row>
     <row r="76" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="146" t="s">
+      <c r="A77" s="144" t="s">
         <v>1005</v>
       </c>
-      <c r="B77" s="147"/>
-      <c r="C77" s="148"/>
+      <c r="B77" s="145"/>
+      <c r="C77" s="146"/>
     </row>
     <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="115">
         <v>1</v>
       </c>
-      <c r="B78" s="142"/>
-      <c r="C78" s="143"/>
+      <c r="B78" s="151"/>
+      <c r="C78" s="152"/>
     </row>
     <row r="79" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="116"/>
@@ -6056,40 +6056,40 @@
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="116"/>
-      <c r="B80" s="144"/>
-      <c r="C80" s="145"/>
+      <c r="B80" s="140"/>
+      <c r="C80" s="141"/>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="116"/>
-      <c r="B81" s="144"/>
-      <c r="C81" s="145"/>
+      <c r="B81" s="140"/>
+      <c r="C81" s="141"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="116"/>
-      <c r="B82" s="144"/>
-      <c r="C82" s="145"/>
+      <c r="B82" s="140"/>
+      <c r="C82" s="141"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="117"/>
-      <c r="B83" s="151"/>
-      <c r="C83" s="152"/>
+      <c r="B83" s="142"/>
+      <c r="C83" s="143"/>
     </row>
     <row r="84" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="146" t="s">
+      <c r="A85" s="144" t="s">
         <v>814</v>
       </c>
-      <c r="B85" s="147"/>
-      <c r="C85" s="148"/>
+      <c r="B85" s="145"/>
+      <c r="C85" s="146"/>
     </row>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="115">
         <v>1</v>
       </c>
-      <c r="B86" s="142" t="s">
+      <c r="B86" s="151" t="s">
         <v>783</v>
       </c>
-      <c r="C86" s="143"/>
+      <c r="C86" s="152"/>
     </row>
     <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="116">
@@ -6104,54 +6104,54 @@
       <c r="A88" s="116">
         <v>3</v>
       </c>
-      <c r="B88" s="144" t="s">
+      <c r="B88" s="140" t="s">
         <v>785</v>
       </c>
-      <c r="C88" s="145"/>
+      <c r="C88" s="141"/>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="116">
         <v>4</v>
       </c>
-      <c r="B89" s="144" t="s">
+      <c r="B89" s="140" t="s">
         <v>786</v>
       </c>
-      <c r="C89" s="145"/>
+      <c r="C89" s="141"/>
     </row>
     <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="116">
         <v>5</v>
       </c>
-      <c r="B90" s="144" t="s">
+      <c r="B90" s="140" t="s">
         <v>787</v>
       </c>
-      <c r="C90" s="145"/>
+      <c r="C90" s="141"/>
     </row>
     <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="117">
         <v>6</v>
       </c>
-      <c r="B91" s="151" t="s">
+      <c r="B91" s="142" t="s">
         <v>791</v>
       </c>
-      <c r="C91" s="152"/>
+      <c r="C91" s="143"/>
     </row>
     <row r="92" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="93" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="146" t="s">
+      <c r="A93" s="144" t="s">
         <v>864</v>
       </c>
-      <c r="B93" s="147"/>
-      <c r="C93" s="148"/>
+      <c r="B93" s="145"/>
+      <c r="C93" s="146"/>
     </row>
     <row r="94" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="115">
         <v>1</v>
       </c>
-      <c r="B94" s="149" t="s">
+      <c r="B94" s="147" t="s">
         <v>101</v>
       </c>
-      <c r="C94" s="150"/>
+      <c r="C94" s="148"/>
     </row>
     <row r="95" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="124"/>
@@ -6324,10 +6324,10 @@
       <c r="A114" s="116">
         <v>2</v>
       </c>
-      <c r="B114" s="140" t="s">
+      <c r="B114" s="149" t="s">
         <v>815</v>
       </c>
-      <c r="C114" s="141"/>
+      <c r="C114" s="150"/>
     </row>
     <row r="115" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="116"/>
@@ -6405,10 +6405,10 @@
       <c r="A123" s="116">
         <v>3</v>
       </c>
-      <c r="B123" s="142" t="s">
+      <c r="B123" s="151" t="s">
         <v>816</v>
       </c>
-      <c r="C123" s="143"/>
+      <c r="C123" s="152"/>
     </row>
     <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="116"/>
@@ -6464,10 +6464,10 @@
       <c r="A130" s="115">
         <v>4</v>
       </c>
-      <c r="B130" s="144" t="s">
+      <c r="B130" s="140" t="s">
         <v>817</v>
       </c>
-      <c r="C130" s="145"/>
+      <c r="C130" s="141"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="124"/>
@@ -6507,20 +6507,20 @@
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="136" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="146" t="s">
+      <c r="A136" s="144" t="s">
         <v>865</v>
       </c>
-      <c r="B136" s="147"/>
-      <c r="C136" s="148"/>
+      <c r="B136" s="145"/>
+      <c r="C136" s="146"/>
     </row>
     <row r="137" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="115">
         <v>1</v>
       </c>
-      <c r="B137" s="149" t="s">
+      <c r="B137" s="147" t="s">
         <v>866</v>
       </c>
-      <c r="C137" s="150"/>
+      <c r="C137" s="148"/>
     </row>
     <row r="138" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="124"/>
@@ -6667,10 +6667,10 @@
       <c r="A157" s="116">
         <v>2</v>
       </c>
-      <c r="B157" s="140" t="s">
+      <c r="B157" s="149" t="s">
         <v>867</v>
       </c>
-      <c r="C157" s="141"/>
+      <c r="C157" s="150"/>
     </row>
     <row r="158" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="116"/>
@@ -6740,10 +6740,10 @@
       <c r="A166" s="116">
         <v>3</v>
       </c>
-      <c r="B166" s="142" t="s">
+      <c r="B166" s="151" t="s">
         <v>868</v>
       </c>
-      <c r="C166" s="143"/>
+      <c r="C166" s="152"/>
     </row>
     <row r="167" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="116"/>
@@ -6797,6 +6797,50 @@
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="A136:C136"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="A93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B37:C37"/>
     <mergeCell ref="B81:C81"/>
     <mergeCell ref="B82:C82"/>
     <mergeCell ref="B83:C83"/>
@@ -6813,50 +6857,6 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B34:C34"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="A93:C93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="A77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="A136:C136"/>
-    <mergeCell ref="B137:C137"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Tidying up spear wall implementation
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716" firstSheet="12" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="TODO - Quick Battle" sheetId="37" r:id="rId1"/>
@@ -643,7 +643,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2240" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="1079">
   <si>
     <t>Fishing</t>
   </si>
@@ -3874,6 +3874,12 @@
   </si>
   <si>
     <t>Fires a dart at target that if hits, does DoT damage as well as initial damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a </t>
+  </si>
+  <si>
+    <t>shield wall</t>
   </si>
 </sst>
 </file>
@@ -5433,8 +5439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5637,10 +5643,10 @@
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="116"/>
       <c r="B24" s="122" t="s">
-        <v>789</v>
+        <v>1077</v>
       </c>
       <c r="C24" s="123" t="s">
-        <v>635</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5654,12 +5660,8 @@
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="116"/>
-      <c r="B26" s="122" t="s">
-        <v>795</v>
-      </c>
-      <c r="C26" s="123" t="s">
-        <v>675</v>
-      </c>
+      <c r="B26" s="122"/>
+      <c r="C26" s="123"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="116"/>
@@ -9501,8 +9503,8 @@
   <dimension ref="A1:X300"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K80" sqref="K80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24088,7 +24090,7 @@
   <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" activeCellId="1" sqref="A18:XFD20 A21:XFD21"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25458,8 +25460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TODO's and tomorrow's tasks
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716" firstSheet="12" activeTab="23"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716"/>
   </bookViews>
   <sheets>
     <sheet name="TODO - Quick Battle" sheetId="37" r:id="rId1"/>
@@ -643,7 +643,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="1079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2232" uniqueCount="1077">
   <si>
     <t>Fishing</t>
   </si>
@@ -3273,9 +3273,6 @@
     <t>Bottlenecks</t>
   </si>
   <si>
-    <t>Pull</t>
-  </si>
-  <si>
     <t>Weenomancer</t>
   </si>
   <si>
@@ -3649,9 +3646,6 @@
   </si>
   <si>
     <t>Soul Farmer</t>
-  </si>
-  <si>
-    <t>attack of opportunity</t>
   </si>
   <si>
     <t>bullets hitting random targets</t>
@@ -4730,7 +4724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5049,16 +5043,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5076,16 +5076,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5132,6 +5126,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5439,8 +5451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C172"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5455,29 +5467,29 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="144" t="s">
+      <c r="A2" s="146" t="s">
         <v>782</v>
       </c>
-      <c r="B2" s="145"/>
-      <c r="C2" s="146"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="148"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="115">
         <v>1</v>
       </c>
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="149" t="s">
         <v>783</v>
       </c>
-      <c r="C3" s="148"/>
+      <c r="C3" s="150"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B4" s="149" t="s">
+      <c r="B4" s="140" t="s">
         <v>784</v>
       </c>
-      <c r="C4" s="150"/>
+      <c r="C4" s="141"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="116"/>
@@ -5512,7 +5524,7 @@
         <v>795</v>
       </c>
       <c r="C8" s="123" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="9" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
@@ -5528,10 +5540,10 @@
       <c r="A10" s="116">
         <v>3</v>
       </c>
-      <c r="B10" s="151" t="s">
+      <c r="B10" s="142" t="s">
         <v>785</v>
       </c>
-      <c r="C10" s="152"/>
+      <c r="C10" s="143"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="116"/>
@@ -5539,17 +5551,17 @@
         <v>788</v>
       </c>
       <c r="C11" s="119" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="12" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="116">
         <v>4</v>
       </c>
-      <c r="B12" s="140" t="s">
+      <c r="B12" s="144" t="s">
         <v>786</v>
       </c>
-      <c r="C12" s="141"/>
+      <c r="C12" s="145"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="116"/>
@@ -5557,17 +5569,17 @@
         <v>788</v>
       </c>
       <c r="C13" s="119" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="14" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="116">
         <v>5</v>
       </c>
-      <c r="B14" s="140" t="s">
+      <c r="B14" s="144" t="s">
         <v>787</v>
       </c>
-      <c r="C14" s="141"/>
+      <c r="C14" s="145"/>
     </row>
     <row r="15" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="116"/>
@@ -5575,17 +5587,17 @@
         <v>788</v>
       </c>
       <c r="C15" s="119" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="16" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="117">
         <v>6</v>
       </c>
-      <c r="B16" s="142" t="s">
+      <c r="B16" s="151" t="s">
         <v>791</v>
       </c>
-      <c r="C16" s="143"/>
+      <c r="C16" s="152"/>
     </row>
     <row r="17" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="116"/>
@@ -5593,68 +5605,68 @@
         <v>788</v>
       </c>
       <c r="C17" s="119" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="18" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="117">
         <v>7</v>
       </c>
-      <c r="B18" s="142" t="s">
-        <v>916</v>
-      </c>
-      <c r="C18" s="143"/>
+      <c r="B18" s="151" t="s">
+        <v>915</v>
+      </c>
+      <c r="C18" s="152"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="132">
         <v>8</v>
       </c>
-      <c r="B19" s="142" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C19" s="143"/>
+      <c r="B19" s="151" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C19" s="152"/>
     </row>
     <row r="20" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="132">
         <v>9</v>
       </c>
-      <c r="B20" s="142" t="s">
-        <v>917</v>
-      </c>
-      <c r="C20" s="143"/>
+      <c r="B20" s="151" t="s">
+        <v>916</v>
+      </c>
+      <c r="C20" s="152"/>
     </row>
     <row r="21" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="144" t="s">
+      <c r="A22" s="146" t="s">
         <v>183</v>
       </c>
-      <c r="B22" s="145"/>
-      <c r="C22" s="146"/>
+      <c r="B22" s="147"/>
+      <c r="C22" s="148"/>
     </row>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="115">
         <v>1</v>
       </c>
-      <c r="B23" s="147" t="s">
+      <c r="B23" s="149" t="s">
         <v>792</v>
       </c>
-      <c r="C23" s="148"/>
+      <c r="C23" s="150"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="116"/>
-      <c r="B24" s="122" t="s">
-        <v>1077</v>
-      </c>
-      <c r="C24" s="123" t="s">
-        <v>1078</v>
+      <c r="B24" s="168" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C24" s="169" t="s">
+        <v>1076</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="116"/>
-      <c r="B25" s="122" t="s">
+      <c r="B25" s="168" t="s">
         <v>793</v>
       </c>
-      <c r="C25" s="123" t="s">
+      <c r="C25" s="169" t="s">
         <v>797</v>
       </c>
     </row>
@@ -5665,65 +5677,53 @@
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="116"/>
-      <c r="B27" s="125" t="s">
-        <v>796</v>
-      </c>
-      <c r="C27" s="126" t="s">
-        <v>658</v>
-      </c>
+      <c r="B27" s="125"/>
+      <c r="C27" s="126"/>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="116"/>
-      <c r="B28" s="125" t="s">
-        <v>829</v>
-      </c>
-      <c r="C28" s="126" t="s">
-        <v>876</v>
-      </c>
+      <c r="B28" s="125"/>
+      <c r="C28" s="126"/>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="144" t="s">
+      <c r="A30" s="146" t="s">
         <v>794</v>
       </c>
-      <c r="B30" s="145"/>
-      <c r="C30" s="146"/>
+      <c r="B30" s="147"/>
+      <c r="C30" s="148"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="115">
         <v>1</v>
       </c>
-      <c r="B31" s="147" t="s">
+      <c r="B31" s="149" t="s">
         <v>782</v>
       </c>
-      <c r="C31" s="148"/>
+      <c r="C31" s="150"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="116"/>
-      <c r="B32" s="122" t="s">
-        <v>788</v>
-      </c>
-      <c r="C32" s="123" t="s">
-        <v>1002</v>
-      </c>
+      <c r="B32" s="122"/>
+      <c r="C32" s="123"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="116"/>
-      <c r="B33" s="122" t="s">
+      <c r="B33" s="168" t="s">
         <v>789</v>
       </c>
-      <c r="C33" s="123" t="s">
-        <v>1003</v>
+      <c r="C33" s="169" t="s">
+        <v>1001</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="116">
         <v>2</v>
       </c>
-      <c r="B34" s="149" t="s">
+      <c r="B34" s="140" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="150"/>
+      <c r="C34" s="141"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="116"/>
@@ -5743,45 +5743,45 @@
       <c r="A37" s="116">
         <v>3</v>
       </c>
-      <c r="B37" s="149" t="s">
-        <v>1005</v>
-      </c>
-      <c r="C37" s="150"/>
+      <c r="B37" s="140" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C37" s="141"/>
     </row>
     <row r="38" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="116"/>
-      <c r="B38" s="118" t="s">
+      <c r="B38" s="170" t="s">
         <v>788</v>
       </c>
-      <c r="C38" s="119" t="s">
-        <v>1006</v>
+      <c r="C38" s="171" t="s">
+        <v>1004</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="116"/>
-      <c r="B39" s="120" t="s">
+      <c r="B39" s="172" t="s">
         <v>789</v>
       </c>
-      <c r="C39" s="121" t="s">
-        <v>1007</v>
+      <c r="C39" s="173" t="s">
+        <v>1005</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="144" t="s">
+      <c r="A41" s="146" t="s">
         <v>799</v>
       </c>
-      <c r="B41" s="145"/>
-      <c r="C41" s="146"/>
+      <c r="B41" s="147"/>
+      <c r="C41" s="148"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="115">
         <v>1</v>
       </c>
-      <c r="B42" s="147" t="s">
+      <c r="B42" s="149" t="s">
         <v>800</v>
       </c>
-      <c r="C42" s="148"/>
+      <c r="C42" s="150"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="116"/>
@@ -5821,20 +5821,20 @@
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="144" t="s">
+      <c r="A48" s="146" t="s">
         <v>804</v>
       </c>
-      <c r="B48" s="145"/>
-      <c r="C48" s="146"/>
+      <c r="B48" s="147"/>
+      <c r="C48" s="148"/>
     </row>
     <row r="49" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="115">
         <v>1</v>
       </c>
-      <c r="B49" s="147" t="s">
+      <c r="B49" s="149" t="s">
         <v>805</v>
       </c>
-      <c r="C49" s="148"/>
+      <c r="C49" s="150"/>
     </row>
     <row r="50" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="116"/>
@@ -5858,10 +5858,10 @@
       <c r="A52" s="115">
         <v>1</v>
       </c>
-      <c r="B52" s="147" t="s">
+      <c r="B52" s="149" t="s">
         <v>807</v>
       </c>
-      <c r="C52" s="148"/>
+      <c r="C52" s="150"/>
     </row>
     <row r="53" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="116"/>
@@ -5897,37 +5897,37 @@
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="144" t="s">
+      <c r="A58" s="146" t="s">
         <v>188</v>
       </c>
-      <c r="B58" s="145"/>
-      <c r="C58" s="146"/>
+      <c r="B58" s="147"/>
+      <c r="C58" s="148"/>
     </row>
     <row r="59" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="115">
         <v>1</v>
       </c>
-      <c r="B59" s="147" t="s">
+      <c r="B59" s="149" t="s">
         <v>812</v>
       </c>
-      <c r="C59" s="148"/>
+      <c r="C59" s="150"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="144" t="s">
+      <c r="A61" s="146" t="s">
         <v>790</v>
       </c>
-      <c r="B61" s="145"/>
-      <c r="C61" s="146"/>
+      <c r="B61" s="147"/>
+      <c r="C61" s="148"/>
     </row>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="115">
         <v>1</v>
       </c>
-      <c r="B62" s="151" t="s">
+      <c r="B62" s="142" t="s">
         <v>783</v>
       </c>
-      <c r="C62" s="152"/>
+      <c r="C62" s="143"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="116">
@@ -5942,54 +5942,54 @@
       <c r="A64" s="116">
         <v>3</v>
       </c>
-      <c r="B64" s="140" t="s">
+      <c r="B64" s="144" t="s">
         <v>785</v>
       </c>
-      <c r="C64" s="141"/>
+      <c r="C64" s="145"/>
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="116">
         <v>4</v>
       </c>
-      <c r="B65" s="140" t="s">
+      <c r="B65" s="144" t="s">
         <v>786</v>
       </c>
-      <c r="C65" s="141"/>
+      <c r="C65" s="145"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="116">
         <v>5</v>
       </c>
-      <c r="B66" s="140" t="s">
+      <c r="B66" s="144" t="s">
         <v>787</v>
       </c>
-      <c r="C66" s="141"/>
+      <c r="C66" s="145"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="117">
         <v>6</v>
       </c>
-      <c r="B67" s="142" t="s">
+      <c r="B67" s="151" t="s">
         <v>791</v>
       </c>
-      <c r="C67" s="143"/>
+      <c r="C67" s="152"/>
     </row>
     <row r="68" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="144" t="s">
+      <c r="A69" s="146" t="s">
         <v>813</v>
       </c>
-      <c r="B69" s="145"/>
-      <c r="C69" s="146"/>
+      <c r="B69" s="147"/>
+      <c r="C69" s="148"/>
     </row>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="115">
         <v>1</v>
       </c>
-      <c r="B70" s="151" t="s">
+      <c r="B70" s="142" t="s">
         <v>783</v>
       </c>
-      <c r="C70" s="152"/>
+      <c r="C70" s="143"/>
     </row>
     <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="116">
@@ -6004,52 +6004,52 @@
       <c r="A72" s="116">
         <v>3</v>
       </c>
-      <c r="B72" s="140" t="s">
+      <c r="B72" s="144" t="s">
         <v>785</v>
       </c>
-      <c r="C72" s="141"/>
+      <c r="C72" s="145"/>
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="116">
         <v>4</v>
       </c>
-      <c r="B73" s="140" t="s">
+      <c r="B73" s="144" t="s">
         <v>786</v>
       </c>
-      <c r="C73" s="141"/>
+      <c r="C73" s="145"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="116">
         <v>5</v>
       </c>
-      <c r="B74" s="140" t="s">
+      <c r="B74" s="144" t="s">
         <v>787</v>
       </c>
-      <c r="C74" s="141"/>
+      <c r="C74" s="145"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="117">
         <v>6</v>
       </c>
-      <c r="B75" s="142" t="s">
+      <c r="B75" s="151" t="s">
         <v>791</v>
       </c>
-      <c r="C75" s="143"/>
+      <c r="C75" s="152"/>
     </row>
     <row r="76" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="144" t="s">
-        <v>1005</v>
-      </c>
-      <c r="B77" s="145"/>
-      <c r="C77" s="146"/>
+      <c r="A77" s="146" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B77" s="147"/>
+      <c r="C77" s="148"/>
     </row>
     <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="115">
         <v>1</v>
       </c>
-      <c r="B78" s="151"/>
-      <c r="C78" s="152"/>
+      <c r="B78" s="142"/>
+      <c r="C78" s="143"/>
     </row>
     <row r="79" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="116"/>
@@ -6058,40 +6058,40 @@
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="116"/>
-      <c r="B80" s="140"/>
-      <c r="C80" s="141"/>
+      <c r="B80" s="144"/>
+      <c r="C80" s="145"/>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="116"/>
-      <c r="B81" s="140"/>
-      <c r="C81" s="141"/>
+      <c r="B81" s="144"/>
+      <c r="C81" s="145"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="116"/>
-      <c r="B82" s="140"/>
-      <c r="C82" s="141"/>
+      <c r="B82" s="144"/>
+      <c r="C82" s="145"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="117"/>
-      <c r="B83" s="142"/>
-      <c r="C83" s="143"/>
+      <c r="B83" s="151"/>
+      <c r="C83" s="152"/>
     </row>
     <row r="84" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="144" t="s">
+      <c r="A85" s="146" t="s">
         <v>814</v>
       </c>
-      <c r="B85" s="145"/>
-      <c r="C85" s="146"/>
+      <c r="B85" s="147"/>
+      <c r="C85" s="148"/>
     </row>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="115">
         <v>1</v>
       </c>
-      <c r="B86" s="151" t="s">
+      <c r="B86" s="142" t="s">
         <v>783</v>
       </c>
-      <c r="C86" s="152"/>
+      <c r="C86" s="143"/>
     </row>
     <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="116">
@@ -6106,54 +6106,54 @@
       <c r="A88" s="116">
         <v>3</v>
       </c>
-      <c r="B88" s="140" t="s">
+      <c r="B88" s="144" t="s">
         <v>785</v>
       </c>
-      <c r="C88" s="141"/>
+      <c r="C88" s="145"/>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="116">
         <v>4</v>
       </c>
-      <c r="B89" s="140" t="s">
+      <c r="B89" s="144" t="s">
         <v>786</v>
       </c>
-      <c r="C89" s="141"/>
+      <c r="C89" s="145"/>
     </row>
     <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="116">
         <v>5</v>
       </c>
-      <c r="B90" s="140" t="s">
+      <c r="B90" s="144" t="s">
         <v>787</v>
       </c>
-      <c r="C90" s="141"/>
+      <c r="C90" s="145"/>
     </row>
     <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="117">
         <v>6</v>
       </c>
-      <c r="B91" s="142" t="s">
+      <c r="B91" s="151" t="s">
         <v>791</v>
       </c>
-      <c r="C91" s="143"/>
+      <c r="C91" s="152"/>
     </row>
     <row r="92" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="93" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="144" t="s">
+      <c r="A93" s="146" t="s">
         <v>864</v>
       </c>
-      <c r="B93" s="145"/>
-      <c r="C93" s="146"/>
+      <c r="B93" s="147"/>
+      <c r="C93" s="148"/>
     </row>
     <row r="94" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="115">
         <v>1</v>
       </c>
-      <c r="B94" s="147" t="s">
+      <c r="B94" s="149" t="s">
         <v>101</v>
       </c>
-      <c r="C94" s="148"/>
+      <c r="C94" s="150"/>
     </row>
     <row r="95" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="124"/>
@@ -6326,10 +6326,10 @@
       <c r="A114" s="116">
         <v>2</v>
       </c>
-      <c r="B114" s="149" t="s">
+      <c r="B114" s="140" t="s">
         <v>815</v>
       </c>
-      <c r="C114" s="150"/>
+      <c r="C114" s="141"/>
     </row>
     <row r="115" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="116"/>
@@ -6407,10 +6407,10 @@
       <c r="A123" s="116">
         <v>3</v>
       </c>
-      <c r="B123" s="151" t="s">
+      <c r="B123" s="142" t="s">
         <v>816</v>
       </c>
-      <c r="C123" s="152"/>
+      <c r="C123" s="143"/>
     </row>
     <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="116"/>
@@ -6466,10 +6466,10 @@
       <c r="A130" s="115">
         <v>4</v>
       </c>
-      <c r="B130" s="140" t="s">
+      <c r="B130" s="144" t="s">
         <v>817</v>
       </c>
-      <c r="C130" s="141"/>
+      <c r="C130" s="145"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="124"/>
@@ -6509,20 +6509,20 @@
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="136" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="144" t="s">
+      <c r="A136" s="146" t="s">
         <v>865</v>
       </c>
-      <c r="B136" s="145"/>
-      <c r="C136" s="146"/>
+      <c r="B136" s="147"/>
+      <c r="C136" s="148"/>
     </row>
     <row r="137" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="115">
         <v>1</v>
       </c>
-      <c r="B137" s="147" t="s">
+      <c r="B137" s="149" t="s">
         <v>866</v>
       </c>
-      <c r="C137" s="148"/>
+      <c r="C137" s="150"/>
     </row>
     <row r="138" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="124"/>
@@ -6669,10 +6669,10 @@
       <c r="A157" s="116">
         <v>2</v>
       </c>
-      <c r="B157" s="149" t="s">
+      <c r="B157" s="140" t="s">
         <v>867</v>
       </c>
-      <c r="C157" s="150"/>
+      <c r="C157" s="141"/>
     </row>
     <row r="158" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="116"/>
@@ -6742,10 +6742,10 @@
       <c r="A166" s="116">
         <v>3</v>
       </c>
-      <c r="B166" s="151" t="s">
+      <c r="B166" s="142" t="s">
         <v>868</v>
       </c>
-      <c r="C166" s="152"/>
+      <c r="C166" s="143"/>
     </row>
     <row r="167" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="116"/>
@@ -6799,12 +6799,44 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="A136:C136"/>
-    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
     <mergeCell ref="B114:C114"/>
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="B75:C75"/>
@@ -6821,44 +6853,12 @@
     <mergeCell ref="B78:C78"/>
     <mergeCell ref="B79:C79"/>
     <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="A136:C136"/>
+    <mergeCell ref="B137:C137"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -8917,7 +8917,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:G6"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13158,7 +13158,7 @@
         <v>658</v>
       </c>
       <c r="X54" s="44" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
@@ -13228,7 +13228,7 @@
         <v>658</v>
       </c>
       <c r="X55" s="44" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
@@ -13298,7 +13298,7 @@
         <v>658</v>
       </c>
       <c r="X56" s="44" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
@@ -13368,7 +13368,7 @@
         <v>658</v>
       </c>
       <c r="X57" s="44" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
@@ -13438,7 +13438,7 @@
         <v>658</v>
       </c>
       <c r="X58" s="44" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
@@ -22211,7 +22211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView topLeftCell="B34" workbookViewId="0">
+    <sheetView topLeftCell="B31" workbookViewId="0">
       <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
@@ -22521,10 +22521,10 @@
     </row>
     <row r="16" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="83" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C16" s="43"/>
       <c r="D16" s="43"/>
@@ -22535,7 +22535,7 @@
       <c r="I16" s="43"/>
       <c r="J16" s="44"/>
       <c r="K16" s="89" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="L16" s="87"/>
     </row>
@@ -22803,7 +22803,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="83" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B30" s="48"/>
       <c r="C30" s="43"/>
@@ -22815,7 +22815,7 @@
       <c r="I30" s="43"/>
       <c r="J30" s="44"/>
       <c r="K30" s="89" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="L30" s="87">
         <v>3</v>
@@ -22903,7 +22903,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="83" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="43"/>
@@ -22915,13 +22915,13 @@
       <c r="I35" s="43"/>
       <c r="J35" s="44"/>
       <c r="K35" s="89" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="L35" s="87"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="83" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="43"/>
@@ -22933,7 +22933,7 @@
       <c r="I36" s="43"/>
       <c r="J36" s="44"/>
       <c r="K36" s="89" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="L36" s="87"/>
     </row>
@@ -22977,10 +22977,10 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="83" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="B39" s="48" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="C39" s="43" t="s">
         <v>745</v>
@@ -22993,7 +22993,7 @@
       <c r="I39" s="43"/>
       <c r="J39" s="44"/>
       <c r="K39" s="89" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="L39" s="87"/>
     </row>
@@ -23093,7 +23093,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="83" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B45" s="48"/>
       <c r="C45" s="43"/>
@@ -23111,7 +23111,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="83" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B46" s="48"/>
       <c r="C46" s="43"/>
@@ -23123,7 +23123,7 @@
       <c r="I46" s="43"/>
       <c r="J46" s="44"/>
       <c r="K46" s="89" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="L46" s="87">
         <v>3</v>
@@ -23131,10 +23131,10 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="83" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="B47" s="48" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="C47" s="43" t="s">
         <v>745</v>
@@ -23147,7 +23147,7 @@
       <c r="I47" s="43"/>
       <c r="J47" s="44"/>
       <c r="K47" s="89" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="L47" s="87"/>
     </row>
@@ -23811,7 +23811,7 @@
       <c r="I81" s="43"/>
       <c r="J81" s="44"/>
       <c r="K81" s="89" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="L81" s="87"/>
     </row>
@@ -24089,8 +24089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24169,7 +24169,7 @@
         <v>372</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="F3" s="129"/>
       <c r="G3" s="31"/>
@@ -24196,7 +24196,7 @@
         <v>382</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="F4" s="129"/>
       <c r="G4" s="31"/>
@@ -24287,7 +24287,7 @@
         <v>492</v>
       </c>
       <c r="E8" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F8" s="133" t="s">
         <v>745</v>
@@ -24695,7 +24695,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="129" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B28" s="129" t="s">
         <v>582</v>
@@ -24704,12 +24704,12 @@
         <v>488</v>
       </c>
       <c r="M28" s="129" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="129" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B29" s="129" t="s">
         <v>582</v>
@@ -24719,7 +24719,7 @@
       </c>
       <c r="L29" s="32"/>
       <c r="M29" s="129" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="N29"/>
     </row>
@@ -24734,22 +24734,22 @@
         <v>488</v>
       </c>
       <c r="M30" s="129" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="129" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="129" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="129" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B33" s="129" t="s">
         <v>582</v>
@@ -24758,15 +24758,15 @@
         <v>488</v>
       </c>
       <c r="E33" s="129" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="M33" s="129" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="129" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B34" s="129" t="s">
         <v>374</v>
@@ -24775,10 +24775,10 @@
         <v>488</v>
       </c>
       <c r="E34" s="129" t="s">
+        <v>893</v>
+      </c>
+      <c r="M34" s="129" t="s">
         <v>894</v>
-      </c>
-      <c r="M34" s="129" t="s">
-        <v>895</v>
       </c>
       <c r="N34" s="34">
         <v>5</v>
@@ -24786,7 +24786,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="129" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B35" s="129" t="s">
         <v>374</v>
@@ -24795,15 +24795,15 @@
         <v>488</v>
       </c>
       <c r="E35" s="129" t="s">
+        <v>896</v>
+      </c>
+      <c r="M35" s="129" t="s">
         <v>897</v>
-      </c>
-      <c r="M35" s="129" t="s">
-        <v>898</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="129" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B36" s="129" t="s">
         <v>374</v>
@@ -24812,15 +24812,15 @@
         <v>488</v>
       </c>
       <c r="E36" s="129" t="s">
+        <v>899</v>
+      </c>
+      <c r="M36" s="129" t="s">
         <v>900</v>
-      </c>
-      <c r="M36" s="129" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="129" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B37" s="129" t="s">
         <v>374</v>
@@ -24829,15 +24829,15 @@
         <v>488</v>
       </c>
       <c r="E37" s="129" t="s">
+        <v>902</v>
+      </c>
+      <c r="M37" s="129" t="s">
         <v>903</v>
-      </c>
-      <c r="M37" s="129" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="129" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B38" s="129" t="s">
         <v>374</v>
@@ -24846,10 +24846,10 @@
         <v>488</v>
       </c>
       <c r="E38" s="129" t="s">
+        <v>905</v>
+      </c>
+      <c r="M38" s="129" t="s">
         <v>906</v>
-      </c>
-      <c r="M38" s="129" t="s">
-        <v>907</v>
       </c>
       <c r="N38" s="34">
         <v>5</v>
@@ -24866,12 +24866,12 @@
         <v>488</v>
       </c>
       <c r="M39" s="130" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="130" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B40" s="130" t="s">
         <v>582</v>
@@ -24880,41 +24880,41 @@
         <v>488</v>
       </c>
       <c r="M40" s="130" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="130" t="s">
+        <v>924</v>
+      </c>
+      <c r="B41" s="130" t="s">
         <v>925</v>
-      </c>
-      <c r="B41" s="130" t="s">
-        <v>926</v>
       </c>
       <c r="D41" s="130" t="s">
         <v>488</v>
       </c>
       <c r="E41" s="130" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="M41" s="130" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="130" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B42" s="130" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D42" s="130" t="s">
         <v>488</v>
       </c>
       <c r="E42" s="130" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="M42" s="130" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="N42" s="34">
         <v>3</v>
@@ -24922,7 +24922,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="131" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B43" s="131" t="s">
         <v>374</v>
@@ -24931,10 +24931,10 @@
         <v>488</v>
       </c>
       <c r="E43" s="131" t="s">
+        <v>932</v>
+      </c>
+      <c r="M43" s="131" t="s">
         <v>933</v>
-      </c>
-      <c r="M43" s="131" t="s">
-        <v>934</v>
       </c>
       <c r="N43" s="34">
         <v>3</v>
@@ -24942,7 +24942,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="131" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B44" s="131" t="s">
         <v>374</v>
@@ -24951,10 +24951,10 @@
         <v>488</v>
       </c>
       <c r="E44" s="131" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="M44" s="131" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="N44" s="34">
         <v>3</v>
@@ -24962,7 +24962,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="131" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B45" s="131" t="s">
         <v>374</v>
@@ -24971,10 +24971,10 @@
         <v>488</v>
       </c>
       <c r="E45" s="131" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="M45" s="131" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="N45" s="34">
         <v>3</v>
@@ -24982,7 +24982,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="133" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B46" s="133" t="s">
         <v>374</v>
@@ -24991,10 +24991,10 @@
         <v>422</v>
       </c>
       <c r="E46" s="133" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="M46" s="133" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="N46" s="34">
         <v>3</v>
@@ -25002,7 +25002,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="134" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B47" s="134" t="s">
         <v>375</v>
@@ -25011,16 +25011,16 @@
         <v>492</v>
       </c>
       <c r="E47" s="134" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F47" s="134" t="s">
         <v>745</v>
       </c>
       <c r="G47" s="134" t="s">
+        <v>945</v>
+      </c>
+      <c r="M47" s="134" t="s">
         <v>946</v>
-      </c>
-      <c r="M47" s="134" t="s">
-        <v>947</v>
       </c>
       <c r="N47" s="34">
         <v>3</v>
@@ -25028,7 +25028,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="134" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B48" s="134" t="s">
         <v>375</v>
@@ -25037,30 +25037,30 @@
         <v>492</v>
       </c>
       <c r="E48" s="134" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F48" s="134" t="s">
         <v>745</v>
       </c>
       <c r="M48" s="134" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="134" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B49" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D49" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E49" s="134" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="M49" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="N49" s="34">
         <v>3</v>
@@ -25068,19 +25068,19 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="134" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B50" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D50" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E50" s="134" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="M50" s="134" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="N50" s="34">
         <v>3</v>
@@ -25088,53 +25088,53 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="134" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B51" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D51" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E51" s="134" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="M51" s="134" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="134" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B52" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D52" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E52" s="134" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="M52" s="134" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="134" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B53" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D53" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E53" s="134" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="M53" s="134" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="N53" s="34">
         <v>3</v>
@@ -25142,19 +25142,19 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="134" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B54" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D54" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E54" s="134" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="M54" s="134" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="N54" s="34">
         <v>3</v>
@@ -25162,19 +25162,19 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="134" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="B55" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D55" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E55" s="134" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="M55" s="135" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="N55" s="136">
         <v>3</v>
@@ -25184,19 +25184,19 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="134" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B56" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D56" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E56" s="134" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="M56" s="134" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="N56" s="34">
         <v>3</v>
@@ -25204,19 +25204,19 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="134" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B57" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D57" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E57" s="134" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="M57" s="134" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="N57" s="34">
         <v>3</v>
@@ -25224,19 +25224,19 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="134" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B58" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D58" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E58" s="134" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="M58" s="134" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="N58" s="34">
         <v>3</v>
@@ -25244,19 +25244,19 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="134" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B59" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D59" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E59" s="134" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="M59" s="134" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="N59" s="34">
         <v>3</v>
@@ -25264,53 +25264,53 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="134" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B60" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D60" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E60" s="134" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="M60" s="134" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="134" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B61" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D61" s="134" t="s">
         <v>382</v>
       </c>
       <c r="E61" s="134" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="M61" s="134" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="134" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="B62" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D62" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E62" s="134" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="M62" s="134" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="N62" s="34">
         <v>3</v>
@@ -25318,19 +25318,19 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="134" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B63" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D63" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E63" s="134" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="M63" s="134" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="N63" s="34">
         <v>3</v>
@@ -25338,19 +25338,19 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="134" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B64" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D64" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E64" s="134" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="M64" s="134" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="N64" s="34">
         <v>4</v>
@@ -25358,19 +25358,19 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="134" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B65" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D65" s="134" t="s">
         <v>422</v>
       </c>
       <c r="E65" s="134" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="M65" s="134" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="N65" s="34">
         <v>3</v>
@@ -25378,36 +25378,36 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="134" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B66" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D66" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E66" s="134" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="M66" s="134" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="134" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B67" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D67" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E67" s="134" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="M67" s="134" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="N67" s="34">
         <v>3</v>
@@ -25415,19 +25415,19 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="134" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B68" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D68" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E68" s="134" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="M68" s="134" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
@@ -25435,16 +25435,16 @@
         <v>483</v>
       </c>
       <c r="B69" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D69" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E69" s="134" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="M69" s="134" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
   </sheetData>
@@ -25460,7 +25460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -25499,34 +25499,34 @@
         <v>363</v>
       </c>
       <c r="B1" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="C1" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="D1" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="E1" s="137" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="F1" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="G1" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="H1" t="s">
         <v>376</v>
       </c>
       <c r="I1" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="J1" t="s">
         <v>491</v>
       </c>
       <c r="K1" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="L1" t="s">
         <v>364</v>
@@ -25535,7 +25535,7 @@
         <v>236</v>
       </c>
       <c r="N1" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="O1" s="3">
         <v>1</v>
@@ -25690,25 +25690,25 @@
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" s="137" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B2" s="137" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="C2" s="137" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="D2" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="137" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="F2" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G2" s="137" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="H2" s="137">
         <v>3</v>
@@ -25721,25 +25721,25 @@
       </c>
       <c r="K2" s="137"/>
       <c r="L2" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="M2" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="N2" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="T2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="X2" t="s">
         <v>1018</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Z2" t="s">
         <v>1019</v>
-      </c>
-      <c r="X2" t="s">
-        <v>1020</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>1021</v>
       </c>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.25">
@@ -25747,22 +25747,22 @@
         <v>501</v>
       </c>
       <c r="B3" s="137" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="C3" s="137" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="D3" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="137" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="F3" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G3" s="137" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="H3" s="137">
         <v>5</v>
@@ -25775,13 +25775,13 @@
       </c>
       <c r="K3" s="137"/>
       <c r="L3" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="M3" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="N3" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="O3" s="138"/>
       <c r="P3" s="138"/>
@@ -25790,25 +25790,25 @@
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="B4" s="137" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="C4" s="137" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="D4" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="137" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="F4" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G4" s="137" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="H4" s="137">
         <v>4</v>
@@ -25821,19 +25821,19 @@
       </c>
       <c r="K4" s="137"/>
       <c r="L4" t="s">
+        <v>1020</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1060</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1013</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1021</v>
+      </c>
+      <c r="AD4" t="s">
         <v>1022</v>
-      </c>
-      <c r="M4" t="s">
-        <v>1062</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1015</v>
-      </c>
-      <c r="R4" t="s">
-        <v>1023</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.25">
@@ -25841,20 +25841,20 @@
         <v>493</v>
       </c>
       <c r="B5" s="137" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="C5" s="137" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="D5" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="137" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="F5" s="137"/>
       <c r="G5" s="137" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="H5" s="137">
         <v>4</v>
@@ -25869,13 +25869,13 @@
         <v>247</v>
       </c>
       <c r="L5" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="M5" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="N5" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="U5" s="138">
         <v>0.18</v>
@@ -25895,20 +25895,20 @@
         <v>497</v>
       </c>
       <c r="B6" s="137" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="C6" s="137" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="D6" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="137" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="F6" s="137"/>
       <c r="G6" s="137" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="H6" s="137">
         <v>3</v>
@@ -25917,19 +25917,19 @@
         <v>1</v>
       </c>
       <c r="J6" s="137" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="K6" s="137" t="s">
         <v>246</v>
       </c>
       <c r="L6" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="M6" s="139" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="N6" s="137" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="T6" s="138"/>
       <c r="X6" s="138"/>
@@ -25940,10 +25940,10 @@
         <v>558</v>
       </c>
       <c r="B7" s="137" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="C7" s="137" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="D7" s="137" t="s">
         <v>33</v>
@@ -25953,7 +25953,7 @@
       </c>
       <c r="F7" s="137"/>
       <c r="G7" s="137" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="H7" s="137">
         <v>4</v>
@@ -25965,46 +25965,46 @@
         <v>3</v>
       </c>
       <c r="K7" s="137" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="L7" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="M7" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="R7" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="V7" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="Z7" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="AD7" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B8" s="137" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C8" s="137" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D8" s="137" t="s">
         <v>1050</v>
       </c>
-      <c r="B8" s="137" t="s">
-        <v>1012</v>
-      </c>
-      <c r="C8" s="137" t="s">
-        <v>1051</v>
-      </c>
-      <c r="D8" s="137" t="s">
-        <v>1052</v>
-      </c>
       <c r="E8" s="137" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="F8" s="137"/>
       <c r="G8" s="137" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="H8" s="137">
         <v>0</v>
@@ -26017,10 +26017,10 @@
       </c>
       <c r="K8" s="137"/>
       <c r="L8" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="M8" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="W8">
         <v>2</v>
@@ -26037,22 +26037,22 @@
         <v>490</v>
       </c>
       <c r="B9" s="137" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="C9" s="137" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="D9" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="137" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="F9" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G9" s="137" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="H9" s="137">
         <v>4</v>
@@ -26067,10 +26067,10 @@
         <v>246</v>
       </c>
       <c r="L9" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="M9" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.25">
@@ -26078,20 +26078,20 @@
         <v>496</v>
       </c>
       <c r="B10" s="137" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="C10" s="137" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="D10" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="137" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="F10" s="137"/>
       <c r="G10" s="137" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="H10" s="137">
         <v>4</v>
@@ -26106,13 +26106,13 @@
         <v>246</v>
       </c>
       <c r="L10" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="M10" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="N10" s="139" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.25">
@@ -26120,10 +26120,10 @@
         <v>565</v>
       </c>
       <c r="B11" s="137" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="C11" s="137" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="D11" s="137" t="s">
         <v>33</v>
@@ -26133,7 +26133,7 @@
       </c>
       <c r="F11" s="137"/>
       <c r="G11" s="137" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="H11" s="137">
         <v>1</v>
@@ -26148,25 +26148,25 @@
         <v>246</v>
       </c>
       <c r="L11" t="s">
+        <v>1071</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1054</v>
+      </c>
+      <c r="N11" s="139" t="s">
+        <v>1072</v>
+      </c>
+      <c r="S11" t="s">
+        <v>1055</v>
+      </c>
+      <c r="X11" t="s">
+        <v>1055</v>
+      </c>
+      <c r="AC11" t="s">
         <v>1073</v>
       </c>
-      <c r="M11" t="s">
-        <v>1056</v>
-      </c>
-      <c r="N11" s="139" t="s">
-        <v>1074</v>
-      </c>
-      <c r="S11" t="s">
-        <v>1057</v>
-      </c>
-      <c r="X11" t="s">
-        <v>1057</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>1075</v>
-      </c>
       <c r="AH11" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.25">
@@ -27647,10 +27647,10 @@
     </row>
     <row r="19" spans="1:15" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="104" t="s">
+        <v>941</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>942</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>943</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -28157,7 +28157,7 @@
         <v>278</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -28410,19 +28410,19 @@
         <v>773</v>
       </c>
       <c r="K61" s="76" t="s">
+        <v>910</v>
+      </c>
+      <c r="L61" s="76" t="s">
         <v>911</v>
       </c>
-      <c r="L61" s="76" t="s">
+      <c r="M61" s="76" t="s">
         <v>912</v>
       </c>
-      <c r="M61" s="76" t="s">
+      <c r="N61" s="76" t="s">
         <v>913</v>
       </c>
-      <c r="N61" s="76" t="s">
+      <c r="O61" s="74" t="s">
         <v>914</v>
-      </c>
-      <c r="O61" s="74" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Implementing shield wall and many fixes
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -643,7 +643,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2232" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2230" uniqueCount="1075">
   <si>
     <t>Fishing</t>
   </si>
@@ -3868,12 +3868,6 @@
   </si>
   <si>
     <t>Fires a dart at target that if hits, does DoT damage as well as initial damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a </t>
-  </si>
-  <si>
-    <t>shield wall</t>
   </si>
 </sst>
 </file>
@@ -3923,7 +3917,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3963,6 +3957,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4724,7 +4724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5043,22 +5043,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5076,10 +5088,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5127,22 +5145,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -5451,8 +5457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5467,29 +5473,29 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="150" t="s">
         <v>782</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="148"/>
+      <c r="B2" s="151"/>
+      <c r="C2" s="152"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="115">
         <v>1</v>
       </c>
-      <c r="B3" s="149" t="s">
+      <c r="B3" s="153" t="s">
         <v>783</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="154"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="155" t="s">
         <v>784</v>
       </c>
-      <c r="C4" s="141"/>
+      <c r="C4" s="156"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="116"/>
@@ -5540,10 +5546,10 @@
       <c r="A10" s="116">
         <v>3</v>
       </c>
-      <c r="B10" s="142" t="s">
+      <c r="B10" s="157" t="s">
         <v>785</v>
       </c>
-      <c r="C10" s="143"/>
+      <c r="C10" s="158"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="116"/>
@@ -5558,10 +5564,10 @@
       <c r="A12" s="116">
         <v>4</v>
       </c>
-      <c r="B12" s="144" t="s">
+      <c r="B12" s="146" t="s">
         <v>786</v>
       </c>
-      <c r="C12" s="145"/>
+      <c r="C12" s="147"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="116"/>
@@ -5576,10 +5582,10 @@
       <c r="A14" s="116">
         <v>5</v>
       </c>
-      <c r="B14" s="144" t="s">
+      <c r="B14" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="C14" s="145"/>
+      <c r="C14" s="147"/>
     </row>
     <row r="15" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="116"/>
@@ -5594,10 +5600,10 @@
       <c r="A16" s="117">
         <v>6</v>
       </c>
-      <c r="B16" s="151" t="s">
+      <c r="B16" s="148" t="s">
         <v>791</v>
       </c>
-      <c r="C16" s="152"/>
+      <c r="C16" s="149"/>
     </row>
     <row r="17" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="116"/>
@@ -5612,61 +5618,57 @@
       <c r="A18" s="117">
         <v>7</v>
       </c>
-      <c r="B18" s="151" t="s">
+      <c r="B18" s="148" t="s">
         <v>915</v>
       </c>
-      <c r="C18" s="152"/>
+      <c r="C18" s="149"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="132">
         <v>8</v>
       </c>
-      <c r="B19" s="151" t="s">
+      <c r="B19" s="148" t="s">
         <v>1002</v>
       </c>
-      <c r="C19" s="152"/>
+      <c r="C19" s="149"/>
     </row>
     <row r="20" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="132">
         <v>9</v>
       </c>
-      <c r="B20" s="151" t="s">
+      <c r="B20" s="148" t="s">
         <v>916</v>
       </c>
-      <c r="C20" s="152"/>
+      <c r="C20" s="149"/>
     </row>
     <row r="21" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="146" t="s">
+      <c r="A22" s="150" t="s">
         <v>183</v>
       </c>
-      <c r="B22" s="147"/>
-      <c r="C22" s="148"/>
+      <c r="B22" s="151"/>
+      <c r="C22" s="152"/>
     </row>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="115">
         <v>1</v>
       </c>
-      <c r="B23" s="149" t="s">
+      <c r="B23" s="153" t="s">
         <v>792</v>
       </c>
-      <c r="C23" s="150"/>
+      <c r="C23" s="154"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="116"/>
-      <c r="B24" s="168" t="s">
-        <v>1075</v>
-      </c>
-      <c r="C24" s="169" t="s">
-        <v>1076</v>
-      </c>
+      <c r="B24" s="174"/>
+      <c r="C24" s="175"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="116"/>
-      <c r="B25" s="168" t="s">
+      <c r="B25" s="140" t="s">
         <v>793</v>
       </c>
-      <c r="C25" s="169" t="s">
+      <c r="C25" s="141" t="s">
         <v>797</v>
       </c>
     </row>
@@ -5687,20 +5689,20 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="146" t="s">
+      <c r="A30" s="150" t="s">
         <v>794</v>
       </c>
-      <c r="B30" s="147"/>
-      <c r="C30" s="148"/>
+      <c r="B30" s="151"/>
+      <c r="C30" s="152"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="115">
         <v>1</v>
       </c>
-      <c r="B31" s="149" t="s">
+      <c r="B31" s="153" t="s">
         <v>782</v>
       </c>
-      <c r="C31" s="150"/>
+      <c r="C31" s="154"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="116"/>
@@ -5709,10 +5711,10 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="116"/>
-      <c r="B33" s="168" t="s">
+      <c r="B33" s="140" t="s">
         <v>789</v>
       </c>
-      <c r="C33" s="169" t="s">
+      <c r="C33" s="141" t="s">
         <v>1001</v>
       </c>
     </row>
@@ -5720,10 +5722,10 @@
       <c r="A34" s="116">
         <v>2</v>
       </c>
-      <c r="B34" s="140" t="s">
+      <c r="B34" s="155" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="141"/>
+      <c r="C34" s="156"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="116"/>
@@ -5743,45 +5745,45 @@
       <c r="A37" s="116">
         <v>3</v>
       </c>
-      <c r="B37" s="140" t="s">
+      <c r="B37" s="155" t="s">
         <v>1003</v>
       </c>
-      <c r="C37" s="141"/>
+      <c r="C37" s="156"/>
     </row>
     <row r="38" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="116"/>
-      <c r="B38" s="170" t="s">
+      <c r="B38" s="142" t="s">
         <v>788</v>
       </c>
-      <c r="C38" s="171" t="s">
+      <c r="C38" s="143" t="s">
         <v>1004</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="116"/>
-      <c r="B39" s="172" t="s">
+      <c r="B39" s="144" t="s">
         <v>789</v>
       </c>
-      <c r="C39" s="173" t="s">
+      <c r="C39" s="145" t="s">
         <v>1005</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="146" t="s">
+      <c r="A41" s="150" t="s">
         <v>799</v>
       </c>
-      <c r="B41" s="147"/>
-      <c r="C41" s="148"/>
+      <c r="B41" s="151"/>
+      <c r="C41" s="152"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="115">
         <v>1</v>
       </c>
-      <c r="B42" s="149" t="s">
+      <c r="B42" s="153" t="s">
         <v>800</v>
       </c>
-      <c r="C42" s="150"/>
+      <c r="C42" s="154"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="116"/>
@@ -5821,20 +5823,20 @@
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="146" t="s">
+      <c r="A48" s="150" t="s">
         <v>804</v>
       </c>
-      <c r="B48" s="147"/>
-      <c r="C48" s="148"/>
+      <c r="B48" s="151"/>
+      <c r="C48" s="152"/>
     </row>
     <row r="49" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="115">
         <v>1</v>
       </c>
-      <c r="B49" s="149" t="s">
+      <c r="B49" s="153" t="s">
         <v>805</v>
       </c>
-      <c r="C49" s="150"/>
+      <c r="C49" s="154"/>
     </row>
     <row r="50" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="116"/>
@@ -5858,10 +5860,10 @@
       <c r="A52" s="115">
         <v>1</v>
       </c>
-      <c r="B52" s="149" t="s">
+      <c r="B52" s="153" t="s">
         <v>807</v>
       </c>
-      <c r="C52" s="150"/>
+      <c r="C52" s="154"/>
     </row>
     <row r="53" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="116"/>
@@ -5897,263 +5899,263 @@
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="146" t="s">
+      <c r="A58" s="150" t="s">
         <v>188</v>
       </c>
-      <c r="B58" s="147"/>
-      <c r="C58" s="148"/>
+      <c r="B58" s="151"/>
+      <c r="C58" s="152"/>
     </row>
     <row r="59" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="115">
         <v>1</v>
       </c>
-      <c r="B59" s="149" t="s">
+      <c r="B59" s="153" t="s">
         <v>812</v>
       </c>
-      <c r="C59" s="150"/>
+      <c r="C59" s="154"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="146" t="s">
+      <c r="A61" s="150" t="s">
         <v>790</v>
       </c>
-      <c r="B61" s="147"/>
-      <c r="C61" s="148"/>
+      <c r="B61" s="151"/>
+      <c r="C61" s="152"/>
     </row>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="115">
         <v>1</v>
       </c>
-      <c r="B62" s="142" t="s">
+      <c r="B62" s="157" t="s">
         <v>783</v>
       </c>
-      <c r="C62" s="143"/>
+      <c r="C62" s="158"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="116">
         <v>2</v>
       </c>
-      <c r="B63" s="153" t="s">
+      <c r="B63" s="159" t="s">
         <v>784</v>
       </c>
-      <c r="C63" s="154"/>
+      <c r="C63" s="160"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="116">
         <v>3</v>
       </c>
-      <c r="B64" s="144" t="s">
+      <c r="B64" s="146" t="s">
         <v>785</v>
       </c>
-      <c r="C64" s="145"/>
+      <c r="C64" s="147"/>
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="116">
         <v>4</v>
       </c>
-      <c r="B65" s="144" t="s">
+      <c r="B65" s="146" t="s">
         <v>786</v>
       </c>
-      <c r="C65" s="145"/>
+      <c r="C65" s="147"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="116">
         <v>5</v>
       </c>
-      <c r="B66" s="144" t="s">
+      <c r="B66" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="C66" s="145"/>
+      <c r="C66" s="147"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="117">
         <v>6</v>
       </c>
-      <c r="B67" s="151" t="s">
+      <c r="B67" s="148" t="s">
         <v>791</v>
       </c>
-      <c r="C67" s="152"/>
+      <c r="C67" s="149"/>
     </row>
     <row r="68" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="146" t="s">
+      <c r="A69" s="150" t="s">
         <v>813</v>
       </c>
-      <c r="B69" s="147"/>
-      <c r="C69" s="148"/>
+      <c r="B69" s="151"/>
+      <c r="C69" s="152"/>
     </row>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="115">
         <v>1</v>
       </c>
-      <c r="B70" s="142" t="s">
+      <c r="B70" s="157" t="s">
         <v>783</v>
       </c>
-      <c r="C70" s="143"/>
+      <c r="C70" s="158"/>
     </row>
     <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="116">
         <v>2</v>
       </c>
-      <c r="B71" s="153" t="s">
+      <c r="B71" s="159" t="s">
         <v>784</v>
       </c>
-      <c r="C71" s="154"/>
+      <c r="C71" s="160"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="116">
         <v>3</v>
       </c>
-      <c r="B72" s="144" t="s">
+      <c r="B72" s="146" t="s">
         <v>785</v>
       </c>
-      <c r="C72" s="145"/>
+      <c r="C72" s="147"/>
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="116">
         <v>4</v>
       </c>
-      <c r="B73" s="144" t="s">
+      <c r="B73" s="146" t="s">
         <v>786</v>
       </c>
-      <c r="C73" s="145"/>
+      <c r="C73" s="147"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="116">
         <v>5</v>
       </c>
-      <c r="B74" s="144" t="s">
+      <c r="B74" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="C74" s="145"/>
+      <c r="C74" s="147"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="117">
         <v>6</v>
       </c>
-      <c r="B75" s="151" t="s">
+      <c r="B75" s="148" t="s">
         <v>791</v>
       </c>
-      <c r="C75" s="152"/>
+      <c r="C75" s="149"/>
     </row>
     <row r="76" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="146" t="s">
+      <c r="A77" s="150" t="s">
         <v>1003</v>
       </c>
-      <c r="B77" s="147"/>
-      <c r="C77" s="148"/>
+      <c r="B77" s="151"/>
+      <c r="C77" s="152"/>
     </row>
     <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="115">
         <v>1</v>
       </c>
-      <c r="B78" s="142"/>
-      <c r="C78" s="143"/>
+      <c r="B78" s="157"/>
+      <c r="C78" s="158"/>
     </row>
     <row r="79" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="116"/>
-      <c r="B79" s="153"/>
-      <c r="C79" s="154"/>
+      <c r="B79" s="159"/>
+      <c r="C79" s="160"/>
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="116"/>
-      <c r="B80" s="144"/>
-      <c r="C80" s="145"/>
+      <c r="B80" s="146"/>
+      <c r="C80" s="147"/>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="116"/>
-      <c r="B81" s="144"/>
-      <c r="C81" s="145"/>
+      <c r="B81" s="146"/>
+      <c r="C81" s="147"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="116"/>
-      <c r="B82" s="144"/>
-      <c r="C82" s="145"/>
+      <c r="B82" s="146"/>
+      <c r="C82" s="147"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="117"/>
-      <c r="B83" s="151"/>
-      <c r="C83" s="152"/>
+      <c r="B83" s="148"/>
+      <c r="C83" s="149"/>
     </row>
     <row r="84" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="146" t="s">
+      <c r="A85" s="150" t="s">
         <v>814</v>
       </c>
-      <c r="B85" s="147"/>
-      <c r="C85" s="148"/>
+      <c r="B85" s="151"/>
+      <c r="C85" s="152"/>
     </row>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="115">
         <v>1</v>
       </c>
-      <c r="B86" s="142" t="s">
+      <c r="B86" s="157" t="s">
         <v>783</v>
       </c>
-      <c r="C86" s="143"/>
+      <c r="C86" s="158"/>
     </row>
     <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="116">
         <v>2</v>
       </c>
-      <c r="B87" s="153" t="s">
+      <c r="B87" s="159" t="s">
         <v>784</v>
       </c>
-      <c r="C87" s="154"/>
+      <c r="C87" s="160"/>
     </row>
     <row r="88" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="116">
         <v>3</v>
       </c>
-      <c r="B88" s="144" t="s">
+      <c r="B88" s="146" t="s">
         <v>785</v>
       </c>
-      <c r="C88" s="145"/>
+      <c r="C88" s="147"/>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="116">
         <v>4</v>
       </c>
-      <c r="B89" s="144" t="s">
+      <c r="B89" s="146" t="s">
         <v>786</v>
       </c>
-      <c r="C89" s="145"/>
+      <c r="C89" s="147"/>
     </row>
     <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="116">
         <v>5</v>
       </c>
-      <c r="B90" s="144" t="s">
+      <c r="B90" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="C90" s="145"/>
+      <c r="C90" s="147"/>
     </row>
     <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="117">
         <v>6</v>
       </c>
-      <c r="B91" s="151" t="s">
+      <c r="B91" s="148" t="s">
         <v>791</v>
       </c>
-      <c r="C91" s="152"/>
+      <c r="C91" s="149"/>
     </row>
     <row r="92" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="93" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="146" t="s">
+      <c r="A93" s="150" t="s">
         <v>864</v>
       </c>
-      <c r="B93" s="147"/>
-      <c r="C93" s="148"/>
+      <c r="B93" s="151"/>
+      <c r="C93" s="152"/>
     </row>
     <row r="94" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="115">
         <v>1</v>
       </c>
-      <c r="B94" s="149" t="s">
+      <c r="B94" s="153" t="s">
         <v>101</v>
       </c>
-      <c r="C94" s="150"/>
+      <c r="C94" s="154"/>
     </row>
     <row r="95" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="124"/>
@@ -6326,10 +6328,10 @@
       <c r="A114" s="116">
         <v>2</v>
       </c>
-      <c r="B114" s="140" t="s">
+      <c r="B114" s="155" t="s">
         <v>815</v>
       </c>
-      <c r="C114" s="141"/>
+      <c r="C114" s="156"/>
     </row>
     <row r="115" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="116"/>
@@ -6407,10 +6409,10 @@
       <c r="A123" s="116">
         <v>3</v>
       </c>
-      <c r="B123" s="142" t="s">
+      <c r="B123" s="157" t="s">
         <v>816</v>
       </c>
-      <c r="C123" s="143"/>
+      <c r="C123" s="158"/>
     </row>
     <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="116"/>
@@ -6466,10 +6468,10 @@
       <c r="A130" s="115">
         <v>4</v>
       </c>
-      <c r="B130" s="144" t="s">
+      <c r="B130" s="146" t="s">
         <v>817</v>
       </c>
-      <c r="C130" s="145"/>
+      <c r="C130" s="147"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="124"/>
@@ -6509,20 +6511,20 @@
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="136" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="146" t="s">
+      <c r="A136" s="150" t="s">
         <v>865</v>
       </c>
-      <c r="B136" s="147"/>
-      <c r="C136" s="148"/>
+      <c r="B136" s="151"/>
+      <c r="C136" s="152"/>
     </row>
     <row r="137" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="115">
         <v>1</v>
       </c>
-      <c r="B137" s="149" t="s">
+      <c r="B137" s="153" t="s">
         <v>866</v>
       </c>
-      <c r="C137" s="150"/>
+      <c r="C137" s="154"/>
     </row>
     <row r="138" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="124"/>
@@ -6669,10 +6671,10 @@
       <c r="A157" s="116">
         <v>2</v>
       </c>
-      <c r="B157" s="140" t="s">
+      <c r="B157" s="155" t="s">
         <v>867</v>
       </c>
-      <c r="C157" s="141"/>
+      <c r="C157" s="156"/>
     </row>
     <row r="158" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="116"/>
@@ -6742,10 +6744,10 @@
       <c r="A166" s="116">
         <v>3</v>
       </c>
-      <c r="B166" s="142" t="s">
+      <c r="B166" s="157" t="s">
         <v>868</v>
       </c>
-      <c r="C166" s="143"/>
+      <c r="C166" s="158"/>
     </row>
     <row r="167" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="116"/>
@@ -6799,6 +6801,50 @@
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="A136:C136"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="A93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B37:C37"/>
     <mergeCell ref="B81:C81"/>
     <mergeCell ref="B82:C82"/>
     <mergeCell ref="B83:C83"/>
@@ -6815,50 +6861,6 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B34:C34"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="A93:C93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="A77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="A136:C136"/>
-    <mergeCell ref="B137:C137"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -8055,31 +8057,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="158" t="s">
+      <c r="B1" s="164" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="159"/>
-      <c r="G1" s="159"/>
-      <c r="H1" s="159"/>
-      <c r="I1" s="159"/>
-      <c r="J1" s="160"/>
-      <c r="K1" s="161" t="s">
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
+      <c r="E1" s="165"/>
+      <c r="F1" s="165"/>
+      <c r="G1" s="165"/>
+      <c r="H1" s="165"/>
+      <c r="I1" s="165"/>
+      <c r="J1" s="166"/>
+      <c r="K1" s="167" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="162"/>
-      <c r="M1" s="162"/>
-      <c r="N1" s="162"/>
-      <c r="O1" s="162"/>
-      <c r="P1" s="162"/>
-      <c r="Q1" s="162"/>
-      <c r="R1" s="162"/>
-      <c r="S1" s="162"/>
-      <c r="T1" s="162"/>
-      <c r="U1" s="162"/>
-      <c r="V1" s="163"/>
+      <c r="L1" s="168"/>
+      <c r="M1" s="168"/>
+      <c r="N1" s="168"/>
+      <c r="O1" s="168"/>
+      <c r="P1" s="168"/>
+      <c r="Q1" s="168"/>
+      <c r="R1" s="168"/>
+      <c r="S1" s="168"/>
+      <c r="T1" s="168"/>
+      <c r="U1" s="168"/>
+      <c r="V1" s="169"/>
     </row>
     <row r="2" spans="1:22" ht="44.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K2" s="66" t="s">
@@ -22231,17 +22233,17 @@
       <c r="A1" s="81" t="s">
         <v>363</v>
       </c>
-      <c r="B1" s="164" t="s">
+      <c r="B1" s="170" t="s">
         <v>365</v>
       </c>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
-      <c r="J1" s="166"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
+      <c r="G1" s="171"/>
+      <c r="H1" s="171"/>
+      <c r="I1" s="171"/>
+      <c r="J1" s="172"/>
       <c r="K1" s="91" t="s">
         <v>364</v>
       </c>
@@ -24108,15 +24110,15 @@
       <c r="C1" t="s">
         <v>701</v>
       </c>
-      <c r="E1" s="167" t="s">
+      <c r="E1" s="173" t="s">
         <v>365</v>
       </c>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="167"/>
-      <c r="J1" s="167"/>
-      <c r="K1" s="167"/>
+      <c r="F1" s="173"/>
+      <c r="G1" s="173"/>
+      <c r="H1" s="173"/>
+      <c r="I1" s="173"/>
+      <c r="J1" s="173"/>
+      <c r="K1" s="173"/>
       <c r="L1" s="31"/>
     </row>
     <row r="2" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
@@ -27233,24 +27235,24 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="100"/>
-      <c r="B1" s="157" t="s">
+      <c r="B1" s="163" t="s">
         <v>702</v>
       </c>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
       <c r="E1" s="101"/>
-      <c r="F1" s="155" t="s">
+      <c r="F1" s="161" t="s">
         <v>350</v>
       </c>
-      <c r="G1" s="155"/>
-      <c r="H1" s="155"/>
-      <c r="I1" s="155"/>
-      <c r="J1" s="155"/>
-      <c r="K1" s="155"/>
-      <c r="L1" s="155"/>
-      <c r="M1" s="155"/>
-      <c r="N1" s="155"/>
-      <c r="O1" s="156"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
+      <c r="K1" s="161"/>
+      <c r="L1" s="161"/>
+      <c r="M1" s="161"/>
+      <c r="N1" s="161"/>
+      <c r="O1" s="162"/>
       <c r="P1" s="30"/>
       <c r="Q1" s="30"/>
       <c r="R1" s="30"/>

</xml_diff>

<commit_message>
Implementing area suppression, introducing bugs to squash
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -643,7 +643,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2230" uniqueCount="1075">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="1073">
   <si>
     <t>Fishing</t>
   </si>
@@ -3021,9 +3021,6 @@
     <t>Finish Trollish</t>
   </si>
   <si>
-    <t>Weapon Abilities</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
@@ -3034,9 +3031,6 @@
   </si>
   <si>
     <t>e</t>
-  </si>
-  <si>
-    <t>Area Suppression</t>
   </si>
   <si>
     <t>Implement</t>
@@ -3917,7 +3911,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3957,12 +3951,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4724,7 +4712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5061,16 +5049,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5088,16 +5082,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5144,12 +5132,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5455,10 +5437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C172"/>
+  <dimension ref="A1:C165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5473,29 +5455,29 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="152" t="s">
         <v>782</v>
       </c>
-      <c r="B2" s="151"/>
-      <c r="C2" s="152"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="154"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="115">
         <v>1</v>
       </c>
-      <c r="B3" s="153" t="s">
+      <c r="B3" s="155" t="s">
         <v>783</v>
       </c>
-      <c r="C3" s="154"/>
+      <c r="C3" s="156"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="146" t="s">
         <v>784</v>
       </c>
-      <c r="C4" s="156"/>
+      <c r="C4" s="147"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="116"/>
@@ -5518,7 +5500,7 @@
     <row r="7" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="116"/>
       <c r="B7" s="122" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C7" s="123" t="s">
         <v>111</v>
@@ -5527,16 +5509,16 @@
     <row r="8" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="116"/>
       <c r="B8" s="122" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C8" s="123" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="9" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="116"/>
       <c r="B9" s="120" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C9" s="121" t="s">
         <v>700</v>
@@ -5546,10 +5528,10 @@
       <c r="A10" s="116">
         <v>3</v>
       </c>
-      <c r="B10" s="157" t="s">
+      <c r="B10" s="148" t="s">
         <v>785</v>
       </c>
-      <c r="C10" s="158"/>
+      <c r="C10" s="149"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="116"/>
@@ -5557,17 +5539,17 @@
         <v>788</v>
       </c>
       <c r="C11" s="119" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="12" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="116">
         <v>4</v>
       </c>
-      <c r="B12" s="146" t="s">
+      <c r="B12" s="150" t="s">
         <v>786</v>
       </c>
-      <c r="C12" s="147"/>
+      <c r="C12" s="151"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="116"/>
@@ -5575,17 +5557,17 @@
         <v>788</v>
       </c>
       <c r="C13" s="119" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="14" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="116">
         <v>5</v>
       </c>
-      <c r="B14" s="146" t="s">
+      <c r="B14" s="150" t="s">
         <v>787</v>
       </c>
-      <c r="C14" s="147"/>
+      <c r="C14" s="151"/>
     </row>
     <row r="15" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="116"/>
@@ -5593,17 +5575,17 @@
         <v>788</v>
       </c>
       <c r="C15" s="119" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="16" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="117">
         <v>6</v>
       </c>
-      <c r="B16" s="148" t="s">
+      <c r="B16" s="157" t="s">
         <v>791</v>
       </c>
-      <c r="C16" s="149"/>
+      <c r="C16" s="158"/>
     </row>
     <row r="17" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="116"/>
@@ -5611,179 +5593,187 @@
         <v>788</v>
       </c>
       <c r="C17" s="119" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="18" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="117">
         <v>7</v>
       </c>
-      <c r="B18" s="148" t="s">
-        <v>915</v>
-      </c>
-      <c r="C18" s="149"/>
+      <c r="B18" s="157" t="s">
+        <v>913</v>
+      </c>
+      <c r="C18" s="158"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="132">
         <v>8</v>
       </c>
-      <c r="B19" s="148" t="s">
-        <v>1002</v>
-      </c>
-      <c r="C19" s="149"/>
+      <c r="B19" s="157" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C19" s="158"/>
     </row>
     <row r="20" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="132">
         <v>9</v>
       </c>
-      <c r="B20" s="148" t="s">
-        <v>916</v>
-      </c>
-      <c r="C20" s="149"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="150" t="s">
-        <v>183</v>
-      </c>
-      <c r="B22" s="151"/>
-      <c r="C22" s="152"/>
-    </row>
+      <c r="B20" s="157" t="s">
+        <v>914</v>
+      </c>
+      <c r="C20" s="158"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="115">
-        <v>1</v>
-      </c>
-      <c r="B23" s="153" t="s">
-        <v>792</v>
-      </c>
+      <c r="A23" s="152" t="s">
+        <v>793</v>
+      </c>
+      <c r="B23" s="153"/>
       <c r="C23" s="154"/>
     </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="116"/>
-      <c r="B24" s="174"/>
-      <c r="C24" s="175"/>
+    <row r="24" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="115">
+        <v>1</v>
+      </c>
+      <c r="B24" s="155" t="s">
+        <v>782</v>
+      </c>
+      <c r="C24" s="156"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="116"/>
-      <c r="B25" s="140" t="s">
-        <v>793</v>
-      </c>
-      <c r="C25" s="141" t="s">
-        <v>797</v>
-      </c>
+      <c r="B25" s="122"/>
+      <c r="C25" s="123"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="116"/>
-      <c r="B26" s="122"/>
-      <c r="C26" s="123"/>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="116"/>
-      <c r="B27" s="125"/>
-      <c r="C27" s="126"/>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="140" t="s">
+        <v>789</v>
+      </c>
+      <c r="C26" s="141" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="116">
+        <v>2</v>
+      </c>
+      <c r="B27" s="146" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="147"/>
+    </row>
+    <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="116"/>
-      <c r="B28" s="125"/>
-      <c r="C28" s="126"/>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="B28" s="118" t="s">
+        <v>788</v>
+      </c>
+      <c r="C28" s="119" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="116"/>
+      <c r="B29" s="120"/>
+      <c r="C29" s="121"/>
+    </row>
     <row r="30" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="150" t="s">
-        <v>794</v>
-      </c>
-      <c r="B30" s="151"/>
-      <c r="C30" s="152"/>
+      <c r="A30" s="116">
+        <v>3</v>
+      </c>
+      <c r="B30" s="146" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C30" s="147"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="115">
-        <v>1</v>
-      </c>
-      <c r="B31" s="153" t="s">
-        <v>782</v>
-      </c>
-      <c r="C31" s="154"/>
+      <c r="A31" s="116"/>
+      <c r="B31" s="142" t="s">
+        <v>788</v>
+      </c>
+      <c r="C31" s="143" t="s">
+        <v>1002</v>
+      </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="116"/>
-      <c r="B32" s="122"/>
-      <c r="C32" s="123"/>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="116"/>
-      <c r="B33" s="140" t="s">
+      <c r="B32" s="144" t="s">
         <v>789</v>
       </c>
-      <c r="C33" s="141" t="s">
-        <v>1001</v>
-      </c>
-    </row>
+      <c r="C32" s="145" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="116">
-        <v>2</v>
-      </c>
-      <c r="B34" s="155" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="156"/>
+      <c r="A34" s="152" t="s">
+        <v>797</v>
+      </c>
+      <c r="B34" s="153"/>
+      <c r="C34" s="154"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="116"/>
-      <c r="B35" s="118" t="s">
+      <c r="A35" s="115">
+        <v>1</v>
+      </c>
+      <c r="B35" s="155" t="s">
+        <v>798</v>
+      </c>
+      <c r="C35" s="156"/>
+    </row>
+    <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="116"/>
+      <c r="B36" s="118" t="s">
         <v>788</v>
       </c>
-      <c r="C35" s="119" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="116"/>
-      <c r="B36" s="120"/>
-      <c r="C36" s="121"/>
-    </row>
-    <row r="37" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="116">
-        <v>3</v>
-      </c>
-      <c r="B37" s="155" t="s">
-        <v>1003</v>
-      </c>
-      <c r="C37" s="156"/>
-    </row>
-    <row r="38" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="119" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="116"/>
+      <c r="B37" s="122" t="s">
+        <v>789</v>
+      </c>
+      <c r="C37" s="123" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="116"/>
-      <c r="B38" s="142" t="s">
-        <v>788</v>
-      </c>
-      <c r="C38" s="143" t="s">
-        <v>1004</v>
+      <c r="B38" s="122" t="s">
+        <v>792</v>
+      </c>
+      <c r="C38" s="123" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="116"/>
-      <c r="B39" s="144" t="s">
-        <v>789</v>
-      </c>
-      <c r="C39" s="145" t="s">
-        <v>1005</v>
+      <c r="B39" s="120" t="s">
+        <v>794</v>
+      </c>
+      <c r="C39" s="121" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="150" t="s">
-        <v>799</v>
-      </c>
-      <c r="B41" s="151"/>
-      <c r="C41" s="152"/>
+      <c r="A41" s="152" t="s">
+        <v>802</v>
+      </c>
+      <c r="B41" s="153"/>
+      <c r="C41" s="154"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="115">
         <v>1</v>
       </c>
-      <c r="B42" s="153" t="s">
-        <v>800</v>
-      </c>
-      <c r="C42" s="154"/>
+      <c r="B42" s="155" t="s">
+        <v>803</v>
+      </c>
+      <c r="C42" s="156"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="116"/>
@@ -5791,502 +5781,508 @@
         <v>788</v>
       </c>
       <c r="C43" s="119" t="s">
-        <v>533</v>
+        <v>804</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="116"/>
-      <c r="B44" s="122" t="s">
+      <c r="A44" s="124"/>
+      <c r="B44" s="120" t="s">
         <v>789</v>
       </c>
-      <c r="C44" s="123" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="116"/>
-      <c r="B45" s="122" t="s">
-        <v>793</v>
-      </c>
-      <c r="C45" s="123" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="121" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="115">
+        <v>1</v>
+      </c>
+      <c r="B45" s="155" t="s">
+        <v>805</v>
+      </c>
+      <c r="C45" s="156"/>
+    </row>
+    <row r="46" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="116"/>
-      <c r="B46" s="120" t="s">
-        <v>795</v>
-      </c>
-      <c r="C46" s="121" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="150" t="s">
-        <v>804</v>
-      </c>
-      <c r="B48" s="151"/>
-      <c r="C48" s="152"/>
-    </row>
-    <row r="49" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="115">
-        <v>1</v>
-      </c>
-      <c r="B49" s="153" t="s">
-        <v>805</v>
-      </c>
-      <c r="C49" s="154"/>
-    </row>
-    <row r="50" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="116"/>
-      <c r="B50" s="118" t="s">
+      <c r="B46" s="118" t="s">
         <v>788</v>
       </c>
-      <c r="C50" s="119" t="s">
+      <c r="C46" s="119" t="s">
         <v>806</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="124"/>
-      <c r="B51" s="120" t="s">
+    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="116"/>
+      <c r="B47" s="122" t="s">
         <v>789</v>
       </c>
-      <c r="C51" s="121" t="s">
-        <v>811</v>
-      </c>
+      <c r="C47" s="123" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="116"/>
+      <c r="B48" s="122" t="s">
+        <v>792</v>
+      </c>
+      <c r="C48" s="123" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="116"/>
+      <c r="B49" s="120"/>
+      <c r="C49" s="121"/>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="152" t="s">
+        <v>188</v>
+      </c>
+      <c r="B51" s="153"/>
+      <c r="C51" s="154"/>
     </row>
     <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="115">
         <v>1</v>
       </c>
-      <c r="B52" s="153" t="s">
-        <v>807</v>
-      </c>
-      <c r="C52" s="154"/>
-    </row>
-    <row r="53" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="116"/>
-      <c r="B53" s="118" t="s">
-        <v>788</v>
-      </c>
-      <c r="C53" s="119" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="116"/>
-      <c r="B54" s="122" t="s">
-        <v>789</v>
-      </c>
-      <c r="C54" s="123" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="116"/>
-      <c r="B55" s="122" t="s">
-        <v>793</v>
-      </c>
-      <c r="C55" s="123" t="s">
+      <c r="B52" s="155" t="s">
         <v>810</v>
       </c>
+      <c r="C52" s="156"/>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="152" t="s">
+        <v>790</v>
+      </c>
+      <c r="B54" s="153"/>
+      <c r="C54" s="154"/>
+    </row>
+    <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="115">
+        <v>1</v>
+      </c>
+      <c r="B55" s="148" t="s">
+        <v>783</v>
+      </c>
+      <c r="C55" s="149"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="116"/>
-      <c r="B56" s="120"/>
-      <c r="C56" s="121"/>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="150" t="s">
-        <v>188</v>
-      </c>
-      <c r="B58" s="151"/>
-      <c r="C58" s="152"/>
-    </row>
-    <row r="59" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="115">
-        <v>1</v>
-      </c>
-      <c r="B59" s="153" t="s">
-        <v>812</v>
-      </c>
-      <c r="C59" s="154"/>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="150" t="s">
-        <v>790</v>
-      </c>
-      <c r="B61" s="151"/>
-      <c r="C61" s="152"/>
-    </row>
+      <c r="A56" s="116">
+        <v>2</v>
+      </c>
+      <c r="B56" s="159" t="s">
+        <v>784</v>
+      </c>
+      <c r="C56" s="160"/>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="116">
+        <v>3</v>
+      </c>
+      <c r="B57" s="150" t="s">
+        <v>785</v>
+      </c>
+      <c r="C57" s="151"/>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="116">
+        <v>4</v>
+      </c>
+      <c r="B58" s="150" t="s">
+        <v>786</v>
+      </c>
+      <c r="C58" s="151"/>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="116">
+        <v>5</v>
+      </c>
+      <c r="B59" s="150" t="s">
+        <v>787</v>
+      </c>
+      <c r="C59" s="151"/>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="117">
+        <v>6</v>
+      </c>
+      <c r="B60" s="157" t="s">
+        <v>791</v>
+      </c>
+      <c r="C60" s="158"/>
+    </row>
+    <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="115">
-        <v>1</v>
-      </c>
-      <c r="B62" s="157" t="s">
+      <c r="A62" s="152" t="s">
+        <v>811</v>
+      </c>
+      <c r="B62" s="153"/>
+      <c r="C62" s="154"/>
+    </row>
+    <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="115">
+        <v>1</v>
+      </c>
+      <c r="B63" s="148" t="s">
         <v>783</v>
       </c>
-      <c r="C62" s="158"/>
-    </row>
-    <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="116">
-        <v>2</v>
-      </c>
-      <c r="B63" s="159" t="s">
-        <v>784</v>
-      </c>
-      <c r="C63" s="160"/>
+      <c r="C63" s="149"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="116">
-        <v>3</v>
-      </c>
-      <c r="B64" s="146" t="s">
-        <v>785</v>
-      </c>
-      <c r="C64" s="147"/>
+        <v>2</v>
+      </c>
+      <c r="B64" s="159" t="s">
+        <v>784</v>
+      </c>
+      <c r="C64" s="160"/>
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="116">
-        <v>4</v>
-      </c>
-      <c r="B65" s="146" t="s">
-        <v>786</v>
-      </c>
-      <c r="C65" s="147"/>
+        <v>3</v>
+      </c>
+      <c r="B65" s="150" t="s">
+        <v>785</v>
+      </c>
+      <c r="C65" s="151"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="116">
+        <v>4</v>
+      </c>
+      <c r="B66" s="150" t="s">
+        <v>786</v>
+      </c>
+      <c r="C66" s="151"/>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="116">
         <v>5</v>
       </c>
-      <c r="B66" s="146" t="s">
+      <c r="B67" s="150" t="s">
         <v>787</v>
       </c>
-      <c r="C66" s="147"/>
-    </row>
-    <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="117">
+      <c r="C67" s="151"/>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="117">
         <v>6</v>
       </c>
-      <c r="B67" s="148" t="s">
+      <c r="B68" s="157" t="s">
         <v>791</v>
       </c>
-      <c r="C67" s="149"/>
-    </row>
-    <row r="68" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="150" t="s">
-        <v>813</v>
-      </c>
-      <c r="B69" s="151"/>
-      <c r="C69" s="152"/>
-    </row>
+      <c r="C68" s="158"/>
+    </row>
+    <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="115">
-        <v>1</v>
-      </c>
-      <c r="B70" s="157" t="s">
+      <c r="A70" s="152" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B70" s="153"/>
+      <c r="C70" s="154"/>
+    </row>
+    <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="115">
+        <v>1</v>
+      </c>
+      <c r="B71" s="148"/>
+      <c r="C71" s="149"/>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="116"/>
+      <c r="B72" s="159"/>
+      <c r="C72" s="160"/>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="116"/>
+      <c r="B73" s="150"/>
+      <c r="C73" s="151"/>
+    </row>
+    <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="116"/>
+      <c r="B74" s="150"/>
+      <c r="C74" s="151"/>
+    </row>
+    <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="116"/>
+      <c r="B75" s="150"/>
+      <c r="C75" s="151"/>
+    </row>
+    <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="117"/>
+      <c r="B76" s="157"/>
+      <c r="C76" s="158"/>
+    </row>
+    <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="152" t="s">
+        <v>812</v>
+      </c>
+      <c r="B78" s="153"/>
+      <c r="C78" s="154"/>
+    </row>
+    <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="115">
+        <v>1</v>
+      </c>
+      <c r="B79" s="148" t="s">
         <v>783</v>
       </c>
-      <c r="C70" s="158"/>
-    </row>
-    <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="116">
+      <c r="C79" s="149"/>
+    </row>
+    <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="116">
         <v>2</v>
       </c>
-      <c r="B71" s="159" t="s">
+      <c r="B80" s="159" t="s">
         <v>784</v>
       </c>
-      <c r="C71" s="160"/>
-    </row>
-    <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="116">
+      <c r="C80" s="160"/>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="116">
         <v>3</v>
       </c>
-      <c r="B72" s="146" t="s">
+      <c r="B81" s="150" t="s">
         <v>785</v>
       </c>
-      <c r="C72" s="147"/>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="116">
+      <c r="C81" s="151"/>
+    </row>
+    <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="116">
         <v>4</v>
       </c>
-      <c r="B73" s="146" t="s">
+      <c r="B82" s="150" t="s">
         <v>786</v>
       </c>
-      <c r="C73" s="147"/>
-    </row>
-    <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="116">
+      <c r="C82" s="151"/>
+    </row>
+    <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="116">
         <v>5</v>
       </c>
-      <c r="B74" s="146" t="s">
+      <c r="B83" s="150" t="s">
         <v>787</v>
       </c>
-      <c r="C74" s="147"/>
-    </row>
-    <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="117">
+      <c r="C83" s="151"/>
+    </row>
+    <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="117">
         <v>6</v>
       </c>
-      <c r="B75" s="148" t="s">
+      <c r="B84" s="157" t="s">
         <v>791</v>
       </c>
-      <c r="C75" s="149"/>
-    </row>
-    <row r="76" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="150" t="s">
-        <v>1003</v>
-      </c>
-      <c r="B77" s="151"/>
-      <c r="C77" s="152"/>
-    </row>
-    <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="115">
-        <v>1</v>
-      </c>
-      <c r="B78" s="157"/>
-      <c r="C78" s="158"/>
-    </row>
-    <row r="79" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="116"/>
-      <c r="B79" s="159"/>
-      <c r="C79" s="160"/>
-    </row>
-    <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="116"/>
-      <c r="B80" s="146"/>
-      <c r="C80" s="147"/>
-    </row>
-    <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="116"/>
-      <c r="B81" s="146"/>
-      <c r="C81" s="147"/>
-    </row>
-    <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="116"/>
-      <c r="B82" s="146"/>
-      <c r="C82" s="147"/>
-    </row>
-    <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="117"/>
-      <c r="B83" s="148"/>
-      <c r="C83" s="149"/>
-    </row>
-    <row r="84" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="150" t="s">
-        <v>814</v>
-      </c>
-      <c r="B85" s="151"/>
-      <c r="C85" s="152"/>
-    </row>
+      <c r="C84" s="158"/>
+    </row>
+    <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="115">
-        <v>1</v>
-      </c>
-      <c r="B86" s="157" t="s">
-        <v>783</v>
-      </c>
-      <c r="C86" s="158"/>
-    </row>
-    <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="116">
-        <v>2</v>
-      </c>
-      <c r="B87" s="159" t="s">
-        <v>784</v>
-      </c>
-      <c r="C87" s="160"/>
-    </row>
-    <row r="88" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="116">
-        <v>3</v>
-      </c>
-      <c r="B88" s="146" t="s">
-        <v>785</v>
-      </c>
-      <c r="C88" s="147"/>
+      <c r="A86" s="152" t="s">
+        <v>862</v>
+      </c>
+      <c r="B86" s="153"/>
+      <c r="C86" s="154"/>
+    </row>
+    <row r="87" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="115">
+        <v>1</v>
+      </c>
+      <c r="B87" s="155" t="s">
+        <v>101</v>
+      </c>
+      <c r="C87" s="156"/>
+    </row>
+    <row r="88" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="124"/>
+      <c r="B88" s="118" t="s">
+        <v>788</v>
+      </c>
+      <c r="C88" s="119" t="s">
+        <v>839</v>
+      </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="116">
-        <v>4</v>
-      </c>
-      <c r="B89" s="146" t="s">
-        <v>786</v>
-      </c>
-      <c r="C89" s="147"/>
+      <c r="A89" s="124"/>
+      <c r="B89" s="127" t="s">
+        <v>789</v>
+      </c>
+      <c r="C89" s="128" t="s">
+        <v>840</v>
+      </c>
     </row>
     <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="116">
-        <v>5</v>
-      </c>
-      <c r="B90" s="146" t="s">
-        <v>787</v>
-      </c>
-      <c r="C90" s="147"/>
+      <c r="A90" s="124"/>
+      <c r="B90" s="127" t="s">
+        <v>792</v>
+      </c>
+      <c r="C90" s="128" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="117">
-        <v>6</v>
-      </c>
-      <c r="B91" s="148" t="s">
-        <v>791</v>
-      </c>
-      <c r="C91" s="149"/>
-    </row>
-    <row r="92" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="93" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="150" t="s">
-        <v>864</v>
-      </c>
-      <c r="B93" s="151"/>
-      <c r="C93" s="152"/>
-    </row>
-    <row r="94" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="115">
-        <v>1</v>
-      </c>
-      <c r="B94" s="153" t="s">
-        <v>101</v>
-      </c>
-      <c r="C94" s="154"/>
-    </row>
-    <row r="95" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="124"/>
+      <c r="B91" s="127" t="s">
+        <v>794</v>
+      </c>
+      <c r="C91" s="128" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="124"/>
+      <c r="B92" s="127" t="s">
+        <v>795</v>
+      </c>
+      <c r="C92" s="128" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="124"/>
+      <c r="B93" s="127" t="s">
+        <v>823</v>
+      </c>
+      <c r="C93" s="128" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="124"/>
+      <c r="B94" s="127" t="s">
+        <v>825</v>
+      </c>
+      <c r="C94" s="128" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="124"/>
-      <c r="B95" s="118" t="s">
-        <v>788</v>
-      </c>
-      <c r="C95" s="119" t="s">
-        <v>841</v>
+      <c r="B95" s="127" t="s">
+        <v>827</v>
+      </c>
+      <c r="C95" s="128" t="s">
+        <v>846</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="124"/>
       <c r="B96" s="127" t="s">
-        <v>789</v>
+        <v>828</v>
       </c>
       <c r="C96" s="128" t="s">
-        <v>842</v>
+        <v>847</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="124"/>
-      <c r="B97" s="127" t="s">
-        <v>793</v>
-      </c>
-      <c r="C97" s="128" t="s">
-        <v>843</v>
+      <c r="A97" s="116"/>
+      <c r="B97" s="122" t="s">
+        <v>829</v>
+      </c>
+      <c r="C97" s="123" t="s">
+        <v>848</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="124"/>
-      <c r="B98" s="127" t="s">
-        <v>795</v>
-      </c>
-      <c r="C98" s="128" t="s">
-        <v>844</v>
+      <c r="A98" s="116"/>
+      <c r="B98" s="122" t="s">
+        <v>830</v>
+      </c>
+      <c r="C98" s="123" t="s">
+        <v>849</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="124"/>
-      <c r="B99" s="127" t="s">
-        <v>796</v>
-      </c>
-      <c r="C99" s="128" t="s">
-        <v>845</v>
+      <c r="A99" s="116"/>
+      <c r="B99" s="122" t="s">
+        <v>831</v>
+      </c>
+      <c r="C99" s="123" t="s">
+        <v>850</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="124"/>
-      <c r="B100" s="127" t="s">
-        <v>825</v>
-      </c>
-      <c r="C100" s="128" t="s">
-        <v>846</v>
+      <c r="A100" s="116"/>
+      <c r="B100" s="122" t="s">
+        <v>832</v>
+      </c>
+      <c r="C100" s="123" t="s">
+        <v>851</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="124"/>
-      <c r="B101" s="127" t="s">
-        <v>827</v>
-      </c>
-      <c r="C101" s="128" t="s">
-        <v>847</v>
+      <c r="A101" s="116"/>
+      <c r="B101" s="122" t="s">
+        <v>833</v>
+      </c>
+      <c r="C101" s="123" t="s">
+        <v>852</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="124"/>
-      <c r="B102" s="127" t="s">
-        <v>829</v>
-      </c>
-      <c r="C102" s="128" t="s">
-        <v>848</v>
+      <c r="A102" s="116"/>
+      <c r="B102" s="122" t="s">
+        <v>834</v>
+      </c>
+      <c r="C102" s="123" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="124"/>
-      <c r="B103" s="127" t="s">
-        <v>830</v>
-      </c>
-      <c r="C103" s="128" t="s">
-        <v>849</v>
+      <c r="A103" s="116"/>
+      <c r="B103" s="122" t="s">
+        <v>835</v>
+      </c>
+      <c r="C103" s="123" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="116"/>
       <c r="B104" s="122" t="s">
-        <v>831</v>
+        <v>836</v>
       </c>
       <c r="C104" s="123" t="s">
-        <v>850</v>
+        <v>854</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="116"/>
       <c r="B105" s="122" t="s">
-        <v>832</v>
-      </c>
-      <c r="C105" s="123" t="s">
-        <v>851</v>
-      </c>
+        <v>837</v>
+      </c>
+      <c r="C105" s="123"/>
     </row>
     <row r="106" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="116"/>
-      <c r="B106" s="122" t="s">
-        <v>833</v>
-      </c>
-      <c r="C106" s="123" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="116"/>
-      <c r="B107" s="122" t="s">
-        <v>834</v>
-      </c>
-      <c r="C107" s="123" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="120" t="s">
+        <v>838</v>
+      </c>
+      <c r="C106" s="121"/>
+    </row>
+    <row r="107" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="116">
+        <v>2</v>
+      </c>
+      <c r="B107" s="146" t="s">
+        <v>813</v>
+      </c>
+      <c r="C107" s="147"/>
+    </row>
+    <row r="108" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="116"/>
-      <c r="B108" s="122" t="s">
-        <v>835</v>
-      </c>
-      <c r="C108" s="123" t="s">
-        <v>854</v>
+      <c r="B108" s="118" t="s">
+        <v>788</v>
+      </c>
+      <c r="C108" s="119" t="s">
+        <v>826</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="116"/>
       <c r="B109" s="122" t="s">
-        <v>836</v>
+        <v>789</v>
       </c>
       <c r="C109" s="123" t="s">
         <v>855</v>
@@ -6295,132 +6291,132 @@
     <row r="110" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="116"/>
       <c r="B110" s="122" t="s">
-        <v>837</v>
+        <v>792</v>
       </c>
       <c r="C110" s="123" t="s">
-        <v>35</v>
+        <v>856</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="116"/>
       <c r="B111" s="122" t="s">
-        <v>838</v>
+        <v>794</v>
       </c>
       <c r="C111" s="123" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="116"/>
       <c r="B112" s="122" t="s">
-        <v>839</v>
-      </c>
-      <c r="C112" s="123"/>
+        <v>795</v>
+      </c>
+      <c r="C112" s="123" t="s">
+        <v>858</v>
+      </c>
     </row>
     <row r="113" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="116"/>
-      <c r="B113" s="120" t="s">
-        <v>840</v>
-      </c>
-      <c r="C113" s="121"/>
-    </row>
-    <row r="114" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="116">
-        <v>2</v>
-      </c>
-      <c r="B114" s="155" t="s">
-        <v>815</v>
-      </c>
-      <c r="C114" s="156"/>
-    </row>
-    <row r="115" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B113" s="125" t="s">
+        <v>823</v>
+      </c>
+      <c r="C113" s="126" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="116"/>
+      <c r="B114" s="125" t="s">
+        <v>825</v>
+      </c>
+      <c r="C114" s="126" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="116"/>
-      <c r="B115" s="118" t="s">
+      <c r="B115" s="120" t="s">
+        <v>827</v>
+      </c>
+      <c r="C115" s="121" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="116">
+        <v>3</v>
+      </c>
+      <c r="B116" s="148" t="s">
+        <v>814</v>
+      </c>
+      <c r="C116" s="149"/>
+    </row>
+    <row r="117" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="116"/>
+      <c r="B117" s="118" t="s">
         <v>788</v>
       </c>
-      <c r="C115" s="119" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="116"/>
-      <c r="B116" s="122" t="s">
-        <v>789</v>
-      </c>
-      <c r="C116" s="123" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="116"/>
-      <c r="B117" s="122" t="s">
-        <v>793</v>
-      </c>
-      <c r="C117" s="123" t="s">
-        <v>858</v>
+      <c r="C117" s="119" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="116"/>
       <c r="B118" s="122" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
       <c r="C118" s="123" t="s">
-        <v>859</v>
+        <v>821</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="116"/>
       <c r="B119" s="122" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C119" s="123" t="s">
-        <v>860</v>
+        <v>89</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="116"/>
       <c r="B120" s="125" t="s">
-        <v>825</v>
+        <v>794</v>
       </c>
       <c r="C120" s="126" t="s">
-        <v>861</v>
+        <v>822</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="116"/>
       <c r="B121" s="125" t="s">
-        <v>827</v>
+        <v>795</v>
       </c>
       <c r="C121" s="126" t="s">
-        <v>862</v>
+        <v>824</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="116"/>
-      <c r="B122" s="120" t="s">
-        <v>829</v>
-      </c>
-      <c r="C122" s="121" t="s">
-        <v>863</v>
-      </c>
+      <c r="B122" s="120"/>
+      <c r="C122" s="121"/>
     </row>
     <row r="123" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="116">
-        <v>3</v>
-      </c>
-      <c r="B123" s="157" t="s">
-        <v>816</v>
-      </c>
-      <c r="C123" s="158"/>
+      <c r="A123" s="115">
+        <v>4</v>
+      </c>
+      <c r="B123" s="150" t="s">
+        <v>815</v>
+      </c>
+      <c r="C123" s="151"/>
     </row>
     <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="116"/>
+      <c r="A124" s="124"/>
       <c r="B124" s="118" t="s">
         <v>788</v>
       </c>
       <c r="C124" s="119" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6429,49 +6425,43 @@
         <v>789</v>
       </c>
       <c r="C125" s="123" t="s">
-        <v>823</v>
+        <v>817</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="116"/>
       <c r="B126" s="122" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C126" s="123" t="s">
-        <v>89</v>
+        <v>818</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="116"/>
-      <c r="B127" s="125" t="s">
-        <v>795</v>
-      </c>
-      <c r="C127" s="126" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="116"/>
-      <c r="B128" s="125" t="s">
-        <v>796</v>
-      </c>
-      <c r="C128" s="126" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="116"/>
-      <c r="B129" s="120"/>
-      <c r="C129" s="121"/>
+      <c r="B127" s="120" t="s">
+        <v>794</v>
+      </c>
+      <c r="C127" s="121" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="129" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="152" t="s">
+        <v>863</v>
+      </c>
+      <c r="B129" s="153"/>
+      <c r="C129" s="154"/>
     </row>
     <row r="130" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="115">
-        <v>4</v>
-      </c>
-      <c r="B130" s="146" t="s">
-        <v>817</v>
-      </c>
-      <c r="C130" s="147"/>
+        <v>1</v>
+      </c>
+      <c r="B130" s="155" t="s">
+        <v>864</v>
+      </c>
+      <c r="C130" s="156"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="124"/>
@@ -6479,380 +6469,281 @@
         <v>788</v>
       </c>
       <c r="C131" s="119" t="s">
-        <v>818</v>
+        <v>101</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="116"/>
-      <c r="B132" s="122" t="s">
+      <c r="A132" s="124"/>
+      <c r="B132" s="127" t="s">
         <v>789</v>
       </c>
-      <c r="C132" s="123" t="s">
-        <v>819</v>
+      <c r="C132" s="128" t="s">
+        <v>813</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="116"/>
-      <c r="B133" s="122" t="s">
-        <v>793</v>
-      </c>
-      <c r="C133" s="123" t="s">
-        <v>820</v>
+      <c r="A133" s="124"/>
+      <c r="B133" s="127" t="s">
+        <v>792</v>
+      </c>
+      <c r="C133" s="128" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="116"/>
-      <c r="B134" s="120" t="s">
+      <c r="A134" s="124"/>
+      <c r="B134" s="127" t="s">
+        <v>794</v>
+      </c>
+      <c r="C134" s="128" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="124"/>
+      <c r="B135" s="127" t="s">
         <v>795</v>
       </c>
-      <c r="C134" s="121" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="136" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="150" t="s">
-        <v>865</v>
-      </c>
-      <c r="B136" s="151"/>
-      <c r="C136" s="152"/>
-    </row>
-    <row r="137" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="115">
-        <v>1</v>
-      </c>
-      <c r="B137" s="153" t="s">
-        <v>866</v>
-      </c>
-      <c r="C137" s="154"/>
-    </row>
-    <row r="138" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C135" s="128"/>
+    </row>
+    <row r="136" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="124"/>
+      <c r="B136" s="127" t="s">
+        <v>823</v>
+      </c>
+      <c r="C136" s="128"/>
+    </row>
+    <row r="137" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="124"/>
+      <c r="B137" s="127" t="s">
+        <v>825</v>
+      </c>
+      <c r="C137" s="128"/>
+    </row>
+    <row r="138" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="124"/>
-      <c r="B138" s="118" t="s">
-        <v>788</v>
-      </c>
-      <c r="C138" s="119" t="s">
-        <v>101</v>
-      </c>
+      <c r="B138" s="127" t="s">
+        <v>827</v>
+      </c>
+      <c r="C138" s="128"/>
     </row>
     <row r="139" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="124"/>
       <c r="B139" s="127" t="s">
-        <v>789</v>
-      </c>
-      <c r="C139" s="128" t="s">
-        <v>815</v>
-      </c>
+        <v>828</v>
+      </c>
+      <c r="C139" s="128"/>
     </row>
     <row r="140" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="124"/>
-      <c r="B140" s="127" t="s">
-        <v>793</v>
-      </c>
-      <c r="C140" s="128" t="s">
-        <v>816</v>
-      </c>
+      <c r="A140" s="116"/>
+      <c r="B140" s="122" t="s">
+        <v>829</v>
+      </c>
+      <c r="C140" s="123"/>
     </row>
     <row r="141" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="124"/>
-      <c r="B141" s="127" t="s">
-        <v>795</v>
-      </c>
-      <c r="C141" s="128" t="s">
-        <v>817</v>
-      </c>
+      <c r="A141" s="116"/>
+      <c r="B141" s="122" t="s">
+        <v>830</v>
+      </c>
+      <c r="C141" s="123"/>
     </row>
     <row r="142" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="124"/>
-      <c r="B142" s="127" t="s">
-        <v>796</v>
-      </c>
-      <c r="C142" s="128"/>
+      <c r="A142" s="116"/>
+      <c r="B142" s="122" t="s">
+        <v>831</v>
+      </c>
+      <c r="C142" s="123"/>
     </row>
     <row r="143" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="124"/>
-      <c r="B143" s="127" t="s">
-        <v>825</v>
-      </c>
-      <c r="C143" s="128"/>
+      <c r="A143" s="116"/>
+      <c r="B143" s="122" t="s">
+        <v>832</v>
+      </c>
+      <c r="C143" s="123"/>
     </row>
     <row r="144" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="124"/>
-      <c r="B144" s="127" t="s">
-        <v>827</v>
-      </c>
-      <c r="C144" s="128"/>
+      <c r="A144" s="116"/>
+      <c r="B144" s="122" t="s">
+        <v>833</v>
+      </c>
+      <c r="C144" s="123"/>
     </row>
     <row r="145" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="124"/>
-      <c r="B145" s="127" t="s">
-        <v>829</v>
-      </c>
-      <c r="C145" s="128"/>
+      <c r="A145" s="116"/>
+      <c r="B145" s="122" t="s">
+        <v>834</v>
+      </c>
+      <c r="C145" s="123"/>
     </row>
     <row r="146" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="124"/>
-      <c r="B146" s="127" t="s">
-        <v>830</v>
-      </c>
-      <c r="C146" s="128"/>
+      <c r="A146" s="116"/>
+      <c r="B146" s="122" t="s">
+        <v>835</v>
+      </c>
+      <c r="C146" s="123"/>
     </row>
     <row r="147" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="116"/>
       <c r="B147" s="122" t="s">
-        <v>831</v>
+        <v>836</v>
       </c>
       <c r="C147" s="123"/>
     </row>
     <row r="148" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="116"/>
       <c r="B148" s="122" t="s">
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="C148" s="123"/>
     </row>
     <row r="149" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="116"/>
-      <c r="B149" s="122" t="s">
-        <v>833</v>
-      </c>
-      <c r="C149" s="123"/>
-    </row>
-    <row r="150" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="116"/>
-      <c r="B150" s="122" t="s">
-        <v>834</v>
-      </c>
-      <c r="C150" s="123"/>
-    </row>
-    <row r="151" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B149" s="120" t="s">
+        <v>838</v>
+      </c>
+      <c r="C149" s="121"/>
+    </row>
+    <row r="150" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="116">
+        <v>2</v>
+      </c>
+      <c r="B150" s="146" t="s">
+        <v>865</v>
+      </c>
+      <c r="C150" s="147"/>
+    </row>
+    <row r="151" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="116"/>
-      <c r="B151" s="122" t="s">
-        <v>835</v>
-      </c>
-      <c r="C151" s="123"/>
+      <c r="B151" s="118" t="s">
+        <v>788</v>
+      </c>
+      <c r="C151" s="119" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="152" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="116"/>
       <c r="B152" s="122" t="s">
-        <v>836</v>
-      </c>
-      <c r="C152" s="123"/>
+        <v>789</v>
+      </c>
+      <c r="C152" s="123" t="s">
+        <v>867</v>
+      </c>
     </row>
     <row r="153" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="116"/>
       <c r="B153" s="122" t="s">
-        <v>837</v>
-      </c>
-      <c r="C153" s="123"/>
+        <v>792</v>
+      </c>
+      <c r="C153" s="123" t="s">
+        <v>868</v>
+      </c>
     </row>
     <row r="154" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="116"/>
       <c r="B154" s="122" t="s">
-        <v>838</v>
-      </c>
-      <c r="C154" s="123"/>
+        <v>794</v>
+      </c>
+      <c r="C154" s="123" t="s">
+        <v>869</v>
+      </c>
     </row>
     <row r="155" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="116"/>
       <c r="B155" s="122" t="s">
-        <v>839</v>
+        <v>795</v>
       </c>
       <c r="C155" s="123"/>
     </row>
     <row r="156" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="116"/>
-      <c r="B156" s="120" t="s">
-        <v>840</v>
-      </c>
-      <c r="C156" s="121"/>
-    </row>
-    <row r="157" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="116">
-        <v>2</v>
-      </c>
-      <c r="B157" s="155" t="s">
-        <v>867</v>
-      </c>
-      <c r="C157" s="156"/>
-    </row>
-    <row r="158" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B156" s="125" t="s">
+        <v>823</v>
+      </c>
+      <c r="C156" s="126"/>
+    </row>
+    <row r="157" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="116"/>
+      <c r="B157" s="125" t="s">
+        <v>825</v>
+      </c>
+      <c r="C157" s="126"/>
+    </row>
+    <row r="158" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="116"/>
-      <c r="B158" s="118" t="s">
+      <c r="B158" s="120" t="s">
+        <v>827</v>
+      </c>
+      <c r="C158" s="121"/>
+    </row>
+    <row r="159" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="116">
+        <v>3</v>
+      </c>
+      <c r="B159" s="148" t="s">
+        <v>866</v>
+      </c>
+      <c r="C159" s="149"/>
+    </row>
+    <row r="160" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="116"/>
+      <c r="B160" s="118" t="s">
         <v>788</v>
       </c>
-      <c r="C158" s="119" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="116"/>
-      <c r="B159" s="122" t="s">
-        <v>789</v>
-      </c>
-      <c r="C159" s="123" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="116"/>
-      <c r="B160" s="122" t="s">
-        <v>793</v>
-      </c>
-      <c r="C160" s="123" t="s">
-        <v>870</v>
+      <c r="C160" s="119" t="s">
+        <v>871</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="116"/>
       <c r="B161" s="122" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
       <c r="C161" s="123" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="116"/>
       <c r="B162" s="122" t="s">
-        <v>796</v>
-      </c>
-      <c r="C162" s="123"/>
+        <v>792</v>
+      </c>
+      <c r="C162" s="123" t="s">
+        <v>872</v>
+      </c>
     </row>
     <row r="163" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="116"/>
       <c r="B163" s="125" t="s">
-        <v>825</v>
-      </c>
-      <c r="C163" s="126"/>
+        <v>794</v>
+      </c>
+      <c r="C163" s="126" t="s">
+        <v>873</v>
+      </c>
     </row>
     <row r="164" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="116"/>
       <c r="B164" s="125" t="s">
-        <v>827</v>
+        <v>795</v>
       </c>
       <c r="C164" s="126"/>
     </row>
     <row r="165" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="116"/>
       <c r="B165" s="120" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
       <c r="C165" s="121"/>
     </row>
-    <row r="166" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="116">
-        <v>3</v>
-      </c>
-      <c r="B166" s="157" t="s">
-        <v>868</v>
-      </c>
-      <c r="C166" s="158"/>
-    </row>
-    <row r="167" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="116"/>
-      <c r="B167" s="118" t="s">
-        <v>788</v>
-      </c>
-      <c r="C167" s="119" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="116"/>
-      <c r="B168" s="122" t="s">
-        <v>789</v>
-      </c>
-      <c r="C168" s="123" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="116"/>
-      <c r="B169" s="122" t="s">
-        <v>793</v>
-      </c>
-      <c r="C169" s="123" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="116"/>
-      <c r="B170" s="125" t="s">
-        <v>795</v>
-      </c>
-      <c r="C170" s="126" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="116"/>
-      <c r="B171" s="125" t="s">
-        <v>796</v>
-      </c>
-      <c r="C171" s="126"/>
-    </row>
-    <row r="172" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="116"/>
-      <c r="B172" s="120" t="s">
-        <v>825</v>
-      </c>
-      <c r="C172" s="121"/>
-    </row>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="A136:C136"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B114:C114"/>
+  <mergeCells count="58">
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="B75:C75"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="A93:C93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="A77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B76:C76"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B12:C12"/>
@@ -6860,7 +6751,51 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="A129:C129"/>
+    <mergeCell ref="B130:C130"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -13160,7 +13095,7 @@
         <v>658</v>
       </c>
       <c r="X54" s="44" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
@@ -13230,7 +13165,7 @@
         <v>658</v>
       </c>
       <c r="X55" s="44" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
@@ -13300,7 +13235,7 @@
         <v>658</v>
       </c>
       <c r="X56" s="44" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
@@ -13370,7 +13305,7 @@
         <v>658</v>
       </c>
       <c r="X57" s="44" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
@@ -13440,7 +13375,7 @@
         <v>658</v>
       </c>
       <c r="X58" s="44" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
@@ -22523,10 +22458,10 @@
     </row>
     <row r="16" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="83" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="C16" s="43"/>
       <c r="D16" s="43"/>
@@ -22537,7 +22472,7 @@
       <c r="I16" s="43"/>
       <c r="J16" s="44"/>
       <c r="K16" s="89" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="L16" s="87"/>
     </row>
@@ -22805,7 +22740,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="83" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="B30" s="48"/>
       <c r="C30" s="43"/>
@@ -22817,7 +22752,7 @@
       <c r="I30" s="43"/>
       <c r="J30" s="44"/>
       <c r="K30" s="89" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="L30" s="87">
         <v>3</v>
@@ -22905,7 +22840,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="83" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="43"/>
@@ -22917,13 +22852,13 @@
       <c r="I35" s="43"/>
       <c r="J35" s="44"/>
       <c r="K35" s="89" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="L35" s="87"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="83" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="43"/>
@@ -22935,7 +22870,7 @@
       <c r="I36" s="43"/>
       <c r="J36" s="44"/>
       <c r="K36" s="89" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="L36" s="87"/>
     </row>
@@ -22979,10 +22914,10 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="83" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="B39" s="48" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="C39" s="43" t="s">
         <v>745</v>
@@ -22995,7 +22930,7 @@
       <c r="I39" s="43"/>
       <c r="J39" s="44"/>
       <c r="K39" s="89" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="L39" s="87"/>
     </row>
@@ -23095,7 +23030,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="83" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="B45" s="48"/>
       <c r="C45" s="43"/>
@@ -23113,7 +23048,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="83" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="B46" s="48"/>
       <c r="C46" s="43"/>
@@ -23125,7 +23060,7 @@
       <c r="I46" s="43"/>
       <c r="J46" s="44"/>
       <c r="K46" s="89" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="L46" s="87">
         <v>3</v>
@@ -23133,10 +23068,10 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="83" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="B47" s="48" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="C47" s="43" t="s">
         <v>745</v>
@@ -23149,7 +23084,7 @@
       <c r="I47" s="43"/>
       <c r="J47" s="44"/>
       <c r="K47" s="89" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="L47" s="87"/>
     </row>
@@ -23813,7 +23748,7 @@
       <c r="I81" s="43"/>
       <c r="J81" s="44"/>
       <c r="K81" s="89" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="L81" s="87"/>
     </row>
@@ -24171,7 +24106,7 @@
         <v>372</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="F3" s="129"/>
       <c r="G3" s="31"/>
@@ -24198,7 +24133,7 @@
         <v>382</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="F4" s="129"/>
       <c r="G4" s="31"/>
@@ -24289,7 +24224,7 @@
         <v>492</v>
       </c>
       <c r="E8" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="F8" s="133" t="s">
         <v>745</v>
@@ -24697,7 +24632,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="129" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="B28" s="129" t="s">
         <v>582</v>
@@ -24706,12 +24641,12 @@
         <v>488</v>
       </c>
       <c r="M28" s="129" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="129" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="B29" s="129" t="s">
         <v>582</v>
@@ -24721,7 +24656,7 @@
       </c>
       <c r="L29" s="32"/>
       <c r="M29" s="129" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="N29"/>
     </row>
@@ -24736,22 +24671,22 @@
         <v>488</v>
       </c>
       <c r="M30" s="129" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="129" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="129" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="129" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B33" s="129" t="s">
         <v>582</v>
@@ -24760,15 +24695,15 @@
         <v>488</v>
       </c>
       <c r="E33" s="129" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="M33" s="129" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="129" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="B34" s="129" t="s">
         <v>374</v>
@@ -24777,10 +24712,10 @@
         <v>488</v>
       </c>
       <c r="E34" s="129" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="M34" s="129" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="N34" s="34">
         <v>5</v>
@@ -24788,7 +24723,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="129" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="B35" s="129" t="s">
         <v>374</v>
@@ -24797,15 +24732,15 @@
         <v>488</v>
       </c>
       <c r="E35" s="129" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="M35" s="129" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="129" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="B36" s="129" t="s">
         <v>374</v>
@@ -24814,15 +24749,15 @@
         <v>488</v>
       </c>
       <c r="E36" s="129" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="M36" s="129" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="129" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="B37" s="129" t="s">
         <v>374</v>
@@ -24831,15 +24766,15 @@
         <v>488</v>
       </c>
       <c r="E37" s="129" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="M37" s="129" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="129" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="B38" s="129" t="s">
         <v>374</v>
@@ -24848,10 +24783,10 @@
         <v>488</v>
       </c>
       <c r="E38" s="129" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="M38" s="129" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="N38" s="34">
         <v>5</v>
@@ -24868,12 +24803,12 @@
         <v>488</v>
       </c>
       <c r="M39" s="130" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="130" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="B40" s="130" t="s">
         <v>582</v>
@@ -24882,41 +24817,41 @@
         <v>488</v>
       </c>
       <c r="M40" s="130" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="130" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="B41" s="130" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="D41" s="130" t="s">
         <v>488</v>
       </c>
       <c r="E41" s="130" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="M41" s="130" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="130" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="B42" s="130" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="D42" s="130" t="s">
         <v>488</v>
       </c>
       <c r="E42" s="130" t="s">
+        <v>926</v>
+      </c>
+      <c r="M42" s="130" t="s">
         <v>928</v>
-      </c>
-      <c r="M42" s="130" t="s">
-        <v>930</v>
       </c>
       <c r="N42" s="34">
         <v>3</v>
@@ -24924,7 +24859,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="131" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="B43" s="131" t="s">
         <v>374</v>
@@ -24933,10 +24868,10 @@
         <v>488</v>
       </c>
       <c r="E43" s="131" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="M43" s="131" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="N43" s="34">
         <v>3</v>
@@ -24944,7 +24879,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="131" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="B44" s="131" t="s">
         <v>374</v>
@@ -24953,10 +24888,10 @@
         <v>488</v>
       </c>
       <c r="E44" s="131" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="M44" s="131" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="N44" s="34">
         <v>3</v>
@@ -24964,7 +24899,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="131" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="B45" s="131" t="s">
         <v>374</v>
@@ -24973,10 +24908,10 @@
         <v>488</v>
       </c>
       <c r="E45" s="131" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="M45" s="131" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="N45" s="34">
         <v>3</v>
@@ -24984,7 +24919,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="133" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="B46" s="133" t="s">
         <v>374</v>
@@ -24993,10 +24928,10 @@
         <v>422</v>
       </c>
       <c r="E46" s="133" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="M46" s="133" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="N46" s="34">
         <v>3</v>
@@ -25004,7 +24939,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="134" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="B47" s="134" t="s">
         <v>375</v>
@@ -25013,16 +24948,16 @@
         <v>492</v>
       </c>
       <c r="E47" s="134" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="F47" s="134" t="s">
         <v>745</v>
       </c>
       <c r="G47" s="134" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="M47" s="134" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="N47" s="34">
         <v>3</v>
@@ -25030,7 +24965,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="134" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="B48" s="134" t="s">
         <v>375</v>
@@ -25039,30 +24974,30 @@
         <v>492</v>
       </c>
       <c r="E48" s="134" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="F48" s="134" t="s">
         <v>745</v>
       </c>
       <c r="M48" s="134" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="134" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="B49" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D49" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E49" s="134" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="M49" s="134" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="N49" s="34">
         <v>3</v>
@@ -25070,19 +25005,19 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="134" t="s">
+        <v>951</v>
+      </c>
+      <c r="B50" s="134" t="s">
         <v>953</v>
-      </c>
-      <c r="B50" s="134" t="s">
-        <v>955</v>
       </c>
       <c r="D50" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E50" s="134" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="M50" s="134" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="N50" s="34">
         <v>3</v>
@@ -25090,53 +25025,53 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="134" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="B51" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D51" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E51" s="134" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="M51" s="134" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="134" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="B52" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D52" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E52" s="134" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="M52" s="134" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="134" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="B53" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D53" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E53" s="134" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="M53" s="134" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="N53" s="34">
         <v>3</v>
@@ -25144,19 +25079,19 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="134" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="B54" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D54" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E54" s="134" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="M54" s="134" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="N54" s="34">
         <v>3</v>
@@ -25164,19 +25099,19 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="134" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="B55" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D55" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E55" s="134" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="M55" s="135" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="N55" s="136">
         <v>3</v>
@@ -25186,19 +25121,19 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="134" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="B56" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D56" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E56" s="134" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="M56" s="134" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="N56" s="34">
         <v>3</v>
@@ -25206,19 +25141,19 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="134" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="B57" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D57" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E57" s="134" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="M57" s="134" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="N57" s="34">
         <v>3</v>
@@ -25226,19 +25161,19 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="134" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="B58" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D58" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E58" s="134" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="M58" s="134" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="N58" s="34">
         <v>3</v>
@@ -25246,19 +25181,19 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="134" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="B59" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D59" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E59" s="134" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="M59" s="134" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="N59" s="34">
         <v>3</v>
@@ -25266,53 +25201,53 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="134" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="B60" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D60" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E60" s="134" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="M60" s="134" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="134" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="B61" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D61" s="134" t="s">
         <v>382</v>
       </c>
       <c r="E61" s="134" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="M61" s="134" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="134" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="B62" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D62" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E62" s="134" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="M62" s="134" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="N62" s="34">
         <v>3</v>
@@ -25320,19 +25255,19 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="134" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="B63" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D63" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E63" s="134" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="M63" s="134" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="N63" s="34">
         <v>3</v>
@@ -25340,19 +25275,19 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="134" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B64" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D64" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E64" s="134" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="M64" s="134" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="N64" s="34">
         <v>4</v>
@@ -25360,19 +25295,19 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="134" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B65" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D65" s="134" t="s">
         <v>422</v>
       </c>
       <c r="E65" s="134" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="M65" s="134" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="N65" s="34">
         <v>3</v>
@@ -25380,36 +25315,36 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="134" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="B66" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D66" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E66" s="134" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="M66" s="134" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="134" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B67" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D67" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E67" s="134" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="M67" s="134" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="N67" s="34">
         <v>3</v>
@@ -25417,19 +25352,19 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="134" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="B68" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D68" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E68" s="134" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="M68" s="134" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
@@ -25437,16 +25372,16 @@
         <v>483</v>
       </c>
       <c r="B69" s="134" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D69" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E69" s="134" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="M69" s="134" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
   </sheetData>
@@ -25501,34 +25436,34 @@
         <v>363</v>
       </c>
       <c r="B1" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="C1" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="D1" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E1" s="137" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="F1" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="G1" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="H1" t="s">
         <v>376</v>
       </c>
       <c r="I1" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="J1" t="s">
         <v>491</v>
       </c>
       <c r="K1" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="L1" t="s">
         <v>364</v>
@@ -25537,7 +25472,7 @@
         <v>236</v>
       </c>
       <c r="N1" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="O1" s="3">
         <v>1</v>
@@ -25692,25 +25627,25 @@
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" s="137" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="B2" s="137" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C2" s="137" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="D2" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="137" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="F2" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G2" s="137" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="H2" s="137">
         <v>3</v>
@@ -25723,25 +25658,25 @@
       </c>
       <c r="K2" s="137"/>
       <c r="L2" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="M2" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="N2" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="T2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="X2" t="s">
         <v>1016</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Z2" t="s">
         <v>1017</v>
-      </c>
-      <c r="X2" t="s">
-        <v>1018</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.25">
@@ -25749,22 +25684,22 @@
         <v>501</v>
       </c>
       <c r="B3" s="137" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C3" s="137" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="D3" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="137" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="F3" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G3" s="137" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="H3" s="137">
         <v>5</v>
@@ -25777,13 +25712,13 @@
       </c>
       <c r="K3" s="137"/>
       <c r="L3" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="M3" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="N3" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="O3" s="138"/>
       <c r="P3" s="138"/>
@@ -25792,25 +25727,25 @@
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="B4" s="137" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C4" s="137" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="D4" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="137" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="F4" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G4" s="137" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="H4" s="137">
         <v>4</v>
@@ -25823,19 +25758,19 @@
       </c>
       <c r="K4" s="137"/>
       <c r="L4" t="s">
+        <v>1018</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1011</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1019</v>
+      </c>
+      <c r="AD4" t="s">
         <v>1020</v>
-      </c>
-      <c r="M4" t="s">
-        <v>1060</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1013</v>
-      </c>
-      <c r="R4" t="s">
-        <v>1021</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>1022</v>
       </c>
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.25">
@@ -25843,20 +25778,20 @@
         <v>493</v>
       </c>
       <c r="B5" s="137" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C5" s="137" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="D5" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="137" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="F5" s="137"/>
       <c r="G5" s="137" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="H5" s="137">
         <v>4</v>
@@ -25871,13 +25806,13 @@
         <v>247</v>
       </c>
       <c r="L5" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="M5" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="N5" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="U5" s="138">
         <v>0.18</v>
@@ -25897,20 +25832,20 @@
         <v>497</v>
       </c>
       <c r="B6" s="137" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C6" s="137" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="D6" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="137" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="F6" s="137"/>
       <c r="G6" s="137" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="H6" s="137">
         <v>3</v>
@@ -25919,19 +25854,19 @@
         <v>1</v>
       </c>
       <c r="J6" s="137" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="K6" s="137" t="s">
         <v>246</v>
       </c>
       <c r="L6" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="M6" s="139" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="N6" s="137" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="T6" s="138"/>
       <c r="X6" s="138"/>
@@ -25942,10 +25877,10 @@
         <v>558</v>
       </c>
       <c r="B7" s="137" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C7" s="137" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="D7" s="137" t="s">
         <v>33</v>
@@ -25955,7 +25890,7 @@
       </c>
       <c r="F7" s="137"/>
       <c r="G7" s="137" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="H7" s="137">
         <v>4</v>
@@ -25967,46 +25902,46 @@
         <v>3</v>
       </c>
       <c r="K7" s="137" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="L7" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="M7" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="R7" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="V7" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="Z7" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="AD7" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B8" s="137" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C8" s="137" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D8" s="137" t="s">
         <v>1048</v>
       </c>
-      <c r="B8" s="137" t="s">
-        <v>1010</v>
-      </c>
-      <c r="C8" s="137" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D8" s="137" t="s">
-        <v>1050</v>
-      </c>
       <c r="E8" s="137" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="F8" s="137"/>
       <c r="G8" s="137" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="H8" s="137">
         <v>0</v>
@@ -26019,10 +25954,10 @@
       </c>
       <c r="K8" s="137"/>
       <c r="L8" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="M8" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="W8">
         <v>2</v>
@@ -26039,22 +25974,22 @@
         <v>490</v>
       </c>
       <c r="B9" s="137" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C9" s="137" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="D9" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="137" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="F9" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G9" s="137" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="H9" s="137">
         <v>4</v>
@@ -26069,10 +26004,10 @@
         <v>246</v>
       </c>
       <c r="L9" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="M9" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.25">
@@ -26080,20 +26015,20 @@
         <v>496</v>
       </c>
       <c r="B10" s="137" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C10" s="137" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="D10" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="137" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="F10" s="137"/>
       <c r="G10" s="137" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="H10" s="137">
         <v>4</v>
@@ -26108,13 +26043,13 @@
         <v>246</v>
       </c>
       <c r="L10" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="M10" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="N10" s="139" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.25">
@@ -26122,10 +26057,10 @@
         <v>565</v>
       </c>
       <c r="B11" s="137" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C11" s="137" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="D11" s="137" t="s">
         <v>33</v>
@@ -26135,7 +26070,7 @@
       </c>
       <c r="F11" s="137"/>
       <c r="G11" s="137" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="H11" s="137">
         <v>1</v>
@@ -26150,25 +26085,25 @@
         <v>246</v>
       </c>
       <c r="L11" t="s">
+        <v>1069</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1052</v>
+      </c>
+      <c r="N11" s="139" t="s">
+        <v>1070</v>
+      </c>
+      <c r="S11" t="s">
+        <v>1053</v>
+      </c>
+      <c r="X11" t="s">
+        <v>1053</v>
+      </c>
+      <c r="AC11" t="s">
         <v>1071</v>
       </c>
-      <c r="M11" t="s">
-        <v>1054</v>
-      </c>
-      <c r="N11" s="139" t="s">
-        <v>1072</v>
-      </c>
-      <c r="S11" t="s">
-        <v>1055</v>
-      </c>
-      <c r="X11" t="s">
-        <v>1055</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>1073</v>
-      </c>
       <c r="AH11" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.25">
@@ -27649,10 +27584,10 @@
     </row>
     <row r="19" spans="1:15" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="104" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -28159,7 +28094,7 @@
         <v>278</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -28412,19 +28347,19 @@
         <v>773</v>
       </c>
       <c r="K61" s="76" t="s">
+        <v>908</v>
+      </c>
+      <c r="L61" s="76" t="s">
+        <v>909</v>
+      </c>
+      <c r="M61" s="76" t="s">
         <v>910</v>
       </c>
-      <c r="L61" s="76" t="s">
+      <c r="N61" s="76" t="s">
         <v>911</v>
       </c>
-      <c r="M61" s="76" t="s">
+      <c r="O61" s="74" t="s">
         <v>912</v>
-      </c>
-      <c r="N61" s="76" t="s">
-        <v>913</v>
-      </c>
-      <c r="O61" s="74" t="s">
-        <v>914</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixing a lot of stuff, adding scatter fatality
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716" firstSheet="12" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="TODO - Quick Battle" sheetId="37" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="Perks" sheetId="34" r:id="rId22"/>
     <sheet name="Abilities" sheetId="35" r:id="rId23"/>
     <sheet name="Spells" sheetId="39" r:id="rId24"/>
+    <sheet name="Level Guide" sheetId="40" r:id="rId25"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -643,7 +644,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="1073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2240" uniqueCount="1085">
   <si>
     <t>Fishing</t>
   </si>
@@ -3862,6 +3863,42 @@
   </si>
   <si>
     <t>Fires a dart at target that if hits, does DoT damage as well as initial damage</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Militia</t>
+  </si>
+  <si>
+    <t>Green Soldier</t>
+  </si>
+  <si>
+    <t>Veteran</t>
+  </si>
+  <si>
+    <t>Experienced</t>
+  </si>
+  <si>
+    <t>Elite</t>
+  </si>
+  <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>Demigod</t>
+  </si>
+  <si>
+    <t>Godling</t>
+  </si>
+  <si>
+    <t>Lesser Deity</t>
+  </si>
+  <si>
+    <t>Deity</t>
+  </si>
+  <si>
+    <t>Greater Deity</t>
   </si>
 </sst>
 </file>
@@ -5049,22 +5086,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5082,10 +5113,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5439,7 +5476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -5455,29 +5492,29 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="152" t="s">
+      <c r="A2" s="150" t="s">
         <v>782</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="154"/>
+      <c r="B2" s="151"/>
+      <c r="C2" s="152"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="115">
         <v>1</v>
       </c>
-      <c r="B3" s="155" t="s">
+      <c r="B3" s="153" t="s">
         <v>783</v>
       </c>
-      <c r="C3" s="156"/>
+      <c r="C3" s="154"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="155" t="s">
         <v>784</v>
       </c>
-      <c r="C4" s="147"/>
+      <c r="C4" s="156"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="116"/>
@@ -5528,10 +5565,10 @@
       <c r="A10" s="116">
         <v>3</v>
       </c>
-      <c r="B10" s="148" t="s">
+      <c r="B10" s="157" t="s">
         <v>785</v>
       </c>
-      <c r="C10" s="149"/>
+      <c r="C10" s="158"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="116"/>
@@ -5546,10 +5583,10 @@
       <c r="A12" s="116">
         <v>4</v>
       </c>
-      <c r="B12" s="150" t="s">
+      <c r="B12" s="146" t="s">
         <v>786</v>
       </c>
-      <c r="C12" s="151"/>
+      <c r="C12" s="147"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="116"/>
@@ -5564,10 +5601,10 @@
       <c r="A14" s="116">
         <v>5</v>
       </c>
-      <c r="B14" s="150" t="s">
+      <c r="B14" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="C14" s="151"/>
+      <c r="C14" s="147"/>
     </row>
     <row r="15" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="116"/>
@@ -5582,10 +5619,10 @@
       <c r="A16" s="117">
         <v>6</v>
       </c>
-      <c r="B16" s="157" t="s">
+      <c r="B16" s="148" t="s">
         <v>791</v>
       </c>
-      <c r="C16" s="158"/>
+      <c r="C16" s="149"/>
     </row>
     <row r="17" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="116"/>
@@ -5600,46 +5637,46 @@
       <c r="A18" s="117">
         <v>7</v>
       </c>
-      <c r="B18" s="157" t="s">
+      <c r="B18" s="148" t="s">
         <v>913</v>
       </c>
-      <c r="C18" s="158"/>
+      <c r="C18" s="149"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="132">
         <v>8</v>
       </c>
-      <c r="B19" s="157" t="s">
+      <c r="B19" s="148" t="s">
         <v>1000</v>
       </c>
-      <c r="C19" s="158"/>
+      <c r="C19" s="149"/>
     </row>
     <row r="20" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="132">
         <v>9</v>
       </c>
-      <c r="B20" s="157" t="s">
+      <c r="B20" s="148" t="s">
         <v>914</v>
       </c>
-      <c r="C20" s="158"/>
+      <c r="C20" s="149"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="152" t="s">
+      <c r="A23" s="150" t="s">
         <v>793</v>
       </c>
-      <c r="B23" s="153"/>
-      <c r="C23" s="154"/>
+      <c r="B23" s="151"/>
+      <c r="C23" s="152"/>
     </row>
     <row r="24" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="115">
         <v>1</v>
       </c>
-      <c r="B24" s="155" t="s">
+      <c r="B24" s="153" t="s">
         <v>782</v>
       </c>
-      <c r="C24" s="156"/>
+      <c r="C24" s="154"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="116"/>
@@ -5659,10 +5696,10 @@
       <c r="A27" s="116">
         <v>2</v>
       </c>
-      <c r="B27" s="146" t="s">
+      <c r="B27" s="155" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="147"/>
+      <c r="C27" s="156"/>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="116"/>
@@ -5682,10 +5719,10 @@
       <c r="A30" s="116">
         <v>3</v>
       </c>
-      <c r="B30" s="146" t="s">
+      <c r="B30" s="155" t="s">
         <v>1001</v>
       </c>
-      <c r="C30" s="147"/>
+      <c r="C30" s="156"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="116"/>
@@ -5707,20 +5744,20 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="152" t="s">
+      <c r="A34" s="150" t="s">
         <v>797</v>
       </c>
-      <c r="B34" s="153"/>
-      <c r="C34" s="154"/>
+      <c r="B34" s="151"/>
+      <c r="C34" s="152"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="115">
         <v>1</v>
       </c>
-      <c r="B35" s="155" t="s">
+      <c r="B35" s="153" t="s">
         <v>798</v>
       </c>
-      <c r="C35" s="156"/>
+      <c r="C35" s="154"/>
     </row>
     <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="116"/>
@@ -5760,20 +5797,20 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="152" t="s">
+      <c r="A41" s="150" t="s">
         <v>802</v>
       </c>
-      <c r="B41" s="153"/>
-      <c r="C41" s="154"/>
+      <c r="B41" s="151"/>
+      <c r="C41" s="152"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="115">
         <v>1</v>
       </c>
-      <c r="B42" s="155" t="s">
+      <c r="B42" s="153" t="s">
         <v>803</v>
       </c>
-      <c r="C42" s="156"/>
+      <c r="C42" s="154"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="116"/>
@@ -5797,10 +5834,10 @@
       <c r="A45" s="115">
         <v>1</v>
       </c>
-      <c r="B45" s="155" t="s">
+      <c r="B45" s="153" t="s">
         <v>805</v>
       </c>
-      <c r="C45" s="156"/>
+      <c r="C45" s="154"/>
     </row>
     <row r="46" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="116"/>
@@ -5836,37 +5873,37 @@
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="152" t="s">
+      <c r="A51" s="150" t="s">
         <v>188</v>
       </c>
-      <c r="B51" s="153"/>
-      <c r="C51" s="154"/>
+      <c r="B51" s="151"/>
+      <c r="C51" s="152"/>
     </row>
     <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="115">
         <v>1</v>
       </c>
-      <c r="B52" s="155" t="s">
+      <c r="B52" s="153" t="s">
         <v>810</v>
       </c>
-      <c r="C52" s="156"/>
+      <c r="C52" s="154"/>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="152" t="s">
+      <c r="A54" s="150" t="s">
         <v>790</v>
       </c>
-      <c r="B54" s="153"/>
-      <c r="C54" s="154"/>
+      <c r="B54" s="151"/>
+      <c r="C54" s="152"/>
     </row>
     <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="115">
         <v>1</v>
       </c>
-      <c r="B55" s="148" t="s">
+      <c r="B55" s="157" t="s">
         <v>783</v>
       </c>
-      <c r="C55" s="149"/>
+      <c r="C55" s="158"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="116">
@@ -5881,54 +5918,54 @@
       <c r="A57" s="116">
         <v>3</v>
       </c>
-      <c r="B57" s="150" t="s">
+      <c r="B57" s="146" t="s">
         <v>785</v>
       </c>
-      <c r="C57" s="151"/>
+      <c r="C57" s="147"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="116">
         <v>4</v>
       </c>
-      <c r="B58" s="150" t="s">
+      <c r="B58" s="146" t="s">
         <v>786</v>
       </c>
-      <c r="C58" s="151"/>
+      <c r="C58" s="147"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="116">
         <v>5</v>
       </c>
-      <c r="B59" s="150" t="s">
+      <c r="B59" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="C59" s="151"/>
+      <c r="C59" s="147"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="117">
         <v>6</v>
       </c>
-      <c r="B60" s="157" t="s">
+      <c r="B60" s="148" t="s">
         <v>791</v>
       </c>
-      <c r="C60" s="158"/>
+      <c r="C60" s="149"/>
     </row>
     <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="152" t="s">
+      <c r="A62" s="150" t="s">
         <v>811</v>
       </c>
-      <c r="B62" s="153"/>
-      <c r="C62" s="154"/>
+      <c r="B62" s="151"/>
+      <c r="C62" s="152"/>
     </row>
     <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="115">
         <v>1</v>
       </c>
-      <c r="B63" s="148" t="s">
+      <c r="B63" s="157" t="s">
         <v>783</v>
       </c>
-      <c r="C63" s="149"/>
+      <c r="C63" s="158"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="116">
@@ -5943,52 +5980,52 @@
       <c r="A65" s="116">
         <v>3</v>
       </c>
-      <c r="B65" s="150" t="s">
+      <c r="B65" s="146" t="s">
         <v>785</v>
       </c>
-      <c r="C65" s="151"/>
+      <c r="C65" s="147"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="116">
         <v>4</v>
       </c>
-      <c r="B66" s="150" t="s">
+      <c r="B66" s="146" t="s">
         <v>786</v>
       </c>
-      <c r="C66" s="151"/>
+      <c r="C66" s="147"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="116">
         <v>5</v>
       </c>
-      <c r="B67" s="150" t="s">
+      <c r="B67" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="C67" s="151"/>
+      <c r="C67" s="147"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="117">
         <v>6</v>
       </c>
-      <c r="B68" s="157" t="s">
+      <c r="B68" s="148" t="s">
         <v>791</v>
       </c>
-      <c r="C68" s="158"/>
+      <c r="C68" s="149"/>
     </row>
     <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="152" t="s">
+      <c r="A70" s="150" t="s">
         <v>1001</v>
       </c>
-      <c r="B70" s="153"/>
-      <c r="C70" s="154"/>
+      <c r="B70" s="151"/>
+      <c r="C70" s="152"/>
     </row>
     <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="115">
         <v>1</v>
       </c>
-      <c r="B71" s="148"/>
-      <c r="C71" s="149"/>
+      <c r="B71" s="157"/>
+      <c r="C71" s="158"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="116"/>
@@ -5997,40 +6034,40 @@
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="116"/>
-      <c r="B73" s="150"/>
-      <c r="C73" s="151"/>
+      <c r="B73" s="146"/>
+      <c r="C73" s="147"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="116"/>
-      <c r="B74" s="150"/>
-      <c r="C74" s="151"/>
+      <c r="B74" s="146"/>
+      <c r="C74" s="147"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="116"/>
-      <c r="B75" s="150"/>
-      <c r="C75" s="151"/>
+      <c r="B75" s="146"/>
+      <c r="C75" s="147"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="117"/>
-      <c r="B76" s="157"/>
-      <c r="C76" s="158"/>
+      <c r="B76" s="148"/>
+      <c r="C76" s="149"/>
     </row>
     <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="152" t="s">
+      <c r="A78" s="150" t="s">
         <v>812</v>
       </c>
-      <c r="B78" s="153"/>
-      <c r="C78" s="154"/>
+      <c r="B78" s="151"/>
+      <c r="C78" s="152"/>
     </row>
     <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="115">
         <v>1</v>
       </c>
-      <c r="B79" s="148" t="s">
+      <c r="B79" s="157" t="s">
         <v>783</v>
       </c>
-      <c r="C79" s="149"/>
+      <c r="C79" s="158"/>
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="116">
@@ -6045,54 +6082,54 @@
       <c r="A81" s="116">
         <v>3</v>
       </c>
-      <c r="B81" s="150" t="s">
+      <c r="B81" s="146" t="s">
         <v>785</v>
       </c>
-      <c r="C81" s="151"/>
+      <c r="C81" s="147"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="116">
         <v>4</v>
       </c>
-      <c r="B82" s="150" t="s">
+      <c r="B82" s="146" t="s">
         <v>786</v>
       </c>
-      <c r="C82" s="151"/>
+      <c r="C82" s="147"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="116">
         <v>5</v>
       </c>
-      <c r="B83" s="150" t="s">
+      <c r="B83" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="C83" s="151"/>
+      <c r="C83" s="147"/>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="117">
         <v>6</v>
       </c>
-      <c r="B84" s="157" t="s">
+      <c r="B84" s="148" t="s">
         <v>791</v>
       </c>
-      <c r="C84" s="158"/>
+      <c r="C84" s="149"/>
     </row>
     <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="152" t="s">
+      <c r="A86" s="150" t="s">
         <v>862</v>
       </c>
-      <c r="B86" s="153"/>
-      <c r="C86" s="154"/>
+      <c r="B86" s="151"/>
+      <c r="C86" s="152"/>
     </row>
     <row r="87" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="115">
         <v>1</v>
       </c>
-      <c r="B87" s="155" t="s">
+      <c r="B87" s="153" t="s">
         <v>101</v>
       </c>
-      <c r="C87" s="156"/>
+      <c r="C87" s="154"/>
     </row>
     <row r="88" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="124"/>
@@ -6265,10 +6302,10 @@
       <c r="A107" s="116">
         <v>2</v>
       </c>
-      <c r="B107" s="146" t="s">
+      <c r="B107" s="155" t="s">
         <v>813</v>
       </c>
-      <c r="C107" s="147"/>
+      <c r="C107" s="156"/>
     </row>
     <row r="108" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="116"/>
@@ -6346,10 +6383,10 @@
       <c r="A116" s="116">
         <v>3</v>
       </c>
-      <c r="B116" s="148" t="s">
+      <c r="B116" s="157" t="s">
         <v>814</v>
       </c>
-      <c r="C116" s="149"/>
+      <c r="C116" s="158"/>
     </row>
     <row r="117" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="116"/>
@@ -6405,10 +6442,10 @@
       <c r="A123" s="115">
         <v>4</v>
       </c>
-      <c r="B123" s="150" t="s">
+      <c r="B123" s="146" t="s">
         <v>815</v>
       </c>
-      <c r="C123" s="151"/>
+      <c r="C123" s="147"/>
     </row>
     <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="124"/>
@@ -6448,20 +6485,20 @@
     </row>
     <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="129" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="152" t="s">
+      <c r="A129" s="150" t="s">
         <v>863</v>
       </c>
-      <c r="B129" s="153"/>
-      <c r="C129" s="154"/>
+      <c r="B129" s="151"/>
+      <c r="C129" s="152"/>
     </row>
     <row r="130" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="115">
         <v>1</v>
       </c>
-      <c r="B130" s="155" t="s">
+      <c r="B130" s="153" t="s">
         <v>864</v>
       </c>
-      <c r="C130" s="156"/>
+      <c r="C130" s="154"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="124"/>
@@ -6608,10 +6645,10 @@
       <c r="A150" s="116">
         <v>2</v>
       </c>
-      <c r="B150" s="146" t="s">
+      <c r="B150" s="155" t="s">
         <v>865</v>
       </c>
-      <c r="C150" s="147"/>
+      <c r="C150" s="156"/>
     </row>
     <row r="151" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="116"/>
@@ -6681,10 +6718,10 @@
       <c r="A159" s="116">
         <v>3</v>
       </c>
-      <c r="B159" s="148" t="s">
+      <c r="B159" s="157" t="s">
         <v>866</v>
       </c>
-      <c r="C159" s="149"/>
+      <c r="C159" s="158"/>
     </row>
     <row r="160" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="116"/>
@@ -6738,6 +6775,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="A129:C129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B42:C42"/>
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
@@ -6754,48 +6833,6 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="A129:C129"/>
-    <mergeCell ref="B130:C130"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -26430,6 +26467,128 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A37"/>

</xml_diff>

<commit_message>
General cleanup, plus editing jomonese values
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -5086,16 +5086,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5113,16 +5119,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5492,29 +5492,29 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="152" t="s">
         <v>782</v>
       </c>
-      <c r="B2" s="151"/>
-      <c r="C2" s="152"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="154"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="115">
         <v>1</v>
       </c>
-      <c r="B3" s="153" t="s">
+      <c r="B3" s="155" t="s">
         <v>783</v>
       </c>
-      <c r="C3" s="154"/>
+      <c r="C3" s="156"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="146" t="s">
         <v>784</v>
       </c>
-      <c r="C4" s="156"/>
+      <c r="C4" s="147"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="116"/>
@@ -5565,10 +5565,10 @@
       <c r="A10" s="116">
         <v>3</v>
       </c>
-      <c r="B10" s="157" t="s">
+      <c r="B10" s="148" t="s">
         <v>785</v>
       </c>
-      <c r="C10" s="158"/>
+      <c r="C10" s="149"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="116"/>
@@ -5583,10 +5583,10 @@
       <c r="A12" s="116">
         <v>4</v>
       </c>
-      <c r="B12" s="146" t="s">
+      <c r="B12" s="150" t="s">
         <v>786</v>
       </c>
-      <c r="C12" s="147"/>
+      <c r="C12" s="151"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="116"/>
@@ -5601,10 +5601,10 @@
       <c r="A14" s="116">
         <v>5</v>
       </c>
-      <c r="B14" s="146" t="s">
+      <c r="B14" s="150" t="s">
         <v>787</v>
       </c>
-      <c r="C14" s="147"/>
+      <c r="C14" s="151"/>
     </row>
     <row r="15" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="116"/>
@@ -5619,10 +5619,10 @@
       <c r="A16" s="117">
         <v>6</v>
       </c>
-      <c r="B16" s="148" t="s">
+      <c r="B16" s="157" t="s">
         <v>791</v>
       </c>
-      <c r="C16" s="149"/>
+      <c r="C16" s="158"/>
     </row>
     <row r="17" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="116"/>
@@ -5637,46 +5637,46 @@
       <c r="A18" s="117">
         <v>7</v>
       </c>
-      <c r="B18" s="148" t="s">
+      <c r="B18" s="157" t="s">
         <v>913</v>
       </c>
-      <c r="C18" s="149"/>
+      <c r="C18" s="158"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="132">
         <v>8</v>
       </c>
-      <c r="B19" s="148" t="s">
+      <c r="B19" s="157" t="s">
         <v>1000</v>
       </c>
-      <c r="C19" s="149"/>
+      <c r="C19" s="158"/>
     </row>
     <row r="20" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="132">
         <v>9</v>
       </c>
-      <c r="B20" s="148" t="s">
+      <c r="B20" s="157" t="s">
         <v>914</v>
       </c>
-      <c r="C20" s="149"/>
+      <c r="C20" s="158"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="150" t="s">
+      <c r="A23" s="152" t="s">
         <v>793</v>
       </c>
-      <c r="B23" s="151"/>
-      <c r="C23" s="152"/>
+      <c r="B23" s="153"/>
+      <c r="C23" s="154"/>
     </row>
     <row r="24" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="115">
         <v>1</v>
       </c>
-      <c r="B24" s="153" t="s">
+      <c r="B24" s="155" t="s">
         <v>782</v>
       </c>
-      <c r="C24" s="154"/>
+      <c r="C24" s="156"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="116"/>
@@ -5696,10 +5696,10 @@
       <c r="A27" s="116">
         <v>2</v>
       </c>
-      <c r="B27" s="155" t="s">
+      <c r="B27" s="146" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="156"/>
+      <c r="C27" s="147"/>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="116"/>
@@ -5719,10 +5719,10 @@
       <c r="A30" s="116">
         <v>3</v>
       </c>
-      <c r="B30" s="155" t="s">
+      <c r="B30" s="146" t="s">
         <v>1001</v>
       </c>
-      <c r="C30" s="156"/>
+      <c r="C30" s="147"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="116"/>
@@ -5744,20 +5744,20 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="150" t="s">
+      <c r="A34" s="152" t="s">
         <v>797</v>
       </c>
-      <c r="B34" s="151"/>
-      <c r="C34" s="152"/>
+      <c r="B34" s="153"/>
+      <c r="C34" s="154"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="115">
         <v>1</v>
       </c>
-      <c r="B35" s="153" t="s">
+      <c r="B35" s="155" t="s">
         <v>798</v>
       </c>
-      <c r="C35" s="154"/>
+      <c r="C35" s="156"/>
     </row>
     <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="116"/>
@@ -5797,20 +5797,20 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="150" t="s">
+      <c r="A41" s="152" t="s">
         <v>802</v>
       </c>
-      <c r="B41" s="151"/>
-      <c r="C41" s="152"/>
+      <c r="B41" s="153"/>
+      <c r="C41" s="154"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="115">
         <v>1</v>
       </c>
-      <c r="B42" s="153" t="s">
+      <c r="B42" s="155" t="s">
         <v>803</v>
       </c>
-      <c r="C42" s="154"/>
+      <c r="C42" s="156"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="116"/>
@@ -5834,10 +5834,10 @@
       <c r="A45" s="115">
         <v>1</v>
       </c>
-      <c r="B45" s="153" t="s">
+      <c r="B45" s="155" t="s">
         <v>805</v>
       </c>
-      <c r="C45" s="154"/>
+      <c r="C45" s="156"/>
     </row>
     <row r="46" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="116"/>
@@ -5873,37 +5873,37 @@
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="150" t="s">
+      <c r="A51" s="152" t="s">
         <v>188</v>
       </c>
-      <c r="B51" s="151"/>
-      <c r="C51" s="152"/>
+      <c r="B51" s="153"/>
+      <c r="C51" s="154"/>
     </row>
     <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="115">
         <v>1</v>
       </c>
-      <c r="B52" s="153" t="s">
+      <c r="B52" s="155" t="s">
         <v>810</v>
       </c>
-      <c r="C52" s="154"/>
+      <c r="C52" s="156"/>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="150" t="s">
+      <c r="A54" s="152" t="s">
         <v>790</v>
       </c>
-      <c r="B54" s="151"/>
-      <c r="C54" s="152"/>
+      <c r="B54" s="153"/>
+      <c r="C54" s="154"/>
     </row>
     <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="115">
         <v>1</v>
       </c>
-      <c r="B55" s="157" t="s">
+      <c r="B55" s="148" t="s">
         <v>783</v>
       </c>
-      <c r="C55" s="158"/>
+      <c r="C55" s="149"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="116">
@@ -5918,54 +5918,54 @@
       <c r="A57" s="116">
         <v>3</v>
       </c>
-      <c r="B57" s="146" t="s">
+      <c r="B57" s="150" t="s">
         <v>785</v>
       </c>
-      <c r="C57" s="147"/>
+      <c r="C57" s="151"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="116">
         <v>4</v>
       </c>
-      <c r="B58" s="146" t="s">
+      <c r="B58" s="150" t="s">
         <v>786</v>
       </c>
-      <c r="C58" s="147"/>
+      <c r="C58" s="151"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="116">
         <v>5</v>
       </c>
-      <c r="B59" s="146" t="s">
+      <c r="B59" s="150" t="s">
         <v>787</v>
       </c>
-      <c r="C59" s="147"/>
+      <c r="C59" s="151"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="117">
         <v>6</v>
       </c>
-      <c r="B60" s="148" t="s">
+      <c r="B60" s="157" t="s">
         <v>791</v>
       </c>
-      <c r="C60" s="149"/>
+      <c r="C60" s="158"/>
     </row>
     <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="150" t="s">
+      <c r="A62" s="152" t="s">
         <v>811</v>
       </c>
-      <c r="B62" s="151"/>
-      <c r="C62" s="152"/>
+      <c r="B62" s="153"/>
+      <c r="C62" s="154"/>
     </row>
     <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="115">
         <v>1</v>
       </c>
-      <c r="B63" s="157" t="s">
+      <c r="B63" s="148" t="s">
         <v>783</v>
       </c>
-      <c r="C63" s="158"/>
+      <c r="C63" s="149"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="116">
@@ -5980,52 +5980,52 @@
       <c r="A65" s="116">
         <v>3</v>
       </c>
-      <c r="B65" s="146" t="s">
+      <c r="B65" s="150" t="s">
         <v>785</v>
       </c>
-      <c r="C65" s="147"/>
+      <c r="C65" s="151"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="116">
         <v>4</v>
       </c>
-      <c r="B66" s="146" t="s">
+      <c r="B66" s="150" t="s">
         <v>786</v>
       </c>
-      <c r="C66" s="147"/>
+      <c r="C66" s="151"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="116">
         <v>5</v>
       </c>
-      <c r="B67" s="146" t="s">
+      <c r="B67" s="150" t="s">
         <v>787</v>
       </c>
-      <c r="C67" s="147"/>
+      <c r="C67" s="151"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="117">
         <v>6</v>
       </c>
-      <c r="B68" s="148" t="s">
+      <c r="B68" s="157" t="s">
         <v>791</v>
       </c>
-      <c r="C68" s="149"/>
+      <c r="C68" s="158"/>
     </row>
     <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="150" t="s">
+      <c r="A70" s="152" t="s">
         <v>1001</v>
       </c>
-      <c r="B70" s="151"/>
-      <c r="C70" s="152"/>
+      <c r="B70" s="153"/>
+      <c r="C70" s="154"/>
     </row>
     <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="115">
         <v>1</v>
       </c>
-      <c r="B71" s="157"/>
-      <c r="C71" s="158"/>
+      <c r="B71" s="148"/>
+      <c r="C71" s="149"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="116"/>
@@ -6034,40 +6034,40 @@
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="116"/>
-      <c r="B73" s="146"/>
-      <c r="C73" s="147"/>
+      <c r="B73" s="150"/>
+      <c r="C73" s="151"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="116"/>
-      <c r="B74" s="146"/>
-      <c r="C74" s="147"/>
+      <c r="B74" s="150"/>
+      <c r="C74" s="151"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="116"/>
-      <c r="B75" s="146"/>
-      <c r="C75" s="147"/>
+      <c r="B75" s="150"/>
+      <c r="C75" s="151"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="117"/>
-      <c r="B76" s="148"/>
-      <c r="C76" s="149"/>
+      <c r="B76" s="157"/>
+      <c r="C76" s="158"/>
     </row>
     <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="150" t="s">
+      <c r="A78" s="152" t="s">
         <v>812</v>
       </c>
-      <c r="B78" s="151"/>
-      <c r="C78" s="152"/>
+      <c r="B78" s="153"/>
+      <c r="C78" s="154"/>
     </row>
     <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="115">
         <v>1</v>
       </c>
-      <c r="B79" s="157" t="s">
+      <c r="B79" s="148" t="s">
         <v>783</v>
       </c>
-      <c r="C79" s="158"/>
+      <c r="C79" s="149"/>
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="116">
@@ -6082,54 +6082,54 @@
       <c r="A81" s="116">
         <v>3</v>
       </c>
-      <c r="B81" s="146" t="s">
+      <c r="B81" s="150" t="s">
         <v>785</v>
       </c>
-      <c r="C81" s="147"/>
+      <c r="C81" s="151"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="116">
         <v>4</v>
       </c>
-      <c r="B82" s="146" t="s">
+      <c r="B82" s="150" t="s">
         <v>786</v>
       </c>
-      <c r="C82" s="147"/>
+      <c r="C82" s="151"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="116">
         <v>5</v>
       </c>
-      <c r="B83" s="146" t="s">
+      <c r="B83" s="150" t="s">
         <v>787</v>
       </c>
-      <c r="C83" s="147"/>
+      <c r="C83" s="151"/>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="117">
         <v>6</v>
       </c>
-      <c r="B84" s="148" t="s">
+      <c r="B84" s="157" t="s">
         <v>791</v>
       </c>
-      <c r="C84" s="149"/>
+      <c r="C84" s="158"/>
     </row>
     <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="150" t="s">
+      <c r="A86" s="152" t="s">
         <v>862</v>
       </c>
-      <c r="B86" s="151"/>
-      <c r="C86" s="152"/>
+      <c r="B86" s="153"/>
+      <c r="C86" s="154"/>
     </row>
     <row r="87" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="115">
         <v>1</v>
       </c>
-      <c r="B87" s="153" t="s">
+      <c r="B87" s="155" t="s">
         <v>101</v>
       </c>
-      <c r="C87" s="154"/>
+      <c r="C87" s="156"/>
     </row>
     <row r="88" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="124"/>
@@ -6302,10 +6302,10 @@
       <c r="A107" s="116">
         <v>2</v>
       </c>
-      <c r="B107" s="155" t="s">
+      <c r="B107" s="146" t="s">
         <v>813</v>
       </c>
-      <c r="C107" s="156"/>
+      <c r="C107" s="147"/>
     </row>
     <row r="108" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="116"/>
@@ -6383,10 +6383,10 @@
       <c r="A116" s="116">
         <v>3</v>
       </c>
-      <c r="B116" s="157" t="s">
+      <c r="B116" s="148" t="s">
         <v>814</v>
       </c>
-      <c r="C116" s="158"/>
+      <c r="C116" s="149"/>
     </row>
     <row r="117" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="116"/>
@@ -6442,10 +6442,10 @@
       <c r="A123" s="115">
         <v>4</v>
       </c>
-      <c r="B123" s="146" t="s">
+      <c r="B123" s="150" t="s">
         <v>815</v>
       </c>
-      <c r="C123" s="147"/>
+      <c r="C123" s="151"/>
     </row>
     <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="124"/>
@@ -6485,20 +6485,20 @@
     </row>
     <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="129" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="150" t="s">
+      <c r="A129" s="152" t="s">
         <v>863</v>
       </c>
-      <c r="B129" s="151"/>
-      <c r="C129" s="152"/>
+      <c r="B129" s="153"/>
+      <c r="C129" s="154"/>
     </row>
     <row r="130" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="115">
         <v>1</v>
       </c>
-      <c r="B130" s="153" t="s">
+      <c r="B130" s="155" t="s">
         <v>864</v>
       </c>
-      <c r="C130" s="154"/>
+      <c r="C130" s="156"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="124"/>
@@ -6645,10 +6645,10 @@
       <c r="A150" s="116">
         <v>2</v>
       </c>
-      <c r="B150" s="155" t="s">
+      <c r="B150" s="146" t="s">
         <v>865</v>
       </c>
-      <c r="C150" s="156"/>
+      <c r="C150" s="147"/>
     </row>
     <row r="151" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="116"/>
@@ -6718,10 +6718,10 @@
       <c r="A159" s="116">
         <v>3</v>
       </c>
-      <c r="B159" s="157" t="s">
+      <c r="B159" s="148" t="s">
         <v>866</v>
       </c>
-      <c r="C159" s="158"/>
+      <c r="C159" s="149"/>
     </row>
     <row r="160" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="116"/>
@@ -6775,12 +6775,42 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="A129:C129"/>
-    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
     <mergeCell ref="B107:C107"/>
     <mergeCell ref="B67:C67"/>
     <mergeCell ref="B68:C68"/>
@@ -6797,42 +6827,12 @@
     <mergeCell ref="B71:C71"/>
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="A129:C129"/>
+    <mergeCell ref="B130:C130"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -26472,7 +26472,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Various changes and tweaks
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716" firstSheet="12" activeTab="24"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716"/>
   </bookViews>
   <sheets>
     <sheet name="TODO - Quick Battle" sheetId="37" r:id="rId1"/>
@@ -644,7 +644,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2240" uniqueCount="1085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="1086">
   <si>
     <t>Fishing</t>
   </si>
@@ -3899,6 +3899,9 @@
   </si>
   <si>
     <t>Greater Deity</t>
+  </si>
+  <si>
+    <t>blink spell (stealth)</t>
   </si>
 </sst>
 </file>
@@ -5086,22 +5089,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5119,10 +5116,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5476,8 +5479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C165"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5492,29 +5495,29 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="152" t="s">
+      <c r="A2" s="150" t="s">
         <v>782</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="154"/>
+      <c r="B2" s="151"/>
+      <c r="C2" s="152"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="115">
         <v>1</v>
       </c>
-      <c r="B3" s="155" t="s">
+      <c r="B3" s="153" t="s">
         <v>783</v>
       </c>
-      <c r="C3" s="156"/>
+      <c r="C3" s="154"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="155" t="s">
         <v>784</v>
       </c>
-      <c r="C4" s="147"/>
+      <c r="C4" s="156"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="116"/>
@@ -5565,10 +5568,10 @@
       <c r="A10" s="116">
         <v>3</v>
       </c>
-      <c r="B10" s="148" t="s">
+      <c r="B10" s="157" t="s">
         <v>785</v>
       </c>
-      <c r="C10" s="149"/>
+      <c r="C10" s="158"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="116"/>
@@ -5583,10 +5586,10 @@
       <c r="A12" s="116">
         <v>4</v>
       </c>
-      <c r="B12" s="150" t="s">
+      <c r="B12" s="146" t="s">
         <v>786</v>
       </c>
-      <c r="C12" s="151"/>
+      <c r="C12" s="147"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="116"/>
@@ -5601,10 +5604,10 @@
       <c r="A14" s="116">
         <v>5</v>
       </c>
-      <c r="B14" s="150" t="s">
+      <c r="B14" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="C14" s="151"/>
+      <c r="C14" s="147"/>
     </row>
     <row r="15" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="116"/>
@@ -5619,10 +5622,10 @@
       <c r="A16" s="117">
         <v>6</v>
       </c>
-      <c r="B16" s="157" t="s">
+      <c r="B16" s="148" t="s">
         <v>791</v>
       </c>
-      <c r="C16" s="158"/>
+      <c r="C16" s="149"/>
     </row>
     <row r="17" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="116"/>
@@ -5637,46 +5640,46 @@
       <c r="A18" s="117">
         <v>7</v>
       </c>
-      <c r="B18" s="157" t="s">
+      <c r="B18" s="148" t="s">
         <v>913</v>
       </c>
-      <c r="C18" s="158"/>
+      <c r="C18" s="149"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="132">
         <v>8</v>
       </c>
-      <c r="B19" s="157" t="s">
+      <c r="B19" s="148" t="s">
         <v>1000</v>
       </c>
-      <c r="C19" s="158"/>
+      <c r="C19" s="149"/>
     </row>
     <row r="20" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="132">
         <v>9</v>
       </c>
-      <c r="B20" s="157" t="s">
+      <c r="B20" s="148" t="s">
         <v>914</v>
       </c>
-      <c r="C20" s="158"/>
+      <c r="C20" s="149"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="152" t="s">
+      <c r="A23" s="150" t="s">
         <v>793</v>
       </c>
-      <c r="B23" s="153"/>
-      <c r="C23" s="154"/>
+      <c r="B23" s="151"/>
+      <c r="C23" s="152"/>
     </row>
     <row r="24" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="115">
         <v>1</v>
       </c>
-      <c r="B24" s="155" t="s">
+      <c r="B24" s="153" t="s">
         <v>782</v>
       </c>
-      <c r="C24" s="156"/>
+      <c r="C24" s="154"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="116"/>
@@ -5696,10 +5699,10 @@
       <c r="A27" s="116">
         <v>2</v>
       </c>
-      <c r="B27" s="146" t="s">
+      <c r="B27" s="155" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="147"/>
+      <c r="C27" s="156"/>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="116"/>
@@ -5712,17 +5715,21 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="116"/>
-      <c r="B29" s="120"/>
-      <c r="C29" s="121"/>
+      <c r="B29" s="120" t="s">
+        <v>789</v>
+      </c>
+      <c r="C29" s="121" t="s">
+        <v>1085</v>
+      </c>
     </row>
     <row r="30" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="116">
         <v>3</v>
       </c>
-      <c r="B30" s="146" t="s">
+      <c r="B30" s="155" t="s">
         <v>1001</v>
       </c>
-      <c r="C30" s="147"/>
+      <c r="C30" s="156"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="116"/>
@@ -5744,20 +5751,20 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="152" t="s">
+      <c r="A34" s="150" t="s">
         <v>797</v>
       </c>
-      <c r="B34" s="153"/>
-      <c r="C34" s="154"/>
+      <c r="B34" s="151"/>
+      <c r="C34" s="152"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="115">
         <v>1</v>
       </c>
-      <c r="B35" s="155" t="s">
+      <c r="B35" s="153" t="s">
         <v>798</v>
       </c>
-      <c r="C35" s="156"/>
+      <c r="C35" s="154"/>
     </row>
     <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="116"/>
@@ -5797,20 +5804,20 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="152" t="s">
+      <c r="A41" s="150" t="s">
         <v>802</v>
       </c>
-      <c r="B41" s="153"/>
-      <c r="C41" s="154"/>
+      <c r="B41" s="151"/>
+      <c r="C41" s="152"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="115">
         <v>1</v>
       </c>
-      <c r="B42" s="155" t="s">
+      <c r="B42" s="153" t="s">
         <v>803</v>
       </c>
-      <c r="C42" s="156"/>
+      <c r="C42" s="154"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="116"/>
@@ -5834,10 +5841,10 @@
       <c r="A45" s="115">
         <v>1</v>
       </c>
-      <c r="B45" s="155" t="s">
+      <c r="B45" s="153" t="s">
         <v>805</v>
       </c>
-      <c r="C45" s="156"/>
+      <c r="C45" s="154"/>
     </row>
     <row r="46" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="116"/>
@@ -5873,37 +5880,37 @@
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="152" t="s">
+      <c r="A51" s="150" t="s">
         <v>188</v>
       </c>
-      <c r="B51" s="153"/>
-      <c r="C51" s="154"/>
+      <c r="B51" s="151"/>
+      <c r="C51" s="152"/>
     </row>
     <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="115">
         <v>1</v>
       </c>
-      <c r="B52" s="155" t="s">
+      <c r="B52" s="153" t="s">
         <v>810</v>
       </c>
-      <c r="C52" s="156"/>
+      <c r="C52" s="154"/>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="152" t="s">
+      <c r="A54" s="150" t="s">
         <v>790</v>
       </c>
-      <c r="B54" s="153"/>
-      <c r="C54" s="154"/>
+      <c r="B54" s="151"/>
+      <c r="C54" s="152"/>
     </row>
     <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="115">
         <v>1</v>
       </c>
-      <c r="B55" s="148" t="s">
+      <c r="B55" s="157" t="s">
         <v>783</v>
       </c>
-      <c r="C55" s="149"/>
+      <c r="C55" s="158"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="116">
@@ -5918,54 +5925,54 @@
       <c r="A57" s="116">
         <v>3</v>
       </c>
-      <c r="B57" s="150" t="s">
+      <c r="B57" s="146" t="s">
         <v>785</v>
       </c>
-      <c r="C57" s="151"/>
+      <c r="C57" s="147"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="116">
         <v>4</v>
       </c>
-      <c r="B58" s="150" t="s">
+      <c r="B58" s="146" t="s">
         <v>786</v>
       </c>
-      <c r="C58" s="151"/>
+      <c r="C58" s="147"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="116">
         <v>5</v>
       </c>
-      <c r="B59" s="150" t="s">
+      <c r="B59" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="C59" s="151"/>
+      <c r="C59" s="147"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="117">
         <v>6</v>
       </c>
-      <c r="B60" s="157" t="s">
+      <c r="B60" s="148" t="s">
         <v>791</v>
       </c>
-      <c r="C60" s="158"/>
+      <c r="C60" s="149"/>
     </row>
     <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="152" t="s">
+      <c r="A62" s="150" t="s">
         <v>811</v>
       </c>
-      <c r="B62" s="153"/>
-      <c r="C62" s="154"/>
+      <c r="B62" s="151"/>
+      <c r="C62" s="152"/>
     </row>
     <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="115">
         <v>1</v>
       </c>
-      <c r="B63" s="148" t="s">
+      <c r="B63" s="157" t="s">
         <v>783</v>
       </c>
-      <c r="C63" s="149"/>
+      <c r="C63" s="158"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="116">
@@ -5980,52 +5987,52 @@
       <c r="A65" s="116">
         <v>3</v>
       </c>
-      <c r="B65" s="150" t="s">
+      <c r="B65" s="146" t="s">
         <v>785</v>
       </c>
-      <c r="C65" s="151"/>
+      <c r="C65" s="147"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="116">
         <v>4</v>
       </c>
-      <c r="B66" s="150" t="s">
+      <c r="B66" s="146" t="s">
         <v>786</v>
       </c>
-      <c r="C66" s="151"/>
+      <c r="C66" s="147"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="116">
         <v>5</v>
       </c>
-      <c r="B67" s="150" t="s">
+      <c r="B67" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="C67" s="151"/>
+      <c r="C67" s="147"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="117">
         <v>6</v>
       </c>
-      <c r="B68" s="157" t="s">
+      <c r="B68" s="148" t="s">
         <v>791</v>
       </c>
-      <c r="C68" s="158"/>
+      <c r="C68" s="149"/>
     </row>
     <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="152" t="s">
+      <c r="A70" s="150" t="s">
         <v>1001</v>
       </c>
-      <c r="B70" s="153"/>
-      <c r="C70" s="154"/>
+      <c r="B70" s="151"/>
+      <c r="C70" s="152"/>
     </row>
     <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="115">
         <v>1</v>
       </c>
-      <c r="B71" s="148"/>
-      <c r="C71" s="149"/>
+      <c r="B71" s="157"/>
+      <c r="C71" s="158"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="116"/>
@@ -6034,40 +6041,40 @@
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="116"/>
-      <c r="B73" s="150"/>
-      <c r="C73" s="151"/>
+      <c r="B73" s="146"/>
+      <c r="C73" s="147"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="116"/>
-      <c r="B74" s="150"/>
-      <c r="C74" s="151"/>
+      <c r="B74" s="146"/>
+      <c r="C74" s="147"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="116"/>
-      <c r="B75" s="150"/>
-      <c r="C75" s="151"/>
+      <c r="B75" s="146"/>
+      <c r="C75" s="147"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="117"/>
-      <c r="B76" s="157"/>
-      <c r="C76" s="158"/>
+      <c r="B76" s="148"/>
+      <c r="C76" s="149"/>
     </row>
     <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="152" t="s">
+      <c r="A78" s="150" t="s">
         <v>812</v>
       </c>
-      <c r="B78" s="153"/>
-      <c r="C78" s="154"/>
+      <c r="B78" s="151"/>
+      <c r="C78" s="152"/>
     </row>
     <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="115">
         <v>1</v>
       </c>
-      <c r="B79" s="148" t="s">
+      <c r="B79" s="157" t="s">
         <v>783</v>
       </c>
-      <c r="C79" s="149"/>
+      <c r="C79" s="158"/>
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="116">
@@ -6082,54 +6089,54 @@
       <c r="A81" s="116">
         <v>3</v>
       </c>
-      <c r="B81" s="150" t="s">
+      <c r="B81" s="146" t="s">
         <v>785</v>
       </c>
-      <c r="C81" s="151"/>
+      <c r="C81" s="147"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="116">
         <v>4</v>
       </c>
-      <c r="B82" s="150" t="s">
+      <c r="B82" s="146" t="s">
         <v>786</v>
       </c>
-      <c r="C82" s="151"/>
+      <c r="C82" s="147"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="116">
         <v>5</v>
       </c>
-      <c r="B83" s="150" t="s">
+      <c r="B83" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="C83" s="151"/>
+      <c r="C83" s="147"/>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="117">
         <v>6</v>
       </c>
-      <c r="B84" s="157" t="s">
+      <c r="B84" s="148" t="s">
         <v>791</v>
       </c>
-      <c r="C84" s="158"/>
+      <c r="C84" s="149"/>
     </row>
     <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="152" t="s">
+      <c r="A86" s="150" t="s">
         <v>862</v>
       </c>
-      <c r="B86" s="153"/>
-      <c r="C86" s="154"/>
+      <c r="B86" s="151"/>
+      <c r="C86" s="152"/>
     </row>
     <row r="87" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="115">
         <v>1</v>
       </c>
-      <c r="B87" s="155" t="s">
+      <c r="B87" s="153" t="s">
         <v>101</v>
       </c>
-      <c r="C87" s="156"/>
+      <c r="C87" s="154"/>
     </row>
     <row r="88" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="124"/>
@@ -6302,10 +6309,10 @@
       <c r="A107" s="116">
         <v>2</v>
       </c>
-      <c r="B107" s="146" t="s">
+      <c r="B107" s="155" t="s">
         <v>813</v>
       </c>
-      <c r="C107" s="147"/>
+      <c r="C107" s="156"/>
     </row>
     <row r="108" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="116"/>
@@ -6383,10 +6390,10 @@
       <c r="A116" s="116">
         <v>3</v>
       </c>
-      <c r="B116" s="148" t="s">
+      <c r="B116" s="157" t="s">
         <v>814</v>
       </c>
-      <c r="C116" s="149"/>
+      <c r="C116" s="158"/>
     </row>
     <row r="117" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="116"/>
@@ -6442,10 +6449,10 @@
       <c r="A123" s="115">
         <v>4</v>
       </c>
-      <c r="B123" s="150" t="s">
+      <c r="B123" s="146" t="s">
         <v>815</v>
       </c>
-      <c r="C123" s="151"/>
+      <c r="C123" s="147"/>
     </row>
     <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="124"/>
@@ -6485,20 +6492,20 @@
     </row>
     <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="129" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="152" t="s">
+      <c r="A129" s="150" t="s">
         <v>863</v>
       </c>
-      <c r="B129" s="153"/>
-      <c r="C129" s="154"/>
+      <c r="B129" s="151"/>
+      <c r="C129" s="152"/>
     </row>
     <row r="130" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="115">
         <v>1</v>
       </c>
-      <c r="B130" s="155" t="s">
+      <c r="B130" s="153" t="s">
         <v>864</v>
       </c>
-      <c r="C130" s="156"/>
+      <c r="C130" s="154"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="124"/>
@@ -6645,10 +6652,10 @@
       <c r="A150" s="116">
         <v>2</v>
       </c>
-      <c r="B150" s="146" t="s">
+      <c r="B150" s="155" t="s">
         <v>865</v>
       </c>
-      <c r="C150" s="147"/>
+      <c r="C150" s="156"/>
     </row>
     <row r="151" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="116"/>
@@ -6718,10 +6725,10 @@
       <c r="A159" s="116">
         <v>3</v>
       </c>
-      <c r="B159" s="148" t="s">
+      <c r="B159" s="157" t="s">
         <v>866</v>
       </c>
-      <c r="C159" s="149"/>
+      <c r="C159" s="158"/>
     </row>
     <row r="160" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="116"/>
@@ -6775,6 +6782,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="A129:C129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B42:C42"/>
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
@@ -6791,48 +6840,6 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="A129:C129"/>
-    <mergeCell ref="B130:C130"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -26471,7 +26478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Combining wpn and ability buttons
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -644,7 +644,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="1086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2240" uniqueCount="1085">
   <si>
     <t>Fishing</t>
   </si>
@@ -3047,9 +3047,6 @@
   </si>
   <si>
     <t>Tropical</t>
-  </si>
-  <si>
-    <t>Lava</t>
   </si>
   <si>
     <t>Combat Map</t>
@@ -5089,16 +5086,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5116,16 +5119,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5479,8 +5476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57:C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5495,29 +5492,29 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="152" t="s">
         <v>782</v>
       </c>
-      <c r="B2" s="151"/>
-      <c r="C2" s="152"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="154"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="115">
         <v>1</v>
       </c>
-      <c r="B3" s="153" t="s">
+      <c r="B3" s="155" t="s">
         <v>783</v>
       </c>
-      <c r="C3" s="154"/>
+      <c r="C3" s="156"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="146" t="s">
         <v>784</v>
       </c>
-      <c r="C4" s="156"/>
+      <c r="C4" s="147"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="116"/>
@@ -5552,7 +5549,7 @@
         <v>794</v>
       </c>
       <c r="C8" s="123" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="9" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
@@ -5568,10 +5565,10 @@
       <c r="A10" s="116">
         <v>3</v>
       </c>
-      <c r="B10" s="157" t="s">
+      <c r="B10" s="148" t="s">
         <v>785</v>
       </c>
-      <c r="C10" s="158"/>
+      <c r="C10" s="149"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="116"/>
@@ -5579,17 +5576,17 @@
         <v>788</v>
       </c>
       <c r="C11" s="119" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="12" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="116">
         <v>4</v>
       </c>
-      <c r="B12" s="146" t="s">
+      <c r="B12" s="150" t="s">
         <v>786</v>
       </c>
-      <c r="C12" s="147"/>
+      <c r="C12" s="151"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="116"/>
@@ -5597,17 +5594,17 @@
         <v>788</v>
       </c>
       <c r="C13" s="119" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="14" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="116">
         <v>5</v>
       </c>
-      <c r="B14" s="146" t="s">
+      <c r="B14" s="150" t="s">
         <v>787</v>
       </c>
-      <c r="C14" s="147"/>
+      <c r="C14" s="151"/>
     </row>
     <row r="15" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="116"/>
@@ -5615,17 +5612,17 @@
         <v>788</v>
       </c>
       <c r="C15" s="119" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="16" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="117">
         <v>6</v>
       </c>
-      <c r="B16" s="148" t="s">
+      <c r="B16" s="157" t="s">
         <v>791</v>
       </c>
-      <c r="C16" s="149"/>
+      <c r="C16" s="158"/>
     </row>
     <row r="17" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="116"/>
@@ -5633,53 +5630,53 @@
         <v>788</v>
       </c>
       <c r="C17" s="119" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="18" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="117">
         <v>7</v>
       </c>
-      <c r="B18" s="148" t="s">
-        <v>913</v>
-      </c>
-      <c r="C18" s="149"/>
+      <c r="B18" s="157" t="s">
+        <v>912</v>
+      </c>
+      <c r="C18" s="158"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="132">
         <v>8</v>
       </c>
-      <c r="B19" s="148" t="s">
-        <v>1000</v>
-      </c>
-      <c r="C19" s="149"/>
+      <c r="B19" s="157" t="s">
+        <v>999</v>
+      </c>
+      <c r="C19" s="158"/>
     </row>
     <row r="20" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="132">
         <v>9</v>
       </c>
-      <c r="B20" s="148" t="s">
-        <v>914</v>
-      </c>
-      <c r="C20" s="149"/>
+      <c r="B20" s="157" t="s">
+        <v>913</v>
+      </c>
+      <c r="C20" s="158"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="150" t="s">
+      <c r="A23" s="152" t="s">
         <v>793</v>
       </c>
-      <c r="B23" s="151"/>
-      <c r="C23" s="152"/>
+      <c r="B23" s="153"/>
+      <c r="C23" s="154"/>
     </row>
     <row r="24" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="115">
         <v>1</v>
       </c>
-      <c r="B24" s="153" t="s">
+      <c r="B24" s="155" t="s">
         <v>782</v>
       </c>
-      <c r="C24" s="154"/>
+      <c r="C24" s="156"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="116"/>
@@ -5692,17 +5689,17 @@
         <v>789</v>
       </c>
       <c r="C26" s="141" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="116">
         <v>2</v>
       </c>
-      <c r="B27" s="155" t="s">
+      <c r="B27" s="146" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="156"/>
+      <c r="C27" s="147"/>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="116"/>
@@ -5719,17 +5716,17 @@
         <v>789</v>
       </c>
       <c r="C29" s="121" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="116">
         <v>3</v>
       </c>
-      <c r="B30" s="155" t="s">
-        <v>1001</v>
-      </c>
-      <c r="C30" s="156"/>
+      <c r="B30" s="146" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C30" s="147"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="116"/>
@@ -5737,7 +5734,7 @@
         <v>788</v>
       </c>
       <c r="C31" s="143" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5746,25 +5743,25 @@
         <v>789</v>
       </c>
       <c r="C32" s="145" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="150" t="s">
+      <c r="A34" s="152" t="s">
         <v>797</v>
       </c>
-      <c r="B34" s="151"/>
-      <c r="C34" s="152"/>
+      <c r="B34" s="153"/>
+      <c r="C34" s="154"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="115">
         <v>1</v>
       </c>
-      <c r="B35" s="153" t="s">
+      <c r="B35" s="155" t="s">
         <v>798</v>
       </c>
-      <c r="C35" s="154"/>
+      <c r="C35" s="156"/>
     </row>
     <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="116"/>
@@ -5795,29 +5792,25 @@
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="116"/>
-      <c r="B39" s="120" t="s">
-        <v>794</v>
-      </c>
-      <c r="C39" s="121" t="s">
-        <v>801</v>
-      </c>
+      <c r="B39" s="120"/>
+      <c r="C39" s="121"/>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="150" t="s">
-        <v>802</v>
-      </c>
-      <c r="B41" s="151"/>
-      <c r="C41" s="152"/>
+      <c r="A41" s="152" t="s">
+        <v>801</v>
+      </c>
+      <c r="B41" s="153"/>
+      <c r="C41" s="154"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="115">
         <v>1</v>
       </c>
-      <c r="B42" s="153" t="s">
-        <v>803</v>
-      </c>
-      <c r="C42" s="154"/>
+      <c r="B42" s="155" t="s">
+        <v>802</v>
+      </c>
+      <c r="C42" s="156"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="116"/>
@@ -5825,7 +5818,7 @@
         <v>788</v>
       </c>
       <c r="C43" s="119" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5834,17 +5827,17 @@
         <v>789</v>
       </c>
       <c r="C44" s="121" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="115">
         <v>1</v>
       </c>
-      <c r="B45" s="153" t="s">
-        <v>805</v>
-      </c>
-      <c r="C45" s="154"/>
+      <c r="B45" s="155" t="s">
+        <v>804</v>
+      </c>
+      <c r="C45" s="156"/>
     </row>
     <row r="46" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="116"/>
@@ -5852,7 +5845,7 @@
         <v>788</v>
       </c>
       <c r="C46" s="119" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5861,7 +5854,7 @@
         <v>789</v>
       </c>
       <c r="C47" s="123" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5870,7 +5863,7 @@
         <v>792</v>
       </c>
       <c r="C48" s="123" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5880,37 +5873,37 @@
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="150" t="s">
+      <c r="A51" s="152" t="s">
         <v>188</v>
       </c>
-      <c r="B51" s="151"/>
-      <c r="C51" s="152"/>
+      <c r="B51" s="153"/>
+      <c r="C51" s="154"/>
     </row>
     <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="115">
         <v>1</v>
       </c>
-      <c r="B52" s="153" t="s">
-        <v>810</v>
-      </c>
-      <c r="C52" s="154"/>
+      <c r="B52" s="155" t="s">
+        <v>809</v>
+      </c>
+      <c r="C52" s="156"/>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="150" t="s">
+      <c r="A54" s="152" t="s">
         <v>790</v>
       </c>
-      <c r="B54" s="151"/>
-      <c r="C54" s="152"/>
+      <c r="B54" s="153"/>
+      <c r="C54" s="154"/>
     </row>
     <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="115">
         <v>1</v>
       </c>
-      <c r="B55" s="157" t="s">
+      <c r="B55" s="148" t="s">
         <v>783</v>
       </c>
-      <c r="C55" s="158"/>
+      <c r="C55" s="149"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="116">
@@ -5925,54 +5918,54 @@
       <c r="A57" s="116">
         <v>3</v>
       </c>
-      <c r="B57" s="146" t="s">
+      <c r="B57" s="150" t="s">
         <v>785</v>
       </c>
-      <c r="C57" s="147"/>
+      <c r="C57" s="151"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="116">
         <v>4</v>
       </c>
-      <c r="B58" s="146" t="s">
+      <c r="B58" s="150" t="s">
         <v>786</v>
       </c>
-      <c r="C58" s="147"/>
+      <c r="C58" s="151"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="116">
         <v>5</v>
       </c>
-      <c r="B59" s="146" t="s">
+      <c r="B59" s="150" t="s">
         <v>787</v>
       </c>
-      <c r="C59" s="147"/>
+      <c r="C59" s="151"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="117">
         <v>6</v>
       </c>
-      <c r="B60" s="148" t="s">
+      <c r="B60" s="157" t="s">
         <v>791</v>
       </c>
-      <c r="C60" s="149"/>
+      <c r="C60" s="158"/>
     </row>
     <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="150" t="s">
-        <v>811</v>
-      </c>
-      <c r="B62" s="151"/>
-      <c r="C62" s="152"/>
+      <c r="A62" s="152" t="s">
+        <v>810</v>
+      </c>
+      <c r="B62" s="153"/>
+      <c r="C62" s="154"/>
     </row>
     <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="115">
         <v>1</v>
       </c>
-      <c r="B63" s="157" t="s">
+      <c r="B63" s="148" t="s">
         <v>783</v>
       </c>
-      <c r="C63" s="158"/>
+      <c r="C63" s="149"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="116">
@@ -5987,52 +5980,52 @@
       <c r="A65" s="116">
         <v>3</v>
       </c>
-      <c r="B65" s="146" t="s">
+      <c r="B65" s="150" t="s">
         <v>785</v>
       </c>
-      <c r="C65" s="147"/>
+      <c r="C65" s="151"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="116">
         <v>4</v>
       </c>
-      <c r="B66" s="146" t="s">
+      <c r="B66" s="150" t="s">
         <v>786</v>
       </c>
-      <c r="C66" s="147"/>
+      <c r="C66" s="151"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="116">
         <v>5</v>
       </c>
-      <c r="B67" s="146" t="s">
+      <c r="B67" s="150" t="s">
         <v>787</v>
       </c>
-      <c r="C67" s="147"/>
+      <c r="C67" s="151"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="117">
         <v>6</v>
       </c>
-      <c r="B68" s="148" t="s">
+      <c r="B68" s="157" t="s">
         <v>791</v>
       </c>
-      <c r="C68" s="149"/>
+      <c r="C68" s="158"/>
     </row>
     <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="150" t="s">
-        <v>1001</v>
-      </c>
-      <c r="B70" s="151"/>
-      <c r="C70" s="152"/>
+      <c r="A70" s="152" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B70" s="153"/>
+      <c r="C70" s="154"/>
     </row>
     <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="115">
         <v>1</v>
       </c>
-      <c r="B71" s="157"/>
-      <c r="C71" s="158"/>
+      <c r="B71" s="148"/>
+      <c r="C71" s="149"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="116"/>
@@ -6041,40 +6034,40 @@
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="116"/>
-      <c r="B73" s="146"/>
-      <c r="C73" s="147"/>
+      <c r="B73" s="150"/>
+      <c r="C73" s="151"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="116"/>
-      <c r="B74" s="146"/>
-      <c r="C74" s="147"/>
+      <c r="B74" s="150"/>
+      <c r="C74" s="151"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="116"/>
-      <c r="B75" s="146"/>
-      <c r="C75" s="147"/>
+      <c r="B75" s="150"/>
+      <c r="C75" s="151"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="117"/>
-      <c r="B76" s="148"/>
-      <c r="C76" s="149"/>
+      <c r="B76" s="157"/>
+      <c r="C76" s="158"/>
     </row>
     <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="150" t="s">
-        <v>812</v>
-      </c>
-      <c r="B78" s="151"/>
-      <c r="C78" s="152"/>
+      <c r="A78" s="152" t="s">
+        <v>811</v>
+      </c>
+      <c r="B78" s="153"/>
+      <c r="C78" s="154"/>
     </row>
     <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="115">
         <v>1</v>
       </c>
-      <c r="B79" s="157" t="s">
+      <c r="B79" s="148" t="s">
         <v>783</v>
       </c>
-      <c r="C79" s="158"/>
+      <c r="C79" s="149"/>
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="116">
@@ -6089,54 +6082,54 @@
       <c r="A81" s="116">
         <v>3</v>
       </c>
-      <c r="B81" s="146" t="s">
+      <c r="B81" s="150" t="s">
         <v>785</v>
       </c>
-      <c r="C81" s="147"/>
+      <c r="C81" s="151"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="116">
         <v>4</v>
       </c>
-      <c r="B82" s="146" t="s">
+      <c r="B82" s="150" t="s">
         <v>786</v>
       </c>
-      <c r="C82" s="147"/>
+      <c r="C82" s="151"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="116">
         <v>5</v>
       </c>
-      <c r="B83" s="146" t="s">
+      <c r="B83" s="150" t="s">
         <v>787</v>
       </c>
-      <c r="C83" s="147"/>
+      <c r="C83" s="151"/>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="117">
         <v>6</v>
       </c>
-      <c r="B84" s="148" t="s">
+      <c r="B84" s="157" t="s">
         <v>791</v>
       </c>
-      <c r="C84" s="149"/>
+      <c r="C84" s="158"/>
     </row>
     <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="150" t="s">
-        <v>862</v>
-      </c>
-      <c r="B86" s="151"/>
-      <c r="C86" s="152"/>
+      <c r="A86" s="152" t="s">
+        <v>861</v>
+      </c>
+      <c r="B86" s="153"/>
+      <c r="C86" s="154"/>
     </row>
     <row r="87" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="115">
         <v>1</v>
       </c>
-      <c r="B87" s="153" t="s">
+      <c r="B87" s="155" t="s">
         <v>101</v>
       </c>
-      <c r="C87" s="154"/>
+      <c r="C87" s="156"/>
     </row>
     <row r="88" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="124"/>
@@ -6144,7 +6137,7 @@
         <v>788</v>
       </c>
       <c r="C88" s="119" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6153,7 +6146,7 @@
         <v>789</v>
       </c>
       <c r="C89" s="128" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6162,7 +6155,7 @@
         <v>792</v>
       </c>
       <c r="C90" s="128" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6171,7 +6164,7 @@
         <v>794</v>
       </c>
       <c r="C91" s="128" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6180,103 +6173,103 @@
         <v>795</v>
       </c>
       <c r="C92" s="128" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="124"/>
       <c r="B93" s="127" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C93" s="128" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="124"/>
       <c r="B94" s="127" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C94" s="128" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="124"/>
       <c r="B95" s="127" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C95" s="128" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="124"/>
       <c r="B96" s="127" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C96" s="128" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="116"/>
       <c r="B97" s="122" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C97" s="123" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="116"/>
       <c r="B98" s="122" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C98" s="123" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="116"/>
       <c r="B99" s="122" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C99" s="123" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="116"/>
       <c r="B100" s="122" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C100" s="123" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="116"/>
       <c r="B101" s="122" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C101" s="123" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="116"/>
       <c r="B102" s="122" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C102" s="123" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="116"/>
       <c r="B103" s="122" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C103" s="123" t="s">
         <v>35</v>
@@ -6285,23 +6278,23 @@
     <row r="104" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="116"/>
       <c r="B104" s="122" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C104" s="123" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="116"/>
       <c r="B105" s="122" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C105" s="123"/>
     </row>
     <row r="106" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="116"/>
       <c r="B106" s="120" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C106" s="121"/>
     </row>
@@ -6309,10 +6302,10 @@
       <c r="A107" s="116">
         <v>2</v>
       </c>
-      <c r="B107" s="155" t="s">
-        <v>813</v>
-      </c>
-      <c r="C107" s="156"/>
+      <c r="B107" s="146" t="s">
+        <v>812</v>
+      </c>
+      <c r="C107" s="147"/>
     </row>
     <row r="108" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="116"/>
@@ -6320,7 +6313,7 @@
         <v>788</v>
       </c>
       <c r="C108" s="119" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6329,7 +6322,7 @@
         <v>789</v>
       </c>
       <c r="C109" s="123" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6338,7 +6331,7 @@
         <v>792</v>
       </c>
       <c r="C110" s="123" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6347,7 +6340,7 @@
         <v>794</v>
       </c>
       <c r="C111" s="123" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6356,44 +6349,44 @@
         <v>795</v>
       </c>
       <c r="C112" s="123" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="116"/>
       <c r="B113" s="125" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C113" s="126" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="116"/>
       <c r="B114" s="125" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C114" s="126" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="116"/>
       <c r="B115" s="120" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C115" s="121" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="116">
         <v>3</v>
       </c>
-      <c r="B116" s="157" t="s">
-        <v>814</v>
-      </c>
-      <c r="C116" s="158"/>
+      <c r="B116" s="148" t="s">
+        <v>813</v>
+      </c>
+      <c r="C116" s="149"/>
     </row>
     <row r="117" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="116"/>
@@ -6401,7 +6394,7 @@
         <v>788</v>
       </c>
       <c r="C117" s="119" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6410,7 +6403,7 @@
         <v>789</v>
       </c>
       <c r="C118" s="123" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6428,7 +6421,7 @@
         <v>794</v>
       </c>
       <c r="C120" s="126" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6437,7 +6430,7 @@
         <v>795</v>
       </c>
       <c r="C121" s="126" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6449,10 +6442,10 @@
       <c r="A123" s="115">
         <v>4</v>
       </c>
-      <c r="B123" s="146" t="s">
-        <v>815</v>
-      </c>
-      <c r="C123" s="147"/>
+      <c r="B123" s="150" t="s">
+        <v>814</v>
+      </c>
+      <c r="C123" s="151"/>
     </row>
     <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="124"/>
@@ -6460,7 +6453,7 @@
         <v>788</v>
       </c>
       <c r="C124" s="119" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6469,7 +6462,7 @@
         <v>789</v>
       </c>
       <c r="C125" s="123" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6478,7 +6471,7 @@
         <v>792</v>
       </c>
       <c r="C126" s="123" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6487,25 +6480,25 @@
         <v>794</v>
       </c>
       <c r="C127" s="121" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="129" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="150" t="s">
-        <v>863</v>
-      </c>
-      <c r="B129" s="151"/>
-      <c r="C129" s="152"/>
+      <c r="A129" s="152" t="s">
+        <v>862</v>
+      </c>
+      <c r="B129" s="153"/>
+      <c r="C129" s="154"/>
     </row>
     <row r="130" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="115">
         <v>1</v>
       </c>
-      <c r="B130" s="153" t="s">
-        <v>864</v>
-      </c>
-      <c r="C130" s="154"/>
+      <c r="B130" s="155" t="s">
+        <v>863</v>
+      </c>
+      <c r="C130" s="156"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="124"/>
@@ -6522,7 +6515,7 @@
         <v>789</v>
       </c>
       <c r="C132" s="128" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6531,7 +6524,7 @@
         <v>792</v>
       </c>
       <c r="C133" s="128" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6540,7 +6533,7 @@
         <v>794</v>
       </c>
       <c r="C134" s="128" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6553,98 +6546,98 @@
     <row r="136" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="124"/>
       <c r="B136" s="127" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C136" s="128"/>
     </row>
     <row r="137" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="124"/>
       <c r="B137" s="127" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C137" s="128"/>
     </row>
     <row r="138" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="124"/>
       <c r="B138" s="127" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C138" s="128"/>
     </row>
     <row r="139" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="124"/>
       <c r="B139" s="127" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C139" s="128"/>
     </row>
     <row r="140" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="116"/>
       <c r="B140" s="122" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C140" s="123"/>
     </row>
     <row r="141" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="116"/>
       <c r="B141" s="122" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C141" s="123"/>
     </row>
     <row r="142" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="116"/>
       <c r="B142" s="122" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C142" s="123"/>
     </row>
     <row r="143" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="116"/>
       <c r="B143" s="122" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C143" s="123"/>
     </row>
     <row r="144" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="116"/>
       <c r="B144" s="122" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C144" s="123"/>
     </row>
     <row r="145" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="116"/>
       <c r="B145" s="122" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C145" s="123"/>
     </row>
     <row r="146" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="116"/>
       <c r="B146" s="122" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C146" s="123"/>
     </row>
     <row r="147" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="116"/>
       <c r="B147" s="122" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C147" s="123"/>
     </row>
     <row r="148" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="116"/>
       <c r="B148" s="122" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C148" s="123"/>
     </row>
     <row r="149" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="116"/>
       <c r="B149" s="120" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C149" s="121"/>
     </row>
@@ -6652,10 +6645,10 @@
       <c r="A150" s="116">
         <v>2</v>
       </c>
-      <c r="B150" s="155" t="s">
-        <v>865</v>
-      </c>
-      <c r="C150" s="156"/>
+      <c r="B150" s="146" t="s">
+        <v>864</v>
+      </c>
+      <c r="C150" s="147"/>
     </row>
     <row r="151" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="116"/>
@@ -6672,7 +6665,7 @@
         <v>789</v>
       </c>
       <c r="C152" s="123" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6681,7 +6674,7 @@
         <v>792</v>
       </c>
       <c r="C153" s="123" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6690,7 +6683,7 @@
         <v>794</v>
       </c>
       <c r="C154" s="123" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6703,21 +6696,21 @@
     <row r="156" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="116"/>
       <c r="B156" s="125" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C156" s="126"/>
     </row>
     <row r="157" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="116"/>
       <c r="B157" s="125" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C157" s="126"/>
     </row>
     <row r="158" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="116"/>
       <c r="B158" s="120" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C158" s="121"/>
     </row>
@@ -6725,10 +6718,10 @@
       <c r="A159" s="116">
         <v>3</v>
       </c>
-      <c r="B159" s="157" t="s">
-        <v>866</v>
-      </c>
-      <c r="C159" s="158"/>
+      <c r="B159" s="148" t="s">
+        <v>865</v>
+      </c>
+      <c r="C159" s="149"/>
     </row>
     <row r="160" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="116"/>
@@ -6736,7 +6729,7 @@
         <v>788</v>
       </c>
       <c r="C160" s="119" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6745,7 +6738,7 @@
         <v>789</v>
       </c>
       <c r="C161" s="123" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6754,7 +6747,7 @@
         <v>792</v>
       </c>
       <c r="C162" s="123" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6763,7 +6756,7 @@
         <v>794</v>
       </c>
       <c r="C163" s="126" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6776,18 +6769,48 @@
     <row r="165" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="116"/>
       <c r="B165" s="120" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C165" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="A129:C129"/>
-    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
     <mergeCell ref="B107:C107"/>
     <mergeCell ref="B67:C67"/>
     <mergeCell ref="B68:C68"/>
@@ -6804,42 +6827,12 @@
     <mergeCell ref="B71:C71"/>
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="A129:C129"/>
+    <mergeCell ref="B130:C130"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -13139,7 +13132,7 @@
         <v>658</v>
       </c>
       <c r="X54" s="44" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
@@ -13209,7 +13202,7 @@
         <v>658</v>
       </c>
       <c r="X55" s="44" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
@@ -13279,7 +13272,7 @@
         <v>658</v>
       </c>
       <c r="X56" s="44" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
@@ -13349,7 +13342,7 @@
         <v>658</v>
       </c>
       <c r="X57" s="44" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
@@ -13419,7 +13412,7 @@
         <v>658</v>
       </c>
       <c r="X58" s="44" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
@@ -22502,10 +22495,10 @@
     </row>
     <row r="16" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="83" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C16" s="43"/>
       <c r="D16" s="43"/>
@@ -22516,7 +22509,7 @@
       <c r="I16" s="43"/>
       <c r="J16" s="44"/>
       <c r="K16" s="89" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="L16" s="87"/>
     </row>
@@ -22784,7 +22777,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="83" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B30" s="48"/>
       <c r="C30" s="43"/>
@@ -22796,7 +22789,7 @@
       <c r="I30" s="43"/>
       <c r="J30" s="44"/>
       <c r="K30" s="89" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="L30" s="87">
         <v>3</v>
@@ -22884,7 +22877,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="83" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="43"/>
@@ -22896,13 +22889,13 @@
       <c r="I35" s="43"/>
       <c r="J35" s="44"/>
       <c r="K35" s="89" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="L35" s="87"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="83" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="43"/>
@@ -22914,7 +22907,7 @@
       <c r="I36" s="43"/>
       <c r="J36" s="44"/>
       <c r="K36" s="89" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="L36" s="87"/>
     </row>
@@ -22958,10 +22951,10 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="83" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B39" s="48" t="s">
         <v>1030</v>
-      </c>
-      <c r="B39" s="48" t="s">
-        <v>1031</v>
       </c>
       <c r="C39" s="43" t="s">
         <v>745</v>
@@ -22974,7 +22967,7 @@
       <c r="I39" s="43"/>
       <c r="J39" s="44"/>
       <c r="K39" s="89" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="L39" s="87"/>
     </row>
@@ -23074,7 +23067,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="83" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B45" s="48"/>
       <c r="C45" s="43"/>
@@ -23092,7 +23085,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="83" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B46" s="48"/>
       <c r="C46" s="43"/>
@@ -23104,7 +23097,7 @@
       <c r="I46" s="43"/>
       <c r="J46" s="44"/>
       <c r="K46" s="89" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="L46" s="87">
         <v>3</v>
@@ -23112,10 +23105,10 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="83" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B47" s="48" t="s">
         <v>1028</v>
-      </c>
-      <c r="B47" s="48" t="s">
-        <v>1029</v>
       </c>
       <c r="C47" s="43" t="s">
         <v>745</v>
@@ -23128,7 +23121,7 @@
       <c r="I47" s="43"/>
       <c r="J47" s="44"/>
       <c r="K47" s="89" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="L47" s="87"/>
     </row>
@@ -23792,7 +23785,7 @@
       <c r="I81" s="43"/>
       <c r="J81" s="44"/>
       <c r="K81" s="89" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="L81" s="87"/>
     </row>
@@ -24150,7 +24143,7 @@
         <v>372</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F3" s="129"/>
       <c r="G3" s="31"/>
@@ -24177,7 +24170,7 @@
         <v>382</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="F4" s="129"/>
       <c r="G4" s="31"/>
@@ -24268,7 +24261,7 @@
         <v>492</v>
       </c>
       <c r="E8" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F8" s="133" t="s">
         <v>745</v>
@@ -24676,7 +24669,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="129" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B28" s="129" t="s">
         <v>582</v>
@@ -24685,12 +24678,12 @@
         <v>488</v>
       </c>
       <c r="M28" s="129" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="129" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B29" s="129" t="s">
         <v>582</v>
@@ -24700,7 +24693,7 @@
       </c>
       <c r="L29" s="32"/>
       <c r="M29" s="129" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="N29"/>
     </row>
@@ -24715,22 +24708,22 @@
         <v>488</v>
       </c>
       <c r="M30" s="129" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="129" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="129" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="129" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B33" s="129" t="s">
         <v>582</v>
@@ -24739,15 +24732,15 @@
         <v>488</v>
       </c>
       <c r="E33" s="129" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="M33" s="129" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="129" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B34" s="129" t="s">
         <v>374</v>
@@ -24756,10 +24749,10 @@
         <v>488</v>
       </c>
       <c r="E34" s="129" t="s">
+        <v>890</v>
+      </c>
+      <c r="M34" s="129" t="s">
         <v>891</v>
-      </c>
-      <c r="M34" s="129" t="s">
-        <v>892</v>
       </c>
       <c r="N34" s="34">
         <v>5</v>
@@ -24767,7 +24760,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="129" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B35" s="129" t="s">
         <v>374</v>
@@ -24776,15 +24769,15 @@
         <v>488</v>
       </c>
       <c r="E35" s="129" t="s">
+        <v>893</v>
+      </c>
+      <c r="M35" s="129" t="s">
         <v>894</v>
-      </c>
-      <c r="M35" s="129" t="s">
-        <v>895</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="129" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B36" s="129" t="s">
         <v>374</v>
@@ -24793,15 +24786,15 @@
         <v>488</v>
       </c>
       <c r="E36" s="129" t="s">
+        <v>896</v>
+      </c>
+      <c r="M36" s="129" t="s">
         <v>897</v>
-      </c>
-      <c r="M36" s="129" t="s">
-        <v>898</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="129" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B37" s="129" t="s">
         <v>374</v>
@@ -24810,15 +24803,15 @@
         <v>488</v>
       </c>
       <c r="E37" s="129" t="s">
+        <v>899</v>
+      </c>
+      <c r="M37" s="129" t="s">
         <v>900</v>
-      </c>
-      <c r="M37" s="129" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="129" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B38" s="129" t="s">
         <v>374</v>
@@ -24827,10 +24820,10 @@
         <v>488</v>
       </c>
       <c r="E38" s="129" t="s">
+        <v>902</v>
+      </c>
+      <c r="M38" s="129" t="s">
         <v>903</v>
-      </c>
-      <c r="M38" s="129" t="s">
-        <v>904</v>
       </c>
       <c r="N38" s="34">
         <v>5</v>
@@ -24847,12 +24840,12 @@
         <v>488</v>
       </c>
       <c r="M39" s="130" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="130" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B40" s="130" t="s">
         <v>582</v>
@@ -24861,41 +24854,41 @@
         <v>488</v>
       </c>
       <c r="M40" s="130" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="130" t="s">
+        <v>921</v>
+      </c>
+      <c r="B41" s="130" t="s">
         <v>922</v>
-      </c>
-      <c r="B41" s="130" t="s">
-        <v>923</v>
       </c>
       <c r="D41" s="130" t="s">
         <v>488</v>
       </c>
       <c r="E41" s="130" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="M41" s="130" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="130" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B42" s="130" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D42" s="130" t="s">
         <v>488</v>
       </c>
       <c r="E42" s="130" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="M42" s="130" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="N42" s="34">
         <v>3</v>
@@ -24903,7 +24896,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="131" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B43" s="131" t="s">
         <v>374</v>
@@ -24912,10 +24905,10 @@
         <v>488</v>
       </c>
       <c r="E43" s="131" t="s">
+        <v>929</v>
+      </c>
+      <c r="M43" s="131" t="s">
         <v>930</v>
-      </c>
-      <c r="M43" s="131" t="s">
-        <v>931</v>
       </c>
       <c r="N43" s="34">
         <v>3</v>
@@ -24923,7 +24916,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="131" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B44" s="131" t="s">
         <v>374</v>
@@ -24932,10 +24925,10 @@
         <v>488</v>
       </c>
       <c r="E44" s="131" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="M44" s="131" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="N44" s="34">
         <v>3</v>
@@ -24943,7 +24936,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="131" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B45" s="131" t="s">
         <v>374</v>
@@ -24952,10 +24945,10 @@
         <v>488</v>
       </c>
       <c r="E45" s="131" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="M45" s="131" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="N45" s="34">
         <v>3</v>
@@ -24963,7 +24956,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="133" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B46" s="133" t="s">
         <v>374</v>
@@ -24972,10 +24965,10 @@
         <v>422</v>
       </c>
       <c r="E46" s="133" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="M46" s="133" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="N46" s="34">
         <v>3</v>
@@ -24983,7 +24976,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="134" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B47" s="134" t="s">
         <v>375</v>
@@ -24992,16 +24985,16 @@
         <v>492</v>
       </c>
       <c r="E47" s="134" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F47" s="134" t="s">
         <v>745</v>
       </c>
       <c r="G47" s="134" t="s">
+        <v>942</v>
+      </c>
+      <c r="M47" s="134" t="s">
         <v>943</v>
-      </c>
-      <c r="M47" s="134" t="s">
-        <v>944</v>
       </c>
       <c r="N47" s="34">
         <v>3</v>
@@ -25009,7 +25002,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="134" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B48" s="134" t="s">
         <v>375</v>
@@ -25018,30 +25011,30 @@
         <v>492</v>
       </c>
       <c r="E48" s="134" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="F48" s="134" t="s">
         <v>745</v>
       </c>
       <c r="M48" s="134" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="134" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B49" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D49" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E49" s="134" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="M49" s="134" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="N49" s="34">
         <v>3</v>
@@ -25049,19 +25042,19 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="134" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B50" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D50" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E50" s="134" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="M50" s="134" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="N50" s="34">
         <v>3</v>
@@ -25069,53 +25062,53 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="134" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B51" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D51" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E51" s="134" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="M51" s="134" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="134" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B52" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D52" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E52" s="134" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="M52" s="134" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="134" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B53" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D53" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E53" s="134" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="M53" s="134" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="N53" s="34">
         <v>3</v>
@@ -25123,19 +25116,19 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="134" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B54" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D54" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E54" s="134" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="M54" s="134" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="N54" s="34">
         <v>3</v>
@@ -25143,19 +25136,19 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="134" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B55" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D55" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E55" s="134" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="M55" s="135" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="N55" s="136">
         <v>3</v>
@@ -25165,19 +25158,19 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="134" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B56" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D56" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E56" s="134" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="M56" s="134" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="N56" s="34">
         <v>3</v>
@@ -25185,19 +25178,19 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="134" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="B57" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D57" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E57" s="134" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="M57" s="134" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="N57" s="34">
         <v>3</v>
@@ -25205,19 +25198,19 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="134" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B58" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D58" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E58" s="134" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="M58" s="134" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="N58" s="34">
         <v>3</v>
@@ -25225,19 +25218,19 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="134" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B59" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D59" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E59" s="134" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="M59" s="134" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="N59" s="34">
         <v>3</v>
@@ -25245,53 +25238,53 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="134" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B60" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D60" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E60" s="134" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="M60" s="134" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="134" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B61" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D61" s="134" t="s">
         <v>382</v>
       </c>
       <c r="E61" s="134" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="M61" s="134" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="134" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B62" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D62" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E62" s="134" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="M62" s="134" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="N62" s="34">
         <v>3</v>
@@ -25299,19 +25292,19 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="134" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B63" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D63" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E63" s="134" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="M63" s="134" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="N63" s="34">
         <v>3</v>
@@ -25319,19 +25312,19 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="134" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B64" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D64" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E64" s="134" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="M64" s="134" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="N64" s="34">
         <v>4</v>
@@ -25339,19 +25332,19 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="134" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B65" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D65" s="134" t="s">
         <v>422</v>
       </c>
       <c r="E65" s="134" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="M65" s="134" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="N65" s="34">
         <v>3</v>
@@ -25359,36 +25352,36 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="134" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B66" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D66" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E66" s="134" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="M66" s="134" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="134" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B67" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D67" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E67" s="134" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="M67" s="134" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="N67" s="34">
         <v>3</v>
@@ -25396,19 +25389,19 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="134" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B68" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D68" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E68" s="134" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="M68" s="134" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
@@ -25416,16 +25409,16 @@
         <v>483</v>
       </c>
       <c r="B69" s="134" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D69" s="134" t="s">
         <v>488</v>
       </c>
       <c r="E69" s="134" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="M69" s="134" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
   </sheetData>
@@ -25480,34 +25473,34 @@
         <v>363</v>
       </c>
       <c r="B1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D1" t="s">
         <v>1004</v>
       </c>
-      <c r="C1" t="s">
-        <v>1025</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1005</v>
-      </c>
       <c r="E1" s="137" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="F1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="G1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="H1" t="s">
         <v>376</v>
       </c>
       <c r="I1" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="J1" t="s">
         <v>491</v>
       </c>
       <c r="K1" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="L1" t="s">
         <v>364</v>
@@ -25516,7 +25509,7 @@
         <v>236</v>
       </c>
       <c r="N1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="O1" s="3">
         <v>1</v>
@@ -25671,25 +25664,25 @@
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" s="137" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B2" s="137" t="s">
         <v>1007</v>
       </c>
-      <c r="B2" s="137" t="s">
-        <v>1008</v>
-      </c>
       <c r="C2" s="137" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D2" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="137" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="F2" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G2" s="137" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="H2" s="137">
         <v>3</v>
@@ -25702,25 +25695,25 @@
       </c>
       <c r="K2" s="137"/>
       <c r="L2" t="s">
+        <v>1009</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="N2" t="s">
         <v>1010</v>
       </c>
-      <c r="M2" t="s">
-        <v>1055</v>
-      </c>
-      <c r="N2" t="s">
-        <v>1011</v>
-      </c>
       <c r="T2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="V2" t="s">
         <v>1014</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>1015</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>1016</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.25">
@@ -25728,22 +25721,22 @@
         <v>501</v>
       </c>
       <c r="B3" s="137" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C3" s="137" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D3" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="137" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="F3" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G3" s="137" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="H3" s="137">
         <v>5</v>
@@ -25756,13 +25749,13 @@
       </c>
       <c r="K3" s="137"/>
       <c r="L3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="M3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="N3" t="s">
         <v>1056</v>
-      </c>
-      <c r="N3" t="s">
-        <v>1057</v>
       </c>
       <c r="O3" s="138"/>
       <c r="P3" s="138"/>
@@ -25771,25 +25764,25 @@
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B4" s="137" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C4" s="137" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D4" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="137" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="F4" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G4" s="137" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="H4" s="137">
         <v>4</v>
@@ -25802,19 +25795,19 @@
       </c>
       <c r="K4" s="137"/>
       <c r="L4" t="s">
+        <v>1017</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1057</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1010</v>
+      </c>
+      <c r="R4" t="s">
         <v>1018</v>
       </c>
-      <c r="M4" t="s">
-        <v>1058</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1011</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="AD4" t="s">
         <v>1019</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.25">
@@ -25822,20 +25815,20 @@
         <v>493</v>
       </c>
       <c r="B5" s="137" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C5" s="137" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="D5" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="137" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="F5" s="137"/>
       <c r="G5" s="137" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="H5" s="137">
         <v>4</v>
@@ -25850,13 +25843,13 @@
         <v>247</v>
       </c>
       <c r="L5" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="M5" t="s">
+        <v>1058</v>
+      </c>
+      <c r="N5" t="s">
         <v>1059</v>
-      </c>
-      <c r="N5" t="s">
-        <v>1060</v>
       </c>
       <c r="U5" s="138">
         <v>0.18</v>
@@ -25876,20 +25869,20 @@
         <v>497</v>
       </c>
       <c r="B6" s="137" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C6" s="137" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D6" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="137" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="F6" s="137"/>
       <c r="G6" s="137" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="H6" s="137">
         <v>3</v>
@@ -25898,19 +25891,19 @@
         <v>1</v>
       </c>
       <c r="J6" s="137" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="K6" s="137" t="s">
         <v>246</v>
       </c>
       <c r="L6" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="M6" s="139" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="N6" s="137" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="T6" s="138"/>
       <c r="X6" s="138"/>
@@ -25921,10 +25914,10 @@
         <v>558</v>
       </c>
       <c r="B7" s="137" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C7" s="137" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D7" s="137" t="s">
         <v>33</v>
@@ -25934,7 +25927,7 @@
       </c>
       <c r="F7" s="137"/>
       <c r="G7" s="137" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="H7" s="137">
         <v>4</v>
@@ -25946,46 +25939,46 @@
         <v>3</v>
       </c>
       <c r="K7" s="137" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="L7" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="M7" t="s">
+        <v>1051</v>
+      </c>
+      <c r="R7" t="s">
         <v>1052</v>
       </c>
-      <c r="R7" t="s">
-        <v>1053</v>
-      </c>
       <c r="V7" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="Z7" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="AD7" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B8" s="137" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C8" s="137" t="s">
         <v>1046</v>
       </c>
-      <c r="B8" s="137" t="s">
-        <v>1008</v>
-      </c>
-      <c r="C8" s="137" t="s">
+      <c r="D8" s="137" t="s">
         <v>1047</v>
       </c>
-      <c r="D8" s="137" t="s">
-        <v>1048</v>
-      </c>
       <c r="E8" s="137" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="F8" s="137"/>
       <c r="G8" s="137" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="H8" s="137">
         <v>0</v>
@@ -25998,10 +25991,10 @@
       </c>
       <c r="K8" s="137"/>
       <c r="L8" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="M8" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="W8">
         <v>2</v>
@@ -26018,22 +26011,22 @@
         <v>490</v>
       </c>
       <c r="B9" s="137" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C9" s="137" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D9" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="137" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="F9" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G9" s="137" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="H9" s="137">
         <v>4</v>
@@ -26048,10 +26041,10 @@
         <v>246</v>
       </c>
       <c r="L9" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="M9" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.25">
@@ -26059,20 +26052,20 @@
         <v>496</v>
       </c>
       <c r="B10" s="137" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C10" s="137" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D10" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="137" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="F10" s="137"/>
       <c r="G10" s="137" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="H10" s="137">
         <v>4</v>
@@ -26087,13 +26080,13 @@
         <v>246</v>
       </c>
       <c r="L10" t="s">
+        <v>1065</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1051</v>
+      </c>
+      <c r="N10" s="139" t="s">
         <v>1066</v>
-      </c>
-      <c r="M10" t="s">
-        <v>1052</v>
-      </c>
-      <c r="N10" s="139" t="s">
-        <v>1067</v>
       </c>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.25">
@@ -26101,10 +26094,10 @@
         <v>565</v>
       </c>
       <c r="B11" s="137" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C11" s="137" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D11" s="137" t="s">
         <v>33</v>
@@ -26114,7 +26107,7 @@
       </c>
       <c r="F11" s="137"/>
       <c r="G11" s="137" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="H11" s="137">
         <v>1</v>
@@ -26129,25 +26122,25 @@
         <v>246</v>
       </c>
       <c r="L11" t="s">
+        <v>1068</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1051</v>
+      </c>
+      <c r="N11" s="139" t="s">
         <v>1069</v>
       </c>
-      <c r="M11" t="s">
+      <c r="S11" t="s">
         <v>1052</v>
       </c>
-      <c r="N11" s="139" t="s">
+      <c r="X11" t="s">
+        <v>1052</v>
+      </c>
+      <c r="AC11" t="s">
         <v>1070</v>
       </c>
-      <c r="S11" t="s">
-        <v>1053</v>
-      </c>
-      <c r="X11" t="s">
-        <v>1053</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>1071</v>
-      </c>
       <c r="AH11" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.25">
@@ -26492,7 +26485,7 @@
         <v>350</v>
       </c>
       <c r="B1" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -26500,7 +26493,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -26508,7 +26501,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -26524,7 +26517,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -26532,7 +26525,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -26540,7 +26533,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -26548,7 +26541,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -26556,7 +26549,7 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -26564,7 +26557,7 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -26572,7 +26565,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -26580,7 +26573,7 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -26588,7 +26581,7 @@
         <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
   </sheetData>
@@ -27750,10 +27743,10 @@
     </row>
     <row r="19" spans="1:15" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="104" t="s">
+        <v>938</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>939</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>940</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -28260,7 +28253,7 @@
         <v>278</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -28513,19 +28506,19 @@
         <v>773</v>
       </c>
       <c r="K61" s="76" t="s">
+        <v>907</v>
+      </c>
+      <c r="L61" s="76" t="s">
         <v>908</v>
       </c>
-      <c r="L61" s="76" t="s">
+      <c r="M61" s="76" t="s">
         <v>909</v>
       </c>
-      <c r="M61" s="76" t="s">
+      <c r="N61" s="76" t="s">
         <v>910</v>
       </c>
-      <c r="N61" s="76" t="s">
+      <c r="O61" s="74" t="s">
         <v>911</v>
-      </c>
-      <c r="O61" s="74" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Implementing deco blocking LoS bullet fire
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -644,7 +644,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2240" uniqueCount="1085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="1084">
   <si>
     <t>Fishing</t>
   </si>
@@ -3638,9 +3638,6 @@
   </si>
   <si>
     <t>Soul Farmer</t>
-  </si>
-  <si>
-    <t>bullets hitting random targets</t>
   </si>
   <si>
     <t>Spells going by levels</t>
@@ -4749,7 +4746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5068,12 +5065,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -5086,22 +5077,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5119,10 +5104,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5476,8 +5467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57:C57"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5492,29 +5483,29 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="152" t="s">
+      <c r="A2" s="148" t="s">
         <v>782</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="154"/>
+      <c r="B2" s="149"/>
+      <c r="C2" s="150"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="115">
         <v>1</v>
       </c>
-      <c r="B3" s="155" t="s">
+      <c r="B3" s="151" t="s">
         <v>783</v>
       </c>
-      <c r="C3" s="156"/>
+      <c r="C3" s="152"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="153" t="s">
         <v>784</v>
       </c>
-      <c r="C4" s="147"/>
+      <c r="C4" s="154"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="116"/>
@@ -5565,10 +5556,10 @@
       <c r="A10" s="116">
         <v>3</v>
       </c>
-      <c r="B10" s="148" t="s">
+      <c r="B10" s="155" t="s">
         <v>785</v>
       </c>
-      <c r="C10" s="149"/>
+      <c r="C10" s="156"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="116"/>
@@ -5583,10 +5574,10 @@
       <c r="A12" s="116">
         <v>4</v>
       </c>
-      <c r="B12" s="150" t="s">
+      <c r="B12" s="144" t="s">
         <v>786</v>
       </c>
-      <c r="C12" s="151"/>
+      <c r="C12" s="145"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="116"/>
@@ -5601,10 +5592,10 @@
       <c r="A14" s="116">
         <v>5</v>
       </c>
-      <c r="B14" s="150" t="s">
+      <c r="B14" s="144" t="s">
         <v>787</v>
       </c>
-      <c r="C14" s="151"/>
+      <c r="C14" s="145"/>
     </row>
     <row r="15" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="116"/>
@@ -5619,10 +5610,10 @@
       <c r="A16" s="117">
         <v>6</v>
       </c>
-      <c r="B16" s="157" t="s">
+      <c r="B16" s="146" t="s">
         <v>791</v>
       </c>
-      <c r="C16" s="158"/>
+      <c r="C16" s="147"/>
     </row>
     <row r="17" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="116"/>
@@ -5637,46 +5628,46 @@
       <c r="A18" s="117">
         <v>7</v>
       </c>
-      <c r="B18" s="157" t="s">
+      <c r="B18" s="146" t="s">
         <v>912</v>
       </c>
-      <c r="C18" s="158"/>
+      <c r="C18" s="147"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="132">
         <v>8</v>
       </c>
-      <c r="B19" s="157" t="s">
-        <v>999</v>
-      </c>
-      <c r="C19" s="158"/>
+      <c r="B19" s="146" t="s">
+        <v>998</v>
+      </c>
+      <c r="C19" s="147"/>
     </row>
     <row r="20" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="132">
         <v>9</v>
       </c>
-      <c r="B20" s="157" t="s">
+      <c r="B20" s="146" t="s">
         <v>913</v>
       </c>
-      <c r="C20" s="158"/>
+      <c r="C20" s="147"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="152" t="s">
+      <c r="A23" s="148" t="s">
         <v>793</v>
       </c>
-      <c r="B23" s="153"/>
-      <c r="C23" s="154"/>
+      <c r="B23" s="149"/>
+      <c r="C23" s="150"/>
     </row>
     <row r="24" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="115">
         <v>1</v>
       </c>
-      <c r="B24" s="155" t="s">
+      <c r="B24" s="151" t="s">
         <v>782</v>
       </c>
-      <c r="C24" s="156"/>
+      <c r="C24" s="152"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="116"/>
@@ -5685,21 +5676,17 @@
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="116"/>
-      <c r="B26" s="140" t="s">
-        <v>789</v>
-      </c>
-      <c r="C26" s="141" t="s">
-        <v>998</v>
-      </c>
+      <c r="B26" s="120"/>
+      <c r="C26" s="121"/>
     </row>
     <row r="27" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="116">
         <v>2</v>
       </c>
-      <c r="B27" s="146" t="s">
+      <c r="B27" s="153" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="147"/>
+      <c r="C27" s="154"/>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="116"/>
@@ -5716,52 +5703,52 @@
         <v>789</v>
       </c>
       <c r="C29" s="121" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="116">
         <v>3</v>
       </c>
-      <c r="B30" s="146" t="s">
-        <v>1000</v>
-      </c>
-      <c r="C30" s="147"/>
+      <c r="B30" s="153" t="s">
+        <v>999</v>
+      </c>
+      <c r="C30" s="154"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="116"/>
-      <c r="B31" s="142" t="s">
+      <c r="B31" s="140" t="s">
         <v>788</v>
       </c>
-      <c r="C31" s="143" t="s">
-        <v>1001</v>
+      <c r="C31" s="141" t="s">
+        <v>1000</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="116"/>
-      <c r="B32" s="144" t="s">
+      <c r="B32" s="142" t="s">
         <v>789</v>
       </c>
-      <c r="C32" s="145" t="s">
-        <v>1002</v>
+      <c r="C32" s="143" t="s">
+        <v>1001</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="152" t="s">
+      <c r="A34" s="148" t="s">
         <v>797</v>
       </c>
-      <c r="B34" s="153"/>
-      <c r="C34" s="154"/>
+      <c r="B34" s="149"/>
+      <c r="C34" s="150"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="115">
         <v>1</v>
       </c>
-      <c r="B35" s="155" t="s">
+      <c r="B35" s="151" t="s">
         <v>798</v>
       </c>
-      <c r="C35" s="156"/>
+      <c r="C35" s="152"/>
     </row>
     <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="116"/>
@@ -5797,20 +5784,20 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="152" t="s">
+      <c r="A41" s="148" t="s">
         <v>801</v>
       </c>
-      <c r="B41" s="153"/>
-      <c r="C41" s="154"/>
+      <c r="B41" s="149"/>
+      <c r="C41" s="150"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="115">
         <v>1</v>
       </c>
-      <c r="B42" s="155" t="s">
+      <c r="B42" s="151" t="s">
         <v>802</v>
       </c>
-      <c r="C42" s="156"/>
+      <c r="C42" s="152"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="116"/>
@@ -5834,10 +5821,10 @@
       <c r="A45" s="115">
         <v>1</v>
       </c>
-      <c r="B45" s="155" t="s">
+      <c r="B45" s="151" t="s">
         <v>804</v>
       </c>
-      <c r="C45" s="156"/>
+      <c r="C45" s="152"/>
     </row>
     <row r="46" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="116"/>
@@ -5873,263 +5860,263 @@
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="152" t="s">
+      <c r="A51" s="148" t="s">
         <v>188</v>
       </c>
-      <c r="B51" s="153"/>
-      <c r="C51" s="154"/>
+      <c r="B51" s="149"/>
+      <c r="C51" s="150"/>
     </row>
     <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="115">
         <v>1</v>
       </c>
-      <c r="B52" s="155" t="s">
+      <c r="B52" s="151" t="s">
         <v>809</v>
       </c>
-      <c r="C52" s="156"/>
+      <c r="C52" s="152"/>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="152" t="s">
+      <c r="A54" s="148" t="s">
         <v>790</v>
       </c>
-      <c r="B54" s="153"/>
-      <c r="C54" s="154"/>
+      <c r="B54" s="149"/>
+      <c r="C54" s="150"/>
     </row>
     <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="115">
         <v>1</v>
       </c>
-      <c r="B55" s="148" t="s">
+      <c r="B55" s="155" t="s">
         <v>783</v>
       </c>
-      <c r="C55" s="149"/>
+      <c r="C55" s="156"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="116">
         <v>2</v>
       </c>
-      <c r="B56" s="159" t="s">
+      <c r="B56" s="157" t="s">
         <v>784</v>
       </c>
-      <c r="C56" s="160"/>
+      <c r="C56" s="158"/>
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="116">
         <v>3</v>
       </c>
-      <c r="B57" s="150" t="s">
+      <c r="B57" s="144" t="s">
         <v>785</v>
       </c>
-      <c r="C57" s="151"/>
+      <c r="C57" s="145"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="116">
         <v>4</v>
       </c>
-      <c r="B58" s="150" t="s">
+      <c r="B58" s="144" t="s">
         <v>786</v>
       </c>
-      <c r="C58" s="151"/>
+      <c r="C58" s="145"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="116">
         <v>5</v>
       </c>
-      <c r="B59" s="150" t="s">
+      <c r="B59" s="144" t="s">
         <v>787</v>
       </c>
-      <c r="C59" s="151"/>
+      <c r="C59" s="145"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="117">
         <v>6</v>
       </c>
-      <c r="B60" s="157" t="s">
+      <c r="B60" s="146" t="s">
         <v>791</v>
       </c>
-      <c r="C60" s="158"/>
+      <c r="C60" s="147"/>
     </row>
     <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="152" t="s">
+      <c r="A62" s="148" t="s">
         <v>810</v>
       </c>
-      <c r="B62" s="153"/>
-      <c r="C62" s="154"/>
+      <c r="B62" s="149"/>
+      <c r="C62" s="150"/>
     </row>
     <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="115">
         <v>1</v>
       </c>
-      <c r="B63" s="148" t="s">
+      <c r="B63" s="155" t="s">
         <v>783</v>
       </c>
-      <c r="C63" s="149"/>
+      <c r="C63" s="156"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="116">
         <v>2</v>
       </c>
-      <c r="B64" s="159" t="s">
+      <c r="B64" s="157" t="s">
         <v>784</v>
       </c>
-      <c r="C64" s="160"/>
+      <c r="C64" s="158"/>
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="116">
         <v>3</v>
       </c>
-      <c r="B65" s="150" t="s">
+      <c r="B65" s="144" t="s">
         <v>785</v>
       </c>
-      <c r="C65" s="151"/>
+      <c r="C65" s="145"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="116">
         <v>4</v>
       </c>
-      <c r="B66" s="150" t="s">
+      <c r="B66" s="144" t="s">
         <v>786</v>
       </c>
-      <c r="C66" s="151"/>
+      <c r="C66" s="145"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="116">
         <v>5</v>
       </c>
-      <c r="B67" s="150" t="s">
+      <c r="B67" s="144" t="s">
         <v>787</v>
       </c>
-      <c r="C67" s="151"/>
+      <c r="C67" s="145"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="117">
         <v>6</v>
       </c>
-      <c r="B68" s="157" t="s">
+      <c r="B68" s="146" t="s">
         <v>791</v>
       </c>
-      <c r="C68" s="158"/>
+      <c r="C68" s="147"/>
     </row>
     <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="152" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B70" s="153"/>
-      <c r="C70" s="154"/>
+      <c r="A70" s="148" t="s">
+        <v>999</v>
+      </c>
+      <c r="B70" s="149"/>
+      <c r="C70" s="150"/>
     </row>
     <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="115">
         <v>1</v>
       </c>
-      <c r="B71" s="148"/>
-      <c r="C71" s="149"/>
+      <c r="B71" s="155"/>
+      <c r="C71" s="156"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="116"/>
-      <c r="B72" s="159"/>
-      <c r="C72" s="160"/>
+      <c r="B72" s="157"/>
+      <c r="C72" s="158"/>
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="116"/>
-      <c r="B73" s="150"/>
-      <c r="C73" s="151"/>
+      <c r="B73" s="144"/>
+      <c r="C73" s="145"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="116"/>
-      <c r="B74" s="150"/>
-      <c r="C74" s="151"/>
+      <c r="B74" s="144"/>
+      <c r="C74" s="145"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="116"/>
-      <c r="B75" s="150"/>
-      <c r="C75" s="151"/>
+      <c r="B75" s="144"/>
+      <c r="C75" s="145"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="117"/>
-      <c r="B76" s="157"/>
-      <c r="C76" s="158"/>
+      <c r="B76" s="146"/>
+      <c r="C76" s="147"/>
     </row>
     <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="152" t="s">
+      <c r="A78" s="148" t="s">
         <v>811</v>
       </c>
-      <c r="B78" s="153"/>
-      <c r="C78" s="154"/>
+      <c r="B78" s="149"/>
+      <c r="C78" s="150"/>
     </row>
     <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="115">
         <v>1</v>
       </c>
-      <c r="B79" s="148" t="s">
+      <c r="B79" s="155" t="s">
         <v>783</v>
       </c>
-      <c r="C79" s="149"/>
+      <c r="C79" s="156"/>
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="116">
         <v>2</v>
       </c>
-      <c r="B80" s="159" t="s">
+      <c r="B80" s="157" t="s">
         <v>784</v>
       </c>
-      <c r="C80" s="160"/>
+      <c r="C80" s="158"/>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="116">
         <v>3</v>
       </c>
-      <c r="B81" s="150" t="s">
+      <c r="B81" s="144" t="s">
         <v>785</v>
       </c>
-      <c r="C81" s="151"/>
+      <c r="C81" s="145"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="116">
         <v>4</v>
       </c>
-      <c r="B82" s="150" t="s">
+      <c r="B82" s="144" t="s">
         <v>786</v>
       </c>
-      <c r="C82" s="151"/>
+      <c r="C82" s="145"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="116">
         <v>5</v>
       </c>
-      <c r="B83" s="150" t="s">
+      <c r="B83" s="144" t="s">
         <v>787</v>
       </c>
-      <c r="C83" s="151"/>
+      <c r="C83" s="145"/>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="117">
         <v>6</v>
       </c>
-      <c r="B84" s="157" t="s">
+      <c r="B84" s="146" t="s">
         <v>791</v>
       </c>
-      <c r="C84" s="158"/>
+      <c r="C84" s="147"/>
     </row>
     <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="152" t="s">
+      <c r="A86" s="148" t="s">
         <v>861</v>
       </c>
-      <c r="B86" s="153"/>
-      <c r="C86" s="154"/>
+      <c r="B86" s="149"/>
+      <c r="C86" s="150"/>
     </row>
     <row r="87" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="115">
         <v>1</v>
       </c>
-      <c r="B87" s="155" t="s">
+      <c r="B87" s="151" t="s">
         <v>101</v>
       </c>
-      <c r="C87" s="156"/>
+      <c r="C87" s="152"/>
     </row>
     <row r="88" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="124"/>
@@ -6302,10 +6289,10 @@
       <c r="A107" s="116">
         <v>2</v>
       </c>
-      <c r="B107" s="146" t="s">
+      <c r="B107" s="153" t="s">
         <v>812</v>
       </c>
-      <c r="C107" s="147"/>
+      <c r="C107" s="154"/>
     </row>
     <row r="108" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="116"/>
@@ -6383,10 +6370,10 @@
       <c r="A116" s="116">
         <v>3</v>
       </c>
-      <c r="B116" s="148" t="s">
+      <c r="B116" s="155" t="s">
         <v>813</v>
       </c>
-      <c r="C116" s="149"/>
+      <c r="C116" s="156"/>
     </row>
     <row r="117" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="116"/>
@@ -6442,10 +6429,10 @@
       <c r="A123" s="115">
         <v>4</v>
       </c>
-      <c r="B123" s="150" t="s">
+      <c r="B123" s="144" t="s">
         <v>814</v>
       </c>
-      <c r="C123" s="151"/>
+      <c r="C123" s="145"/>
     </row>
     <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="124"/>
@@ -6485,20 +6472,20 @@
     </row>
     <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="129" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="152" t="s">
+      <c r="A129" s="148" t="s">
         <v>862</v>
       </c>
-      <c r="B129" s="153"/>
-      <c r="C129" s="154"/>
+      <c r="B129" s="149"/>
+      <c r="C129" s="150"/>
     </row>
     <row r="130" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="115">
         <v>1</v>
       </c>
-      <c r="B130" s="155" t="s">
+      <c r="B130" s="151" t="s">
         <v>863</v>
       </c>
-      <c r="C130" s="156"/>
+      <c r="C130" s="152"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="124"/>
@@ -6645,10 +6632,10 @@
       <c r="A150" s="116">
         <v>2</v>
       </c>
-      <c r="B150" s="146" t="s">
+      <c r="B150" s="153" t="s">
         <v>864</v>
       </c>
-      <c r="C150" s="147"/>
+      <c r="C150" s="154"/>
     </row>
     <row r="151" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="116"/>
@@ -6718,10 +6705,10 @@
       <c r="A159" s="116">
         <v>3</v>
       </c>
-      <c r="B159" s="148" t="s">
+      <c r="B159" s="155" t="s">
         <v>865</v>
       </c>
-      <c r="C159" s="149"/>
+      <c r="C159" s="156"/>
     </row>
     <row r="160" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="116"/>
@@ -6775,6 +6762,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="A129:C129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B42:C42"/>
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
@@ -6791,48 +6820,6 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="A129:C129"/>
-    <mergeCell ref="B130:C130"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -8029,31 +8016,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="164" t="s">
+      <c r="B1" s="162" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="167" t="s">
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
+      <c r="J1" s="164"/>
+      <c r="K1" s="165" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="168"/>
-      <c r="M1" s="168"/>
-      <c r="N1" s="168"/>
-      <c r="O1" s="168"/>
-      <c r="P1" s="168"/>
-      <c r="Q1" s="168"/>
-      <c r="R1" s="168"/>
-      <c r="S1" s="168"/>
-      <c r="T1" s="168"/>
-      <c r="U1" s="168"/>
-      <c r="V1" s="169"/>
+      <c r="L1" s="166"/>
+      <c r="M1" s="166"/>
+      <c r="N1" s="166"/>
+      <c r="O1" s="166"/>
+      <c r="P1" s="166"/>
+      <c r="Q1" s="166"/>
+      <c r="R1" s="166"/>
+      <c r="S1" s="166"/>
+      <c r="T1" s="166"/>
+      <c r="U1" s="166"/>
+      <c r="V1" s="167"/>
     </row>
     <row r="2" spans="1:22" ht="44.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K2" s="66" t="s">
@@ -22205,17 +22192,17 @@
       <c r="A1" s="81" t="s">
         <v>363</v>
       </c>
-      <c r="B1" s="170" t="s">
+      <c r="B1" s="168" t="s">
         <v>365</v>
       </c>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="171"/>
-      <c r="H1" s="171"/>
-      <c r="I1" s="171"/>
-      <c r="J1" s="172"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="169"/>
+      <c r="I1" s="169"/>
+      <c r="J1" s="170"/>
       <c r="K1" s="91" t="s">
         <v>364</v>
       </c>
@@ -22951,10 +22938,10 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="83" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B39" s="48" t="s">
         <v>1029</v>
-      </c>
-      <c r="B39" s="48" t="s">
-        <v>1030</v>
       </c>
       <c r="C39" s="43" t="s">
         <v>745</v>
@@ -22967,7 +22954,7 @@
       <c r="I39" s="43"/>
       <c r="J39" s="44"/>
       <c r="K39" s="89" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="L39" s="87"/>
     </row>
@@ -23105,10 +23092,10 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="83" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B47" s="48" t="s">
         <v>1027</v>
-      </c>
-      <c r="B47" s="48" t="s">
-        <v>1028</v>
       </c>
       <c r="C47" s="43" t="s">
         <v>745</v>
@@ -23121,7 +23108,7 @@
       <c r="I47" s="43"/>
       <c r="J47" s="44"/>
       <c r="K47" s="89" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="L47" s="87"/>
     </row>
@@ -24082,15 +24069,15 @@
       <c r="C1" t="s">
         <v>701</v>
       </c>
-      <c r="E1" s="173" t="s">
+      <c r="E1" s="171" t="s">
         <v>365</v>
       </c>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="J1" s="173"/>
-      <c r="K1" s="173"/>
+      <c r="F1" s="171"/>
+      <c r="G1" s="171"/>
+      <c r="H1" s="171"/>
+      <c r="I1" s="171"/>
+      <c r="J1" s="171"/>
+      <c r="K1" s="171"/>
       <c r="L1" s="31"/>
     </row>
     <row r="2" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
@@ -25473,34 +25460,34 @@
         <v>363</v>
       </c>
       <c r="B1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D1" t="s">
         <v>1003</v>
       </c>
-      <c r="C1" t="s">
-        <v>1024</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1004</v>
-      </c>
       <c r="E1" s="137" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="F1" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="G1" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="H1" t="s">
         <v>376</v>
       </c>
       <c r="I1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="J1" t="s">
         <v>491</v>
       </c>
       <c r="K1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="L1" t="s">
         <v>364</v>
@@ -25509,7 +25496,7 @@
         <v>236</v>
       </c>
       <c r="N1" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="O1" s="3">
         <v>1</v>
@@ -25664,25 +25651,25 @@
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" s="137" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B2" s="137" t="s">
         <v>1006</v>
       </c>
-      <c r="B2" s="137" t="s">
-        <v>1007</v>
-      </c>
       <c r="C2" s="137" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D2" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="137" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="F2" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G2" s="137" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="H2" s="137">
         <v>3</v>
@@ -25695,25 +25682,25 @@
       </c>
       <c r="K2" s="137"/>
       <c r="L2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1053</v>
+      </c>
+      <c r="N2" t="s">
         <v>1009</v>
       </c>
-      <c r="M2" t="s">
-        <v>1054</v>
-      </c>
-      <c r="N2" t="s">
-        <v>1010</v>
-      </c>
       <c r="T2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="V2" t="s">
         <v>1013</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>1014</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>1015</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>1016</v>
       </c>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.25">
@@ -25721,22 +25708,22 @@
         <v>501</v>
       </c>
       <c r="B3" s="137" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C3" s="137" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D3" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="137" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="F3" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G3" s="137" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="H3" s="137">
         <v>5</v>
@@ -25749,13 +25736,13 @@
       </c>
       <c r="K3" s="137"/>
       <c r="L3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="M3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="N3" t="s">
         <v>1055</v>
-      </c>
-      <c r="N3" t="s">
-        <v>1056</v>
       </c>
       <c r="O3" s="138"/>
       <c r="P3" s="138"/>
@@ -25764,25 +25751,25 @@
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B4" s="137" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C4" s="137" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D4" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="137" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="F4" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G4" s="137" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="H4" s="137">
         <v>4</v>
@@ -25795,19 +25782,19 @@
       </c>
       <c r="K4" s="137"/>
       <c r="L4" t="s">
+        <v>1016</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1056</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1009</v>
+      </c>
+      <c r="R4" t="s">
         <v>1017</v>
       </c>
-      <c r="M4" t="s">
-        <v>1057</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1010</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="AD4" t="s">
         <v>1018</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.25">
@@ -25815,20 +25802,20 @@
         <v>493</v>
       </c>
       <c r="B5" s="137" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C5" s="137" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D5" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="137" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F5" s="137"/>
       <c r="G5" s="137" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="H5" s="137">
         <v>4</v>
@@ -25843,13 +25830,13 @@
         <v>247</v>
       </c>
       <c r="L5" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="M5" t="s">
+        <v>1057</v>
+      </c>
+      <c r="N5" t="s">
         <v>1058</v>
-      </c>
-      <c r="N5" t="s">
-        <v>1059</v>
       </c>
       <c r="U5" s="138">
         <v>0.18</v>
@@ -25869,20 +25856,20 @@
         <v>497</v>
       </c>
       <c r="B6" s="137" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C6" s="137" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D6" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="137" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F6" s="137"/>
       <c r="G6" s="137" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="H6" s="137">
         <v>3</v>
@@ -25891,19 +25878,19 @@
         <v>1</v>
       </c>
       <c r="J6" s="137" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="K6" s="137" t="s">
         <v>246</v>
       </c>
       <c r="L6" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="M6" s="139" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="N6" s="137" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="T6" s="138"/>
       <c r="X6" s="138"/>
@@ -25914,10 +25901,10 @@
         <v>558</v>
       </c>
       <c r="B7" s="137" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C7" s="137" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D7" s="137" t="s">
         <v>33</v>
@@ -25927,7 +25914,7 @@
       </c>
       <c r="F7" s="137"/>
       <c r="G7" s="137" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="H7" s="137">
         <v>4</v>
@@ -25939,46 +25926,46 @@
         <v>3</v>
       </c>
       <c r="K7" s="137" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="L7" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="M7" t="s">
+        <v>1050</v>
+      </c>
+      <c r="R7" t="s">
         <v>1051</v>
       </c>
-      <c r="R7" t="s">
-        <v>1052</v>
-      </c>
       <c r="V7" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="Z7" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="AD7" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B8" s="137" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C8" s="137" t="s">
         <v>1045</v>
       </c>
-      <c r="B8" s="137" t="s">
-        <v>1007</v>
-      </c>
-      <c r="C8" s="137" t="s">
+      <c r="D8" s="137" t="s">
         <v>1046</v>
       </c>
-      <c r="D8" s="137" t="s">
-        <v>1047</v>
-      </c>
       <c r="E8" s="137" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="F8" s="137"/>
       <c r="G8" s="137" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="H8" s="137">
         <v>0</v>
@@ -25991,10 +25978,10 @@
       </c>
       <c r="K8" s="137"/>
       <c r="L8" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="M8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="W8">
         <v>2</v>
@@ -26011,22 +25998,22 @@
         <v>490</v>
       </c>
       <c r="B9" s="137" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C9" s="137" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D9" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="137" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="F9" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G9" s="137" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="H9" s="137">
         <v>4</v>
@@ -26041,10 +26028,10 @@
         <v>246</v>
       </c>
       <c r="L9" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="M9" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.25">
@@ -26052,20 +26039,20 @@
         <v>496</v>
       </c>
       <c r="B10" s="137" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C10" s="137" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D10" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="137" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="F10" s="137"/>
       <c r="G10" s="137" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="H10" s="137">
         <v>4</v>
@@ -26080,13 +26067,13 @@
         <v>246</v>
       </c>
       <c r="L10" t="s">
+        <v>1064</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1050</v>
+      </c>
+      <c r="N10" s="139" t="s">
         <v>1065</v>
-      </c>
-      <c r="M10" t="s">
-        <v>1051</v>
-      </c>
-      <c r="N10" s="139" t="s">
-        <v>1066</v>
       </c>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.25">
@@ -26094,10 +26081,10 @@
         <v>565</v>
       </c>
       <c r="B11" s="137" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C11" s="137" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D11" s="137" t="s">
         <v>33</v>
@@ -26107,7 +26094,7 @@
       </c>
       <c r="F11" s="137"/>
       <c r="G11" s="137" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="H11" s="137">
         <v>1</v>
@@ -26122,25 +26109,25 @@
         <v>246</v>
       </c>
       <c r="L11" t="s">
+        <v>1067</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1050</v>
+      </c>
+      <c r="N11" s="139" t="s">
         <v>1068</v>
       </c>
-      <c r="M11" t="s">
+      <c r="S11" t="s">
         <v>1051</v>
       </c>
-      <c r="N11" s="139" t="s">
+      <c r="X11" t="s">
+        <v>1051</v>
+      </c>
+      <c r="AC11" t="s">
         <v>1069</v>
       </c>
-      <c r="S11" t="s">
-        <v>1052</v>
-      </c>
-      <c r="X11" t="s">
-        <v>1052</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>1070</v>
-      </c>
       <c r="AH11" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.25">
@@ -26485,7 +26472,7 @@
         <v>350</v>
       </c>
       <c r="B1" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -26493,7 +26480,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -26501,7 +26488,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -26517,7 +26504,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -26525,7 +26512,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -26533,7 +26520,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -26541,7 +26528,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -26549,7 +26536,7 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -26557,7 +26544,7 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -26565,7 +26552,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -26573,7 +26560,7 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -26581,7 +26568,7 @@
         <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
   </sheetData>
@@ -27329,24 +27316,24 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="100"/>
-      <c r="B1" s="163" t="s">
+      <c r="B1" s="161" t="s">
         <v>702</v>
       </c>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
       <c r="E1" s="101"/>
-      <c r="F1" s="161" t="s">
+      <c r="F1" s="159" t="s">
         <v>350</v>
       </c>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="161"/>
-      <c r="J1" s="161"/>
-      <c r="K1" s="161"/>
-      <c r="L1" s="161"/>
-      <c r="M1" s="161"/>
-      <c r="N1" s="161"/>
-      <c r="O1" s="162"/>
+      <c r="G1" s="159"/>
+      <c r="H1" s="159"/>
+      <c r="I1" s="159"/>
+      <c r="J1" s="159"/>
+      <c r="K1" s="159"/>
+      <c r="L1" s="159"/>
+      <c r="M1" s="159"/>
+      <c r="N1" s="159"/>
+      <c r="O1" s="160"/>
       <c r="P1" s="30"/>
       <c r="Q1" s="30"/>
       <c r="R1" s="30"/>

</xml_diff>

<commit_message>
Tweaking orc culture parameters
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -5077,16 +5077,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5104,16 +5110,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5467,8 +5467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5483,29 +5483,29 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="150" t="s">
         <v>782</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="150"/>
+      <c r="B2" s="151"/>
+      <c r="C2" s="152"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="115">
         <v>1</v>
       </c>
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="153" t="s">
         <v>783</v>
       </c>
-      <c r="C3" s="152"/>
+      <c r="C3" s="154"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B4" s="153" t="s">
+      <c r="B4" s="144" t="s">
         <v>784</v>
       </c>
-      <c r="C4" s="154"/>
+      <c r="C4" s="145"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="116"/>
@@ -5556,10 +5556,10 @@
       <c r="A10" s="116">
         <v>3</v>
       </c>
-      <c r="B10" s="155" t="s">
+      <c r="B10" s="146" t="s">
         <v>785</v>
       </c>
-      <c r="C10" s="156"/>
+      <c r="C10" s="147"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="116"/>
@@ -5574,10 +5574,10 @@
       <c r="A12" s="116">
         <v>4</v>
       </c>
-      <c r="B12" s="144" t="s">
+      <c r="B12" s="148" t="s">
         <v>786</v>
       </c>
-      <c r="C12" s="145"/>
+      <c r="C12" s="149"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="116"/>
@@ -5592,10 +5592,10 @@
       <c r="A14" s="116">
         <v>5</v>
       </c>
-      <c r="B14" s="144" t="s">
+      <c r="B14" s="148" t="s">
         <v>787</v>
       </c>
-      <c r="C14" s="145"/>
+      <c r="C14" s="149"/>
     </row>
     <row r="15" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="116"/>
@@ -5610,10 +5610,10 @@
       <c r="A16" s="117">
         <v>6</v>
       </c>
-      <c r="B16" s="146" t="s">
+      <c r="B16" s="155" t="s">
         <v>791</v>
       </c>
-      <c r="C16" s="147"/>
+      <c r="C16" s="156"/>
     </row>
     <row r="17" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="116"/>
@@ -5628,46 +5628,46 @@
       <c r="A18" s="117">
         <v>7</v>
       </c>
-      <c r="B18" s="146" t="s">
+      <c r="B18" s="155" t="s">
         <v>912</v>
       </c>
-      <c r="C18" s="147"/>
+      <c r="C18" s="156"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="132">
         <v>8</v>
       </c>
-      <c r="B19" s="146" t="s">
+      <c r="B19" s="155" t="s">
         <v>998</v>
       </c>
-      <c r="C19" s="147"/>
+      <c r="C19" s="156"/>
     </row>
     <row r="20" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="132">
         <v>9</v>
       </c>
-      <c r="B20" s="146" t="s">
+      <c r="B20" s="155" t="s">
         <v>913</v>
       </c>
-      <c r="C20" s="147"/>
+      <c r="C20" s="156"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="148" t="s">
+      <c r="A23" s="150" t="s">
         <v>793</v>
       </c>
-      <c r="B23" s="149"/>
-      <c r="C23" s="150"/>
+      <c r="B23" s="151"/>
+      <c r="C23" s="152"/>
     </row>
     <row r="24" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="115">
         <v>1</v>
       </c>
-      <c r="B24" s="151" t="s">
+      <c r="B24" s="153" t="s">
         <v>782</v>
       </c>
-      <c r="C24" s="152"/>
+      <c r="C24" s="154"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="116"/>
@@ -5683,10 +5683,10 @@
       <c r="A27" s="116">
         <v>2</v>
       </c>
-      <c r="B27" s="153" t="s">
+      <c r="B27" s="144" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="154"/>
+      <c r="C27" s="145"/>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="116"/>
@@ -5710,10 +5710,10 @@
       <c r="A30" s="116">
         <v>3</v>
       </c>
-      <c r="B30" s="153" t="s">
+      <c r="B30" s="144" t="s">
         <v>999</v>
       </c>
-      <c r="C30" s="154"/>
+      <c r="C30" s="145"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="116"/>
@@ -5735,20 +5735,20 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="148" t="s">
+      <c r="A34" s="150" t="s">
         <v>797</v>
       </c>
-      <c r="B34" s="149"/>
-      <c r="C34" s="150"/>
+      <c r="B34" s="151"/>
+      <c r="C34" s="152"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="115">
         <v>1</v>
       </c>
-      <c r="B35" s="151" t="s">
+      <c r="B35" s="153" t="s">
         <v>798</v>
       </c>
-      <c r="C35" s="152"/>
+      <c r="C35" s="154"/>
     </row>
     <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="116"/>
@@ -5784,20 +5784,20 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="148" t="s">
+      <c r="A41" s="150" t="s">
         <v>801</v>
       </c>
-      <c r="B41" s="149"/>
-      <c r="C41" s="150"/>
+      <c r="B41" s="151"/>
+      <c r="C41" s="152"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="115">
         <v>1</v>
       </c>
-      <c r="B42" s="151" t="s">
+      <c r="B42" s="153" t="s">
         <v>802</v>
       </c>
-      <c r="C42" s="152"/>
+      <c r="C42" s="154"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="116"/>
@@ -5821,10 +5821,10 @@
       <c r="A45" s="115">
         <v>1</v>
       </c>
-      <c r="B45" s="151" t="s">
+      <c r="B45" s="153" t="s">
         <v>804</v>
       </c>
-      <c r="C45" s="152"/>
+      <c r="C45" s="154"/>
     </row>
     <row r="46" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="116"/>
@@ -5860,37 +5860,37 @@
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="148" t="s">
+      <c r="A51" s="150" t="s">
         <v>188</v>
       </c>
-      <c r="B51" s="149"/>
-      <c r="C51" s="150"/>
+      <c r="B51" s="151"/>
+      <c r="C51" s="152"/>
     </row>
     <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="115">
         <v>1</v>
       </c>
-      <c r="B52" s="151" t="s">
+      <c r="B52" s="153" t="s">
         <v>809</v>
       </c>
-      <c r="C52" s="152"/>
+      <c r="C52" s="154"/>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="148" t="s">
+      <c r="A54" s="150" t="s">
         <v>790</v>
       </c>
-      <c r="B54" s="149"/>
-      <c r="C54" s="150"/>
+      <c r="B54" s="151"/>
+      <c r="C54" s="152"/>
     </row>
     <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="115">
         <v>1</v>
       </c>
-      <c r="B55" s="155" t="s">
+      <c r="B55" s="146" t="s">
         <v>783</v>
       </c>
-      <c r="C55" s="156"/>
+      <c r="C55" s="147"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="116">
@@ -5905,54 +5905,54 @@
       <c r="A57" s="116">
         <v>3</v>
       </c>
-      <c r="B57" s="144" t="s">
+      <c r="B57" s="148" t="s">
         <v>785</v>
       </c>
-      <c r="C57" s="145"/>
+      <c r="C57" s="149"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="116">
         <v>4</v>
       </c>
-      <c r="B58" s="144" t="s">
+      <c r="B58" s="148" t="s">
         <v>786</v>
       </c>
-      <c r="C58" s="145"/>
+      <c r="C58" s="149"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="116">
         <v>5</v>
       </c>
-      <c r="B59" s="144" t="s">
+      <c r="B59" s="148" t="s">
         <v>787</v>
       </c>
-      <c r="C59" s="145"/>
+      <c r="C59" s="149"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="117">
         <v>6</v>
       </c>
-      <c r="B60" s="146" t="s">
+      <c r="B60" s="155" t="s">
         <v>791</v>
       </c>
-      <c r="C60" s="147"/>
+      <c r="C60" s="156"/>
     </row>
     <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="148" t="s">
+      <c r="A62" s="150" t="s">
         <v>810</v>
       </c>
-      <c r="B62" s="149"/>
-      <c r="C62" s="150"/>
+      <c r="B62" s="151"/>
+      <c r="C62" s="152"/>
     </row>
     <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="115">
         <v>1</v>
       </c>
-      <c r="B63" s="155" t="s">
+      <c r="B63" s="146" t="s">
         <v>783</v>
       </c>
-      <c r="C63" s="156"/>
+      <c r="C63" s="147"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="116">
@@ -5967,52 +5967,52 @@
       <c r="A65" s="116">
         <v>3</v>
       </c>
-      <c r="B65" s="144" t="s">
+      <c r="B65" s="148" t="s">
         <v>785</v>
       </c>
-      <c r="C65" s="145"/>
+      <c r="C65" s="149"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="116">
         <v>4</v>
       </c>
-      <c r="B66" s="144" t="s">
+      <c r="B66" s="148" t="s">
         <v>786</v>
       </c>
-      <c r="C66" s="145"/>
+      <c r="C66" s="149"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="116">
         <v>5</v>
       </c>
-      <c r="B67" s="144" t="s">
+      <c r="B67" s="148" t="s">
         <v>787</v>
       </c>
-      <c r="C67" s="145"/>
+      <c r="C67" s="149"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="117">
         <v>6</v>
       </c>
-      <c r="B68" s="146" t="s">
+      <c r="B68" s="155" t="s">
         <v>791</v>
       </c>
-      <c r="C68" s="147"/>
+      <c r="C68" s="156"/>
     </row>
     <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="148" t="s">
+      <c r="A70" s="150" t="s">
         <v>999</v>
       </c>
-      <c r="B70" s="149"/>
-      <c r="C70" s="150"/>
+      <c r="B70" s="151"/>
+      <c r="C70" s="152"/>
     </row>
     <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="115">
         <v>1</v>
       </c>
-      <c r="B71" s="155"/>
-      <c r="C71" s="156"/>
+      <c r="B71" s="146"/>
+      <c r="C71" s="147"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="116"/>
@@ -6021,40 +6021,40 @@
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="116"/>
-      <c r="B73" s="144"/>
-      <c r="C73" s="145"/>
+      <c r="B73" s="148"/>
+      <c r="C73" s="149"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="116"/>
-      <c r="B74" s="144"/>
-      <c r="C74" s="145"/>
+      <c r="B74" s="148"/>
+      <c r="C74" s="149"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="116"/>
-      <c r="B75" s="144"/>
-      <c r="C75" s="145"/>
+      <c r="B75" s="148"/>
+      <c r="C75" s="149"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="117"/>
-      <c r="B76" s="146"/>
-      <c r="C76" s="147"/>
+      <c r="B76" s="155"/>
+      <c r="C76" s="156"/>
     </row>
     <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="148" t="s">
+      <c r="A78" s="150" t="s">
         <v>811</v>
       </c>
-      <c r="B78" s="149"/>
-      <c r="C78" s="150"/>
+      <c r="B78" s="151"/>
+      <c r="C78" s="152"/>
     </row>
     <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="115">
         <v>1</v>
       </c>
-      <c r="B79" s="155" t="s">
+      <c r="B79" s="146" t="s">
         <v>783</v>
       </c>
-      <c r="C79" s="156"/>
+      <c r="C79" s="147"/>
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="116">
@@ -6069,54 +6069,54 @@
       <c r="A81" s="116">
         <v>3</v>
       </c>
-      <c r="B81" s="144" t="s">
+      <c r="B81" s="148" t="s">
         <v>785</v>
       </c>
-      <c r="C81" s="145"/>
+      <c r="C81" s="149"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="116">
         <v>4</v>
       </c>
-      <c r="B82" s="144" t="s">
+      <c r="B82" s="148" t="s">
         <v>786</v>
       </c>
-      <c r="C82" s="145"/>
+      <c r="C82" s="149"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="116">
         <v>5</v>
       </c>
-      <c r="B83" s="144" t="s">
+      <c r="B83" s="148" t="s">
         <v>787</v>
       </c>
-      <c r="C83" s="145"/>
+      <c r="C83" s="149"/>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="117">
         <v>6</v>
       </c>
-      <c r="B84" s="146" t="s">
+      <c r="B84" s="155" t="s">
         <v>791</v>
       </c>
-      <c r="C84" s="147"/>
+      <c r="C84" s="156"/>
     </row>
     <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="148" t="s">
+      <c r="A86" s="150" t="s">
         <v>861</v>
       </c>
-      <c r="B86" s="149"/>
-      <c r="C86" s="150"/>
+      <c r="B86" s="151"/>
+      <c r="C86" s="152"/>
     </row>
     <row r="87" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="115">
         <v>1</v>
       </c>
-      <c r="B87" s="151" t="s">
+      <c r="B87" s="153" t="s">
         <v>101</v>
       </c>
-      <c r="C87" s="152"/>
+      <c r="C87" s="154"/>
     </row>
     <row r="88" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="124"/>
@@ -6289,10 +6289,10 @@
       <c r="A107" s="116">
         <v>2</v>
       </c>
-      <c r="B107" s="153" t="s">
+      <c r="B107" s="144" t="s">
         <v>812</v>
       </c>
-      <c r="C107" s="154"/>
+      <c r="C107" s="145"/>
     </row>
     <row r="108" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="116"/>
@@ -6370,10 +6370,10 @@
       <c r="A116" s="116">
         <v>3</v>
       </c>
-      <c r="B116" s="155" t="s">
+      <c r="B116" s="146" t="s">
         <v>813</v>
       </c>
-      <c r="C116" s="156"/>
+      <c r="C116" s="147"/>
     </row>
     <row r="117" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="116"/>
@@ -6429,10 +6429,10 @@
       <c r="A123" s="115">
         <v>4</v>
       </c>
-      <c r="B123" s="144" t="s">
+      <c r="B123" s="148" t="s">
         <v>814</v>
       </c>
-      <c r="C123" s="145"/>
+      <c r="C123" s="149"/>
     </row>
     <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="124"/>
@@ -6472,20 +6472,20 @@
     </row>
     <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="129" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="148" t="s">
+      <c r="A129" s="150" t="s">
         <v>862</v>
       </c>
-      <c r="B129" s="149"/>
-      <c r="C129" s="150"/>
+      <c r="B129" s="151"/>
+      <c r="C129" s="152"/>
     </row>
     <row r="130" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="115">
         <v>1</v>
       </c>
-      <c r="B130" s="151" t="s">
+      <c r="B130" s="153" t="s">
         <v>863</v>
       </c>
-      <c r="C130" s="152"/>
+      <c r="C130" s="154"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="124"/>
@@ -6632,10 +6632,10 @@
       <c r="A150" s="116">
         <v>2</v>
       </c>
-      <c r="B150" s="153" t="s">
+      <c r="B150" s="144" t="s">
         <v>864</v>
       </c>
-      <c r="C150" s="154"/>
+      <c r="C150" s="145"/>
     </row>
     <row r="151" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="116"/>
@@ -6705,10 +6705,10 @@
       <c r="A159" s="116">
         <v>3</v>
       </c>
-      <c r="B159" s="155" t="s">
+      <c r="B159" s="146" t="s">
         <v>865</v>
       </c>
-      <c r="C159" s="156"/>
+      <c r="C159" s="147"/>
     </row>
     <row r="160" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="116"/>
@@ -6762,12 +6762,42 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="A129:C129"/>
-    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
     <mergeCell ref="B107:C107"/>
     <mergeCell ref="B67:C67"/>
     <mergeCell ref="B68:C68"/>
@@ -6784,42 +6814,12 @@
     <mergeCell ref="B71:C71"/>
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="A129:C129"/>
+    <mergeCell ref="B130:C130"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -26459,7 +26459,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Creating attacks of opportunity on char creation
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716" firstSheet="13" activeTab="23"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TODO - Quick Battle" sheetId="37" r:id="rId1"/>
@@ -644,7 +644,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2346" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2461" uniqueCount="1176">
   <si>
     <t>Fishing</t>
   </si>
@@ -4040,6 +4040,138 @@
   </si>
   <si>
     <t>Restores Target Stamina</t>
+  </si>
+  <si>
+    <t>Holy Dampening</t>
+  </si>
+  <si>
+    <t>Target damag received is lowered by 20%</t>
+  </si>
+  <si>
+    <t>Increases amount</t>
+  </si>
+  <si>
+    <t>Healing Dawn</t>
+  </si>
+  <si>
+    <t>Heal 4 random nearby allies</t>
+  </si>
+  <si>
+    <t>Increases healing</t>
+  </si>
+  <si>
+    <t>Increases number heaed</t>
+  </si>
+  <si>
+    <t>Shield Ward</t>
+  </si>
+  <si>
+    <t>Target gains a ward that produces a shield when damaged</t>
+  </si>
+  <si>
+    <t>Minor Shield</t>
+  </si>
+  <si>
+    <t>Target gains a shield</t>
+  </si>
+  <si>
+    <t>Reassuring Touch</t>
+  </si>
+  <si>
+    <t>Target gains morale</t>
+  </si>
+  <si>
+    <t>Nearby allies gain morale</t>
+  </si>
+  <si>
+    <t>Prayer of Morale</t>
+  </si>
+  <si>
+    <t>Healing Beacon</t>
+  </si>
+  <si>
+    <t>Target receives buff that doubles heals received.  Nearby allies receive small % of heals</t>
+  </si>
+  <si>
+    <t>Caster receives buff.  Each turn, caster heals all adjacent allies</t>
+  </si>
+  <si>
+    <t>Prayer of Battle</t>
+  </si>
+  <si>
+    <t>Nearby allies gain parry, block, and melee skill</t>
+  </si>
+  <si>
+    <t>Champion's Boon</t>
+  </si>
+  <si>
+    <t>Ally gains a boon that buffs target with constitution on each attack</t>
+  </si>
+  <si>
+    <t>Holy Emanation</t>
+  </si>
+  <si>
+    <t>Regrowth</t>
+  </si>
+  <si>
+    <t>Nature</t>
+  </si>
+  <si>
+    <t>Grass</t>
+  </si>
+  <si>
+    <t>Grass 3</t>
+  </si>
+  <si>
+    <t>Heals target and gives target a HoT</t>
+  </si>
+  <si>
+    <t>Rejuvenation</t>
+  </si>
+  <si>
+    <t>Grass 1</t>
+  </si>
+  <si>
+    <t>Nourish</t>
+  </si>
+  <si>
+    <t>Grass 2</t>
+  </si>
+  <si>
+    <t>Hot</t>
+  </si>
+  <si>
+    <t>Lifebloom</t>
+  </si>
+  <si>
+    <t>Grass 4</t>
+  </si>
+  <si>
+    <t>HoT.  When HoT expires, it heals target</t>
+  </si>
+  <si>
+    <t>Swiftmend</t>
+  </si>
+  <si>
+    <t>Grass 5</t>
+  </si>
+  <si>
+    <t>Drastically heals target.  Consumes HoTs on target for 1/2 HoT remaining.  Can only use on target with HoT</t>
+  </si>
+  <si>
+    <t>Immunity</t>
+  </si>
+  <si>
+    <t>Light 7</t>
+  </si>
+  <si>
+    <t>Target is immune to all damage and negative effects for duration</t>
+  </si>
+  <si>
+    <t>Shelter</t>
+  </si>
+  <si>
+    <t>Caster and adjacent allies gain shields</t>
   </si>
 </sst>
 </file>
@@ -4890,7 +5022,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5228,6 +5360,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5636,29 +5771,29 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="154" t="s">
         <v>781</v>
       </c>
-      <c r="B2" s="154"/>
-      <c r="C2" s="155"/>
+      <c r="B2" s="155"/>
+      <c r="C2" s="156"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="115">
         <v>1</v>
       </c>
-      <c r="B3" s="156" t="s">
+      <c r="B3" s="157" t="s">
         <v>782</v>
       </c>
-      <c r="C3" s="157"/>
+      <c r="C3" s="158"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B4" s="147" t="s">
+      <c r="B4" s="148" t="s">
         <v>783</v>
       </c>
-      <c r="C4" s="148"/>
+      <c r="C4" s="149"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="116"/>
@@ -5709,10 +5844,10 @@
       <c r="A10" s="116">
         <v>3</v>
       </c>
-      <c r="B10" s="149" t="s">
+      <c r="B10" s="150" t="s">
         <v>784</v>
       </c>
-      <c r="C10" s="150"/>
+      <c r="C10" s="151"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="116"/>
@@ -5727,10 +5862,10 @@
       <c r="A12" s="116">
         <v>4</v>
       </c>
-      <c r="B12" s="151" t="s">
+      <c r="B12" s="152" t="s">
         <v>785</v>
       </c>
-      <c r="C12" s="152"/>
+      <c r="C12" s="153"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="116"/>
@@ -5745,10 +5880,10 @@
       <c r="A14" s="116">
         <v>5</v>
       </c>
-      <c r="B14" s="151" t="s">
+      <c r="B14" s="152" t="s">
         <v>786</v>
       </c>
-      <c r="C14" s="152"/>
+      <c r="C14" s="153"/>
     </row>
     <row r="15" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="116"/>
@@ -5763,10 +5898,10 @@
       <c r="A16" s="117">
         <v>6</v>
       </c>
-      <c r="B16" s="158" t="s">
+      <c r="B16" s="159" t="s">
         <v>790</v>
       </c>
-      <c r="C16" s="159"/>
+      <c r="C16" s="160"/>
     </row>
     <row r="17" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="116"/>
@@ -5781,46 +5916,46 @@
       <c r="A18" s="117">
         <v>7</v>
       </c>
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="159" t="s">
         <v>911</v>
       </c>
-      <c r="C18" s="159"/>
+      <c r="C18" s="160"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="132">
         <v>8</v>
       </c>
-      <c r="B19" s="158" t="s">
+      <c r="B19" s="159" t="s">
         <v>996</v>
       </c>
-      <c r="C19" s="159"/>
+      <c r="C19" s="160"/>
     </row>
     <row r="20" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="132">
         <v>9</v>
       </c>
-      <c r="B20" s="158" t="s">
+      <c r="B20" s="159" t="s">
         <v>912</v>
       </c>
-      <c r="C20" s="159"/>
+      <c r="C20" s="160"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="153" t="s">
+      <c r="A23" s="154" t="s">
         <v>792</v>
       </c>
-      <c r="B23" s="154"/>
-      <c r="C23" s="155"/>
+      <c r="B23" s="155"/>
+      <c r="C23" s="156"/>
     </row>
     <row r="24" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="115">
         <v>1</v>
       </c>
-      <c r="B24" s="156" t="s">
+      <c r="B24" s="157" t="s">
         <v>781</v>
       </c>
-      <c r="C24" s="157"/>
+      <c r="C24" s="158"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="116"/>
@@ -5836,10 +5971,10 @@
       <c r="A27" s="116">
         <v>2</v>
       </c>
-      <c r="B27" s="147" t="s">
+      <c r="B27" s="148" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="148"/>
+      <c r="C27" s="149"/>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="116"/>
@@ -5863,10 +5998,10 @@
       <c r="A30" s="116">
         <v>3</v>
       </c>
-      <c r="B30" s="147" t="s">
+      <c r="B30" s="148" t="s">
         <v>997</v>
       </c>
-      <c r="C30" s="148"/>
+      <c r="C30" s="149"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="116"/>
@@ -5888,20 +6023,20 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="153" t="s">
+      <c r="A34" s="154" t="s">
         <v>796</v>
       </c>
-      <c r="B34" s="154"/>
-      <c r="C34" s="155"/>
+      <c r="B34" s="155"/>
+      <c r="C34" s="156"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="115">
         <v>1</v>
       </c>
-      <c r="B35" s="156" t="s">
+      <c r="B35" s="157" t="s">
         <v>797</v>
       </c>
-      <c r="C35" s="157"/>
+      <c r="C35" s="158"/>
     </row>
     <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="116"/>
@@ -5937,20 +6072,20 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="153" t="s">
+      <c r="A41" s="154" t="s">
         <v>800</v>
       </c>
-      <c r="B41" s="154"/>
-      <c r="C41" s="155"/>
+      <c r="B41" s="155"/>
+      <c r="C41" s="156"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="115">
         <v>1</v>
       </c>
-      <c r="B42" s="156" t="s">
+      <c r="B42" s="157" t="s">
         <v>801</v>
       </c>
-      <c r="C42" s="157"/>
+      <c r="C42" s="158"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="116"/>
@@ -5974,10 +6109,10 @@
       <c r="A45" s="115">
         <v>1</v>
       </c>
-      <c r="B45" s="156" t="s">
+      <c r="B45" s="157" t="s">
         <v>803</v>
       </c>
-      <c r="C45" s="157"/>
+      <c r="C45" s="158"/>
     </row>
     <row r="46" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="116"/>
@@ -6013,263 +6148,263 @@
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="153" t="s">
+      <c r="A51" s="154" t="s">
         <v>188</v>
       </c>
-      <c r="B51" s="154"/>
-      <c r="C51" s="155"/>
+      <c r="B51" s="155"/>
+      <c r="C51" s="156"/>
     </row>
     <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="115">
         <v>1</v>
       </c>
-      <c r="B52" s="156" t="s">
+      <c r="B52" s="157" t="s">
         <v>808</v>
       </c>
-      <c r="C52" s="157"/>
+      <c r="C52" s="158"/>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="153" t="s">
+      <c r="A54" s="154" t="s">
         <v>789</v>
       </c>
-      <c r="B54" s="154"/>
-      <c r="C54" s="155"/>
+      <c r="B54" s="155"/>
+      <c r="C54" s="156"/>
     </row>
     <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="115">
         <v>1</v>
       </c>
-      <c r="B55" s="149" t="s">
+      <c r="B55" s="150" t="s">
         <v>782</v>
       </c>
-      <c r="C55" s="150"/>
+      <c r="C55" s="151"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="116">
         <v>2</v>
       </c>
-      <c r="B56" s="160" t="s">
+      <c r="B56" s="161" t="s">
         <v>783</v>
       </c>
-      <c r="C56" s="161"/>
+      <c r="C56" s="162"/>
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="116">
         <v>3</v>
       </c>
-      <c r="B57" s="151" t="s">
+      <c r="B57" s="152" t="s">
         <v>784</v>
       </c>
-      <c r="C57" s="152"/>
+      <c r="C57" s="153"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="116">
         <v>4</v>
       </c>
-      <c r="B58" s="151" t="s">
+      <c r="B58" s="152" t="s">
         <v>785</v>
       </c>
-      <c r="C58" s="152"/>
+      <c r="C58" s="153"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="116">
         <v>5</v>
       </c>
-      <c r="B59" s="151" t="s">
+      <c r="B59" s="152" t="s">
         <v>786</v>
       </c>
-      <c r="C59" s="152"/>
+      <c r="C59" s="153"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="117">
         <v>6</v>
       </c>
-      <c r="B60" s="158" t="s">
+      <c r="B60" s="159" t="s">
         <v>790</v>
       </c>
-      <c r="C60" s="159"/>
+      <c r="C60" s="160"/>
     </row>
     <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="153" t="s">
+      <c r="A62" s="154" t="s">
         <v>809</v>
       </c>
-      <c r="B62" s="154"/>
-      <c r="C62" s="155"/>
+      <c r="B62" s="155"/>
+      <c r="C62" s="156"/>
     </row>
     <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="115">
         <v>1</v>
       </c>
-      <c r="B63" s="149" t="s">
+      <c r="B63" s="150" t="s">
         <v>782</v>
       </c>
-      <c r="C63" s="150"/>
+      <c r="C63" s="151"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="116">
         <v>2</v>
       </c>
-      <c r="B64" s="160" t="s">
+      <c r="B64" s="161" t="s">
         <v>783</v>
       </c>
-      <c r="C64" s="161"/>
+      <c r="C64" s="162"/>
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="116">
         <v>3</v>
       </c>
-      <c r="B65" s="151" t="s">
+      <c r="B65" s="152" t="s">
         <v>784</v>
       </c>
-      <c r="C65" s="152"/>
+      <c r="C65" s="153"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="116">
         <v>4</v>
       </c>
-      <c r="B66" s="151" t="s">
+      <c r="B66" s="152" t="s">
         <v>785</v>
       </c>
-      <c r="C66" s="152"/>
+      <c r="C66" s="153"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="116">
         <v>5</v>
       </c>
-      <c r="B67" s="151" t="s">
+      <c r="B67" s="152" t="s">
         <v>786</v>
       </c>
-      <c r="C67" s="152"/>
+      <c r="C67" s="153"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="117">
         <v>6</v>
       </c>
-      <c r="B68" s="158" t="s">
+      <c r="B68" s="159" t="s">
         <v>790</v>
       </c>
-      <c r="C68" s="159"/>
+      <c r="C68" s="160"/>
     </row>
     <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="153" t="s">
+      <c r="A70" s="154" t="s">
         <v>997</v>
       </c>
-      <c r="B70" s="154"/>
-      <c r="C70" s="155"/>
+      <c r="B70" s="155"/>
+      <c r="C70" s="156"/>
     </row>
     <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="115">
         <v>1</v>
       </c>
-      <c r="B71" s="149"/>
-      <c r="C71" s="150"/>
+      <c r="B71" s="150"/>
+      <c r="C71" s="151"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="116"/>
-      <c r="B72" s="160"/>
-      <c r="C72" s="161"/>
+      <c r="B72" s="161"/>
+      <c r="C72" s="162"/>
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="116"/>
-      <c r="B73" s="151"/>
-      <c r="C73" s="152"/>
+      <c r="B73" s="152"/>
+      <c r="C73" s="153"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="116"/>
-      <c r="B74" s="151"/>
-      <c r="C74" s="152"/>
+      <c r="B74" s="152"/>
+      <c r="C74" s="153"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="116"/>
-      <c r="B75" s="151"/>
-      <c r="C75" s="152"/>
+      <c r="B75" s="152"/>
+      <c r="C75" s="153"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="117"/>
-      <c r="B76" s="158"/>
-      <c r="C76" s="159"/>
+      <c r="B76" s="159"/>
+      <c r="C76" s="160"/>
     </row>
     <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="153" t="s">
+      <c r="A78" s="154" t="s">
         <v>810</v>
       </c>
-      <c r="B78" s="154"/>
-      <c r="C78" s="155"/>
+      <c r="B78" s="155"/>
+      <c r="C78" s="156"/>
     </row>
     <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="115">
         <v>1</v>
       </c>
-      <c r="B79" s="149" t="s">
+      <c r="B79" s="150" t="s">
         <v>782</v>
       </c>
-      <c r="C79" s="150"/>
+      <c r="C79" s="151"/>
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="116">
         <v>2</v>
       </c>
-      <c r="B80" s="160" t="s">
+      <c r="B80" s="161" t="s">
         <v>783</v>
       </c>
-      <c r="C80" s="161"/>
+      <c r="C80" s="162"/>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="116">
         <v>3</v>
       </c>
-      <c r="B81" s="151" t="s">
+      <c r="B81" s="152" t="s">
         <v>784</v>
       </c>
-      <c r="C81" s="152"/>
+      <c r="C81" s="153"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="116">
         <v>4</v>
       </c>
-      <c r="B82" s="151" t="s">
+      <c r="B82" s="152" t="s">
         <v>785</v>
       </c>
-      <c r="C82" s="152"/>
+      <c r="C82" s="153"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="116">
         <v>5</v>
       </c>
-      <c r="B83" s="151" t="s">
+      <c r="B83" s="152" t="s">
         <v>786</v>
       </c>
-      <c r="C83" s="152"/>
+      <c r="C83" s="153"/>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="117">
         <v>6</v>
       </c>
-      <c r="B84" s="158" t="s">
+      <c r="B84" s="159" t="s">
         <v>790</v>
       </c>
-      <c r="C84" s="159"/>
+      <c r="C84" s="160"/>
     </row>
     <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="153" t="s">
+      <c r="A86" s="154" t="s">
         <v>860</v>
       </c>
-      <c r="B86" s="154"/>
-      <c r="C86" s="155"/>
+      <c r="B86" s="155"/>
+      <c r="C86" s="156"/>
     </row>
     <row r="87" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="115">
         <v>1</v>
       </c>
-      <c r="B87" s="156" t="s">
+      <c r="B87" s="157" t="s">
         <v>101</v>
       </c>
-      <c r="C87" s="157"/>
+      <c r="C87" s="158"/>
     </row>
     <row r="88" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="124"/>
@@ -6442,10 +6577,10 @@
       <c r="A107" s="116">
         <v>2</v>
       </c>
-      <c r="B107" s="147" t="s">
+      <c r="B107" s="148" t="s">
         <v>811</v>
       </c>
-      <c r="C107" s="148"/>
+      <c r="C107" s="149"/>
     </row>
     <row r="108" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="116"/>
@@ -6523,10 +6658,10 @@
       <c r="A116" s="116">
         <v>3</v>
       </c>
-      <c r="B116" s="149" t="s">
+      <c r="B116" s="150" t="s">
         <v>812</v>
       </c>
-      <c r="C116" s="150"/>
+      <c r="C116" s="151"/>
     </row>
     <row r="117" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="116"/>
@@ -6582,10 +6717,10 @@
       <c r="A123" s="115">
         <v>4</v>
       </c>
-      <c r="B123" s="151" t="s">
+      <c r="B123" s="152" t="s">
         <v>813</v>
       </c>
-      <c r="C123" s="152"/>
+      <c r="C123" s="153"/>
     </row>
     <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="124"/>
@@ -6625,20 +6760,20 @@
     </row>
     <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="129" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="153" t="s">
+      <c r="A129" s="154" t="s">
         <v>861</v>
       </c>
-      <c r="B129" s="154"/>
-      <c r="C129" s="155"/>
+      <c r="B129" s="155"/>
+      <c r="C129" s="156"/>
     </row>
     <row r="130" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="115">
         <v>1</v>
       </c>
-      <c r="B130" s="156" t="s">
+      <c r="B130" s="157" t="s">
         <v>862</v>
       </c>
-      <c r="C130" s="157"/>
+      <c r="C130" s="158"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="124"/>
@@ -6785,10 +6920,10 @@
       <c r="A150" s="116">
         <v>2</v>
       </c>
-      <c r="B150" s="147" t="s">
+      <c r="B150" s="148" t="s">
         <v>863</v>
       </c>
-      <c r="C150" s="148"/>
+      <c r="C150" s="149"/>
     </row>
     <row r="151" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="116"/>
@@ -6858,10 +6993,10 @@
       <c r="A159" s="116">
         <v>3</v>
       </c>
-      <c r="B159" s="149" t="s">
+      <c r="B159" s="150" t="s">
         <v>864</v>
       </c>
-      <c r="C159" s="150"/>
+      <c r="C159" s="151"/>
     </row>
     <row r="160" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="116"/>
@@ -6983,8 +7118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7168,7 +7303,9 @@
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
@@ -7698,7 +7835,7 @@
   <dimension ref="A1:A40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8169,31 +8306,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="165" t="s">
+      <c r="B1" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="167"/>
-      <c r="K1" s="168" t="s">
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="168"/>
+      <c r="K1" s="169" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="169"/>
-      <c r="M1" s="169"/>
-      <c r="N1" s="169"/>
-      <c r="O1" s="169"/>
-      <c r="P1" s="169"/>
-      <c r="Q1" s="169"/>
-      <c r="R1" s="169"/>
-      <c r="S1" s="169"/>
-      <c r="T1" s="169"/>
-      <c r="U1" s="169"/>
-      <c r="V1" s="170"/>
+      <c r="L1" s="170"/>
+      <c r="M1" s="170"/>
+      <c r="N1" s="170"/>
+      <c r="O1" s="170"/>
+      <c r="P1" s="170"/>
+      <c r="Q1" s="170"/>
+      <c r="R1" s="170"/>
+      <c r="S1" s="170"/>
+      <c r="T1" s="170"/>
+      <c r="U1" s="170"/>
+      <c r="V1" s="171"/>
     </row>
     <row r="2" spans="1:22" ht="44.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K2" s="66" t="s">
@@ -22325,8 +22462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22345,17 +22482,17 @@
       <c r="A1" s="81" t="s">
         <v>363</v>
       </c>
-      <c r="B1" s="171" t="s">
+      <c r="B1" s="172" t="s">
         <v>365</v>
       </c>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172"/>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172"/>
-      <c r="I1" s="172"/>
-      <c r="J1" s="173"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
+      <c r="G1" s="173"/>
+      <c r="H1" s="173"/>
+      <c r="I1" s="173"/>
+      <c r="J1" s="174"/>
       <c r="K1" s="91" t="s">
         <v>364</v>
       </c>
@@ -24203,7 +24340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -24222,15 +24359,15 @@
       <c r="C1" t="s">
         <v>700</v>
       </c>
-      <c r="E1" s="174" t="s">
+      <c r="E1" s="175" t="s">
         <v>365</v>
       </c>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
-      <c r="H1" s="174"/>
-      <c r="I1" s="174"/>
-      <c r="J1" s="174"/>
-      <c r="K1" s="174"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
+      <c r="H1" s="175"/>
+      <c r="I1" s="175"/>
+      <c r="J1" s="175"/>
+      <c r="K1" s="175"/>
       <c r="L1" s="31"/>
     </row>
     <row r="2" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
@@ -25550,10 +25687,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL40"/>
+  <dimension ref="A1:BL44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26785,158 +26922,580 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="137"/>
+      <c r="A27" s="146" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B27" s="137" t="s">
+        <v>1083</v>
+      </c>
       <c r="C27" s="137"/>
-      <c r="D27" s="137"/>
+      <c r="D27" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E27" s="137" t="s">
+        <v>1085</v>
+      </c>
       <c r="F27" s="137"/>
-      <c r="G27" s="137"/>
-      <c r="H27" s="137"/>
-      <c r="I27" s="137"/>
-      <c r="J27" s="137"/>
+      <c r="G27" s="137" t="s">
+        <v>1086</v>
+      </c>
+      <c r="H27" s="137">
+        <v>3</v>
+      </c>
+      <c r="I27" s="137">
+        <v>1</v>
+      </c>
+      <c r="J27" s="137">
+        <v>3</v>
+      </c>
       <c r="K27" s="137"/>
+      <c r="L27" t="s">
+        <v>1133</v>
+      </c>
+      <c r="M27" t="s">
+        <v>1134</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="137"/>
+      <c r="A28" s="146" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B28" s="137" t="s">
+        <v>1083</v>
+      </c>
       <c r="C28" s="137"/>
-      <c r="D28" s="137"/>
+      <c r="D28" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E28" s="137" t="s">
+        <v>1085</v>
+      </c>
       <c r="F28" s="137"/>
-      <c r="G28" s="137"/>
-      <c r="H28" s="137"/>
-      <c r="I28" s="137"/>
+      <c r="G28" s="137" t="s">
+        <v>1097</v>
+      </c>
+      <c r="H28" s="137">
+        <v>0</v>
+      </c>
+      <c r="I28" s="137">
+        <v>1</v>
+      </c>
       <c r="J28" s="137"/>
       <c r="K28" s="137"/>
+      <c r="L28" t="s">
+        <v>1136</v>
+      </c>
+      <c r="M28" t="s">
+        <v>1137</v>
+      </c>
+      <c r="N28" t="s">
+        <v>1138</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="137"/>
+      <c r="A29" s="146" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B29" s="137" t="s">
+        <v>1083</v>
+      </c>
       <c r="C29" s="137"/>
-      <c r="D29" s="137"/>
+      <c r="D29" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E29" s="137" t="s">
+        <v>1085</v>
+      </c>
       <c r="F29" s="137"/>
-      <c r="G29" s="137"/>
-      <c r="H29" s="137"/>
-      <c r="I29" s="137"/>
-      <c r="J29" s="137"/>
+      <c r="G29" s="137" t="s">
+        <v>1097</v>
+      </c>
+      <c r="H29" s="137">
+        <v>3</v>
+      </c>
+      <c r="I29" s="137">
+        <v>1</v>
+      </c>
+      <c r="J29" s="137">
+        <v>3</v>
+      </c>
       <c r="K29" s="137"/>
+      <c r="L29" t="s">
+        <v>1140</v>
+      </c>
+      <c r="M29" t="s">
+        <v>1107</v>
+      </c>
+      <c r="N29" t="s">
+        <v>1128</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="137"/>
+      <c r="A30" s="146" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B30" s="137" t="s">
+        <v>1004</v>
+      </c>
       <c r="C30" s="137"/>
-      <c r="D30" s="137"/>
+      <c r="D30" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E30" s="137" t="s">
+        <v>1085</v>
+      </c>
       <c r="F30" s="137"/>
-      <c r="G30" s="137"/>
-      <c r="H30" s="137"/>
-      <c r="I30" s="137"/>
-      <c r="J30" s="137"/>
+      <c r="G30" s="137" t="s">
+        <v>1086</v>
+      </c>
+      <c r="H30" s="137">
+        <v>3</v>
+      </c>
+      <c r="I30" s="137">
+        <v>1</v>
+      </c>
+      <c r="J30" s="137">
+        <v>3</v>
+      </c>
       <c r="K30" s="137"/>
+      <c r="L30" t="s">
+        <v>1142</v>
+      </c>
+      <c r="M30" t="s">
+        <v>1107</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="137"/>
+      <c r="A31" s="146" t="s">
+        <v>888</v>
+      </c>
+      <c r="B31" s="137" t="s">
+        <v>1004</v>
+      </c>
       <c r="C31" s="137"/>
-      <c r="D31" s="137"/>
+      <c r="D31" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E31" s="137" t="s">
+        <v>1085</v>
+      </c>
       <c r="F31" s="137"/>
-      <c r="G31" s="137"/>
-      <c r="H31" s="137"/>
-      <c r="I31" s="137"/>
-      <c r="J31" s="137"/>
+      <c r="G31" s="137" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H31" s="137">
+        <v>3</v>
+      </c>
+      <c r="I31" s="137">
+        <v>1</v>
+      </c>
+      <c r="J31" s="137">
+        <v>4</v>
+      </c>
       <c r="K31" s="137"/>
+      <c r="L31" t="s">
+        <v>1142</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="137"/>
+      <c r="A32" s="146" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B32" s="137" t="s">
+        <v>1083</v>
+      </c>
       <c r="C32" s="137"/>
-      <c r="D32" s="137"/>
+      <c r="D32" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E32" s="137" t="s">
+        <v>1085</v>
+      </c>
       <c r="F32" s="137"/>
-      <c r="G32" s="137"/>
-      <c r="H32" s="137"/>
-      <c r="I32" s="137"/>
+      <c r="G32" s="137" t="s">
+        <v>1090</v>
+      </c>
+      <c r="H32" s="137">
+        <v>1</v>
+      </c>
+      <c r="I32" s="137">
+        <v>0</v>
+      </c>
       <c r="J32" s="137"/>
       <c r="K32" s="137"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="137"/>
+      <c r="L32" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="146" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B33" s="137" t="s">
+        <v>1083</v>
+      </c>
       <c r="C33" s="137"/>
-      <c r="D33" s="137"/>
+      <c r="D33" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E33" s="137" t="s">
+        <v>1085</v>
+      </c>
       <c r="F33" s="137"/>
-      <c r="G33" s="137"/>
-      <c r="H33" s="137"/>
-      <c r="I33" s="137"/>
+      <c r="G33" s="137" t="s">
+        <v>1086</v>
+      </c>
+      <c r="H33" s="137">
+        <v>0</v>
+      </c>
+      <c r="I33" s="137">
+        <v>0</v>
+      </c>
       <c r="J33" s="137"/>
       <c r="K33" s="137"/>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="137"/>
+      <c r="L33" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="146" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B34" s="137" t="s">
+        <v>1083</v>
+      </c>
       <c r="C34" s="137"/>
-      <c r="D34" s="137"/>
+      <c r="D34" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E34" s="137" t="s">
+        <v>1085</v>
+      </c>
       <c r="F34" s="137"/>
-      <c r="G34" s="137"/>
-      <c r="H34" s="137"/>
-      <c r="I34" s="137"/>
-      <c r="J34" s="137"/>
+      <c r="G34" s="137" t="s">
+        <v>1124</v>
+      </c>
+      <c r="H34" s="137">
+        <v>3</v>
+      </c>
+      <c r="I34" s="137">
+        <v>2</v>
+      </c>
+      <c r="J34" s="137">
+        <v>4</v>
+      </c>
       <c r="K34" s="137"/>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="137"/>
+      <c r="L34" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="146" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B35" s="137" t="s">
+        <v>1083</v>
+      </c>
       <c r="C35" s="137"/>
-      <c r="D35" s="137"/>
+      <c r="D35" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E35" s="137" t="s">
+        <v>1085</v>
+      </c>
       <c r="F35" s="137"/>
-      <c r="G35" s="137"/>
-      <c r="H35" s="137"/>
-      <c r="I35" s="137"/>
-      <c r="J35" s="137"/>
+      <c r="G35" s="137" t="s">
+        <v>1124</v>
+      </c>
+      <c r="H35" s="137">
+        <v>0</v>
+      </c>
+      <c r="I35" s="137">
+        <v>2</v>
+      </c>
+      <c r="J35" s="137">
+        <v>4</v>
+      </c>
       <c r="K35" s="137"/>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="137"/>
+      <c r="L35" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="146" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B36" s="137" t="s">
+        <v>1083</v>
+      </c>
       <c r="C36" s="137"/>
-      <c r="D36" s="137"/>
+      <c r="D36" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E36" s="137" t="s">
+        <v>1085</v>
+      </c>
       <c r="F36" s="137"/>
-      <c r="G36" s="137"/>
-      <c r="H36" s="137"/>
-      <c r="I36" s="137"/>
-      <c r="J36" s="137"/>
+      <c r="G36" s="137" t="s">
+        <v>1086</v>
+      </c>
+      <c r="H36" s="137">
+        <v>0</v>
+      </c>
+      <c r="I36" s="137">
+        <v>1</v>
+      </c>
+      <c r="J36" s="137">
+        <v>3</v>
+      </c>
       <c r="K36" s="137"/>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="137"/>
+      <c r="L36" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="146" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B37" s="137" t="s">
+        <v>1083</v>
+      </c>
       <c r="C37" s="137"/>
-      <c r="D37" s="137"/>
+      <c r="D37" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E37" s="137" t="s">
+        <v>1085</v>
+      </c>
       <c r="F37" s="137"/>
-      <c r="G37" s="137"/>
-      <c r="H37" s="137"/>
-      <c r="I37" s="137"/>
-      <c r="J37" s="137"/>
+      <c r="G37" s="137" t="s">
+        <v>1097</v>
+      </c>
+      <c r="H37" s="137">
+        <v>3</v>
+      </c>
+      <c r="I37" s="137">
+        <v>1</v>
+      </c>
+      <c r="J37" s="137">
+        <v>3</v>
+      </c>
       <c r="K37" s="137"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="137"/>
+      <c r="L37" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="146" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B38" s="137" t="s">
+        <v>1156</v>
+      </c>
       <c r="C38" s="137"/>
-      <c r="D38" s="137"/>
+      <c r="D38" s="137" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E38" s="137" t="s">
+        <v>1085</v>
+      </c>
       <c r="F38" s="137"/>
-      <c r="G38" s="137"/>
-      <c r="H38" s="137"/>
-      <c r="I38" s="137"/>
-      <c r="J38" s="137"/>
+      <c r="G38" s="137" t="s">
+        <v>1158</v>
+      </c>
+      <c r="H38" s="137">
+        <v>3</v>
+      </c>
+      <c r="I38" s="137">
+        <v>1</v>
+      </c>
+      <c r="J38" s="137">
+        <v>3</v>
+      </c>
       <c r="K38" s="137"/>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="137"/>
+      <c r="L38" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="146" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B39" s="137" t="s">
+        <v>1156</v>
+      </c>
       <c r="C39" s="137"/>
-      <c r="D39" s="137"/>
+      <c r="D39" s="137" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E39" s="137" t="s">
+        <v>1085</v>
+      </c>
       <c r="F39" s="137"/>
-      <c r="G39" s="137"/>
-      <c r="H39" s="137"/>
-      <c r="I39" s="137"/>
-      <c r="J39" s="137"/>
+      <c r="G39" s="137" t="s">
+        <v>1161</v>
+      </c>
+      <c r="H39" s="137">
+        <v>3</v>
+      </c>
+      <c r="I39" s="137">
+        <v>0</v>
+      </c>
+      <c r="J39" s="137">
+        <v>3</v>
+      </c>
       <c r="K39" s="137"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="137"/>
+      <c r="L39" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="146" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B40" s="137" t="s">
+        <v>1156</v>
+      </c>
       <c r="C40" s="137"/>
-      <c r="D40" s="137"/>
+      <c r="D40" s="137" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E40" s="137" t="s">
+        <v>1085</v>
+      </c>
       <c r="F40" s="137"/>
-      <c r="G40" s="137"/>
-      <c r="H40" s="137"/>
-      <c r="I40" s="137"/>
-      <c r="J40" s="137"/>
+      <c r="G40" s="137" t="s">
+        <v>1163</v>
+      </c>
+      <c r="H40" s="137">
+        <v>3</v>
+      </c>
+      <c r="I40" s="137">
+        <v>1</v>
+      </c>
+      <c r="J40" s="137">
+        <v>6</v>
+      </c>
       <c r="K40" s="137"/>
+      <c r="L40" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="146" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B41" s="147" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D41" s="147" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E41" s="137" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G41" s="147" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H41" s="147">
+        <v>3</v>
+      </c>
+      <c r="I41" s="147">
+        <v>1</v>
+      </c>
+      <c r="J41" s="147">
+        <v>5</v>
+      </c>
+      <c r="L41" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="146" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B42" s="147" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D42" s="147" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E42" s="137" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G42" s="147" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H42" s="147">
+        <v>3</v>
+      </c>
+      <c r="I42" s="147">
+        <v>1</v>
+      </c>
+      <c r="J42" s="147">
+        <v>0</v>
+      </c>
+      <c r="L42" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="146" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B43" s="147" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D43" s="147" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E43" s="137" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G43" s="147" t="s">
+        <v>1172</v>
+      </c>
+      <c r="H43" s="147">
+        <v>2</v>
+      </c>
+      <c r="I43" s="147">
+        <v>1</v>
+      </c>
+      <c r="J43" s="147">
+        <v>1</v>
+      </c>
+      <c r="L43" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="146" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B44" s="147" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D44" s="147" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E44" s="137" t="s">
+        <v>422</v>
+      </c>
+      <c r="G44" s="147" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H44" s="147">
+        <v>0</v>
+      </c>
+      <c r="I44" s="147">
+        <v>1</v>
+      </c>
+      <c r="J44" s="147">
+        <v>4</v>
+      </c>
+      <c r="L44" t="s">
+        <v>1175</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27805,24 +28364,24 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="100"/>
-      <c r="B1" s="164" t="s">
+      <c r="B1" s="165" t="s">
         <v>701</v>
       </c>
-      <c r="C1" s="164"/>
-      <c r="D1" s="164"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
       <c r="E1" s="101"/>
-      <c r="F1" s="162" t="s">
+      <c r="F1" s="163" t="s">
         <v>350</v>
       </c>
-      <c r="G1" s="162"/>
-      <c r="H1" s="162"/>
-      <c r="I1" s="162"/>
-      <c r="J1" s="162"/>
-      <c r="K1" s="162"/>
-      <c r="L1" s="162"/>
-      <c r="M1" s="162"/>
-      <c r="N1" s="162"/>
-      <c r="O1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
+      <c r="J1" s="163"/>
+      <c r="K1" s="163"/>
+      <c r="L1" s="163"/>
+      <c r="M1" s="163"/>
+      <c r="N1" s="163"/>
+      <c r="O1" s="164"/>
       <c r="P1" s="30"/>
       <c r="Q1" s="30"/>
       <c r="R1" s="30"/>

</xml_diff>

<commit_message>
Adding rejuvenation ability and implementing HoTs
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716" activeTab="9"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716" firstSheet="13" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="TODO - Quick Battle" sheetId="37" r:id="rId1"/>
@@ -3961,9 +3961,6 @@
     <t>Remove all buffs on target, caster gains a Ghost DoT for each buff removed</t>
   </si>
   <si>
-    <t>Quick Shield</t>
-  </si>
-  <si>
     <t>Shield target with a massive, short duration shield</t>
   </si>
   <si>
@@ -4172,6 +4169,9 @@
   </si>
   <si>
     <t>Caster and adjacent allies gain shields</t>
+  </si>
+  <si>
+    <t>Quick Barrier</t>
   </si>
 </sst>
 </file>
@@ -5365,22 +5365,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5398,10 +5392,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5771,29 +5771,29 @@
       <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="154" t="s">
+      <c r="A2" s="152" t="s">
         <v>781</v>
       </c>
-      <c r="B2" s="155"/>
-      <c r="C2" s="156"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="154"/>
     </row>
     <row r="3" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="115">
         <v>1</v>
       </c>
-      <c r="B3" s="157" t="s">
+      <c r="B3" s="155" t="s">
         <v>782</v>
       </c>
-      <c r="C3" s="158"/>
+      <c r="C3" s="156"/>
     </row>
     <row r="4" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B4" s="148" t="s">
+      <c r="B4" s="157" t="s">
         <v>783</v>
       </c>
-      <c r="C4" s="149"/>
+      <c r="C4" s="158"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="116"/>
@@ -5844,10 +5844,10 @@
       <c r="A10" s="116">
         <v>3</v>
       </c>
-      <c r="B10" s="150" t="s">
+      <c r="B10" s="159" t="s">
         <v>784</v>
       </c>
-      <c r="C10" s="151"/>
+      <c r="C10" s="160"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="116"/>
@@ -5862,10 +5862,10 @@
       <c r="A12" s="116">
         <v>4</v>
       </c>
-      <c r="B12" s="152" t="s">
+      <c r="B12" s="148" t="s">
         <v>785</v>
       </c>
-      <c r="C12" s="153"/>
+      <c r="C12" s="149"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="116"/>
@@ -5880,10 +5880,10 @@
       <c r="A14" s="116">
         <v>5</v>
       </c>
-      <c r="B14" s="152" t="s">
+      <c r="B14" s="148" t="s">
         <v>786</v>
       </c>
-      <c r="C14" s="153"/>
+      <c r="C14" s="149"/>
     </row>
     <row r="15" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="116"/>
@@ -5898,10 +5898,10 @@
       <c r="A16" s="117">
         <v>6</v>
       </c>
-      <c r="B16" s="159" t="s">
+      <c r="B16" s="150" t="s">
         <v>790</v>
       </c>
-      <c r="C16" s="160"/>
+      <c r="C16" s="151"/>
     </row>
     <row r="17" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="116"/>
@@ -5916,46 +5916,46 @@
       <c r="A18" s="117">
         <v>7</v>
       </c>
-      <c r="B18" s="159" t="s">
+      <c r="B18" s="150" t="s">
         <v>911</v>
       </c>
-      <c r="C18" s="160"/>
+      <c r="C18" s="151"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="132">
         <v>8</v>
       </c>
-      <c r="B19" s="159" t="s">
+      <c r="B19" s="150" t="s">
         <v>996</v>
       </c>
-      <c r="C19" s="160"/>
+      <c r="C19" s="151"/>
     </row>
     <row r="20" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="132">
         <v>9</v>
       </c>
-      <c r="B20" s="159" t="s">
+      <c r="B20" s="150" t="s">
         <v>912</v>
       </c>
-      <c r="C20" s="160"/>
+      <c r="C20" s="151"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="154" t="s">
+      <c r="A23" s="152" t="s">
         <v>792</v>
       </c>
-      <c r="B23" s="155"/>
-      <c r="C23" s="156"/>
+      <c r="B23" s="153"/>
+      <c r="C23" s="154"/>
     </row>
     <row r="24" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="115">
         <v>1</v>
       </c>
-      <c r="B24" s="157" t="s">
+      <c r="B24" s="155" t="s">
         <v>781</v>
       </c>
-      <c r="C24" s="158"/>
+      <c r="C24" s="156"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="116"/>
@@ -5971,10 +5971,10 @@
       <c r="A27" s="116">
         <v>2</v>
       </c>
-      <c r="B27" s="148" t="s">
+      <c r="B27" s="157" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="149"/>
+      <c r="C27" s="158"/>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="116"/>
@@ -5998,10 +5998,10 @@
       <c r="A30" s="116">
         <v>3</v>
       </c>
-      <c r="B30" s="148" t="s">
+      <c r="B30" s="157" t="s">
         <v>997</v>
       </c>
-      <c r="C30" s="149"/>
+      <c r="C30" s="158"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="116"/>
@@ -6023,20 +6023,20 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="154" t="s">
+      <c r="A34" s="152" t="s">
         <v>796</v>
       </c>
-      <c r="B34" s="155"/>
-      <c r="C34" s="156"/>
+      <c r="B34" s="153"/>
+      <c r="C34" s="154"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="115">
         <v>1</v>
       </c>
-      <c r="B35" s="157" t="s">
+      <c r="B35" s="155" t="s">
         <v>797</v>
       </c>
-      <c r="C35" s="158"/>
+      <c r="C35" s="156"/>
     </row>
     <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="116"/>
@@ -6072,20 +6072,20 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="154" t="s">
+      <c r="A41" s="152" t="s">
         <v>800</v>
       </c>
-      <c r="B41" s="155"/>
-      <c r="C41" s="156"/>
+      <c r="B41" s="153"/>
+      <c r="C41" s="154"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="115">
         <v>1</v>
       </c>
-      <c r="B42" s="157" t="s">
+      <c r="B42" s="155" t="s">
         <v>801</v>
       </c>
-      <c r="C42" s="158"/>
+      <c r="C42" s="156"/>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="116"/>
@@ -6109,10 +6109,10 @@
       <c r="A45" s="115">
         <v>1</v>
       </c>
-      <c r="B45" s="157" t="s">
+      <c r="B45" s="155" t="s">
         <v>803</v>
       </c>
-      <c r="C45" s="158"/>
+      <c r="C45" s="156"/>
     </row>
     <row r="46" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="116"/>
@@ -6148,37 +6148,37 @@
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="154" t="s">
+      <c r="A51" s="152" t="s">
         <v>188</v>
       </c>
-      <c r="B51" s="155"/>
-      <c r="C51" s="156"/>
+      <c r="B51" s="153"/>
+      <c r="C51" s="154"/>
     </row>
     <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="115">
         <v>1</v>
       </c>
-      <c r="B52" s="157" t="s">
+      <c r="B52" s="155" t="s">
         <v>808</v>
       </c>
-      <c r="C52" s="158"/>
+      <c r="C52" s="156"/>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="154" t="s">
+      <c r="A54" s="152" t="s">
         <v>789</v>
       </c>
-      <c r="B54" s="155"/>
-      <c r="C54" s="156"/>
+      <c r="B54" s="153"/>
+      <c r="C54" s="154"/>
     </row>
     <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="115">
         <v>1</v>
       </c>
-      <c r="B55" s="150" t="s">
+      <c r="B55" s="159" t="s">
         <v>782</v>
       </c>
-      <c r="C55" s="151"/>
+      <c r="C55" s="160"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="116">
@@ -6193,54 +6193,54 @@
       <c r="A57" s="116">
         <v>3</v>
       </c>
-      <c r="B57" s="152" t="s">
+      <c r="B57" s="148" t="s">
         <v>784</v>
       </c>
-      <c r="C57" s="153"/>
+      <c r="C57" s="149"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="116">
         <v>4</v>
       </c>
-      <c r="B58" s="152" t="s">
+      <c r="B58" s="148" t="s">
         <v>785</v>
       </c>
-      <c r="C58" s="153"/>
+      <c r="C58" s="149"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="116">
         <v>5</v>
       </c>
-      <c r="B59" s="152" t="s">
+      <c r="B59" s="148" t="s">
         <v>786</v>
       </c>
-      <c r="C59" s="153"/>
+      <c r="C59" s="149"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="117">
         <v>6</v>
       </c>
-      <c r="B60" s="159" t="s">
+      <c r="B60" s="150" t="s">
         <v>790</v>
       </c>
-      <c r="C60" s="160"/>
+      <c r="C60" s="151"/>
     </row>
     <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="154" t="s">
+      <c r="A62" s="152" t="s">
         <v>809</v>
       </c>
-      <c r="B62" s="155"/>
-      <c r="C62" s="156"/>
+      <c r="B62" s="153"/>
+      <c r="C62" s="154"/>
     </row>
     <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="115">
         <v>1</v>
       </c>
-      <c r="B63" s="150" t="s">
+      <c r="B63" s="159" t="s">
         <v>782</v>
       </c>
-      <c r="C63" s="151"/>
+      <c r="C63" s="160"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="116">
@@ -6255,52 +6255,52 @@
       <c r="A65" s="116">
         <v>3</v>
       </c>
-      <c r="B65" s="152" t="s">
+      <c r="B65" s="148" t="s">
         <v>784</v>
       </c>
-      <c r="C65" s="153"/>
+      <c r="C65" s="149"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="116">
         <v>4</v>
       </c>
-      <c r="B66" s="152" t="s">
+      <c r="B66" s="148" t="s">
         <v>785</v>
       </c>
-      <c r="C66" s="153"/>
+      <c r="C66" s="149"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="116">
         <v>5</v>
       </c>
-      <c r="B67" s="152" t="s">
+      <c r="B67" s="148" t="s">
         <v>786</v>
       </c>
-      <c r="C67" s="153"/>
+      <c r="C67" s="149"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="117">
         <v>6</v>
       </c>
-      <c r="B68" s="159" t="s">
+      <c r="B68" s="150" t="s">
         <v>790</v>
       </c>
-      <c r="C68" s="160"/>
+      <c r="C68" s="151"/>
     </row>
     <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="154" t="s">
+      <c r="A70" s="152" t="s">
         <v>997</v>
       </c>
-      <c r="B70" s="155"/>
-      <c r="C70" s="156"/>
+      <c r="B70" s="153"/>
+      <c r="C70" s="154"/>
     </row>
     <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="115">
         <v>1</v>
       </c>
-      <c r="B71" s="150"/>
-      <c r="C71" s="151"/>
+      <c r="B71" s="159"/>
+      <c r="C71" s="160"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="116"/>
@@ -6309,40 +6309,40 @@
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="116"/>
-      <c r="B73" s="152"/>
-      <c r="C73" s="153"/>
+      <c r="B73" s="148"/>
+      <c r="C73" s="149"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="116"/>
-      <c r="B74" s="152"/>
-      <c r="C74" s="153"/>
+      <c r="B74" s="148"/>
+      <c r="C74" s="149"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="116"/>
-      <c r="B75" s="152"/>
-      <c r="C75" s="153"/>
+      <c r="B75" s="148"/>
+      <c r="C75" s="149"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="117"/>
-      <c r="B76" s="159"/>
-      <c r="C76" s="160"/>
+      <c r="B76" s="150"/>
+      <c r="C76" s="151"/>
     </row>
     <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="154" t="s">
+      <c r="A78" s="152" t="s">
         <v>810</v>
       </c>
-      <c r="B78" s="155"/>
-      <c r="C78" s="156"/>
+      <c r="B78" s="153"/>
+      <c r="C78" s="154"/>
     </row>
     <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="115">
         <v>1</v>
       </c>
-      <c r="B79" s="150" t="s">
+      <c r="B79" s="159" t="s">
         <v>782</v>
       </c>
-      <c r="C79" s="151"/>
+      <c r="C79" s="160"/>
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="116">
@@ -6357,54 +6357,54 @@
       <c r="A81" s="116">
         <v>3</v>
       </c>
-      <c r="B81" s="152" t="s">
+      <c r="B81" s="148" t="s">
         <v>784</v>
       </c>
-      <c r="C81" s="153"/>
+      <c r="C81" s="149"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="116">
         <v>4</v>
       </c>
-      <c r="B82" s="152" t="s">
+      <c r="B82" s="148" t="s">
         <v>785</v>
       </c>
-      <c r="C82" s="153"/>
+      <c r="C82" s="149"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="116">
         <v>5</v>
       </c>
-      <c r="B83" s="152" t="s">
+      <c r="B83" s="148" t="s">
         <v>786</v>
       </c>
-      <c r="C83" s="153"/>
+      <c r="C83" s="149"/>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="117">
         <v>6</v>
       </c>
-      <c r="B84" s="159" t="s">
+      <c r="B84" s="150" t="s">
         <v>790</v>
       </c>
-      <c r="C84" s="160"/>
+      <c r="C84" s="151"/>
     </row>
     <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="154" t="s">
+      <c r="A86" s="152" t="s">
         <v>860</v>
       </c>
-      <c r="B86" s="155"/>
-      <c r="C86" s="156"/>
+      <c r="B86" s="153"/>
+      <c r="C86" s="154"/>
     </row>
     <row r="87" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="115">
         <v>1</v>
       </c>
-      <c r="B87" s="157" t="s">
+      <c r="B87" s="155" t="s">
         <v>101</v>
       </c>
-      <c r="C87" s="158"/>
+      <c r="C87" s="156"/>
     </row>
     <row r="88" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="124"/>
@@ -6577,10 +6577,10 @@
       <c r="A107" s="116">
         <v>2</v>
       </c>
-      <c r="B107" s="148" t="s">
+      <c r="B107" s="157" t="s">
         <v>811</v>
       </c>
-      <c r="C107" s="149"/>
+      <c r="C107" s="158"/>
     </row>
     <row r="108" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="116"/>
@@ -6658,10 +6658,10 @@
       <c r="A116" s="116">
         <v>3</v>
       </c>
-      <c r="B116" s="150" t="s">
+      <c r="B116" s="159" t="s">
         <v>812</v>
       </c>
-      <c r="C116" s="151"/>
+      <c r="C116" s="160"/>
     </row>
     <row r="117" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="116"/>
@@ -6717,10 +6717,10 @@
       <c r="A123" s="115">
         <v>4</v>
       </c>
-      <c r="B123" s="152" t="s">
+      <c r="B123" s="148" t="s">
         <v>813</v>
       </c>
-      <c r="C123" s="153"/>
+      <c r="C123" s="149"/>
     </row>
     <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="124"/>
@@ -6760,20 +6760,20 @@
     </row>
     <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="129" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="154" t="s">
+      <c r="A129" s="152" t="s">
         <v>861</v>
       </c>
-      <c r="B129" s="155"/>
-      <c r="C129" s="156"/>
+      <c r="B129" s="153"/>
+      <c r="C129" s="154"/>
     </row>
     <row r="130" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="115">
         <v>1</v>
       </c>
-      <c r="B130" s="157" t="s">
+      <c r="B130" s="155" t="s">
         <v>862</v>
       </c>
-      <c r="C130" s="158"/>
+      <c r="C130" s="156"/>
     </row>
     <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="124"/>
@@ -6920,10 +6920,10 @@
       <c r="A150" s="116">
         <v>2</v>
       </c>
-      <c r="B150" s="148" t="s">
+      <c r="B150" s="157" t="s">
         <v>863</v>
       </c>
-      <c r="C150" s="149"/>
+      <c r="C150" s="158"/>
     </row>
     <row r="151" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="116"/>
@@ -6993,10 +6993,10 @@
       <c r="A159" s="116">
         <v>3</v>
       </c>
-      <c r="B159" s="150" t="s">
+      <c r="B159" s="159" t="s">
         <v>864</v>
       </c>
-      <c r="C159" s="151"/>
+      <c r="C159" s="160"/>
     </row>
     <row r="160" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="116"/>
@@ -7050,6 +7050,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="A129:C129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B42:C42"/>
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
@@ -7066,48 +7108,6 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="A129:C129"/>
-    <mergeCell ref="B130:C130"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -7118,7 +7118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
@@ -24340,7 +24340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -25689,8 +25689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26595,8 +26595,8 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="146" t="s">
-        <v>1105</v>
+      <c r="A17" s="136" t="s">
+        <v>1175</v>
       </c>
       <c r="B17" s="137" t="s">
         <v>1083</v>
@@ -26623,18 +26623,18 @@
       </c>
       <c r="K17" s="137"/>
       <c r="L17" t="s">
+        <v>1105</v>
+      </c>
+      <c r="M17" t="s">
         <v>1106</v>
       </c>
-      <c r="M17" t="s">
-        <v>1107</v>
-      </c>
       <c r="N17" s="144" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="146" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B18" s="137" t="s">
         <v>1083</v>
@@ -26659,12 +26659,12 @@
       <c r="J18" s="137"/>
       <c r="K18" s="137"/>
       <c r="L18" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="146" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B19" s="137" t="s">
         <v>1083</v>
@@ -26678,7 +26678,7 @@
       </c>
       <c r="F19" s="137"/>
       <c r="G19" s="137" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="H19" s="137">
         <v>1</v>
@@ -26689,12 +26689,12 @@
       <c r="J19" s="137"/>
       <c r="K19" s="137"/>
       <c r="L19" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="146" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B20" s="137" t="s">
         <v>1083</v>
@@ -26710,7 +26710,7 @@
       </c>
       <c r="F20" s="137"/>
       <c r="G20" s="137" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="H20" s="137">
         <v>4</v>
@@ -26721,7 +26721,7 @@
       <c r="J20" s="137"/>
       <c r="K20" s="137"/>
       <c r="L20" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="M20" t="s">
         <v>1048</v>
@@ -26729,7 +26729,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="146" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B21" s="137" t="s">
         <v>1083</v>
@@ -26754,18 +26754,18 @@
       <c r="J21" s="137"/>
       <c r="K21" s="137"/>
       <c r="L21" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="M21" t="s">
         <v>1092</v>
       </c>
       <c r="N21" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="146" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B22" s="137" t="s">
         <v>1083</v>
@@ -26790,12 +26790,12 @@
       <c r="J22" s="137"/>
       <c r="K22" s="137"/>
       <c r="L22" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="146" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B23" s="137" t="s">
         <v>1083</v>
@@ -26820,12 +26820,12 @@
       <c r="J23" s="137"/>
       <c r="K23" s="137"/>
       <c r="L23" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="146" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B24" s="137" t="s">
         <v>1083</v>
@@ -26839,7 +26839,7 @@
       </c>
       <c r="F24" s="137"/>
       <c r="G24" s="137" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="H24" s="137">
         <v>3</v>
@@ -26850,12 +26850,12 @@
       <c r="J24" s="137"/>
       <c r="K24" s="137"/>
       <c r="L24" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="146" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B25" s="137" t="s">
         <v>1083</v>
@@ -26882,18 +26882,18 @@
       </c>
       <c r="K25" s="137"/>
       <c r="L25" t="s">
+        <v>1125</v>
+      </c>
+      <c r="M25" t="s">
         <v>1126</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>1127</v>
-      </c>
-      <c r="N25" t="s">
-        <v>1128</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="146" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B26" s="137" t="s">
         <v>1083</v>
@@ -26918,12 +26918,12 @@
       <c r="J26" s="137"/>
       <c r="K26" s="137"/>
       <c r="L26" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="146" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="B27" s="137" t="s">
         <v>1083</v>
@@ -26950,15 +26950,15 @@
       </c>
       <c r="K27" s="137"/>
       <c r="L27" t="s">
+        <v>1132</v>
+      </c>
+      <c r="M27" t="s">
         <v>1133</v>
-      </c>
-      <c r="M27" t="s">
-        <v>1134</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="146" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B28" s="137" t="s">
         <v>1083</v>
@@ -26983,18 +26983,18 @@
       <c r="J28" s="137"/>
       <c r="K28" s="137"/>
       <c r="L28" t="s">
+        <v>1135</v>
+      </c>
+      <c r="M28" t="s">
         <v>1136</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>1137</v>
-      </c>
-      <c r="N28" t="s">
-        <v>1138</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="146" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B29" s="137" t="s">
         <v>1083</v>
@@ -27021,18 +27021,18 @@
       </c>
       <c r="K29" s="137"/>
       <c r="L29" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="M29" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="N29" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="146" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B30" s="137" t="s">
         <v>1004</v>
@@ -27059,10 +27059,10 @@
       </c>
       <c r="K30" s="137"/>
       <c r="L30" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="M30" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -27094,12 +27094,12 @@
       </c>
       <c r="K31" s="137"/>
       <c r="L31" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="146" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B32" s="137" t="s">
         <v>1083</v>
@@ -27124,12 +27124,12 @@
       <c r="J32" s="137"/>
       <c r="K32" s="137"/>
       <c r="L32" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="146" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="B33" s="137" t="s">
         <v>1083</v>
@@ -27154,12 +27154,12 @@
       <c r="J33" s="137"/>
       <c r="K33" s="137"/>
       <c r="L33" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="146" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="B34" s="137" t="s">
         <v>1083</v>
@@ -27173,7 +27173,7 @@
       </c>
       <c r="F34" s="137"/>
       <c r="G34" s="137" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="H34" s="137">
         <v>3</v>
@@ -27186,12 +27186,12 @@
       </c>
       <c r="K34" s="137"/>
       <c r="L34" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="146" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B35" s="137" t="s">
         <v>1083</v>
@@ -27205,7 +27205,7 @@
       </c>
       <c r="F35" s="137"/>
       <c r="G35" s="137" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="H35" s="137">
         <v>0</v>
@@ -27218,12 +27218,12 @@
       </c>
       <c r="K35" s="137"/>
       <c r="L35" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="146" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B36" s="137" t="s">
         <v>1083</v>
@@ -27250,12 +27250,12 @@
       </c>
       <c r="K36" s="137"/>
       <c r="L36" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="146" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B37" s="137" t="s">
         <v>1083</v>
@@ -27282,26 +27282,26 @@
       </c>
       <c r="K37" s="137"/>
       <c r="L37" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="146" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B38" s="137" t="s">
         <v>1155</v>
-      </c>
-      <c r="B38" s="137" t="s">
-        <v>1156</v>
       </c>
       <c r="C38" s="137"/>
       <c r="D38" s="137" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="E38" s="137" t="s">
         <v>1085</v>
       </c>
       <c r="F38" s="137"/>
       <c r="G38" s="137" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="H38" s="137">
         <v>3</v>
@@ -27314,26 +27314,26 @@
       </c>
       <c r="K38" s="137"/>
       <c r="L38" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="146" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B39" s="137" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C39" s="137"/>
       <c r="D39" s="137" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="E39" s="137" t="s">
         <v>1085</v>
       </c>
       <c r="F39" s="137"/>
       <c r="G39" s="137" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="H39" s="137">
         <v>3</v>
@@ -27351,21 +27351,21 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="146" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="B40" s="137" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C40" s="137"/>
       <c r="D40" s="137" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="E40" s="137" t="s">
         <v>1085</v>
       </c>
       <c r="F40" s="137"/>
       <c r="G40" s="137" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="H40" s="137">
         <v>3</v>
@@ -27378,24 +27378,24 @@
       </c>
       <c r="K40" s="137"/>
       <c r="L40" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="146" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="B41" s="147" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D41" s="147" t="s">
         <v>1156</v>
-      </c>
-      <c r="D41" s="147" t="s">
-        <v>1157</v>
       </c>
       <c r="E41" s="137" t="s">
         <v>1085</v>
       </c>
       <c r="G41" s="147" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="H41" s="147">
         <v>3</v>
@@ -27407,24 +27407,24 @@
         <v>5</v>
       </c>
       <c r="L41" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="146" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="B42" s="147" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D42" s="147" t="s">
         <v>1156</v>
-      </c>
-      <c r="D42" s="147" t="s">
-        <v>1157</v>
       </c>
       <c r="E42" s="137" t="s">
         <v>1085</v>
       </c>
       <c r="G42" s="147" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="H42" s="147">
         <v>3</v>
@@ -27436,12 +27436,12 @@
         <v>0</v>
       </c>
       <c r="L42" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="146" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="B43" s="147" t="s">
         <v>1083</v>
@@ -27453,7 +27453,7 @@
         <v>1085</v>
       </c>
       <c r="G43" s="147" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="H43" s="147">
         <v>2</v>
@@ -27465,12 +27465,12 @@
         <v>1</v>
       </c>
       <c r="L43" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="146" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B44" s="147" t="s">
         <v>1083</v>
@@ -27494,7 +27494,7 @@
         <v>4</v>
       </c>
       <c r="L44" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding stun functionality to new turn
</commit_message>
<xml_diff>
--- a/Spreadsheets/Spreadsheet.xlsx
+++ b/Spreadsheets/Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716" firstSheet="13" activeTab="23"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="10515" windowHeight="7230" tabRatio="716"/>
   </bookViews>
   <sheets>
     <sheet name="TODO - Quick Battle" sheetId="37" r:id="rId1"/>
@@ -644,7 +644,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2461" uniqueCount="1176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2459" uniqueCount="1175">
   <si>
     <t>Fishing</t>
   </si>
@@ -3638,9 +3638,6 @@
   </si>
   <si>
     <t>Spells</t>
-  </si>
-  <si>
-    <t>taking turns</t>
   </si>
   <si>
     <t>interrupts</t>
@@ -5022,7 +5019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5341,12 +5338,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -5365,16 +5356,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5392,16 +5389,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5753,10 +5744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C165"/>
+  <dimension ref="A1:C164"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5790,10 +5781,10 @@
       <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B4" s="157" t="s">
+      <c r="B4" s="146" t="s">
         <v>783</v>
       </c>
-      <c r="C4" s="158"/>
+      <c r="C4" s="147"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="116"/>
@@ -5844,10 +5835,10 @@
       <c r="A10" s="116">
         <v>3</v>
       </c>
-      <c r="B10" s="159" t="s">
+      <c r="B10" s="148" t="s">
         <v>784</v>
       </c>
-      <c r="C10" s="160"/>
+      <c r="C10" s="149"/>
     </row>
     <row r="11" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="116"/>
@@ -5862,10 +5853,10 @@
       <c r="A12" s="116">
         <v>4</v>
       </c>
-      <c r="B12" s="148" t="s">
+      <c r="B12" s="150" t="s">
         <v>785</v>
       </c>
-      <c r="C12" s="149"/>
+      <c r="C12" s="151"/>
     </row>
     <row r="13" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="116"/>
@@ -5880,10 +5871,10 @@
       <c r="A14" s="116">
         <v>5</v>
       </c>
-      <c r="B14" s="148" t="s">
+      <c r="B14" s="150" t="s">
         <v>786</v>
       </c>
-      <c r="C14" s="149"/>
+      <c r="C14" s="151"/>
     </row>
     <row r="15" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="116"/>
@@ -5898,10 +5889,10 @@
       <c r="A16" s="117">
         <v>6</v>
       </c>
-      <c r="B16" s="150" t="s">
+      <c r="B16" s="157" t="s">
         <v>790</v>
       </c>
-      <c r="C16" s="151"/>
+      <c r="C16" s="158"/>
     </row>
     <row r="17" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="116"/>
@@ -5916,28 +5907,28 @@
       <c r="A18" s="117">
         <v>7</v>
       </c>
-      <c r="B18" s="150" t="s">
+      <c r="B18" s="157" t="s">
         <v>911</v>
       </c>
-      <c r="C18" s="151"/>
+      <c r="C18" s="158"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="132">
         <v>8</v>
       </c>
-      <c r="B19" s="150" t="s">
+      <c r="B19" s="157" t="s">
         <v>996</v>
       </c>
-      <c r="C19" s="151"/>
+      <c r="C19" s="158"/>
     </row>
     <row r="20" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="132">
         <v>9</v>
       </c>
-      <c r="B20" s="150" t="s">
+      <c r="B20" s="157" t="s">
         <v>912</v>
       </c>
-      <c r="C20" s="151"/>
+      <c r="C20" s="158"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5971,10 +5962,10 @@
       <c r="A27" s="116">
         <v>2</v>
       </c>
-      <c r="B27" s="157" t="s">
+      <c r="B27" s="146" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="158"/>
+      <c r="C27" s="147"/>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="116"/>
@@ -5991,1110 +5982,1059 @@
         <v>788</v>
       </c>
       <c r="C29" s="121" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="116">
         <v>3</v>
       </c>
-      <c r="B30" s="157" t="s">
+      <c r="B30" s="146" t="s">
         <v>997</v>
       </c>
-      <c r="C30" s="158"/>
-    </row>
-    <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="147"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="116"/>
       <c r="B31" s="140" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C31" s="141" t="s">
         <v>998</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="116"/>
-      <c r="B32" s="142" t="s">
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="152" t="s">
+        <v>796</v>
+      </c>
+      <c r="B33" s="153"/>
+      <c r="C33" s="154"/>
+    </row>
+    <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="115">
+        <v>1</v>
+      </c>
+      <c r="B34" s="155" t="s">
+        <v>797</v>
+      </c>
+      <c r="C34" s="156"/>
+    </row>
+    <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="116"/>
+      <c r="B35" s="118" t="s">
+        <v>787</v>
+      </c>
+      <c r="C35" s="119" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="116"/>
+      <c r="B36" s="122" t="s">
         <v>788</v>
       </c>
-      <c r="C32" s="143" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="152" t="s">
-        <v>796</v>
-      </c>
-      <c r="B34" s="153"/>
-      <c r="C34" s="154"/>
-    </row>
-    <row r="35" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="115">
-        <v>1</v>
-      </c>
-      <c r="B35" s="155" t="s">
-        <v>797</v>
-      </c>
-      <c r="C35" s="156"/>
-    </row>
-    <row r="36" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="116"/>
-      <c r="B36" s="118" t="s">
-        <v>787</v>
-      </c>
-      <c r="C36" s="119" t="s">
-        <v>532</v>
+      <c r="C36" s="123" t="s">
+        <v>798</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="116"/>
       <c r="B37" s="122" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="C37" s="123" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="116"/>
-      <c r="B38" s="122" t="s">
-        <v>791</v>
-      </c>
-      <c r="C38" s="123" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="116"/>
-      <c r="B39" s="120"/>
-      <c r="C39" s="121"/>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="B38" s="120"/>
+      <c r="C38" s="121"/>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="152" t="s">
+        <v>800</v>
+      </c>
+      <c r="B40" s="153"/>
+      <c r="C40" s="154"/>
+    </row>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="152" t="s">
-        <v>800</v>
-      </c>
-      <c r="B41" s="153"/>
-      <c r="C41" s="154"/>
+      <c r="A41" s="115">
+        <v>1</v>
+      </c>
+      <c r="B41" s="155" t="s">
+        <v>801</v>
+      </c>
+      <c r="C41" s="156"/>
     </row>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="115">
-        <v>1</v>
-      </c>
-      <c r="B42" s="155" t="s">
-        <v>801</v>
-      </c>
-      <c r="C42" s="156"/>
-    </row>
-    <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="116"/>
-      <c r="B43" s="118" t="s">
+      <c r="A42" s="116"/>
+      <c r="B42" s="118" t="s">
         <v>787</v>
       </c>
-      <c r="C43" s="119" t="s">
+      <c r="C42" s="119" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="124"/>
-      <c r="B44" s="120" t="s">
+    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="124"/>
+      <c r="B43" s="120" t="s">
         <v>788</v>
       </c>
-      <c r="C44" s="121" t="s">
+      <c r="C43" s="121" t="s">
         <v>807</v>
       </c>
     </row>
+    <row r="44" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="115">
+        <v>1</v>
+      </c>
+      <c r="B44" s="155" t="s">
+        <v>803</v>
+      </c>
+      <c r="C44" s="156"/>
+    </row>
     <row r="45" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="115">
-        <v>1</v>
-      </c>
-      <c r="B45" s="155" t="s">
-        <v>803</v>
-      </c>
-      <c r="C45" s="156"/>
-    </row>
-    <row r="46" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="116"/>
+      <c r="B45" s="118" t="s">
+        <v>787</v>
+      </c>
+      <c r="C45" s="119" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="116"/>
-      <c r="B46" s="118" t="s">
-        <v>787</v>
-      </c>
-      <c r="C46" s="119" t="s">
-        <v>804</v>
+      <c r="B46" s="122" t="s">
+        <v>788</v>
+      </c>
+      <c r="C46" s="123" t="s">
+        <v>805</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="116"/>
       <c r="B47" s="122" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="C47" s="123" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="116"/>
-      <c r="B48" s="122" t="s">
-        <v>791</v>
-      </c>
-      <c r="C48" s="123" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="116"/>
-      <c r="B49" s="120"/>
-      <c r="C49" s="121"/>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="B48" s="120"/>
+      <c r="C48" s="121"/>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="152" t="s">
+        <v>188</v>
+      </c>
+      <c r="B50" s="153"/>
+      <c r="C50" s="154"/>
+    </row>
     <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="152" t="s">
-        <v>188</v>
-      </c>
-      <c r="B51" s="153"/>
-      <c r="C51" s="154"/>
-    </row>
-    <row r="52" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="115">
-        <v>1</v>
-      </c>
-      <c r="B52" s="155" t="s">
+      <c r="A51" s="115">
+        <v>1</v>
+      </c>
+      <c r="B51" s="155" t="s">
         <v>808</v>
       </c>
-      <c r="C52" s="156"/>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="C51" s="156"/>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="152" t="s">
+        <v>789</v>
+      </c>
+      <c r="B53" s="153"/>
+      <c r="C53" s="154"/>
+    </row>
     <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="152" t="s">
-        <v>789</v>
-      </c>
-      <c r="B54" s="153"/>
-      <c r="C54" s="154"/>
-    </row>
-    <row r="55" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="115">
-        <v>1</v>
+      <c r="A54" s="115">
+        <v>1</v>
+      </c>
+      <c r="B54" s="148" t="s">
+        <v>782</v>
+      </c>
+      <c r="C54" s="149"/>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="116">
+        <v>2</v>
       </c>
       <c r="B55" s="159" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C55" s="160"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="116">
-        <v>2</v>
-      </c>
-      <c r="B56" s="161" t="s">
-        <v>783</v>
-      </c>
-      <c r="C56" s="162"/>
+        <v>3</v>
+      </c>
+      <c r="B56" s="150" t="s">
+        <v>784</v>
+      </c>
+      <c r="C56" s="151"/>
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="116">
-        <v>3</v>
-      </c>
-      <c r="B57" s="148" t="s">
-        <v>784</v>
-      </c>
-      <c r="C57" s="149"/>
+        <v>4</v>
+      </c>
+      <c r="B57" s="150" t="s">
+        <v>785</v>
+      </c>
+      <c r="C57" s="151"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="116">
-        <v>4</v>
-      </c>
-      <c r="B58" s="148" t="s">
-        <v>785</v>
-      </c>
-      <c r="C58" s="149"/>
+        <v>5</v>
+      </c>
+      <c r="B58" s="150" t="s">
+        <v>786</v>
+      </c>
+      <c r="C58" s="151"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="116">
-        <v>5</v>
-      </c>
-      <c r="B59" s="148" t="s">
-        <v>786</v>
-      </c>
-      <c r="C59" s="149"/>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="117">
+      <c r="A59" s="117">
         <v>6</v>
       </c>
-      <c r="B60" s="150" t="s">
+      <c r="B59" s="157" t="s">
         <v>790</v>
       </c>
-      <c r="C60" s="151"/>
-    </row>
-    <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="C59" s="158"/>
+    </row>
+    <row r="60" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="152" t="s">
+        <v>809</v>
+      </c>
+      <c r="B61" s="153"/>
+      <c r="C61" s="154"/>
+    </row>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="152" t="s">
-        <v>809</v>
-      </c>
-      <c r="B62" s="153"/>
-      <c r="C62" s="154"/>
-    </row>
-    <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="115">
-        <v>1</v>
+      <c r="A62" s="115">
+        <v>1</v>
+      </c>
+      <c r="B62" s="148" t="s">
+        <v>782</v>
+      </c>
+      <c r="C62" s="149"/>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="116">
+        <v>2</v>
       </c>
       <c r="B63" s="159" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C63" s="160"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="116">
-        <v>2</v>
-      </c>
-      <c r="B64" s="161" t="s">
-        <v>783</v>
-      </c>
-      <c r="C64" s="162"/>
+        <v>3</v>
+      </c>
+      <c r="B64" s="150" t="s">
+        <v>784</v>
+      </c>
+      <c r="C64" s="151"/>
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="116">
-        <v>3</v>
-      </c>
-      <c r="B65" s="148" t="s">
-        <v>784</v>
-      </c>
-      <c r="C65" s="149"/>
+        <v>4</v>
+      </c>
+      <c r="B65" s="150" t="s">
+        <v>785</v>
+      </c>
+      <c r="C65" s="151"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="116">
-        <v>4</v>
-      </c>
-      <c r="B66" s="148" t="s">
-        <v>785</v>
-      </c>
-      <c r="C66" s="149"/>
+        <v>5</v>
+      </c>
+      <c r="B66" s="150" t="s">
+        <v>786</v>
+      </c>
+      <c r="C66" s="151"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="116">
-        <v>5</v>
-      </c>
-      <c r="B67" s="148" t="s">
-        <v>786</v>
-      </c>
-      <c r="C67" s="149"/>
-    </row>
-    <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="117">
+      <c r="A67" s="117">
         <v>6</v>
       </c>
-      <c r="B68" s="150" t="s">
+      <c r="B67" s="157" t="s">
         <v>790</v>
       </c>
-      <c r="C68" s="151"/>
-    </row>
-    <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="C67" s="158"/>
+    </row>
+    <row r="68" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="152" t="s">
+        <v>997</v>
+      </c>
+      <c r="B69" s="153"/>
+      <c r="C69" s="154"/>
+    </row>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="152" t="s">
-        <v>997</v>
-      </c>
-      <c r="B70" s="153"/>
-      <c r="C70" s="154"/>
-    </row>
-    <row r="71" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="115">
-        <v>1</v>
-      </c>
+      <c r="A70" s="115">
+        <v>1</v>
+      </c>
+      <c r="B70" s="148"/>
+      <c r="C70" s="149"/>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="116"/>
       <c r="B71" s="159"/>
       <c r="C71" s="160"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="116"/>
-      <c r="B72" s="161"/>
-      <c r="C72" s="162"/>
+      <c r="B72" s="150"/>
+      <c r="C72" s="151"/>
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="116"/>
-      <c r="B73" s="148"/>
-      <c r="C73" s="149"/>
+      <c r="B73" s="150"/>
+      <c r="C73" s="151"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="116"/>
-      <c r="B74" s="148"/>
-      <c r="C74" s="149"/>
+      <c r="B74" s="150"/>
+      <c r="C74" s="151"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="116"/>
-      <c r="B75" s="148"/>
-      <c r="C75" s="149"/>
-    </row>
-    <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="117"/>
-      <c r="B76" s="150"/>
-      <c r="C76" s="151"/>
-    </row>
-    <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="A75" s="117"/>
+      <c r="B75" s="157"/>
+      <c r="C75" s="158"/>
+    </row>
+    <row r="76" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="152" t="s">
+        <v>810</v>
+      </c>
+      <c r="B77" s="153"/>
+      <c r="C77" s="154"/>
+    </row>
     <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="152" t="s">
-        <v>810</v>
-      </c>
-      <c r="B78" s="153"/>
-      <c r="C78" s="154"/>
-    </row>
-    <row r="79" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="115">
-        <v>1</v>
+      <c r="A78" s="115">
+        <v>1</v>
+      </c>
+      <c r="B78" s="148" t="s">
+        <v>782</v>
+      </c>
+      <c r="C78" s="149"/>
+    </row>
+    <row r="79" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="116">
+        <v>2</v>
       </c>
       <c r="B79" s="159" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C79" s="160"/>
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="116">
-        <v>2</v>
-      </c>
-      <c r="B80" s="161" t="s">
-        <v>783</v>
-      </c>
-      <c r="C80" s="162"/>
+        <v>3</v>
+      </c>
+      <c r="B80" s="150" t="s">
+        <v>784</v>
+      </c>
+      <c r="C80" s="151"/>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="116">
-        <v>3</v>
-      </c>
-      <c r="B81" s="148" t="s">
-        <v>784</v>
-      </c>
-      <c r="C81" s="149"/>
+        <v>4</v>
+      </c>
+      <c r="B81" s="150" t="s">
+        <v>785</v>
+      </c>
+      <c r="C81" s="151"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="116">
-        <v>4</v>
-      </c>
-      <c r="B82" s="148" t="s">
-        <v>785</v>
-      </c>
-      <c r="C82" s="149"/>
+        <v>5</v>
+      </c>
+      <c r="B82" s="150" t="s">
+        <v>786</v>
+      </c>
+      <c r="C82" s="151"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="116">
-        <v>5</v>
-      </c>
-      <c r="B83" s="148" t="s">
-        <v>786</v>
-      </c>
-      <c r="C83" s="149"/>
-    </row>
-    <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="117">
+      <c r="A83" s="117">
         <v>6</v>
       </c>
-      <c r="B84" s="150" t="s">
+      <c r="B83" s="157" t="s">
         <v>790</v>
       </c>
-      <c r="C84" s="151"/>
-    </row>
-    <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="C83" s="158"/>
+    </row>
+    <row r="84" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="152" t="s">
+        <v>860</v>
+      </c>
+      <c r="B85" s="153"/>
+      <c r="C85" s="154"/>
+    </row>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="152" t="s">
-        <v>860</v>
-      </c>
-      <c r="B86" s="153"/>
-      <c r="C86" s="154"/>
+      <c r="A86" s="115">
+        <v>1</v>
+      </c>
+      <c r="B86" s="155" t="s">
+        <v>101</v>
+      </c>
+      <c r="C86" s="156"/>
     </row>
     <row r="87" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="115">
-        <v>1</v>
-      </c>
-      <c r="B87" s="155" t="s">
-        <v>101</v>
-      </c>
-      <c r="C87" s="156"/>
-    </row>
-    <row r="88" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="124"/>
+      <c r="B87" s="118" t="s">
+        <v>787</v>
+      </c>
+      <c r="C87" s="119" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="124"/>
-      <c r="B88" s="118" t="s">
-        <v>787</v>
-      </c>
-      <c r="C88" s="119" t="s">
-        <v>837</v>
+      <c r="B88" s="127" t="s">
+        <v>788</v>
+      </c>
+      <c r="C88" s="128" t="s">
+        <v>838</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="124"/>
       <c r="B89" s="127" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="C89" s="128" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="124"/>
       <c r="B90" s="127" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="C90" s="128" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="124"/>
       <c r="B91" s="127" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C91" s="128" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="124"/>
       <c r="B92" s="127" t="s">
-        <v>794</v>
+        <v>821</v>
       </c>
       <c r="C92" s="128" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="124"/>
       <c r="B93" s="127" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="C93" s="128" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="124"/>
       <c r="B94" s="127" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="C94" s="128" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="124"/>
       <c r="B95" s="127" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C95" s="128" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="124"/>
-      <c r="B96" s="127" t="s">
-        <v>826</v>
-      </c>
-      <c r="C96" s="128" t="s">
-        <v>845</v>
+      <c r="A96" s="116"/>
+      <c r="B96" s="122" t="s">
+        <v>827</v>
+      </c>
+      <c r="C96" s="123" t="s">
+        <v>846</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="116"/>
       <c r="B97" s="122" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C97" s="123" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="116"/>
       <c r="B98" s="122" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="C98" s="123" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="116"/>
       <c r="B99" s="122" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C99" s="123" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="116"/>
       <c r="B100" s="122" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C100" s="123" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="116"/>
       <c r="B101" s="122" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C101" s="123" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="116"/>
       <c r="B102" s="122" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C102" s="123" t="s">
-        <v>851</v>
+        <v>35</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="116"/>
       <c r="B103" s="122" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C103" s="123" t="s">
-        <v>35</v>
+        <v>852</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="116"/>
       <c r="B104" s="122" t="s">
-        <v>834</v>
-      </c>
-      <c r="C104" s="123" t="s">
-        <v>852</v>
-      </c>
+        <v>835</v>
+      </c>
+      <c r="C104" s="123"/>
     </row>
     <row r="105" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="116"/>
-      <c r="B105" s="122" t="s">
-        <v>835</v>
-      </c>
-      <c r="C105" s="123"/>
-    </row>
-    <row r="106" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="116"/>
-      <c r="B106" s="120" t="s">
+      <c r="B105" s="120" t="s">
         <v>836</v>
       </c>
-      <c r="C106" s="121"/>
+      <c r="C105" s="121"/>
+    </row>
+    <row r="106" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="116">
+        <v>2</v>
+      </c>
+      <c r="B106" s="146" t="s">
+        <v>811</v>
+      </c>
+      <c r="C106" s="147"/>
     </row>
     <row r="107" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="116">
-        <v>2</v>
-      </c>
-      <c r="B107" s="157" t="s">
-        <v>811</v>
-      </c>
-      <c r="C107" s="158"/>
-    </row>
-    <row r="108" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="116"/>
+      <c r="B107" s="118" t="s">
+        <v>787</v>
+      </c>
+      <c r="C107" s="119" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="116"/>
-      <c r="B108" s="118" t="s">
-        <v>787</v>
-      </c>
-      <c r="C108" s="119" t="s">
-        <v>824</v>
+      <c r="B108" s="122" t="s">
+        <v>788</v>
+      </c>
+      <c r="C108" s="123" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="116"/>
       <c r="B109" s="122" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="C109" s="123" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="116"/>
       <c r="B110" s="122" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="C110" s="123" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="116"/>
       <c r="B111" s="122" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C111" s="123" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="116"/>
-      <c r="B112" s="122" t="s">
-        <v>794</v>
-      </c>
-      <c r="C112" s="123" t="s">
-        <v>856</v>
+      <c r="B112" s="125" t="s">
+        <v>821</v>
+      </c>
+      <c r="C112" s="126" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="116"/>
       <c r="B113" s="125" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="C113" s="126" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="116"/>
-      <c r="B114" s="125" t="s">
-        <v>823</v>
-      </c>
-      <c r="C114" s="126" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="116"/>
-      <c r="B115" s="120" t="s">
+      <c r="B114" s="120" t="s">
         <v>825</v>
       </c>
-      <c r="C115" s="121" t="s">
+      <c r="C114" s="121" t="s">
         <v>859</v>
       </c>
     </row>
+    <row r="115" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="116">
+        <v>3</v>
+      </c>
+      <c r="B115" s="148" t="s">
+        <v>812</v>
+      </c>
+      <c r="C115" s="149"/>
+    </row>
     <row r="116" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="116">
-        <v>3</v>
-      </c>
-      <c r="B116" s="159" t="s">
-        <v>812</v>
-      </c>
-      <c r="C116" s="160"/>
-    </row>
-    <row r="117" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="116"/>
+      <c r="B116" s="118" t="s">
+        <v>787</v>
+      </c>
+      <c r="C116" s="119" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="116"/>
-      <c r="B117" s="118" t="s">
-        <v>787</v>
-      </c>
-      <c r="C117" s="119" t="s">
-        <v>818</v>
+      <c r="B117" s="122" t="s">
+        <v>788</v>
+      </c>
+      <c r="C117" s="123" t="s">
+        <v>819</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="116"/>
       <c r="B118" s="122" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="C118" s="123" t="s">
-        <v>819</v>
+        <v>89</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="116"/>
-      <c r="B119" s="122" t="s">
-        <v>791</v>
-      </c>
-      <c r="C119" s="123" t="s">
-        <v>89</v>
+      <c r="B119" s="125" t="s">
+        <v>793</v>
+      </c>
+      <c r="C119" s="126" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="116"/>
       <c r="B120" s="125" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C120" s="126" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="116"/>
-      <c r="B121" s="125" t="s">
-        <v>794</v>
-      </c>
-      <c r="C121" s="126" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="116"/>
-      <c r="B122" s="120"/>
-      <c r="C122" s="121"/>
+      <c r="B121" s="120"/>
+      <c r="C121" s="121"/>
+    </row>
+    <row r="122" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="115">
+        <v>4</v>
+      </c>
+      <c r="B122" s="150" t="s">
+        <v>813</v>
+      </c>
+      <c r="C122" s="151"/>
     </row>
     <row r="123" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="115">
-        <v>4</v>
-      </c>
-      <c r="B123" s="148" t="s">
-        <v>813</v>
-      </c>
-      <c r="C123" s="149"/>
-    </row>
-    <row r="124" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="124"/>
-      <c r="B124" s="118" t="s">
+      <c r="A123" s="124"/>
+      <c r="B123" s="118" t="s">
         <v>787</v>
       </c>
-      <c r="C124" s="119" t="s">
+      <c r="C123" s="119" t="s">
         <v>814</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="116"/>
+      <c r="B124" s="122" t="s">
+        <v>788</v>
+      </c>
+      <c r="C124" s="123" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="116"/>
       <c r="B125" s="122" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="C125" s="123" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="116"/>
-      <c r="B126" s="122" t="s">
-        <v>791</v>
-      </c>
-      <c r="C126" s="123" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="116"/>
-      <c r="B127" s="120" t="s">
+      <c r="B126" s="120" t="s">
         <v>793</v>
       </c>
-      <c r="C127" s="121" t="s">
+      <c r="C126" s="121" t="s">
         <v>817</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="128" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="152" t="s">
+        <v>861</v>
+      </c>
+      <c r="B128" s="153"/>
+      <c r="C128" s="154"/>
+    </row>
     <row r="129" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="152" t="s">
-        <v>861</v>
-      </c>
-      <c r="B129" s="153"/>
-      <c r="C129" s="154"/>
+      <c r="A129" s="115">
+        <v>1</v>
+      </c>
+      <c r="B129" s="155" t="s">
+        <v>862</v>
+      </c>
+      <c r="C129" s="156"/>
     </row>
     <row r="130" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="115">
-        <v>1</v>
-      </c>
-      <c r="B130" s="155" t="s">
-        <v>862</v>
-      </c>
-      <c r="C130" s="156"/>
-    </row>
-    <row r="131" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="124"/>
+      <c r="B130" s="118" t="s">
+        <v>787</v>
+      </c>
+      <c r="C130" s="119" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="124"/>
-      <c r="B131" s="118" t="s">
-        <v>787</v>
-      </c>
-      <c r="C131" s="119" t="s">
-        <v>101</v>
+      <c r="B131" s="127" t="s">
+        <v>788</v>
+      </c>
+      <c r="C131" s="128" t="s">
+        <v>811</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="124"/>
       <c r="B132" s="127" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="C132" s="128" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="124"/>
       <c r="B133" s="127" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="C133" s="128" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="124"/>
       <c r="B134" s="127" t="s">
-        <v>793</v>
-      </c>
-      <c r="C134" s="128" t="s">
-        <v>813</v>
-      </c>
+        <v>794</v>
+      </c>
+      <c r="C134" s="128"/>
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="124"/>
       <c r="B135" s="127" t="s">
-        <v>794</v>
+        <v>821</v>
       </c>
       <c r="C135" s="128"/>
     </row>
     <row r="136" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="124"/>
       <c r="B136" s="127" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="C136" s="128"/>
     </row>
     <row r="137" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="124"/>
       <c r="B137" s="127" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="C137" s="128"/>
     </row>
     <row r="138" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="124"/>
       <c r="B138" s="127" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C138" s="128"/>
     </row>
     <row r="139" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="124"/>
-      <c r="B139" s="127" t="s">
-        <v>826</v>
-      </c>
-      <c r="C139" s="128"/>
+      <c r="A139" s="116"/>
+      <c r="B139" s="122" t="s">
+        <v>827</v>
+      </c>
+      <c r="C139" s="123"/>
     </row>
     <row r="140" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="116"/>
       <c r="B140" s="122" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C140" s="123"/>
     </row>
     <row r="141" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="116"/>
       <c r="B141" s="122" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="C141" s="123"/>
     </row>
     <row r="142" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="116"/>
       <c r="B142" s="122" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C142" s="123"/>
     </row>
     <row r="143" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="116"/>
       <c r="B143" s="122" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C143" s="123"/>
     </row>
     <row r="144" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="116"/>
       <c r="B144" s="122" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C144" s="123"/>
     </row>
     <row r="145" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="116"/>
       <c r="B145" s="122" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C145" s="123"/>
     </row>
     <row r="146" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="116"/>
       <c r="B146" s="122" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C146" s="123"/>
     </row>
     <row r="147" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="116"/>
       <c r="B147" s="122" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C147" s="123"/>
     </row>
     <row r="148" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="116"/>
-      <c r="B148" s="122" t="s">
-        <v>835</v>
-      </c>
-      <c r="C148" s="123"/>
-    </row>
-    <row r="149" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="116"/>
-      <c r="B149" s="120" t="s">
+      <c r="B148" s="120" t="s">
         <v>836</v>
       </c>
-      <c r="C149" s="121"/>
+      <c r="C148" s="121"/>
+    </row>
+    <row r="149" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="116">
+        <v>2</v>
+      </c>
+      <c r="B149" s="146" t="s">
+        <v>863</v>
+      </c>
+      <c r="C149" s="147"/>
     </row>
     <row r="150" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="116">
-        <v>2</v>
-      </c>
-      <c r="B150" s="157" t="s">
-        <v>863</v>
-      </c>
-      <c r="C150" s="158"/>
-    </row>
-    <row r="151" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="116"/>
+      <c r="B150" s="118" t="s">
+        <v>787</v>
+      </c>
+      <c r="C150" s="119" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="116"/>
-      <c r="B151" s="118" t="s">
-        <v>787</v>
-      </c>
-      <c r="C151" s="119" t="s">
-        <v>241</v>
+      <c r="B151" s="122" t="s">
+        <v>788</v>
+      </c>
+      <c r="C151" s="123" t="s">
+        <v>865</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="116"/>
       <c r="B152" s="122" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="C152" s="123" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="116"/>
       <c r="B153" s="122" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="C153" s="123" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="116"/>
       <c r="B154" s="122" t="s">
-        <v>793</v>
-      </c>
-      <c r="C154" s="123" t="s">
-        <v>867</v>
-      </c>
+        <v>794</v>
+      </c>
+      <c r="C154" s="123"/>
     </row>
     <row r="155" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="116"/>
-      <c r="B155" s="122" t="s">
-        <v>794</v>
-      </c>
-      <c r="C155" s="123"/>
+      <c r="B155" s="125" t="s">
+        <v>821</v>
+      </c>
+      <c r="C155" s="126"/>
     </row>
     <row r="156" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="116"/>
       <c r="B156" s="125" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="C156" s="126"/>
     </row>
     <row r="157" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="116"/>
-      <c r="B157" s="125" t="s">
-        <v>823</v>
-      </c>
-      <c r="C157" s="126"/>
-    </row>
-    <row r="158" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="116"/>
-      <c r="B158" s="120" t="s">
+      <c r="B157" s="120" t="s">
         <v>825</v>
       </c>
-      <c r="C158" s="121"/>
+      <c r="C157" s="121"/>
+    </row>
+    <row r="158" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="116">
+        <v>3</v>
+      </c>
+      <c r="B158" s="148" t="s">
+        <v>864</v>
+      </c>
+      <c r="C158" s="149"/>
     </row>
     <row r="159" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="116">
-        <v>3</v>
-      </c>
-      <c r="B159" s="159" t="s">
-        <v>864</v>
-      </c>
-      <c r="C159" s="160"/>
-    </row>
-    <row r="160" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="116"/>
+      <c r="B159" s="118" t="s">
+        <v>787</v>
+      </c>
+      <c r="C159" s="119" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="116"/>
-      <c r="B160" s="118" t="s">
-        <v>787</v>
-      </c>
-      <c r="C160" s="119" t="s">
-        <v>869</v>
+      <c r="B160" s="122" t="s">
+        <v>788</v>
+      </c>
+      <c r="C160" s="123" t="s">
+        <v>868</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="116"/>
       <c r="B161" s="122" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="C161" s="123" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="116"/>
-      <c r="B162" s="122" t="s">
-        <v>791</v>
-      </c>
-      <c r="C162" s="123" t="s">
-        <v>870</v>
+      <c r="B162" s="125" t="s">
+        <v>793</v>
+      </c>
+      <c r="C162" s="126" t="s">
+        <v>871</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="116"/>
       <c r="B163" s="125" t="s">
-        <v>793</v>
-      </c>
-      <c r="C163" s="126" t="s">
-        <v>871</v>
-      </c>
+        <v>794</v>
+      </c>
+      <c r="C163" s="126"/>
     </row>
     <row r="164" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="116"/>
-      <c r="B164" s="125" t="s">
-        <v>794</v>
-      </c>
-      <c r="C164" s="126"/>
-    </row>
-    <row r="165" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="116"/>
-      <c r="B165" s="120" t="s">
+      <c r="B164" s="120" t="s">
         <v>821</v>
       </c>
-      <c r="C165" s="121"/>
+      <c r="C164" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="A129:C129"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B42:C42"/>
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B16:C16"/>
@@ -7108,6 +7048,48 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B158:C158"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="A128:C128"/>
+    <mergeCell ref="B129:C129"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -8306,31 +8288,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="166" t="s">
+      <c r="B1" s="164" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="167"/>
-      <c r="J1" s="168"/>
-      <c r="K1" s="169" t="s">
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
+      <c r="E1" s="165"/>
+      <c r="F1" s="165"/>
+      <c r="G1" s="165"/>
+      <c r="H1" s="165"/>
+      <c r="I1" s="165"/>
+      <c r="J1" s="166"/>
+      <c r="K1" s="167" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
-      <c r="P1" s="170"/>
-      <c r="Q1" s="170"/>
-      <c r="R1" s="170"/>
-      <c r="S1" s="170"/>
-      <c r="T1" s="170"/>
-      <c r="U1" s="170"/>
-      <c r="V1" s="171"/>
+      <c r="L1" s="168"/>
+      <c r="M1" s="168"/>
+      <c r="N1" s="168"/>
+      <c r="O1" s="168"/>
+      <c r="P1" s="168"/>
+      <c r="Q1" s="168"/>
+      <c r="R1" s="168"/>
+      <c r="S1" s="168"/>
+      <c r="T1" s="168"/>
+      <c r="U1" s="168"/>
+      <c r="V1" s="169"/>
     </row>
     <row r="2" spans="1:22" ht="44.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K2" s="66" t="s">
@@ -22482,17 +22464,17 @@
       <c r="A1" s="81" t="s">
         <v>363</v>
       </c>
-      <c r="B1" s="172" t="s">
+      <c r="B1" s="170" t="s">
         <v>365</v>
       </c>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="J1" s="174"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
+      <c r="G1" s="171"/>
+      <c r="H1" s="171"/>
+      <c r="I1" s="171"/>
+      <c r="J1" s="172"/>
       <c r="K1" s="91" t="s">
         <v>364</v>
       </c>
@@ -23228,10 +23210,10 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="83" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B39" s="48" t="s">
         <v>1026</v>
-      </c>
-      <c r="B39" s="48" t="s">
-        <v>1027</v>
       </c>
       <c r="C39" s="43" t="s">
         <v>744</v>
@@ -23244,7 +23226,7 @@
       <c r="I39" s="43"/>
       <c r="J39" s="44"/>
       <c r="K39" s="89" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="L39" s="87"/>
     </row>
@@ -23382,10 +23364,10 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="83" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B47" s="48" t="s">
         <v>1024</v>
-      </c>
-      <c r="B47" s="48" t="s">
-        <v>1025</v>
       </c>
       <c r="C47" s="43" t="s">
         <v>744</v>
@@ -23398,7 +23380,7 @@
       <c r="I47" s="43"/>
       <c r="J47" s="44"/>
       <c r="K47" s="89" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="L47" s="87"/>
     </row>
@@ -24359,15 +24341,15 @@
       <c r="C1" t="s">
         <v>700</v>
       </c>
-      <c r="E1" s="175" t="s">
+      <c r="E1" s="173" t="s">
         <v>365</v>
       </c>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
+      <c r="F1" s="173"/>
+      <c r="G1" s="173"/>
+      <c r="H1" s="173"/>
+      <c r="I1" s="173"/>
+      <c r="J1" s="173"/>
+      <c r="K1" s="173"/>
       <c r="L1" s="31"/>
     </row>
     <row r="2" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
@@ -25425,7 +25407,7 @@
         <v>983</v>
       </c>
       <c r="M55" s="134" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="N55" s="34">
         <v>3</v>
@@ -25689,7 +25671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -25723,48 +25705,48 @@
     <col min="31" max="64" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="145" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+    <row r="1" spans="1:64" s="143" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="143" t="s">
         <v>363</v>
       </c>
-      <c r="B1" s="145" t="s">
+      <c r="B1" s="143" t="s">
+        <v>999</v>
+      </c>
+      <c r="C1" s="143" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D1" s="143" t="s">
         <v>1000</v>
       </c>
-      <c r="C1" s="145" t="s">
-        <v>1021</v>
-      </c>
-      <c r="D1" s="145" t="s">
+      <c r="E1" s="143" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F1" s="143" t="s">
+        <v>1016</v>
+      </c>
+      <c r="G1" s="143" t="s">
+        <v>1004</v>
+      </c>
+      <c r="H1" s="143" t="s">
+        <v>376</v>
+      </c>
+      <c r="I1" s="143" t="s">
         <v>1001</v>
       </c>
-      <c r="E1" s="145" t="s">
-        <v>1031</v>
-      </c>
-      <c r="F1" s="145" t="s">
-        <v>1017</v>
-      </c>
-      <c r="G1" s="145" t="s">
-        <v>1005</v>
-      </c>
-      <c r="H1" s="145" t="s">
-        <v>376</v>
-      </c>
-      <c r="I1" s="145" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J1" s="145" t="s">
+      <c r="J1" s="143" t="s">
         <v>491</v>
       </c>
-      <c r="K1" s="145" t="s">
-        <v>1040</v>
-      </c>
-      <c r="L1" s="145" t="s">
+      <c r="K1" s="143" t="s">
+        <v>1039</v>
+      </c>
+      <c r="L1" s="143" t="s">
         <v>364</v>
       </c>
-      <c r="M1" s="145" t="s">
+      <c r="M1" s="143" t="s">
         <v>236</v>
       </c>
-      <c r="N1" s="145" t="s">
-        <v>1050</v>
+      <c r="N1" s="143" t="s">
+        <v>1049</v>
       </c>
       <c r="O1" s="3">
         <v>1</v>
@@ -25918,26 +25900,26 @@
       </c>
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="144" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B2" s="137" t="s">
         <v>1003</v>
       </c>
-      <c r="B2" s="137" t="s">
-        <v>1004</v>
-      </c>
       <c r="C2" s="137" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="D2" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="137" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="F2" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G2" s="137" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="H2" s="137">
         <v>3</v>
@@ -25950,48 +25932,48 @@
       </c>
       <c r="K2" s="137"/>
       <c r="L2" t="s">
+        <v>1005</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1050</v>
+      </c>
+      <c r="N2" t="s">
         <v>1006</v>
       </c>
-      <c r="M2" t="s">
-        <v>1051</v>
-      </c>
-      <c r="N2" t="s">
-        <v>1007</v>
-      </c>
       <c r="T2" t="s">
+        <v>1009</v>
+      </c>
+      <c r="V2" t="s">
         <v>1010</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>1011</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>1012</v>
       </c>
-      <c r="Z2" t="s">
-        <v>1013</v>
-      </c>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A3" s="146" t="s">
+      <c r="A3" s="144" t="s">
         <v>501</v>
       </c>
       <c r="B3" s="137" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C3" s="137" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="D3" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="137" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F3" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G3" s="137" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="H3" s="137">
         <v>5</v>
@@ -26004,13 +25986,13 @@
       </c>
       <c r="K3" s="137"/>
       <c r="L3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="M3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="N3" t="s">
         <v>1052</v>
-      </c>
-      <c r="N3" t="s">
-        <v>1053</v>
       </c>
       <c r="O3" s="138"/>
       <c r="P3" s="138"/>
@@ -26018,26 +26000,26 @@
       <c r="R3" s="138"/>
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A4" s="146" t="s">
-        <v>1008</v>
+      <c r="A4" s="144" t="s">
+        <v>1007</v>
       </c>
       <c r="B4" s="137" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C4" s="137" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="D4" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="137" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="F4" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G4" s="137" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="H4" s="137">
         <v>4</v>
@@ -26050,40 +26032,40 @@
       </c>
       <c r="K4" s="137"/>
       <c r="L4" t="s">
+        <v>1013</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1053</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1006</v>
+      </c>
+      <c r="R4" t="s">
         <v>1014</v>
       </c>
-      <c r="M4" t="s">
-        <v>1054</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1007</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="AD4" t="s">
         <v>1015</v>
       </c>
-      <c r="AD4" t="s">
-        <v>1016</v>
-      </c>
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A5" s="146" t="s">
+      <c r="A5" s="144" t="s">
         <v>493</v>
       </c>
       <c r="B5" s="137" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C5" s="137" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D5" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="137" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="F5" s="137"/>
       <c r="G5" s="137" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="H5" s="137">
         <v>4</v>
@@ -26098,13 +26080,13 @@
         <v>247</v>
       </c>
       <c r="L5" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="M5" t="s">
+        <v>1054</v>
+      </c>
+      <c r="N5" t="s">
         <v>1055</v>
-      </c>
-      <c r="N5" t="s">
-        <v>1056</v>
       </c>
       <c r="U5" s="138">
         <v>0.18</v>
@@ -26120,24 +26102,24 @@
       </c>
     </row>
     <row r="6" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A6" s="146" t="s">
+      <c r="A6" s="144" t="s">
         <v>497</v>
       </c>
       <c r="B6" s="137" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C6" s="137" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D6" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="137" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="F6" s="137"/>
       <c r="G6" s="137" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="H6" s="137">
         <v>3</v>
@@ -26146,33 +26128,33 @@
         <v>1</v>
       </c>
       <c r="J6" s="137" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="K6" s="137" t="s">
         <v>246</v>
       </c>
       <c r="L6" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="M6" s="139" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="N6" s="137" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="T6" s="138"/>
       <c r="X6" s="138"/>
       <c r="AB6" s="138"/>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A7" s="146" t="s">
+      <c r="A7" s="144" t="s">
         <v>557</v>
       </c>
       <c r="B7" s="137" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C7" s="137" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D7" s="137" t="s">
         <v>33</v>
@@ -26182,7 +26164,7 @@
       </c>
       <c r="F7" s="137"/>
       <c r="G7" s="137" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="H7" s="137">
         <v>4</v>
@@ -26194,46 +26176,46 @@
         <v>3</v>
       </c>
       <c r="K7" s="137" t="s">
+        <v>1040</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1067</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1047</v>
+      </c>
+      <c r="R7" t="s">
+        <v>1048</v>
+      </c>
+      <c r="V7" t="s">
+        <v>1048</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>1048</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A8" s="144" t="s">
         <v>1041</v>
       </c>
-      <c r="L7" t="s">
-        <v>1068</v>
-      </c>
-      <c r="M7" t="s">
-        <v>1048</v>
-      </c>
-      <c r="R7" t="s">
-        <v>1049</v>
-      </c>
-      <c r="V7" t="s">
-        <v>1049</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>1049</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A8" s="146" t="s">
+      <c r="B8" s="137" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C8" s="137" t="s">
         <v>1042</v>
       </c>
-      <c r="B8" s="137" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C8" s="137" t="s">
+      <c r="D8" s="137" t="s">
         <v>1043</v>
       </c>
-      <c r="D8" s="137" t="s">
-        <v>1044</v>
-      </c>
       <c r="E8" s="137" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F8" s="137"/>
       <c r="G8" s="137" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="H8" s="137">
         <v>0</v>
@@ -26246,10 +26228,10 @@
       </c>
       <c r="K8" s="137"/>
       <c r="L8" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="M8" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="W8">
         <v>2</v>
@@ -26262,26 +26244,26 @@
       </c>
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A9" s="146" t="s">
+      <c r="A9" s="144" t="s">
         <v>490</v>
       </c>
       <c r="B9" s="137" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C9" s="137" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D9" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="137" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="F9" s="137" t="s">
         <v>278</v>
       </c>
       <c r="G9" s="137" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="H9" s="137">
         <v>4</v>
@@ -26296,31 +26278,31 @@
         <v>246</v>
       </c>
       <c r="L9" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="M9" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A10" s="146" t="s">
+      <c r="A10" s="144" t="s">
         <v>496</v>
       </c>
       <c r="B10" s="137" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C10" s="137" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D10" s="137" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="137" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="F10" s="137"/>
       <c r="G10" s="137" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="H10" s="137">
         <v>4</v>
@@ -26335,24 +26317,24 @@
         <v>246</v>
       </c>
       <c r="L10" t="s">
+        <v>1061</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1047</v>
+      </c>
+      <c r="N10" s="139" t="s">
         <v>1062</v>
       </c>
-      <c r="M10" t="s">
-        <v>1048</v>
-      </c>
-      <c r="N10" s="139" t="s">
-        <v>1063</v>
-      </c>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A11" s="146" t="s">
+      <c r="A11" s="144" t="s">
         <v>564</v>
       </c>
       <c r="B11" s="137" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C11" s="137" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D11" s="137" t="s">
         <v>33</v>
@@ -26362,7 +26344,7 @@
       </c>
       <c r="F11" s="137"/>
       <c r="G11" s="137" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="H11" s="137">
         <v>1</v>
@@ -26377,44 +26359,44 @@
         <v>246</v>
       </c>
       <c r="L11" t="s">
+        <v>1064</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1047</v>
+      </c>
+      <c r="N11" s="139" t="s">
         <v>1065</v>
       </c>
-      <c r="M11" t="s">
+      <c r="S11" t="s">
         <v>1048</v>
       </c>
-      <c r="N11" s="139" t="s">
+      <c r="X11" t="s">
+        <v>1048</v>
+      </c>
+      <c r="AC11" t="s">
         <v>1066</v>
       </c>
-      <c r="S11" t="s">
-        <v>1049</v>
-      </c>
-      <c r="X11" t="s">
-        <v>1049</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>1067</v>
-      </c>
       <c r="AH11" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A12" s="136" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B12" s="137" t="s">
         <v>1082</v>
-      </c>
-      <c r="B12" s="137" t="s">
-        <v>1083</v>
       </c>
       <c r="C12" s="137"/>
       <c r="D12" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E12" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E12" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F12" s="137"/>
       <c r="G12" s="137" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H12" s="137">
         <v>2</v>
@@ -26425,32 +26407,32 @@
       <c r="J12" s="137"/>
       <c r="K12" s="137"/>
       <c r="L12" t="s">
+        <v>1086</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1047</v>
+      </c>
+      <c r="N12" t="s">
         <v>1087</v>
-      </c>
-      <c r="M12" t="s">
-        <v>1048</v>
-      </c>
-      <c r="N12" t="s">
-        <v>1088</v>
       </c>
     </row>
     <row r="13" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A13" s="136" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B13" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C13" s="137"/>
       <c r="D13" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E13" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E13" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F13" s="137"/>
       <c r="G13" s="137" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="H13" s="137">
         <v>1</v>
@@ -26461,34 +26443,34 @@
       <c r="J13" s="137"/>
       <c r="K13" s="137"/>
       <c r="L13" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="M13" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="N13" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="14" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A14" s="146" t="s">
+      <c r="A14" s="144" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B14" s="137" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C14" s="137" t="s">
         <v>1093</v>
       </c>
-      <c r="B14" s="137" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C14" s="137" t="s">
-        <v>1094</v>
-      </c>
       <c r="D14" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E14" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E14" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F14" s="137"/>
       <c r="G14" s="137" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H14" s="137">
         <v>3</v>
@@ -26500,37 +26482,37 @@
         <v>3</v>
       </c>
       <c r="K14" s="137" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="L14" t="s">
+        <v>1094</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1047</v>
+      </c>
+      <c r="N14" s="142" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A15" s="144" t="s">
         <v>1095</v>
       </c>
-      <c r="M14" t="s">
-        <v>1048</v>
-      </c>
-      <c r="N14" s="144" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A15" s="146" t="s">
-        <v>1096</v>
-      </c>
       <c r="B15" s="137" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C15" s="137" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D15" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E15" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E15" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F15" s="137"/>
       <c r="G15" s="137" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="H15" s="137">
         <v>3</v>
@@ -26542,37 +26524,37 @@
         <v>6</v>
       </c>
       <c r="K15" s="137" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="L15" t="s">
+        <v>1097</v>
+      </c>
+      <c r="M15" t="s">
         <v>1098</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" s="142" t="s">
         <v>1099</v>
       </c>
-      <c r="N15" s="144" t="s">
+    </row>
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A16" s="144" t="s">
         <v>1100</v>
       </c>
-    </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A16" s="146" t="s">
-        <v>1101</v>
-      </c>
       <c r="B16" s="137" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C16" s="137" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D16" s="137" t="s">
         <v>1083</v>
       </c>
-      <c r="C16" s="137" t="s">
-        <v>1094</v>
-      </c>
-      <c r="D16" s="137" t="s">
+      <c r="E16" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E16" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F16" s="137"/>
       <c r="G16" s="137" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="H16" s="137">
         <v>3</v>
@@ -26585,32 +26567,32 @@
         <v>247</v>
       </c>
       <c r="L16" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="M16" t="s">
-        <v>1048</v>
-      </c>
-      <c r="N16" s="144" t="s">
-        <v>1092</v>
+        <v>1047</v>
+      </c>
+      <c r="N16" s="142" t="s">
+        <v>1091</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="136" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="B17" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C17" s="137"/>
       <c r="D17" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E17" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E17" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F17" s="137"/>
       <c r="G17" s="137" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H17" s="137">
         <v>2</v>
@@ -26623,32 +26605,32 @@
       </c>
       <c r="K17" s="137"/>
       <c r="L17" t="s">
+        <v>1104</v>
+      </c>
+      <c r="M17" t="s">
         <v>1105</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" s="142" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="144" t="s">
         <v>1106</v>
       </c>
-      <c r="N17" s="144" t="s">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="146" t="s">
-        <v>1107</v>
-      </c>
       <c r="B18" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C18" s="137"/>
       <c r="D18" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E18" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E18" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F18" s="137"/>
       <c r="G18" s="137" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="H18" s="137">
         <v>3</v>
@@ -26659,26 +26641,26 @@
       <c r="J18" s="137"/>
       <c r="K18" s="137"/>
       <c r="L18" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="144" t="s">
         <v>1108</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="146" t="s">
-        <v>1109</v>
-      </c>
       <c r="B19" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C19" s="137"/>
       <c r="D19" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E19" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E19" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F19" s="137"/>
       <c r="G19" s="137" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="H19" s="137">
         <v>1</v>
@@ -26689,28 +26671,28 @@
       <c r="J19" s="137"/>
       <c r="K19" s="137"/>
       <c r="L19" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="144" t="s">
         <v>1111</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="146" t="s">
-        <v>1112</v>
-      </c>
       <c r="B20" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C20" s="137" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D20" s="137" t="s">
         <v>375</v>
       </c>
       <c r="E20" s="137" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="F20" s="137"/>
       <c r="G20" s="137" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="H20" s="137">
         <v>4</v>
@@ -26721,29 +26703,29 @@
       <c r="J20" s="137"/>
       <c r="K20" s="137"/>
       <c r="L20" t="s">
+        <v>1113</v>
+      </c>
+      <c r="M20" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="144" t="s">
         <v>1114</v>
       </c>
-      <c r="M20" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="146" t="s">
-        <v>1115</v>
-      </c>
       <c r="B21" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C21" s="137"/>
       <c r="D21" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E21" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E21" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F21" s="137"/>
       <c r="G21" s="137" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="H21" s="137">
         <v>4</v>
@@ -26754,32 +26736,32 @@
       <c r="J21" s="137"/>
       <c r="K21" s="137"/>
       <c r="L21" t="s">
+        <v>1115</v>
+      </c>
+      <c r="M21" t="s">
+        <v>1091</v>
+      </c>
+      <c r="N21" t="s">
         <v>1116</v>
       </c>
-      <c r="M21" t="s">
-        <v>1092</v>
-      </c>
-      <c r="N21" t="s">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="144" t="s">
         <v>1117</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="146" t="s">
-        <v>1118</v>
-      </c>
       <c r="B22" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C22" s="137"/>
       <c r="D22" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E22" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E22" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F22" s="137"/>
       <c r="G22" s="137" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H22" s="137">
         <v>3</v>
@@ -26790,26 +26772,26 @@
       <c r="J22" s="137"/>
       <c r="K22" s="137"/>
       <c r="L22" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="144" t="s">
         <v>1119</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="146" t="s">
-        <v>1120</v>
-      </c>
       <c r="B23" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C23" s="137"/>
       <c r="D23" s="137" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="E23" s="137" t="s">
         <v>422</v>
       </c>
       <c r="F23" s="137"/>
       <c r="G23" s="137" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="H23" s="137">
         <v>3</v>
@@ -26820,26 +26802,26 @@
       <c r="J23" s="137"/>
       <c r="K23" s="137"/>
       <c r="L23" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="144" t="s">
         <v>1121</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="146" t="s">
-        <v>1122</v>
-      </c>
       <c r="B24" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C24" s="137"/>
       <c r="D24" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E24" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E24" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F24" s="137"/>
       <c r="G24" s="137" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="H24" s="137">
         <v>3</v>
@@ -26850,26 +26832,26 @@
       <c r="J24" s="137"/>
       <c r="K24" s="137"/>
       <c r="L24" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="146" t="s">
-        <v>1128</v>
+      <c r="A25" s="144" t="s">
+        <v>1127</v>
       </c>
       <c r="B25" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C25" s="137"/>
       <c r="D25" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E25" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E25" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F25" s="137"/>
       <c r="G25" s="137" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="H25" s="137">
         <v>3</v>
@@ -26882,32 +26864,32 @@
       </c>
       <c r="K25" s="137"/>
       <c r="L25" t="s">
+        <v>1124</v>
+      </c>
+      <c r="M25" t="s">
         <v>1125</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>1126</v>
       </c>
-      <c r="N25" t="s">
-        <v>1127</v>
-      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="146" t="s">
-        <v>1129</v>
+      <c r="A26" s="144" t="s">
+        <v>1128</v>
       </c>
       <c r="B26" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C26" s="137"/>
       <c r="D26" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E26" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E26" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F26" s="137"/>
       <c r="G26" s="137" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="H26" s="137">
         <v>1</v>
@@ -26918,26 +26900,26 @@
       <c r="J26" s="137"/>
       <c r="K26" s="137"/>
       <c r="L26" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="144" t="s">
         <v>1130</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="146" t="s">
-        <v>1131</v>
-      </c>
       <c r="B27" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C27" s="137"/>
       <c r="D27" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E27" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E27" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F27" s="137"/>
       <c r="G27" s="137" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H27" s="137">
         <v>3</v>
@@ -26950,29 +26932,29 @@
       </c>
       <c r="K27" s="137"/>
       <c r="L27" t="s">
+        <v>1131</v>
+      </c>
+      <c r="M27" t="s">
         <v>1132</v>
       </c>
-      <c r="M27" t="s">
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="144" t="s">
         <v>1133</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="146" t="s">
-        <v>1134</v>
-      </c>
       <c r="B28" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C28" s="137"/>
       <c r="D28" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E28" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E28" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F28" s="137"/>
       <c r="G28" s="137" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="H28" s="137">
         <v>0</v>
@@ -26983,32 +26965,32 @@
       <c r="J28" s="137"/>
       <c r="K28" s="137"/>
       <c r="L28" t="s">
+        <v>1134</v>
+      </c>
+      <c r="M28" t="s">
         <v>1135</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>1136</v>
       </c>
-      <c r="N28" t="s">
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="144" t="s">
         <v>1137</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="146" t="s">
-        <v>1138</v>
-      </c>
       <c r="B29" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C29" s="137"/>
       <c r="D29" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E29" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E29" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F29" s="137"/>
       <c r="G29" s="137" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="H29" s="137">
         <v>3</v>
@@ -27021,32 +27003,32 @@
       </c>
       <c r="K29" s="137"/>
       <c r="L29" t="s">
+        <v>1138</v>
+      </c>
+      <c r="M29" t="s">
+        <v>1105</v>
+      </c>
+      <c r="N29" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="144" t="s">
         <v>1139</v>
       </c>
-      <c r="M29" t="s">
-        <v>1106</v>
-      </c>
-      <c r="N29" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="146" t="s">
-        <v>1140</v>
-      </c>
       <c r="B30" s="137" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C30" s="137"/>
       <c r="D30" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E30" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E30" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F30" s="137"/>
       <c r="G30" s="137" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H30" s="137">
         <v>3</v>
@@ -27059,29 +27041,29 @@
       </c>
       <c r="K30" s="137"/>
       <c r="L30" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="M30" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="146" t="s">
+      <c r="A31" s="144" t="s">
         <v>888</v>
       </c>
       <c r="B31" s="137" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C31" s="137"/>
       <c r="D31" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E31" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E31" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F31" s="137"/>
       <c r="G31" s="137" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="H31" s="137">
         <v>3</v>
@@ -27094,26 +27076,26 @@
       </c>
       <c r="K31" s="137"/>
       <c r="L31" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="144" t="s">
         <v>1141</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="146" t="s">
-        <v>1142</v>
-      </c>
       <c r="B32" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C32" s="137"/>
       <c r="D32" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E32" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E32" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F32" s="137"/>
       <c r="G32" s="137" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="H32" s="137">
         <v>1</v>
@@ -27124,26 +27106,26 @@
       <c r="J32" s="137"/>
       <c r="K32" s="137"/>
       <c r="L32" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="146" t="s">
-        <v>1145</v>
+      <c r="A33" s="144" t="s">
+        <v>1144</v>
       </c>
       <c r="B33" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C33" s="137"/>
       <c r="D33" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E33" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E33" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F33" s="137"/>
       <c r="G33" s="137" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H33" s="137">
         <v>0</v>
@@ -27154,26 +27136,26 @@
       <c r="J33" s="137"/>
       <c r="K33" s="137"/>
       <c r="L33" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="146" t="s">
-        <v>1146</v>
+      <c r="A34" s="144" t="s">
+        <v>1145</v>
       </c>
       <c r="B34" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C34" s="137"/>
       <c r="D34" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E34" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E34" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F34" s="137"/>
       <c r="G34" s="137" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="H34" s="137">
         <v>3</v>
@@ -27186,26 +27168,26 @@
       </c>
       <c r="K34" s="137"/>
       <c r="L34" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="146" t="s">
-        <v>1153</v>
+      <c r="A35" s="144" t="s">
+        <v>1152</v>
       </c>
       <c r="B35" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C35" s="137"/>
       <c r="D35" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E35" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E35" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F35" s="137"/>
       <c r="G35" s="137" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="H35" s="137">
         <v>0</v>
@@ -27218,26 +27200,26 @@
       </c>
       <c r="K35" s="137"/>
       <c r="L35" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="144" t="s">
         <v>1148</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="146" t="s">
-        <v>1149</v>
-      </c>
       <c r="B36" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C36" s="137"/>
       <c r="D36" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E36" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E36" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F36" s="137"/>
       <c r="G36" s="137" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H36" s="137">
         <v>0</v>
@@ -27250,26 +27232,26 @@
       </c>
       <c r="K36" s="137"/>
       <c r="L36" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="144" t="s">
         <v>1150</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="146" t="s">
-        <v>1151</v>
-      </c>
       <c r="B37" s="137" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C37" s="137"/>
       <c r="D37" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E37" s="137" t="s">
         <v>1084</v>
-      </c>
-      <c r="E37" s="137" t="s">
-        <v>1085</v>
       </c>
       <c r="F37" s="137"/>
       <c r="G37" s="137" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="H37" s="137">
         <v>3</v>
@@ -27282,26 +27264,26 @@
       </c>
       <c r="K37" s="137"/>
       <c r="L37" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="146" t="s">
+      <c r="A38" s="144" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B38" s="137" t="s">
         <v>1154</v>
-      </c>
-      <c r="B38" s="137" t="s">
-        <v>1155</v>
       </c>
       <c r="C38" s="137"/>
       <c r="D38" s="137" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="E38" s="137" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="F38" s="137"/>
       <c r="G38" s="137" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="H38" s="137">
         <v>3</v>
@@ -27314,26 +27296,26 @@
       </c>
       <c r="K38" s="137"/>
       <c r="L38" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="144" t="s">
         <v>1158</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="146" t="s">
-        <v>1159</v>
-      </c>
       <c r="B39" s="137" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="C39" s="137"/>
       <c r="D39" s="137" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="E39" s="137" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="F39" s="137"/>
       <c r="G39" s="137" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="H39" s="137">
         <v>3</v>
@@ -27350,22 +27332,22 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="146" t="s">
-        <v>1161</v>
+      <c r="A40" s="144" t="s">
+        <v>1160</v>
       </c>
       <c r="B40" s="137" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="C40" s="137"/>
       <c r="D40" s="137" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="E40" s="137" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="F40" s="137"/>
       <c r="G40" s="137" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="H40" s="137">
         <v>3</v>
@@ -27378,123 +27360,123 @@
       </c>
       <c r="K40" s="137"/>
       <c r="L40" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="144" t="s">
         <v>1163</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="146" t="s">
+      <c r="B41" s="145" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D41" s="145" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E41" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G41" s="145" t="s">
         <v>1164</v>
       </c>
-      <c r="B41" s="147" t="s">
+      <c r="H41" s="145">
+        <v>3</v>
+      </c>
+      <c r="I41" s="145">
+        <v>1</v>
+      </c>
+      <c r="J41" s="145">
+        <v>5</v>
+      </c>
+      <c r="L41" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="144" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B42" s="145" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D42" s="145" t="s">
         <v>1155</v>
       </c>
-      <c r="D41" s="147" t="s">
-        <v>1156</v>
-      </c>
-      <c r="E41" s="137" t="s">
-        <v>1085</v>
-      </c>
-      <c r="G41" s="147" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H41" s="147">
+      <c r="E42" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G42" s="145" t="s">
+        <v>1167</v>
+      </c>
+      <c r="H42" s="145">
         <v>3</v>
       </c>
-      <c r="I41" s="147">
-        <v>1</v>
-      </c>
-      <c r="J41" s="147">
-        <v>5</v>
-      </c>
-      <c r="L41" t="s">
-        <v>1166</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="146" t="s">
-        <v>1167</v>
-      </c>
-      <c r="B42" s="147" t="s">
-        <v>1155</v>
-      </c>
-      <c r="D42" s="147" t="s">
-        <v>1156</v>
-      </c>
-      <c r="E42" s="137" t="s">
-        <v>1085</v>
-      </c>
-      <c r="G42" s="147" t="s">
+      <c r="I42" s="145">
+        <v>1</v>
+      </c>
+      <c r="J42" s="145">
+        <v>0</v>
+      </c>
+      <c r="L42" t="s">
         <v>1168</v>
       </c>
-      <c r="H42" s="147">
-        <v>3</v>
-      </c>
-      <c r="I42" s="147">
-        <v>1</v>
-      </c>
-      <c r="J42" s="147">
-        <v>0</v>
-      </c>
-      <c r="L42" t="s">
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="144" t="s">
         <v>1169</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="146" t="s">
+      <c r="B43" s="145" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D43" s="145" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E43" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G43" s="145" t="s">
         <v>1170</v>
       </c>
-      <c r="B43" s="147" t="s">
+      <c r="H43" s="145">
+        <v>2</v>
+      </c>
+      <c r="I43" s="145">
+        <v>1</v>
+      </c>
+      <c r="J43" s="145">
+        <v>1</v>
+      </c>
+      <c r="L43" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="144" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B44" s="145" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D44" s="145" t="s">
         <v>1083</v>
-      </c>
-      <c r="D43" s="147" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E43" s="137" t="s">
-        <v>1085</v>
-      </c>
-      <c r="G43" s="147" t="s">
-        <v>1171</v>
-      </c>
-      <c r="H43" s="147">
-        <v>2</v>
-      </c>
-      <c r="I43" s="147">
-        <v>1</v>
-      </c>
-      <c r="J43" s="147">
-        <v>1</v>
-      </c>
-      <c r="L43" t="s">
-        <v>1172</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="146" t="s">
-        <v>1173</v>
-      </c>
-      <c r="B44" s="147" t="s">
-        <v>1083</v>
-      </c>
-      <c r="D44" s="147" t="s">
-        <v>1084</v>
       </c>
       <c r="E44" s="137" t="s">
         <v>422</v>
       </c>
-      <c r="G44" s="147" t="s">
-        <v>1102</v>
-      </c>
-      <c r="H44" s="147">
+      <c r="G44" s="145" t="s">
+        <v>1101</v>
+      </c>
+      <c r="H44" s="145">
         <v>0</v>
       </c>
-      <c r="I44" s="147">
-        <v>1</v>
-      </c>
-      <c r="J44" s="147">
+      <c r="I44" s="145">
+        <v>1</v>
+      </c>
+      <c r="J44" s="145">
         <v>4</v>
       </c>
       <c r="L44" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
   </sheetData>
@@ -27520,7 +27502,7 @@
         <v>350</v>
       </c>
       <c r="B1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -27528,7 +27510,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -27536,7 +27518,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -27552,7 +27534,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -27560,7 +27542,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -27568,7 +27550,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -27576,7 +27558,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -27584,7 +27566,7 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -27592,7 +27574,7 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -27600,7 +27582,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -27608,7 +27590,7 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -27616,7 +27598,7 @@
         <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
   </sheetData>
@@ -28364,24 +28346,24 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="100"/>
-      <c r="B1" s="165" t="s">
+      <c r="B1" s="163" t="s">
         <v>701</v>
       </c>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
       <c r="E1" s="101"/>
-      <c r="F1" s="163" t="s">
+      <c r="F1" s="161" t="s">
         <v>350</v>
       </c>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="164"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
+      <c r="K1" s="161"/>
+      <c r="L1" s="161"/>
+      <c r="M1" s="161"/>
+      <c r="N1" s="161"/>
+      <c r="O1" s="162"/>
       <c r="P1" s="30"/>
       <c r="Q1" s="30"/>
       <c r="R1" s="30"/>

</xml_diff>